<commit_message>
[Slot Doc] PC04 and PC05 are used on both QFN40 and QFN32 as ADC inputs. PC04 and PC05 could be used (to clarify) on Master as PTI (with PC06 as PTI_CLK).
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501D9068-9073-44E0-8DD9-B332F42CB512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFE1393-3DBE-4346-8FA1-C96FC09D4315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="427">
   <si>
     <t>Timing Slot EFR32x</t>
   </si>
@@ -1222,9 +1222,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>2)</t>
-  </si>
-  <si>
     <t>1)</t>
   </si>
   <si>
@@ -1280,12 +1277,6 @@
   </si>
   <si>
     <t>Single A/D</t>
-  </si>
-  <si>
-    <t>3)</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Debug/Download</t>
@@ -1344,7 +1335,28 @@
     <t>LFXTAL</t>
   </si>
   <si>
-    <t>LF 32.768kHz</t>
+    <t>Spare</t>
+  </si>
+  <si>
+    <t>P19/F9</t>
+  </si>
+  <si>
+    <t>P21/F8</t>
+  </si>
+  <si>
+    <t>VCOM RTS</t>
+  </si>
+  <si>
+    <t>VCOM CTS</t>
+  </si>
+  <si>
+    <t>Button 0</t>
+  </si>
+  <si>
+    <t>N/A (Slave)</t>
+  </si>
+  <si>
+    <t>LF 32.768kHz Is used?</t>
   </si>
 </sst>
 </file>
@@ -1957,7 +1969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2192,16 +2204,34 @@
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2210,38 +2240,41 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2250,6 +2283,81 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2294,15 +2402,6 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2312,107 +2411,28 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2442,13 +2462,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2079167</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:colOff>2247255</xdr:colOff>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2486,13 +2506,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>2009910</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:colOff>2200409</xdr:colOff>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2530,13 +2550,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2596,13 +2616,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2662,13 +2682,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2728,13 +2748,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2794,13 +2814,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>249530</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>173313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>589442</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>116163</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2860,13 +2880,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>281280</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>166963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>621192</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>109813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3490,10 +3510,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE40"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39:U40"/>
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3501,13 +3521,14 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="5"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="33.7109375" customWidth="1"/>
     <col min="10" max="10" width="1.5703125" style="87" customWidth="1"/>
     <col min="11" max="11" width="5.140625" customWidth="1"/>
     <col min="12" max="12" width="1.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" customWidth="1"/>
+    <col min="18" max="18" width="2.85546875" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.140625" customWidth="1"/>
@@ -3518,14 +3539,14 @@
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N1" s="5"/>
       <c r="AA1" s="17" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -3588,14 +3609,14 @@
         <v>54</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AD3" s="3" t="str">
         <f>Q3</f>
         <v>CPU Port</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -3611,8 +3632,8 @@
       <c r="D4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>63</v>
+      <c r="E4" s="91" t="s">
+        <v>60</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>379</v>
@@ -3620,14 +3641,14 @@
       <c r="G4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="91" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>409</v>
-      </c>
-      <c r="K4" s="90" t="s">
-        <v>387</v>
+        <v>408</v>
+      </c>
+      <c r="K4" s="89" t="s">
+        <v>388</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>59</v>
@@ -3654,17 +3675,9 @@
         <v>62</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>409</v>
-      </c>
-      <c r="V4" s="96" t="s">
-        <v>410</v>
-      </c>
-      <c r="W4" s="99" t="s">
-        <v>392</v>
-      </c>
-      <c r="X4" s="97" t="s">
-        <v>60</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="V4" s="96"/>
       <c r="Y4" s="95" t="s">
         <v>389</v>
       </c>
@@ -3685,7 +3698,7 @@
         <v>PC04</v>
       </c>
       <c r="AE4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -3701,8 +3714,8 @@
       <c r="D5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>64</v>
+      <c r="E5" s="91" t="s">
+        <v>61</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>379</v>
@@ -3710,14 +3723,14 @@
       <c r="G5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="91" t="s">
         <v>62</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>409</v>
-      </c>
-      <c r="K5" s="90" t="s">
-        <v>387</v>
+        <v>408</v>
+      </c>
+      <c r="K5" s="89" t="s">
+        <v>388</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>59</v>
@@ -3744,17 +3757,9 @@
         <v>62</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>409</v>
-      </c>
-      <c r="V5" s="96" t="s">
-        <v>390</v>
-      </c>
-      <c r="W5" s="99" t="s">
-        <v>392</v>
-      </c>
-      <c r="X5" s="97" t="s">
-        <v>61</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="V5" s="96"/>
       <c r="Y5" s="95" t="s">
         <v>389</v>
       </c>
@@ -3775,7 +3780,7 @@
         <v>PC05</v>
       </c>
       <c r="AE5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -3920,10 +3925,10 @@
       </c>
       <c r="V8" s="96"/>
       <c r="W8" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y8" s="98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -3952,7 +3957,7 @@
         <v>62</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="K9" s="90" t="s">
         <v>387</v>
@@ -3980,13 +3985,13 @@
         <v>62</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="W9" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y9" s="98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -4018,7 +4023,7 @@
         <v>62</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K11" s="89" t="s">
         <v>388</v>
@@ -4048,7 +4053,7 @@
         <v>62</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="Y11" s="95" t="s">
         <v>389</v>
@@ -4070,7 +4075,7 @@
         <v>PA01</v>
       </c>
       <c r="AE11" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -4099,7 +4104,7 @@
         <v>62</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K12" s="89" t="s">
         <v>388</v>
@@ -4129,7 +4134,7 @@
         <v>62</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="Y12" s="95" t="s">
         <v>389</v>
@@ -4151,7 +4156,7 @@
         <v>PA02</v>
       </c>
       <c r="AE12" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -4180,7 +4185,7 @@
         <v>62</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K13" s="89" t="s">
         <v>388</v>
@@ -4210,7 +4215,7 @@
         <v>62</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="Y13" s="95" t="s">
         <v>389</v>
@@ -4232,7 +4237,7 @@
         <v>PA03</v>
       </c>
       <c r="AE13" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -4263,7 +4268,9 @@
       <c r="H15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K15" s="89" t="s">
         <v>388</v>
       </c>
@@ -4291,7 +4298,9 @@
       <c r="T15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="U15" s="9"/>
+      <c r="U15" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="Y15" s="95" t="s">
         <v>389</v>
       </c>
@@ -4312,7 +4321,7 @@
         <v>PB00</v>
       </c>
       <c r="AE15" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -4389,7 +4398,7 @@
         <v>PA04</v>
       </c>
       <c r="AE16" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -4454,7 +4463,7 @@
         <v>119</v>
       </c>
       <c r="X18" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Y18" s="95" t="s">
         <v>389</v>
@@ -4476,7 +4485,7 @@
         <v>PA00</v>
       </c>
       <c r="AE18" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -4492,7 +4501,7 @@
       <c r="D19" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="91" t="s">
         <v>115</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -4501,7 +4510,7 @@
       <c r="G19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="91" t="s">
         <v>62</v>
       </c>
       <c r="I19" s="9" t="s">
@@ -4537,10 +4546,10 @@
       </c>
       <c r="V19" s="96"/>
       <c r="W19" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y19" s="98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -4761,10 +4770,10 @@
       </c>
       <c r="U23" s="91"/>
       <c r="V23" s="96" t="s">
+        <v>390</v>
+      </c>
+      <c r="W23" s="99" t="s">
         <v>391</v>
-      </c>
-      <c r="W23" s="99" t="s">
-        <v>392</v>
       </c>
       <c r="X23" s="97" t="s">
         <v>72</v>
@@ -4789,7 +4798,7 @@
         <v>PB04</v>
       </c>
       <c r="AE23" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -4850,13 +4859,13 @@
       </c>
       <c r="U25" s="9"/>
       <c r="V25" s="96" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="X25" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y25" s="98" t="s">
         <v>394</v>
-      </c>
-      <c r="Y25" s="98" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -4912,10 +4921,10 @@
       </c>
       <c r="U26" s="91"/>
       <c r="W26" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y26" s="98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -4975,10 +4984,10 @@
         <v>146</v>
       </c>
       <c r="W27" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y27" s="98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
@@ -5010,7 +5019,7 @@
         <v>62</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K29" s="89" t="s">
         <v>388</v>
@@ -5040,7 +5049,7 @@
         <v>62</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y29" s="95" t="s">
         <v>389</v>
@@ -5062,7 +5071,7 @@
         <v>PC00</v>
       </c>
       <c r="AE29" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -5073,7 +5082,7 @@
         <v>101</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>111</v>
@@ -5091,7 +5100,7 @@
         <v>62</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K30" s="89" t="s">
         <v>388</v>
@@ -5103,7 +5112,7 @@
         <v>101</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="P30" s="7" t="s">
         <v>111</v>
@@ -5121,7 +5130,7 @@
         <v>62</v>
       </c>
       <c r="U30" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y30" s="95" t="s">
         <v>389</v>
@@ -5143,7 +5152,7 @@
         <v>PC01</v>
       </c>
       <c r="AE30" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
@@ -5172,7 +5181,7 @@
         <v>62</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K31" s="89" t="s">
         <v>388</v>
@@ -5202,7 +5211,7 @@
         <v>62</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y31" s="95" t="s">
         <v>389</v>
@@ -5224,7 +5233,7 @@
         <v>PC02</v>
       </c>
       <c r="AE31" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
@@ -5232,7 +5241,7 @@
         <v>103</v>
       </c>
       <c r="B32" s="119" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C32" s="118" t="s">
         <v>46</v>
@@ -5251,7 +5260,7 @@
         <v>62</v>
       </c>
       <c r="I32" s="118" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K32" s="89" t="s">
         <v>388</v>
@@ -5260,7 +5269,7 @@
         <v>103</v>
       </c>
       <c r="N32" s="119" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O32" s="118" t="s">
         <v>46</v>
@@ -5279,11 +5288,11 @@
         <v>62</v>
       </c>
       <c r="U32" s="118" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="V32" s="96"/>
       <c r="Y32" s="98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
@@ -5291,7 +5300,7 @@
         <v>103</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>121</v>
@@ -5312,7 +5321,7 @@
         <v>62</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K33" s="89" t="s">
         <v>388</v>
@@ -5321,7 +5330,7 @@
         <v>103</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="O33" s="7" t="s">
         <v>121</v>
@@ -5342,7 +5351,7 @@
         <v>62</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="V33" s="96"/>
       <c r="W33" s="96"/>
@@ -5366,7 +5375,7 @@
         <v>PC03</v>
       </c>
       <c r="AE33" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
@@ -5388,10 +5397,10 @@
       <c r="E35" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="93" t="s">
+      <c r="F35" s="194" t="s">
         <v>379</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="93" t="s">
         <v>62</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -5429,13 +5438,13 @@
         <v>128</v>
       </c>
       <c r="W35" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="X35" s="99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y35" s="98" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
@@ -5451,13 +5460,13 @@
       <c r="D36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="93" t="s">
         <v>61</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="93" t="s">
         <v>62</v>
       </c>
       <c r="H36" s="7" t="s">
@@ -5496,11 +5505,9 @@
       <c r="U36" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="V36" s="96" t="s">
-        <v>390</v>
-      </c>
+      <c r="V36" s="96"/>
       <c r="Y36" s="98" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
@@ -5516,13 +5523,13 @@
       <c r="D37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="93" t="s">
         <v>60</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="93" t="s">
         <v>62</v>
       </c>
       <c r="H37" s="7" t="s">
@@ -5561,138 +5568,192 @@
       <c r="U37" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="V37" s="96" t="s">
-        <v>410</v>
-      </c>
+      <c r="V37" s="96"/>
       <c r="Y37" s="98" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N38" s="5"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="195" t="s">
+        <v>418</v>
+      </c>
+      <c r="B39" s="196" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="195" t="s">
         <v>129</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="195" t="s">
         <v>379</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>422</v>
+      <c r="G39" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="H39" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="I39" s="195" t="s">
+        <v>426</v>
       </c>
       <c r="K39" s="89" t="s">
         <v>388</v>
       </c>
-      <c r="M39" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="N39" s="10" t="s">
+      <c r="M39" s="195" t="s">
+        <v>418</v>
+      </c>
+      <c r="N39" s="196" t="s">
         <v>46</v>
       </c>
-      <c r="O39" s="9" t="s">
+      <c r="O39" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="P39" s="9" t="s">
+      <c r="P39" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="Q39" s="9" t="s">
+      <c r="Q39" s="195" t="s">
         <v>129</v>
       </c>
-      <c r="R39" s="9" t="s">
+      <c r="R39" s="195" t="s">
         <v>379</v>
       </c>
-      <c r="S39" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="T39" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="U39" s="9" t="s">
-        <v>422</v>
+      <c r="S39" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="T39" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="U39" s="195" t="s">
+        <v>426</v>
       </c>
       <c r="Y39" s="95" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="195" t="s">
+        <v>418</v>
+      </c>
+      <c r="B40" s="196" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="195" t="s">
         <v>130</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="195" t="s">
         <v>379</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>422</v>
+      <c r="G40" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="H40" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="I40" s="195" t="s">
+        <v>426</v>
       </c>
       <c r="K40" s="89" t="s">
         <v>388</v>
       </c>
-      <c r="M40" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="N40" s="10" t="s">
+      <c r="M40" s="195" t="s">
+        <v>418</v>
+      </c>
+      <c r="N40" s="196" t="s">
         <v>46</v>
       </c>
-      <c r="O40" s="9" t="s">
+      <c r="O40" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="P40" s="9" t="s">
+      <c r="P40" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="Q40" s="9" t="s">
+      <c r="Q40" s="195" t="s">
         <v>130</v>
       </c>
-      <c r="R40" s="9" t="s">
+      <c r="R40" s="195" t="s">
         <v>379</v>
       </c>
-      <c r="S40" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="T40" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="U40" s="9" t="s">
-        <v>422</v>
+      <c r="S40" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="T40" s="195" t="s">
+        <v>391</v>
+      </c>
+      <c r="U40" s="195" t="s">
+        <v>426</v>
       </c>
       <c r="Y40" s="95" t="s">
         <v>389</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B42" s="197"/>
+      <c r="C42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="K42" s="90" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B43" s="197"/>
+      <c r="C43" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="K43" s="90" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -5849,21 +5910,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="123"/>
-      <c r="O3" s="123"/>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="123"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="192"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="192"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -5971,45 +6032,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="181" t="s">
+      <c r="E5" s="148" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182"/>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="183"/>
-      <c r="K5" s="172" t="s">
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="150"/>
+      <c r="K5" s="152" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="189"/>
-      <c r="M5" s="189"/>
-      <c r="N5" s="189"/>
-      <c r="O5" s="173"/>
-      <c r="P5" s="172" t="s">
+      <c r="L5" s="155"/>
+      <c r="M5" s="155"/>
+      <c r="N5" s="155"/>
+      <c r="O5" s="153"/>
+      <c r="P5" s="152" t="s">
         <v>276</v>
       </c>
-      <c r="Q5" s="173"/>
-      <c r="R5" s="174" t="s">
+      <c r="Q5" s="153"/>
+      <c r="R5" s="156" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="175"/>
-      <c r="T5" s="175"/>
-      <c r="U5" s="175"/>
-      <c r="V5" s="175"/>
-      <c r="W5" s="176"/>
-      <c r="X5" s="172" t="s">
+      <c r="S5" s="157"/>
+      <c r="T5" s="157"/>
+      <c r="U5" s="157"/>
+      <c r="V5" s="157"/>
+      <c r="W5" s="158"/>
+      <c r="X5" s="152" t="s">
         <v>270</v>
       </c>
-      <c r="Y5" s="173"/>
-      <c r="Z5" s="181" t="s">
+      <c r="Y5" s="153"/>
+      <c r="Z5" s="148" t="s">
         <v>339</v>
       </c>
-      <c r="AA5" s="182"/>
-      <c r="AB5" s="182"/>
-      <c r="AC5" s="182"/>
-      <c r="AD5" s="182"/>
-      <c r="AE5" s="183"/>
+      <c r="AA5" s="149"/>
+      <c r="AB5" s="149"/>
+      <c r="AC5" s="149"/>
+      <c r="AD5" s="149"/>
+      <c r="AE5" s="150"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -6044,45 +6105,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="188" t="s">
-        <v>396</v>
-      </c>
-      <c r="F6" s="188"/>
-      <c r="G6" s="188"/>
-      <c r="H6" s="188"/>
-      <c r="I6" s="188"/>
-      <c r="J6" s="188"/>
-      <c r="K6" s="187" t="s">
+      <c r="E6" s="129" t="s">
+        <v>395</v>
+      </c>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="139" t="s">
         <v>336</v>
       </c>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187" t="s">
+      <c r="L6" s="139"/>
+      <c r="M6" s="139"/>
+      <c r="N6" s="139"/>
+      <c r="O6" s="139"/>
+      <c r="P6" s="139" t="s">
         <v>338</v>
       </c>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="188" t="s">
+      <c r="Q6" s="139"/>
+      <c r="R6" s="129" t="s">
         <v>271</v>
       </c>
-      <c r="S6" s="188"/>
-      <c r="T6" s="188"/>
-      <c r="U6" s="188"/>
-      <c r="V6" s="188"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188" t="s">
+      <c r="S6" s="129"/>
+      <c r="T6" s="129"/>
+      <c r="U6" s="129"/>
+      <c r="V6" s="129"/>
+      <c r="W6" s="129"/>
+      <c r="X6" s="129" t="s">
         <v>338</v>
       </c>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188" t="s">
-        <v>396</v>
-      </c>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="188"/>
-      <c r="AC6" s="188"/>
-      <c r="AD6" s="188"/>
-      <c r="AE6" s="188"/>
+      <c r="Y6" s="129"/>
+      <c r="Z6" s="129" t="s">
+        <v>395</v>
+      </c>
+      <c r="AA6" s="129"/>
+      <c r="AB6" s="129"/>
+      <c r="AC6" s="129"/>
+      <c r="AD6" s="129"/>
+      <c r="AE6" s="129"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -6123,29 +6184,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="180" t="s">
+      <c r="K7" s="154" t="s">
         <v>337</v>
       </c>
-      <c r="L7" s="180"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="180"/>
-      <c r="P7" s="180" t="s">
+      <c r="L7" s="154"/>
+      <c r="M7" s="154"/>
+      <c r="N7" s="154"/>
+      <c r="O7" s="154"/>
+      <c r="P7" s="154" t="s">
         <v>337</v>
       </c>
-      <c r="Q7" s="180"/>
-      <c r="R7" s="180" t="s">
+      <c r="Q7" s="154"/>
+      <c r="R7" s="154" t="s">
         <v>278</v>
       </c>
-      <c r="S7" s="180"/>
-      <c r="T7" s="180"/>
-      <c r="U7" s="180"/>
-      <c r="V7" s="180"/>
-      <c r="W7" s="180"/>
-      <c r="X7" s="180" t="s">
+      <c r="S7" s="154"/>
+      <c r="T7" s="154"/>
+      <c r="U7" s="154"/>
+      <c r="V7" s="154"/>
+      <c r="W7" s="154"/>
+      <c r="X7" s="154" t="s">
         <v>337</v>
       </c>
-      <c r="Y7" s="180"/>
+      <c r="Y7" s="154"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -6581,7 +6642,7 @@
       <c r="E14" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="128"/>
+      <c r="F14" s="193"/>
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
@@ -6609,7 +6670,7 @@
       <c r="AE14" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="128"/>
+      <c r="AF14" s="193"/>
       <c r="AG14" s="104"/>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
@@ -6652,67 +6713,67 @@
       <c r="G15" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H15" s="129" t="s">
+      <c r="H15" s="125" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="130"/>
-      <c r="J15" s="131" t="s">
+      <c r="I15" s="126"/>
+      <c r="J15" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="132"/>
-      <c r="L15" s="190"/>
-      <c r="M15" s="191"/>
-      <c r="N15" s="191"/>
-      <c r="O15" s="191"/>
-      <c r="P15" s="191"/>
-      <c r="Q15" s="191"/>
-      <c r="R15" s="191"/>
-      <c r="S15" s="191"/>
-      <c r="T15" s="191"/>
-      <c r="U15" s="191"/>
-      <c r="V15" s="191"/>
-      <c r="W15" s="191"/>
-      <c r="X15" s="191"/>
-      <c r="Y15" s="191"/>
-      <c r="Z15" s="191"/>
-      <c r="AA15" s="191"/>
-      <c r="AB15" s="191"/>
-      <c r="AC15" s="191"/>
-      <c r="AD15" s="191"/>
-      <c r="AE15" s="191"/>
-      <c r="AF15" s="192"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="121"/>
+      <c r="N15" s="121"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="121"/>
+      <c r="R15" s="121"/>
+      <c r="S15" s="121"/>
+      <c r="T15" s="121"/>
+      <c r="U15" s="121"/>
+      <c r="V15" s="121"/>
+      <c r="W15" s="121"/>
+      <c r="X15" s="121"/>
+      <c r="Y15" s="121"/>
+      <c r="Z15" s="121"/>
+      <c r="AA15" s="121"/>
+      <c r="AB15" s="121"/>
+      <c r="AC15" s="121"/>
+      <c r="AD15" s="121"/>
+      <c r="AE15" s="121"/>
+      <c r="AF15" s="122"/>
       <c r="AG15" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="AH15" s="129" t="s">
+      <c r="AH15" s="125" t="s">
         <v>279</v>
       </c>
-      <c r="AI15" s="130"/>
-      <c r="AJ15" s="131" t="s">
+      <c r="AI15" s="126"/>
+      <c r="AJ15" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AK15" s="132"/>
-      <c r="AL15" s="190"/>
-      <c r="AM15" s="191"/>
-      <c r="AN15" s="191"/>
-      <c r="AO15" s="191"/>
-      <c r="AP15" s="191"/>
-      <c r="AQ15" s="191"/>
-      <c r="AR15" s="191"/>
-      <c r="AS15" s="191"/>
-      <c r="AT15" s="191"/>
-      <c r="AU15" s="191"/>
-      <c r="AV15" s="191"/>
-      <c r="AW15" s="191"/>
-      <c r="AX15" s="191"/>
-      <c r="AY15" s="191"/>
-      <c r="AZ15" s="191"/>
-      <c r="BA15" s="191"/>
-      <c r="BB15" s="191"/>
-      <c r="BC15" s="191"/>
-      <c r="BD15" s="191"/>
-      <c r="BE15" s="191"/>
-      <c r="BF15" s="191"/>
+      <c r="AK15" s="124"/>
+      <c r="AL15" s="120"/>
+      <c r="AM15" s="121"/>
+      <c r="AN15" s="121"/>
+      <c r="AO15" s="121"/>
+      <c r="AP15" s="121"/>
+      <c r="AQ15" s="121"/>
+      <c r="AR15" s="121"/>
+      <c r="AS15" s="121"/>
+      <c r="AT15" s="121"/>
+      <c r="AU15" s="121"/>
+      <c r="AV15" s="121"/>
+      <c r="AW15" s="121"/>
+      <c r="AX15" s="121"/>
+      <c r="AY15" s="121"/>
+      <c r="AZ15" s="121"/>
+      <c r="BA15" s="121"/>
+      <c r="BB15" s="121"/>
+      <c r="BC15" s="121"/>
+      <c r="BD15" s="121"/>
+      <c r="BE15" s="121"/>
+      <c r="BF15" s="121"/>
       <c r="BG15" s="103"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -6733,33 +6794,33 @@
         <v>287</v>
       </c>
       <c r="I16" s="110"/>
-      <c r="J16" s="129" t="s">
+      <c r="J16" s="125" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="130"/>
-      <c r="L16" s="131" t="s">
+      <c r="K16" s="126"/>
+      <c r="L16" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="M16" s="132"/>
-      <c r="N16" s="190"/>
-      <c r="O16" s="191"/>
-      <c r="P16" s="191"/>
-      <c r="Q16" s="191"/>
-      <c r="R16" s="191"/>
-      <c r="S16" s="191"/>
-      <c r="T16" s="191"/>
-      <c r="U16" s="191"/>
-      <c r="V16" s="191"/>
-      <c r="W16" s="191"/>
-      <c r="X16" s="191"/>
-      <c r="Y16" s="191"/>
-      <c r="Z16" s="191"/>
-      <c r="AA16" s="191"/>
-      <c r="AB16" s="191"/>
-      <c r="AC16" s="191"/>
-      <c r="AD16" s="191"/>
-      <c r="AE16" s="191"/>
-      <c r="AF16" s="192"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="121"/>
+      <c r="Q16" s="121"/>
+      <c r="R16" s="121"/>
+      <c r="S16" s="121"/>
+      <c r="T16" s="121"/>
+      <c r="U16" s="121"/>
+      <c r="V16" s="121"/>
+      <c r="W16" s="121"/>
+      <c r="X16" s="121"/>
+      <c r="Y16" s="121"/>
+      <c r="Z16" s="121"/>
+      <c r="AA16" s="121"/>
+      <c r="AB16" s="121"/>
+      <c r="AC16" s="121"/>
+      <c r="AD16" s="121"/>
+      <c r="AE16" s="121"/>
+      <c r="AF16" s="122"/>
       <c r="AG16" s="106" t="s">
         <v>274</v>
       </c>
@@ -6767,33 +6828,33 @@
         <v>287</v>
       </c>
       <c r="AI16" s="110"/>
-      <c r="AJ16" s="129" t="s">
+      <c r="AJ16" s="125" t="s">
         <v>280</v>
       </c>
-      <c r="AK16" s="130"/>
-      <c r="AL16" s="131" t="s">
+      <c r="AK16" s="126"/>
+      <c r="AL16" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AM16" s="132"/>
-      <c r="AN16" s="190"/>
-      <c r="AO16" s="191"/>
-      <c r="AP16" s="191"/>
-      <c r="AQ16" s="191"/>
-      <c r="AR16" s="191"/>
-      <c r="AS16" s="191"/>
-      <c r="AT16" s="191"/>
-      <c r="AU16" s="191"/>
-      <c r="AV16" s="191"/>
-      <c r="AW16" s="191"/>
-      <c r="AX16" s="191"/>
-      <c r="AY16" s="191"/>
-      <c r="AZ16" s="191"/>
-      <c r="BA16" s="191"/>
-      <c r="BB16" s="191"/>
-      <c r="BC16" s="191"/>
-      <c r="BD16" s="191"/>
-      <c r="BE16" s="191"/>
-      <c r="BF16" s="191"/>
+      <c r="AM16" s="124"/>
+      <c r="AN16" s="120"/>
+      <c r="AO16" s="121"/>
+      <c r="AP16" s="121"/>
+      <c r="AQ16" s="121"/>
+      <c r="AR16" s="121"/>
+      <c r="AS16" s="121"/>
+      <c r="AT16" s="121"/>
+      <c r="AU16" s="121"/>
+      <c r="AV16" s="121"/>
+      <c r="AW16" s="121"/>
+      <c r="AX16" s="121"/>
+      <c r="AY16" s="121"/>
+      <c r="AZ16" s="121"/>
+      <c r="BA16" s="121"/>
+      <c r="BB16" s="121"/>
+      <c r="BC16" s="121"/>
+      <c r="BD16" s="121"/>
+      <c r="BE16" s="121"/>
+      <c r="BF16" s="121"/>
       <c r="BG16" s="103"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -6811,70 +6872,70 @@
         <v>274</v>
       </c>
       <c r="H17" s="100" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
       <c r="K17" s="110"/>
-      <c r="L17" s="129" t="s">
+      <c r="L17" s="125" t="s">
         <v>281</v>
       </c>
-      <c r="M17" s="130"/>
-      <c r="N17" s="131" t="s">
+      <c r="M17" s="126"/>
+      <c r="N17" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="O17" s="132"/>
-      <c r="P17" s="190"/>
-      <c r="Q17" s="191"/>
-      <c r="R17" s="191"/>
-      <c r="S17" s="191"/>
-      <c r="T17" s="191"/>
-      <c r="U17" s="191"/>
-      <c r="V17" s="191"/>
-      <c r="W17" s="191"/>
-      <c r="X17" s="191"/>
-      <c r="Y17" s="191"/>
-      <c r="Z17" s="191"/>
-      <c r="AA17" s="191"/>
-      <c r="AB17" s="191"/>
-      <c r="AC17" s="191"/>
-      <c r="AD17" s="191"/>
-      <c r="AE17" s="191"/>
-      <c r="AF17" s="192"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="120"/>
+      <c r="Q17" s="121"/>
+      <c r="R17" s="121"/>
+      <c r="S17" s="121"/>
+      <c r="T17" s="121"/>
+      <c r="U17" s="121"/>
+      <c r="V17" s="121"/>
+      <c r="W17" s="121"/>
+      <c r="X17" s="121"/>
+      <c r="Y17" s="121"/>
+      <c r="Z17" s="121"/>
+      <c r="AA17" s="121"/>
+      <c r="AB17" s="121"/>
+      <c r="AC17" s="121"/>
+      <c r="AD17" s="121"/>
+      <c r="AE17" s="121"/>
+      <c r="AF17" s="122"/>
       <c r="AG17" s="106" t="s">
         <v>274</v>
       </c>
       <c r="AH17" s="100" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AI17" s="111"/>
       <c r="AJ17" s="111"/>
       <c r="AK17" s="110"/>
-      <c r="AL17" s="129" t="s">
+      <c r="AL17" s="125" t="s">
         <v>281</v>
       </c>
-      <c r="AM17" s="130"/>
-      <c r="AN17" s="131" t="s">
+      <c r="AM17" s="126"/>
+      <c r="AN17" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AO17" s="132"/>
-      <c r="AP17" s="190"/>
-      <c r="AQ17" s="191"/>
-      <c r="AR17" s="191"/>
-      <c r="AS17" s="191"/>
-      <c r="AT17" s="191"/>
-      <c r="AU17" s="191"/>
-      <c r="AV17" s="191"/>
-      <c r="AW17" s="191"/>
-      <c r="AX17" s="191"/>
-      <c r="AY17" s="191"/>
-      <c r="AZ17" s="191"/>
-      <c r="BA17" s="191"/>
-      <c r="BB17" s="191"/>
-      <c r="BC17" s="191"/>
-      <c r="BD17" s="191"/>
-      <c r="BE17" s="191"/>
-      <c r="BF17" s="191"/>
+      <c r="AO17" s="124"/>
+      <c r="AP17" s="120"/>
+      <c r="AQ17" s="121"/>
+      <c r="AR17" s="121"/>
+      <c r="AS17" s="121"/>
+      <c r="AT17" s="121"/>
+      <c r="AU17" s="121"/>
+      <c r="AV17" s="121"/>
+      <c r="AW17" s="121"/>
+      <c r="AX17" s="121"/>
+      <c r="AY17" s="121"/>
+      <c r="AZ17" s="121"/>
+      <c r="BA17" s="121"/>
+      <c r="BB17" s="121"/>
+      <c r="BC17" s="121"/>
+      <c r="BD17" s="121"/>
+      <c r="BE17" s="121"/>
+      <c r="BF17" s="121"/>
       <c r="BG17" s="103"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -6892,7 +6953,7 @@
         <v>274</v>
       </c>
       <c r="H18" s="100" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I18" s="111"/>
       <c r="J18" s="111"/>
@@ -6902,29 +6963,29 @@
       <c r="N18" s="127" t="s">
         <v>282</v>
       </c>
-      <c r="O18" s="136"/>
-      <c r="P18" s="190"/>
-      <c r="Q18" s="191"/>
-      <c r="R18" s="191"/>
-      <c r="S18" s="191"/>
-      <c r="T18" s="191"/>
-      <c r="U18" s="191"/>
-      <c r="V18" s="191"/>
-      <c r="W18" s="191"/>
-      <c r="X18" s="191"/>
-      <c r="Y18" s="191"/>
-      <c r="Z18" s="191"/>
-      <c r="AA18" s="191"/>
-      <c r="AB18" s="191"/>
-      <c r="AC18" s="191"/>
-      <c r="AD18" s="191"/>
-      <c r="AE18" s="191"/>
-      <c r="AF18" s="192"/>
+      <c r="O18" s="128"/>
+      <c r="P18" s="120"/>
+      <c r="Q18" s="121"/>
+      <c r="R18" s="121"/>
+      <c r="S18" s="121"/>
+      <c r="T18" s="121"/>
+      <c r="U18" s="121"/>
+      <c r="V18" s="121"/>
+      <c r="W18" s="121"/>
+      <c r="X18" s="121"/>
+      <c r="Y18" s="121"/>
+      <c r="Z18" s="121"/>
+      <c r="AA18" s="121"/>
+      <c r="AB18" s="121"/>
+      <c r="AC18" s="121"/>
+      <c r="AD18" s="121"/>
+      <c r="AE18" s="121"/>
+      <c r="AF18" s="122"/>
       <c r="AG18" s="106" t="s">
         <v>274</v>
       </c>
       <c r="AH18" s="100" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AI18" s="111"/>
       <c r="AJ18" s="111"/>
@@ -6934,24 +6995,24 @@
       <c r="AN18" s="127" t="s">
         <v>282</v>
       </c>
-      <c r="AO18" s="136"/>
-      <c r="AP18" s="190"/>
-      <c r="AQ18" s="191"/>
-      <c r="AR18" s="191"/>
-      <c r="AS18" s="191"/>
-      <c r="AT18" s="191"/>
-      <c r="AU18" s="191"/>
-      <c r="AV18" s="191"/>
-      <c r="AW18" s="191"/>
-      <c r="AX18" s="191"/>
-      <c r="AY18" s="191"/>
-      <c r="AZ18" s="191"/>
-      <c r="BA18" s="191"/>
-      <c r="BB18" s="191"/>
-      <c r="BC18" s="191"/>
-      <c r="BD18" s="191"/>
-      <c r="BE18" s="191"/>
-      <c r="BF18" s="191"/>
+      <c r="AO18" s="128"/>
+      <c r="AP18" s="120"/>
+      <c r="AQ18" s="121"/>
+      <c r="AR18" s="121"/>
+      <c r="AS18" s="121"/>
+      <c r="AT18" s="121"/>
+      <c r="AU18" s="121"/>
+      <c r="AV18" s="121"/>
+      <c r="AW18" s="121"/>
+      <c r="AX18" s="121"/>
+      <c r="AY18" s="121"/>
+      <c r="AZ18" s="121"/>
+      <c r="BA18" s="121"/>
+      <c r="BB18" s="121"/>
+      <c r="BC18" s="121"/>
+      <c r="BD18" s="121"/>
+      <c r="BE18" s="121"/>
+      <c r="BF18" s="121"/>
       <c r="BG18" s="103"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -7164,7 +7225,7 @@
         <v>274</v>
       </c>
       <c r="H22" s="100" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I22" s="111"/>
       <c r="J22" s="111"/>
@@ -7177,28 +7238,28 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
       <c r="S22" s="110"/>
-      <c r="T22" s="129" t="s">
+      <c r="T22" s="125" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="130"/>
-      <c r="V22" s="131" t="s">
+      <c r="U22" s="126"/>
+      <c r="V22" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="W22" s="132"/>
-      <c r="X22" s="190"/>
-      <c r="Y22" s="191"/>
-      <c r="Z22" s="191"/>
-      <c r="AA22" s="191"/>
-      <c r="AB22" s="191"/>
-      <c r="AC22" s="191"/>
-      <c r="AD22" s="191"/>
-      <c r="AE22" s="191"/>
-      <c r="AF22" s="192"/>
+      <c r="W22" s="124"/>
+      <c r="X22" s="120"/>
+      <c r="Y22" s="121"/>
+      <c r="Z22" s="121"/>
+      <c r="AA22" s="121"/>
+      <c r="AB22" s="121"/>
+      <c r="AC22" s="121"/>
+      <c r="AD22" s="121"/>
+      <c r="AE22" s="121"/>
+      <c r="AF22" s="122"/>
       <c r="AG22" s="106" t="s">
         <v>274</v>
       </c>
       <c r="AH22" s="100" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AI22" s="111"/>
       <c r="AJ22" s="111"/>
@@ -7211,23 +7272,23 @@
       <c r="AQ22" s="111"/>
       <c r="AR22" s="111"/>
       <c r="AS22" s="110"/>
-      <c r="AT22" s="129" t="s">
+      <c r="AT22" s="125" t="s">
         <v>283</v>
       </c>
-      <c r="AU22" s="130"/>
-      <c r="AV22" s="131" t="s">
+      <c r="AU22" s="126"/>
+      <c r="AV22" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AW22" s="132"/>
-      <c r="AX22" s="190"/>
-      <c r="AY22" s="191"/>
-      <c r="AZ22" s="191"/>
-      <c r="BA22" s="191"/>
-      <c r="BB22" s="191"/>
-      <c r="BC22" s="191"/>
-      <c r="BD22" s="191"/>
-      <c r="BE22" s="191"/>
-      <c r="BF22" s="191"/>
+      <c r="AW22" s="124"/>
+      <c r="AX22" s="120"/>
+      <c r="AY22" s="121"/>
+      <c r="AZ22" s="121"/>
+      <c r="BA22" s="121"/>
+      <c r="BB22" s="121"/>
+      <c r="BC22" s="121"/>
+      <c r="BD22" s="121"/>
+      <c r="BE22" s="121"/>
+      <c r="BF22" s="121"/>
       <c r="BG22" s="103"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -7245,7 +7306,7 @@
         <v>274</v>
       </c>
       <c r="H23" s="100" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I23" s="111"/>
       <c r="J23" s="111"/>
@@ -7260,26 +7321,26 @@
       <c r="S23" s="111"/>
       <c r="T23" s="111"/>
       <c r="U23" s="110"/>
-      <c r="V23" s="129" t="s">
+      <c r="V23" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="W23" s="130"/>
-      <c r="X23" s="131" t="s">
+      <c r="W23" s="126"/>
+      <c r="X23" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="Y23" s="132"/>
-      <c r="Z23" s="190"/>
-      <c r="AA23" s="191"/>
-      <c r="AB23" s="191"/>
-      <c r="AC23" s="191"/>
-      <c r="AD23" s="191"/>
-      <c r="AE23" s="191"/>
-      <c r="AF23" s="192"/>
+      <c r="Y23" s="124"/>
+      <c r="Z23" s="120"/>
+      <c r="AA23" s="121"/>
+      <c r="AB23" s="121"/>
+      <c r="AC23" s="121"/>
+      <c r="AD23" s="121"/>
+      <c r="AE23" s="121"/>
+      <c r="AF23" s="122"/>
       <c r="AG23" s="106" t="s">
         <v>274</v>
       </c>
       <c r="AH23" s="100" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AI23" s="111"/>
       <c r="AJ23" s="111"/>
@@ -7294,21 +7355,21 @@
       <c r="AS23" s="111"/>
       <c r="AT23" s="111"/>
       <c r="AU23" s="110"/>
-      <c r="AV23" s="129" t="s">
+      <c r="AV23" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="AW23" s="130"/>
-      <c r="AX23" s="131" t="s">
+      <c r="AW23" s="126"/>
+      <c r="AX23" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AY23" s="132"/>
-      <c r="AZ23" s="190"/>
-      <c r="BA23" s="191"/>
-      <c r="BB23" s="191"/>
-      <c r="BC23" s="191"/>
-      <c r="BD23" s="191"/>
-      <c r="BE23" s="191"/>
-      <c r="BF23" s="191"/>
+      <c r="AY23" s="124"/>
+      <c r="AZ23" s="120"/>
+      <c r="BA23" s="121"/>
+      <c r="BB23" s="121"/>
+      <c r="BC23" s="121"/>
+      <c r="BD23" s="121"/>
+      <c r="BE23" s="121"/>
+      <c r="BF23" s="121"/>
       <c r="BG23" s="103"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -7326,7 +7387,7 @@
         <v>274</v>
       </c>
       <c r="H24" s="100" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I24" s="111"/>
       <c r="J24" s="111"/>
@@ -7343,24 +7404,24 @@
       <c r="U24" s="111"/>
       <c r="V24" s="111"/>
       <c r="W24" s="110"/>
-      <c r="X24" s="129" t="s">
+      <c r="X24" s="125" t="s">
         <v>285</v>
       </c>
-      <c r="Y24" s="130"/>
-      <c r="Z24" s="131" t="s">
+      <c r="Y24" s="126"/>
+      <c r="Z24" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AA24" s="132"/>
-      <c r="AB24" s="190"/>
-      <c r="AC24" s="191"/>
-      <c r="AD24" s="191"/>
-      <c r="AE24" s="191"/>
-      <c r="AF24" s="192"/>
+      <c r="AA24" s="124"/>
+      <c r="AB24" s="120"/>
+      <c r="AC24" s="121"/>
+      <c r="AD24" s="121"/>
+      <c r="AE24" s="121"/>
+      <c r="AF24" s="122"/>
       <c r="AG24" s="106" t="s">
         <v>274</v>
       </c>
       <c r="AH24" s="100" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AI24" s="111"/>
       <c r="AJ24" s="111"/>
@@ -7377,19 +7438,19 @@
       <c r="AU24" s="111"/>
       <c r="AV24" s="111"/>
       <c r="AW24" s="110"/>
-      <c r="AX24" s="129" t="s">
+      <c r="AX24" s="125" t="s">
         <v>285</v>
       </c>
-      <c r="AY24" s="130"/>
-      <c r="AZ24" s="131" t="s">
+      <c r="AY24" s="126"/>
+      <c r="AZ24" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="BA24" s="132"/>
-      <c r="BB24" s="190"/>
-      <c r="BC24" s="191"/>
-      <c r="BD24" s="191"/>
-      <c r="BE24" s="191"/>
-      <c r="BF24" s="191"/>
+      <c r="BA24" s="124"/>
+      <c r="BB24" s="120"/>
+      <c r="BC24" s="121"/>
+      <c r="BD24" s="121"/>
+      <c r="BE24" s="121"/>
+      <c r="BF24" s="121"/>
       <c r="BG24" s="103"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -7407,7 +7468,7 @@
         <v>274</v>
       </c>
       <c r="H25" s="100" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I25" s="111"/>
       <c r="J25" s="111"/>
@@ -7429,19 +7490,19 @@
       <c r="Z25" s="127" t="s">
         <v>286</v>
       </c>
-      <c r="AA25" s="136"/>
-      <c r="AB25" s="131" t="s">
+      <c r="AA25" s="128"/>
+      <c r="AB25" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AC25" s="132"/>
-      <c r="AD25" s="190"/>
-      <c r="AE25" s="191"/>
-      <c r="AF25" s="192"/>
+      <c r="AC25" s="124"/>
+      <c r="AD25" s="120"/>
+      <c r="AE25" s="121"/>
+      <c r="AF25" s="122"/>
       <c r="AG25" s="106" t="s">
         <v>274</v>
       </c>
       <c r="AH25" s="100" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AI25" s="111"/>
       <c r="AJ25" s="111"/>
@@ -7463,14 +7524,14 @@
       <c r="AZ25" s="127" t="s">
         <v>286</v>
       </c>
-      <c r="BA25" s="136"/>
-      <c r="BB25" s="131" t="s">
+      <c r="BA25" s="128"/>
+      <c r="BB25" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="BC25" s="132"/>
-      <c r="BD25" s="190"/>
-      <c r="BE25" s="191"/>
-      <c r="BF25" s="191"/>
+      <c r="BC25" s="124"/>
+      <c r="BD25" s="120"/>
+      <c r="BE25" s="121"/>
+      <c r="BF25" s="121"/>
       <c r="BG25" s="103"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -7728,29 +7789,29 @@
         <v>318</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="133" t="s">
+      <c r="E30" s="170" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="134"/>
+      <c r="F30" s="171"/>
       <c r="G30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="133" t="s">
+      <c r="H30" s="170" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="134"/>
-      <c r="J30" s="133" t="s">
+      <c r="I30" s="171"/>
+      <c r="J30" s="170" t="s">
         <v>280</v>
       </c>
-      <c r="K30" s="134"/>
-      <c r="L30" s="133" t="s">
+      <c r="K30" s="171"/>
+      <c r="L30" s="170" t="s">
         <v>281</v>
       </c>
-      <c r="M30" s="134"/>
-      <c r="N30" s="133" t="s">
+      <c r="M30" s="171"/>
+      <c r="N30" s="170" t="s">
         <v>282</v>
       </c>
-      <c r="O30" s="134"/>
+      <c r="O30" s="171"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>239</v>
@@ -7759,50 +7820,50 @@
         <v>239</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="133" t="s">
+      <c r="T30" s="170" t="s">
         <v>283</v>
       </c>
-      <c r="U30" s="134"/>
-      <c r="V30" s="133" t="s">
+      <c r="U30" s="171"/>
+      <c r="V30" s="170" t="s">
         <v>284</v>
       </c>
-      <c r="W30" s="134"/>
-      <c r="X30" s="133" t="s">
+      <c r="W30" s="171"/>
+      <c r="X30" s="170" t="s">
         <v>285</v>
       </c>
-      <c r="Y30" s="134"/>
-      <c r="Z30" s="133" t="s">
+      <c r="Y30" s="171"/>
+      <c r="Z30" s="170" t="s">
         <v>286</v>
       </c>
-      <c r="AA30" s="134"/>
-      <c r="AB30" s="137" t="s">
+      <c r="AA30" s="171"/>
+      <c r="AB30" s="144" t="s">
         <v>297</v>
       </c>
-      <c r="AC30" s="138"/>
-      <c r="AD30" s="139"/>
-      <c r="AE30" s="133" t="s">
+      <c r="AC30" s="145"/>
+      <c r="AD30" s="146"/>
+      <c r="AE30" s="170" t="s">
         <v>273</v>
       </c>
-      <c r="AF30" s="134"/>
+      <c r="AF30" s="171"/>
       <c r="AG30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="AH30" s="133" t="s">
+      <c r="AH30" s="170" t="s">
         <v>279</v>
       </c>
-      <c r="AI30" s="134"/>
-      <c r="AJ30" s="133" t="s">
+      <c r="AI30" s="171"/>
+      <c r="AJ30" s="170" t="s">
         <v>280</v>
       </c>
-      <c r="AK30" s="134"/>
-      <c r="AL30" s="133" t="s">
+      <c r="AK30" s="171"/>
+      <c r="AL30" s="170" t="s">
         <v>281</v>
       </c>
-      <c r="AM30" s="134"/>
-      <c r="AN30" s="133" t="s">
+      <c r="AM30" s="171"/>
+      <c r="AN30" s="170" t="s">
         <v>282</v>
       </c>
-      <c r="AO30" s="134"/>
+      <c r="AO30" s="171"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>239</v>
@@ -7811,27 +7872,27 @@
         <v>239</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="133" t="s">
+      <c r="AT30" s="170" t="s">
         <v>283</v>
       </c>
-      <c r="AU30" s="134"/>
-      <c r="AV30" s="133" t="s">
+      <c r="AU30" s="171"/>
+      <c r="AV30" s="170" t="s">
         <v>284</v>
       </c>
-      <c r="AW30" s="134"/>
-      <c r="AX30" s="133" t="s">
+      <c r="AW30" s="171"/>
+      <c r="AX30" s="170" t="s">
         <v>285</v>
       </c>
-      <c r="AY30" s="134"/>
-      <c r="AZ30" s="133" t="s">
+      <c r="AY30" s="171"/>
+      <c r="AZ30" s="170" t="s">
         <v>286</v>
       </c>
-      <c r="BA30" s="134"/>
-      <c r="BB30" s="137" t="s">
+      <c r="BA30" s="171"/>
+      <c r="BB30" s="144" t="s">
         <v>297</v>
       </c>
-      <c r="BC30" s="138"/>
-      <c r="BD30" s="139"/>
+      <c r="BC30" s="145"/>
+      <c r="BD30" s="146"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -7843,10 +7904,10 @@
         <v>317</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="135" t="s">
+      <c r="E31" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="F31" s="135"/>
+      <c r="F31" s="147"/>
       <c r="G31" s="22" t="s">
         <v>324</v>
       </c>
@@ -7873,10 +7934,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="135" t="s">
+      <c r="AE31" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="AF31" s="135"/>
+      <c r="AF31" s="147"/>
       <c r="AG31" s="22" t="s">
         <v>324</v>
       </c>
@@ -7986,75 +8047,75 @@
       <c r="G33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="H33" s="163" t="s">
+      <c r="H33" s="167" t="s">
         <v>319</v>
       </c>
-      <c r="I33" s="164"/>
-      <c r="J33" s="164"/>
-      <c r="K33" s="164"/>
-      <c r="L33" s="164"/>
-      <c r="M33" s="164"/>
-      <c r="N33" s="164"/>
-      <c r="O33" s="164"/>
-      <c r="P33" s="164"/>
-      <c r="Q33" s="164"/>
-      <c r="R33" s="164"/>
-      <c r="S33" s="165"/>
-      <c r="T33" s="133" t="s">
+      <c r="I33" s="168"/>
+      <c r="J33" s="168"/>
+      <c r="K33" s="168"/>
+      <c r="L33" s="168"/>
+      <c r="M33" s="168"/>
+      <c r="N33" s="168"/>
+      <c r="O33" s="168"/>
+      <c r="P33" s="168"/>
+      <c r="Q33" s="168"/>
+      <c r="R33" s="168"/>
+      <c r="S33" s="169"/>
+      <c r="T33" s="170" t="s">
         <v>275</v>
       </c>
-      <c r="U33" s="134"/>
-      <c r="V33" s="137" t="s">
+      <c r="U33" s="171"/>
+      <c r="V33" s="144" t="s">
         <v>297</v>
       </c>
-      <c r="W33" s="139"/>
-      <c r="X33" s="163" t="s">
+      <c r="W33" s="146"/>
+      <c r="X33" s="167" t="s">
         <v>319</v>
       </c>
-      <c r="Y33" s="164"/>
-      <c r="Z33" s="164"/>
-      <c r="AA33" s="164"/>
-      <c r="AB33" s="164"/>
-      <c r="AC33" s="164"/>
-      <c r="AD33" s="164"/>
-      <c r="AE33" s="165"/>
+      <c r="Y33" s="168"/>
+      <c r="Z33" s="168"/>
+      <c r="AA33" s="168"/>
+      <c r="AB33" s="168"/>
+      <c r="AC33" s="168"/>
+      <c r="AD33" s="168"/>
+      <c r="AE33" s="169"/>
       <c r="AF33" s="24" t="s">
         <v>273</v>
       </c>
       <c r="AG33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="AH33" s="163" t="s">
+      <c r="AH33" s="167" t="s">
         <v>319</v>
       </c>
-      <c r="AI33" s="164"/>
-      <c r="AJ33" s="164"/>
-      <c r="AK33" s="164"/>
-      <c r="AL33" s="164"/>
-      <c r="AM33" s="164"/>
-      <c r="AN33" s="164"/>
-      <c r="AO33" s="164"/>
-      <c r="AP33" s="164"/>
-      <c r="AQ33" s="164"/>
-      <c r="AR33" s="164"/>
-      <c r="AS33" s="165"/>
-      <c r="AT33" s="133" t="s">
+      <c r="AI33" s="168"/>
+      <c r="AJ33" s="168"/>
+      <c r="AK33" s="168"/>
+      <c r="AL33" s="168"/>
+      <c r="AM33" s="168"/>
+      <c r="AN33" s="168"/>
+      <c r="AO33" s="168"/>
+      <c r="AP33" s="168"/>
+      <c r="AQ33" s="168"/>
+      <c r="AR33" s="168"/>
+      <c r="AS33" s="169"/>
+      <c r="AT33" s="170" t="s">
         <v>275</v>
       </c>
-      <c r="AU33" s="134"/>
-      <c r="AV33" s="137" t="s">
+      <c r="AU33" s="171"/>
+      <c r="AV33" s="144" t="s">
         <v>297</v>
       </c>
-      <c r="AW33" s="139"/>
-      <c r="AX33" s="163" t="s">
+      <c r="AW33" s="146"/>
+      <c r="AX33" s="167" t="s">
         <v>319</v>
       </c>
-      <c r="AY33" s="164"/>
-      <c r="AZ33" s="164"/>
-      <c r="BA33" s="164"/>
-      <c r="BB33" s="164"/>
-      <c r="BC33" s="164"/>
-      <c r="BD33" s="165"/>
+      <c r="AY33" s="168"/>
+      <c r="AZ33" s="168"/>
+      <c r="BA33" s="168"/>
+      <c r="BB33" s="168"/>
+      <c r="BC33" s="168"/>
+      <c r="BD33" s="169"/>
       <c r="BE33" s="7"/>
       <c r="BF33" s="7"/>
       <c r="BG33" s="7"/>
@@ -8066,10 +8127,10 @@
         <v>317</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="135" t="s">
+      <c r="E34" s="147" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="135"/>
+      <c r="F34" s="147"/>
       <c r="G34" s="22" t="s">
         <v>321</v>
       </c>
@@ -8085,10 +8146,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="135" t="s">
+      <c r="T34" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="U34" s="135"/>
+      <c r="U34" s="147"/>
       <c r="V34" s="22" t="s">
         <v>325</v>
       </c>
@@ -8117,10 +8178,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="135" t="s">
+      <c r="AT34" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="AU34" s="135"/>
+      <c r="AU34" s="147"/>
       <c r="AV34" s="22" t="s">
         <v>320</v>
       </c>
@@ -8391,33 +8452,33 @@
         <v>326</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="166" t="s">
+      <c r="E39" s="162" t="s">
         <v>273</v>
       </c>
-      <c r="F39" s="167"/>
-      <c r="G39" s="168" t="s">
+      <c r="F39" s="163"/>
+      <c r="G39" s="165" t="s">
         <v>273</v>
       </c>
-      <c r="H39" s="169"/>
+      <c r="H39" s="166"/>
       <c r="I39" s="100" t="s">
         <v>319</v>
       </c>
       <c r="J39" s="127" t="s">
         <v>279</v>
       </c>
-      <c r="K39" s="136"/>
+      <c r="K39" s="128"/>
       <c r="L39" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="M39" s="136"/>
+      <c r="M39" s="128"/>
       <c r="N39" s="127" t="s">
         <v>281</v>
       </c>
-      <c r="O39" s="136"/>
+      <c r="O39" s="128"/>
       <c r="P39" s="127" t="s">
         <v>282</v>
       </c>
-      <c r="Q39" s="136"/>
+      <c r="Q39" s="128"/>
       <c r="R39" s="103"/>
       <c r="S39" s="103" t="s">
         <v>239</v>
@@ -8429,47 +8490,47 @@
       <c r="V39" s="127" t="s">
         <v>283</v>
       </c>
-      <c r="W39" s="136"/>
+      <c r="W39" s="128"/>
       <c r="X39" s="127" t="s">
         <v>284</v>
       </c>
-      <c r="Y39" s="136"/>
+      <c r="Y39" s="128"/>
       <c r="Z39" s="127" t="s">
         <v>285</v>
       </c>
-      <c r="AA39" s="136"/>
+      <c r="AA39" s="128"/>
       <c r="AB39" s="127" t="s">
         <v>286</v>
       </c>
-      <c r="AC39" s="136"/>
-      <c r="AD39" s="131" t="s">
+      <c r="AC39" s="128"/>
+      <c r="AD39" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AE39" s="171"/>
-      <c r="AF39" s="132"/>
+      <c r="AE39" s="164"/>
+      <c r="AF39" s="124"/>
       <c r="AG39" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="AH39" s="136"/>
+      <c r="AH39" s="128"/>
       <c r="AI39" s="112" t="s">
         <v>319</v>
       </c>
       <c r="AJ39" s="127" t="s">
         <v>279</v>
       </c>
-      <c r="AK39" s="136"/>
+      <c r="AK39" s="128"/>
       <c r="AL39" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="AM39" s="136"/>
+      <c r="AM39" s="128"/>
       <c r="AN39" s="127" t="s">
         <v>281</v>
       </c>
-      <c r="AO39" s="136"/>
+      <c r="AO39" s="128"/>
       <c r="AP39" s="127" t="s">
         <v>282</v>
       </c>
-      <c r="AQ39" s="136"/>
+      <c r="AQ39" s="128"/>
       <c r="AR39" s="103"/>
       <c r="AS39" s="103" t="s">
         <v>239</v>
@@ -8498,14 +8559,14 @@
         <v>351</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="170" t="s">
+      <c r="E40" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="170"/>
-      <c r="G40" s="170" t="s">
+      <c r="F40" s="140"/>
+      <c r="G40" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="H40" s="170"/>
+      <c r="H40" s="140"/>
       <c r="I40" s="113" t="s">
         <v>324</v>
       </c>
@@ -8532,10 +8593,10 @@
       <c r="AD40" s="103"/>
       <c r="AE40" s="103"/>
       <c r="AF40" s="103"/>
-      <c r="AG40" s="170" t="s">
+      <c r="AG40" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="AH40" s="170"/>
+      <c r="AH40" s="140"/>
       <c r="AI40" s="113" t="s">
         <v>328</v>
       </c>
@@ -8574,24 +8635,24 @@
       <c r="E41" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="136"/>
+      <c r="F41" s="128"/>
       <c r="G41" s="100" t="s">
         <v>319</v>
       </c>
       <c r="H41" s="127" t="s">
         <v>279</v>
       </c>
-      <c r="I41" s="136"/>
+      <c r="I41" s="128"/>
       <c r="J41" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="K41" s="136"/>
-      <c r="L41" s="166"/>
-      <c r="M41" s="167"/>
-      <c r="N41" s="168" t="s">
+      <c r="K41" s="128"/>
+      <c r="L41" s="162"/>
+      <c r="M41" s="163"/>
+      <c r="N41" s="165" t="s">
         <v>282</v>
       </c>
-      <c r="O41" s="169"/>
+      <c r="O41" s="166"/>
       <c r="P41" s="103"/>
       <c r="Q41" s="103" t="s">
         <v>239</v>
@@ -8603,47 +8664,47 @@
       <c r="T41" s="127" t="s">
         <v>283</v>
       </c>
-      <c r="U41" s="136"/>
+      <c r="U41" s="128"/>
       <c r="V41" s="127" t="s">
         <v>284</v>
       </c>
-      <c r="W41" s="136"/>
+      <c r="W41" s="128"/>
       <c r="X41" s="127" t="s">
         <v>285</v>
       </c>
-      <c r="Y41" s="136"/>
+      <c r="Y41" s="128"/>
       <c r="Z41" s="127" t="s">
         <v>286</v>
       </c>
-      <c r="AA41" s="136"/>
-      <c r="AB41" s="131" t="s">
+      <c r="AA41" s="128"/>
+      <c r="AB41" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AC41" s="171"/>
-      <c r="AD41" s="132"/>
+      <c r="AC41" s="164"/>
+      <c r="AD41" s="124"/>
       <c r="AE41" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="AF41" s="136"/>
+      <c r="AF41" s="128"/>
       <c r="AG41" s="100" t="s">
         <v>319</v>
       </c>
       <c r="AH41" s="127" t="s">
         <v>279</v>
       </c>
-      <c r="AI41" s="136"/>
+      <c r="AI41" s="128"/>
       <c r="AJ41" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="AK41" s="136"/>
+      <c r="AK41" s="128"/>
       <c r="AL41" s="127" t="s">
         <v>281</v>
       </c>
-      <c r="AM41" s="136"/>
+      <c r="AM41" s="128"/>
       <c r="AN41" s="127" t="s">
         <v>282</v>
       </c>
-      <c r="AO41" s="136"/>
+      <c r="AO41" s="128"/>
       <c r="AP41" s="103"/>
       <c r="AQ41" s="103" t="s">
         <v>239</v>
@@ -8655,24 +8716,24 @@
       <c r="AT41" s="127" t="s">
         <v>283</v>
       </c>
-      <c r="AU41" s="136"/>
+      <c r="AU41" s="128"/>
       <c r="AV41" s="127" t="s">
         <v>284</v>
       </c>
-      <c r="AW41" s="136"/>
+      <c r="AW41" s="128"/>
       <c r="AX41" s="127" t="s">
         <v>285</v>
       </c>
-      <c r="AY41" s="136"/>
+      <c r="AY41" s="128"/>
       <c r="AZ41" s="127" t="s">
         <v>286</v>
       </c>
-      <c r="BA41" s="136"/>
-      <c r="BB41" s="131" t="s">
+      <c r="BA41" s="128"/>
+      <c r="BB41" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="BC41" s="171"/>
-      <c r="BD41" s="132"/>
+      <c r="BC41" s="164"/>
+      <c r="BD41" s="124"/>
       <c r="BE41" s="103"/>
       <c r="BF41" s="103"/>
       <c r="BG41" s="103"/>
@@ -8684,10 +8745,10 @@
         <v>352</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="170" t="s">
+      <c r="E42" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="170"/>
+      <c r="F42" s="140"/>
       <c r="G42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8714,10 +8775,10 @@
       <c r="AB42" s="103"/>
       <c r="AC42" s="103"/>
       <c r="AD42" s="103"/>
-      <c r="AE42" s="170" t="s">
+      <c r="AE42" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="AF42" s="170"/>
+      <c r="AF42" s="140"/>
       <c r="AG42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8827,75 +8888,75 @@
       <c r="G44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="177" t="s">
+      <c r="H44" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="I44" s="178"/>
-      <c r="J44" s="178"/>
-      <c r="K44" s="178"/>
-      <c r="L44" s="178"/>
-      <c r="M44" s="178"/>
-      <c r="N44" s="178"/>
-      <c r="O44" s="178"/>
-      <c r="P44" s="178"/>
-      <c r="Q44" s="178"/>
-      <c r="R44" s="178"/>
-      <c r="S44" s="179"/>
-      <c r="T44" s="166" t="s">
+      <c r="I44" s="160"/>
+      <c r="J44" s="160"/>
+      <c r="K44" s="160"/>
+      <c r="L44" s="160"/>
+      <c r="M44" s="160"/>
+      <c r="N44" s="160"/>
+      <c r="O44" s="160"/>
+      <c r="P44" s="160"/>
+      <c r="Q44" s="160"/>
+      <c r="R44" s="160"/>
+      <c r="S44" s="161"/>
+      <c r="T44" s="162" t="s">
         <v>275</v>
       </c>
-      <c r="U44" s="167"/>
-      <c r="V44" s="131" t="s">
+      <c r="U44" s="163"/>
+      <c r="V44" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="W44" s="132"/>
-      <c r="X44" s="177" t="s">
+      <c r="W44" s="124"/>
+      <c r="X44" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="Y44" s="178"/>
-      <c r="Z44" s="178"/>
-      <c r="AA44" s="178"/>
-      <c r="AB44" s="178"/>
-      <c r="AC44" s="178"/>
-      <c r="AD44" s="178"/>
-      <c r="AE44" s="179"/>
+      <c r="Y44" s="160"/>
+      <c r="Z44" s="160"/>
+      <c r="AA44" s="160"/>
+      <c r="AB44" s="160"/>
+      <c r="AC44" s="160"/>
+      <c r="AD44" s="160"/>
+      <c r="AE44" s="161"/>
       <c r="AF44" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH44" s="177" t="s">
+      <c r="AH44" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="AI44" s="178"/>
-      <c r="AJ44" s="178"/>
-      <c r="AK44" s="178"/>
-      <c r="AL44" s="178"/>
-      <c r="AM44" s="178"/>
-      <c r="AN44" s="178"/>
-      <c r="AO44" s="178"/>
-      <c r="AP44" s="178"/>
-      <c r="AQ44" s="178"/>
-      <c r="AR44" s="178"/>
-      <c r="AS44" s="179"/>
+      <c r="AI44" s="160"/>
+      <c r="AJ44" s="160"/>
+      <c r="AK44" s="160"/>
+      <c r="AL44" s="160"/>
+      <c r="AM44" s="160"/>
+      <c r="AN44" s="160"/>
+      <c r="AO44" s="160"/>
+      <c r="AP44" s="160"/>
+      <c r="AQ44" s="160"/>
+      <c r="AR44" s="160"/>
+      <c r="AS44" s="161"/>
       <c r="AT44" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="AU44" s="136"/>
-      <c r="AV44" s="131" t="s">
+      <c r="AU44" s="128"/>
+      <c r="AV44" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AW44" s="132"/>
-      <c r="AX44" s="177" t="s">
+      <c r="AW44" s="124"/>
+      <c r="AX44" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="AY44" s="178"/>
-      <c r="AZ44" s="178"/>
-      <c r="BA44" s="178"/>
-      <c r="BB44" s="178"/>
-      <c r="BC44" s="178"/>
-      <c r="BD44" s="179"/>
+      <c r="AY44" s="160"/>
+      <c r="AZ44" s="160"/>
+      <c r="BA44" s="160"/>
+      <c r="BB44" s="160"/>
+      <c r="BC44" s="160"/>
+      <c r="BD44" s="161"/>
       <c r="BE44" s="103"/>
       <c r="BF44" s="103"/>
       <c r="BG44" s="103"/>
@@ -8907,10 +8968,10 @@
         <v>352</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="170" t="s">
+      <c r="E45" s="140" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="170"/>
+      <c r="F45" s="140"/>
       <c r="G45" s="113" t="s">
         <v>321</v>
       </c>
@@ -8926,10 +8987,10 @@
       <c r="Q45" s="116"/>
       <c r="R45" s="116"/>
       <c r="S45" s="103"/>
-      <c r="T45" s="170" t="s">
+      <c r="T45" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="U45" s="170"/>
+      <c r="U45" s="140"/>
       <c r="V45" s="113" t="s">
         <v>325</v>
       </c>
@@ -8958,10 +9019,10 @@
       <c r="AQ45" s="116"/>
       <c r="AR45" s="116"/>
       <c r="AS45" s="103"/>
-      <c r="AT45" s="170" t="s">
+      <c r="AT45" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="AU45" s="170"/>
+      <c r="AU45" s="140"/>
       <c r="AV45" s="113" t="s">
         <v>320</v>
       </c>
@@ -8990,70 +9051,70 @@
       <c r="F46" s="117" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="177" t="s">
+      <c r="G46" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="H46" s="178"/>
-      <c r="I46" s="178"/>
-      <c r="J46" s="178"/>
-      <c r="K46" s="178"/>
-      <c r="L46" s="178"/>
-      <c r="M46" s="178"/>
-      <c r="N46" s="178"/>
-      <c r="O46" s="178"/>
-      <c r="P46" s="178"/>
-      <c r="Q46" s="178"/>
-      <c r="R46" s="178"/>
-      <c r="S46" s="178"/>
-      <c r="T46" s="178"/>
-      <c r="U46" s="178"/>
-      <c r="V46" s="178"/>
-      <c r="W46" s="178"/>
-      <c r="X46" s="178"/>
-      <c r="Y46" s="178"/>
-      <c r="Z46" s="178"/>
-      <c r="AA46" s="178"/>
-      <c r="AB46" s="178"/>
-      <c r="AC46" s="178"/>
-      <c r="AD46" s="178"/>
-      <c r="AE46" s="179"/>
+      <c r="H46" s="160"/>
+      <c r="I46" s="160"/>
+      <c r="J46" s="160"/>
+      <c r="K46" s="160"/>
+      <c r="L46" s="160"/>
+      <c r="M46" s="160"/>
+      <c r="N46" s="160"/>
+      <c r="O46" s="160"/>
+      <c r="P46" s="160"/>
+      <c r="Q46" s="160"/>
+      <c r="R46" s="160"/>
+      <c r="S46" s="160"/>
+      <c r="T46" s="160"/>
+      <c r="U46" s="160"/>
+      <c r="V46" s="160"/>
+      <c r="W46" s="160"/>
+      <c r="X46" s="160"/>
+      <c r="Y46" s="160"/>
+      <c r="Z46" s="160"/>
+      <c r="AA46" s="160"/>
+      <c r="AB46" s="160"/>
+      <c r="AC46" s="160"/>
+      <c r="AD46" s="160"/>
+      <c r="AE46" s="161"/>
       <c r="AF46" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG46" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH46" s="177" t="s">
+      <c r="AH46" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="AI46" s="178"/>
-      <c r="AJ46" s="178"/>
-      <c r="AK46" s="178"/>
-      <c r="AL46" s="178"/>
-      <c r="AM46" s="178"/>
-      <c r="AN46" s="178"/>
-      <c r="AO46" s="178"/>
-      <c r="AP46" s="178"/>
-      <c r="AQ46" s="178"/>
-      <c r="AR46" s="178"/>
-      <c r="AS46" s="179"/>
+      <c r="AI46" s="160"/>
+      <c r="AJ46" s="160"/>
+      <c r="AK46" s="160"/>
+      <c r="AL46" s="160"/>
+      <c r="AM46" s="160"/>
+      <c r="AN46" s="160"/>
+      <c r="AO46" s="160"/>
+      <c r="AP46" s="160"/>
+      <c r="AQ46" s="160"/>
+      <c r="AR46" s="160"/>
+      <c r="AS46" s="161"/>
       <c r="AT46" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="AU46" s="136"/>
-      <c r="AV46" s="131" t="s">
+      <c r="AU46" s="128"/>
+      <c r="AV46" s="123" t="s">
         <v>297</v>
       </c>
-      <c r="AW46" s="132"/>
-      <c r="AX46" s="177" t="s">
+      <c r="AW46" s="124"/>
+      <c r="AX46" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="AY46" s="178"/>
-      <c r="AZ46" s="178"/>
-      <c r="BA46" s="178"/>
-      <c r="BB46" s="178"/>
-      <c r="BC46" s="178"/>
-      <c r="BD46" s="179"/>
+      <c r="AY46" s="160"/>
+      <c r="AZ46" s="160"/>
+      <c r="BA46" s="160"/>
+      <c r="BB46" s="160"/>
+      <c r="BC46" s="160"/>
+      <c r="BD46" s="161"/>
       <c r="BE46" s="103"/>
       <c r="BF46" s="103"/>
       <c r="BG46" s="103"/>
@@ -9110,10 +9171,10 @@
       <c r="AQ47" s="116"/>
       <c r="AR47" s="116"/>
       <c r="AS47" s="103"/>
-      <c r="AT47" s="170" t="s">
+      <c r="AT47" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="AU47" s="170"/>
+      <c r="AU47" s="140"/>
       <c r="AV47" s="113" t="s">
         <v>320</v>
       </c>
@@ -9504,20 +9565,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="124" t="s">
+      <c r="E54" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="125"/>
-      <c r="G54" s="125"/>
-      <c r="H54" s="125"/>
-      <c r="I54" s="125"/>
-      <c r="J54" s="125"/>
-      <c r="K54" s="126"/>
-      <c r="L54" s="124" t="s">
+      <c r="F54" s="131"/>
+      <c r="G54" s="131"/>
+      <c r="H54" s="131"/>
+      <c r="I54" s="131"/>
+      <c r="J54" s="131"/>
+      <c r="K54" s="151"/>
+      <c r="L54" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="125"/>
-      <c r="N54" s="193"/>
+      <c r="M54" s="131"/>
+      <c r="N54" s="132"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -9638,20 +9699,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="184" t="s">
+      <c r="E56" s="133" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="186"/>
-      <c r="G56" s="186"/>
-      <c r="H56" s="186"/>
-      <c r="I56" s="186"/>
-      <c r="J56" s="186"/>
-      <c r="K56" s="185"/>
-      <c r="L56" s="184" t="s">
+      <c r="F56" s="134"/>
+      <c r="G56" s="134"/>
+      <c r="H56" s="134"/>
+      <c r="I56" s="134"/>
+      <c r="J56" s="134"/>
+      <c r="K56" s="135"/>
+      <c r="L56" s="133" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="186"/>
-      <c r="N56" s="185"/>
+      <c r="M56" s="134"/>
+      <c r="N56" s="135"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -12123,68 +12184,68 @@
         <v>364</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="124" t="s">
+      <c r="E95" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="125"/>
-      <c r="G95" s="125"/>
-      <c r="H95" s="125"/>
-      <c r="I95" s="125"/>
-      <c r="J95" s="125"/>
-      <c r="K95" s="126"/>
-      <c r="L95" s="124" t="s">
+      <c r="F95" s="131"/>
+      <c r="G95" s="131"/>
+      <c r="H95" s="131"/>
+      <c r="I95" s="131"/>
+      <c r="J95" s="131"/>
+      <c r="K95" s="151"/>
+      <c r="L95" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="125"/>
-      <c r="N95" s="126"/>
-      <c r="O95" s="160" t="s">
+      <c r="M95" s="131"/>
+      <c r="N95" s="151"/>
+      <c r="O95" s="141" t="s">
         <v>260</v>
       </c>
-      <c r="P95" s="161"/>
-      <c r="Q95" s="161"/>
-      <c r="R95" s="161"/>
-      <c r="S95" s="161"/>
-      <c r="T95" s="162"/>
-      <c r="U95" s="160" t="s">
+      <c r="P95" s="142"/>
+      <c r="Q95" s="142"/>
+      <c r="R95" s="142"/>
+      <c r="S95" s="142"/>
+      <c r="T95" s="143"/>
+      <c r="U95" s="141" t="s">
         <v>260</v>
       </c>
-      <c r="V95" s="161"/>
-      <c r="W95" s="161"/>
-      <c r="X95" s="161"/>
-      <c r="Y95" s="161"/>
-      <c r="Z95" s="161"/>
-      <c r="AA95" s="161"/>
-      <c r="AB95" s="162"/>
-      <c r="AC95" s="160" t="s">
+      <c r="V95" s="142"/>
+      <c r="W95" s="142"/>
+      <c r="X95" s="142"/>
+      <c r="Y95" s="142"/>
+      <c r="Z95" s="142"/>
+      <c r="AA95" s="142"/>
+      <c r="AB95" s="143"/>
+      <c r="AC95" s="141" t="s">
         <v>260</v>
       </c>
-      <c r="AD95" s="161"/>
-      <c r="AE95" s="161"/>
-      <c r="AF95" s="161"/>
-      <c r="AG95" s="161"/>
-      <c r="AH95" s="161"/>
-      <c r="AI95" s="161"/>
-      <c r="AJ95" s="162"/>
-      <c r="AK95" s="160" t="s">
+      <c r="AD95" s="142"/>
+      <c r="AE95" s="142"/>
+      <c r="AF95" s="142"/>
+      <c r="AG95" s="142"/>
+      <c r="AH95" s="142"/>
+      <c r="AI95" s="142"/>
+      <c r="AJ95" s="143"/>
+      <c r="AK95" s="141" t="s">
         <v>260</v>
       </c>
-      <c r="AL95" s="161"/>
-      <c r="AM95" s="161"/>
-      <c r="AN95" s="161"/>
-      <c r="AO95" s="161"/>
-      <c r="AP95" s="161"/>
-      <c r="AQ95" s="161"/>
-      <c r="AR95" s="162"/>
-      <c r="AS95" s="157" t="s">
+      <c r="AL95" s="142"/>
+      <c r="AM95" s="142"/>
+      <c r="AN95" s="142"/>
+      <c r="AO95" s="142"/>
+      <c r="AP95" s="142"/>
+      <c r="AQ95" s="142"/>
+      <c r="AR95" s="143"/>
+      <c r="AS95" s="186" t="s">
         <v>356</v>
       </c>
-      <c r="AT95" s="158"/>
-      <c r="AU95" s="158"/>
-      <c r="AV95" s="158"/>
-      <c r="AW95" s="158"/>
-      <c r="AX95" s="158"/>
-      <c r="AY95" s="158"/>
-      <c r="AZ95" s="159"/>
+      <c r="AT95" s="187"/>
+      <c r="AU95" s="187"/>
+      <c r="AV95" s="187"/>
+      <c r="AW95" s="187"/>
+      <c r="AX95" s="187"/>
+      <c r="AY95" s="187"/>
+      <c r="AZ95" s="188"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -12289,68 +12350,68 @@
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="184" t="s">
+      <c r="E97" s="133" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="186"/>
-      <c r="G97" s="186"/>
-      <c r="H97" s="186"/>
-      <c r="I97" s="186"/>
-      <c r="J97" s="186"/>
-      <c r="K97" s="185"/>
-      <c r="L97" s="184" t="s">
+      <c r="F97" s="134"/>
+      <c r="G97" s="134"/>
+      <c r="H97" s="134"/>
+      <c r="I97" s="134"/>
+      <c r="J97" s="134"/>
+      <c r="K97" s="135"/>
+      <c r="L97" s="133" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="186"/>
-      <c r="N97" s="186"/>
-      <c r="O97" s="184" t="s">
+      <c r="M97" s="134"/>
+      <c r="N97" s="134"/>
+      <c r="O97" s="133" t="s">
         <v>272</v>
       </c>
-      <c r="P97" s="186"/>
-      <c r="Q97" s="186"/>
-      <c r="R97" s="186"/>
-      <c r="S97" s="186"/>
-      <c r="T97" s="185"/>
-      <c r="U97" s="184" t="s">
+      <c r="P97" s="134"/>
+      <c r="Q97" s="134"/>
+      <c r="R97" s="134"/>
+      <c r="S97" s="134"/>
+      <c r="T97" s="135"/>
+      <c r="U97" s="133" t="s">
         <v>229</v>
       </c>
-      <c r="V97" s="186"/>
-      <c r="W97" s="186"/>
-      <c r="X97" s="186"/>
-      <c r="Y97" s="186"/>
-      <c r="Z97" s="186"/>
-      <c r="AA97" s="186"/>
-      <c r="AB97" s="185"/>
-      <c r="AC97" s="184" t="s">
+      <c r="V97" s="134"/>
+      <c r="W97" s="134"/>
+      <c r="X97" s="134"/>
+      <c r="Y97" s="134"/>
+      <c r="Z97" s="134"/>
+      <c r="AA97" s="134"/>
+      <c r="AB97" s="135"/>
+      <c r="AC97" s="133" t="s">
         <v>229</v>
       </c>
-      <c r="AD97" s="186"/>
-      <c r="AE97" s="186"/>
-      <c r="AF97" s="186"/>
-      <c r="AG97" s="186"/>
-      <c r="AH97" s="186"/>
-      <c r="AI97" s="186"/>
-      <c r="AJ97" s="185"/>
-      <c r="AK97" s="184" t="s">
+      <c r="AD97" s="134"/>
+      <c r="AE97" s="134"/>
+      <c r="AF97" s="134"/>
+      <c r="AG97" s="134"/>
+      <c r="AH97" s="134"/>
+      <c r="AI97" s="134"/>
+      <c r="AJ97" s="135"/>
+      <c r="AK97" s="133" t="s">
         <v>229</v>
       </c>
-      <c r="AL97" s="186"/>
-      <c r="AM97" s="186"/>
-      <c r="AN97" s="186"/>
-      <c r="AO97" s="186"/>
-      <c r="AP97" s="186"/>
-      <c r="AQ97" s="186"/>
-      <c r="AR97" s="185"/>
-      <c r="AS97" s="186" t="s">
+      <c r="AL97" s="134"/>
+      <c r="AM97" s="134"/>
+      <c r="AN97" s="134"/>
+      <c r="AO97" s="134"/>
+      <c r="AP97" s="134"/>
+      <c r="AQ97" s="134"/>
+      <c r="AR97" s="135"/>
+      <c r="AS97" s="134" t="s">
         <v>229</v>
       </c>
-      <c r="AT97" s="186"/>
-      <c r="AU97" s="186"/>
-      <c r="AV97" s="186"/>
-      <c r="AW97" s="186"/>
-      <c r="AX97" s="186"/>
-      <c r="AY97" s="186"/>
-      <c r="AZ97" s="185"/>
+      <c r="AT97" s="134"/>
+      <c r="AU97" s="134"/>
+      <c r="AV97" s="134"/>
+      <c r="AW97" s="134"/>
+      <c r="AX97" s="134"/>
+      <c r="AY97" s="134"/>
+      <c r="AZ97" s="135"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -12425,68 +12486,68 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="151" t="s">
-        <v>403</v>
-      </c>
-      <c r="F99" s="152"/>
-      <c r="G99" s="152"/>
-      <c r="H99" s="152"/>
-      <c r="I99" s="152"/>
-      <c r="J99" s="152"/>
-      <c r="K99" s="153"/>
-      <c r="L99" s="154" t="s">
+      <c r="E99" s="183" t="s">
+        <v>402</v>
+      </c>
+      <c r="F99" s="184"/>
+      <c r="G99" s="184"/>
+      <c r="H99" s="184"/>
+      <c r="I99" s="184"/>
+      <c r="J99" s="184"/>
+      <c r="K99" s="185"/>
+      <c r="L99" s="136" t="s">
         <v>246</v>
       </c>
-      <c r="M99" s="155"/>
-      <c r="N99" s="156"/>
-      <c r="O99" s="148" t="s">
+      <c r="M99" s="137"/>
+      <c r="N99" s="138"/>
+      <c r="O99" s="180" t="s">
         <v>235</v>
       </c>
-      <c r="P99" s="149"/>
-      <c r="Q99" s="149"/>
-      <c r="R99" s="149"/>
-      <c r="S99" s="149"/>
-      <c r="T99" s="150"/>
-      <c r="U99" s="148" t="s">
+      <c r="P99" s="181"/>
+      <c r="Q99" s="181"/>
+      <c r="R99" s="181"/>
+      <c r="S99" s="181"/>
+      <c r="T99" s="182"/>
+      <c r="U99" s="180" t="s">
         <v>235</v>
       </c>
-      <c r="V99" s="149"/>
-      <c r="W99" s="149"/>
-      <c r="X99" s="149"/>
-      <c r="Y99" s="149"/>
-      <c r="Z99" s="149"/>
-      <c r="AA99" s="149"/>
-      <c r="AB99" s="150"/>
-      <c r="AC99" s="148" t="s">
+      <c r="V99" s="181"/>
+      <c r="W99" s="181"/>
+      <c r="X99" s="181"/>
+      <c r="Y99" s="181"/>
+      <c r="Z99" s="181"/>
+      <c r="AA99" s="181"/>
+      <c r="AB99" s="182"/>
+      <c r="AC99" s="180" t="s">
         <v>235</v>
       </c>
-      <c r="AD99" s="149"/>
-      <c r="AE99" s="149"/>
-      <c r="AF99" s="149"/>
-      <c r="AG99" s="149"/>
-      <c r="AH99" s="149"/>
-      <c r="AI99" s="149"/>
-      <c r="AJ99" s="150"/>
-      <c r="AK99" s="148" t="s">
+      <c r="AD99" s="181"/>
+      <c r="AE99" s="181"/>
+      <c r="AF99" s="181"/>
+      <c r="AG99" s="181"/>
+      <c r="AH99" s="181"/>
+      <c r="AI99" s="181"/>
+      <c r="AJ99" s="182"/>
+      <c r="AK99" s="180" t="s">
         <v>235</v>
       </c>
-      <c r="AL99" s="149"/>
-      <c r="AM99" s="149"/>
-      <c r="AN99" s="149"/>
-      <c r="AO99" s="149"/>
-      <c r="AP99" s="149"/>
-      <c r="AQ99" s="149"/>
-      <c r="AR99" s="150"/>
-      <c r="AS99" s="148" t="s">
+      <c r="AL99" s="181"/>
+      <c r="AM99" s="181"/>
+      <c r="AN99" s="181"/>
+      <c r="AO99" s="181"/>
+      <c r="AP99" s="181"/>
+      <c r="AQ99" s="181"/>
+      <c r="AR99" s="182"/>
+      <c r="AS99" s="180" t="s">
         <v>301</v>
       </c>
-      <c r="AT99" s="149"/>
-      <c r="AU99" s="149"/>
-      <c r="AV99" s="149"/>
-      <c r="AW99" s="149"/>
-      <c r="AX99" s="149"/>
-      <c r="AY99" s="149"/>
-      <c r="AZ99" s="150"/>
+      <c r="AT99" s="181"/>
+      <c r="AU99" s="181"/>
+      <c r="AV99" s="181"/>
+      <c r="AW99" s="181"/>
+      <c r="AX99" s="181"/>
+      <c r="AY99" s="181"/>
+      <c r="AZ99" s="182"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -12628,68 +12689,68 @@
         <v>367</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="124" t="s">
+      <c r="E102" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="125"/>
-      <c r="G102" s="125"/>
-      <c r="H102" s="125"/>
-      <c r="I102" s="125"/>
-      <c r="J102" s="125"/>
-      <c r="K102" s="126"/>
-      <c r="L102" s="124" t="s">
+      <c r="F102" s="131"/>
+      <c r="G102" s="131"/>
+      <c r="H102" s="131"/>
+      <c r="I102" s="131"/>
+      <c r="J102" s="131"/>
+      <c r="K102" s="151"/>
+      <c r="L102" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="M102" s="125"/>
-      <c r="N102" s="126"/>
-      <c r="O102" s="124" t="s">
+      <c r="M102" s="131"/>
+      <c r="N102" s="151"/>
+      <c r="O102" s="130" t="s">
         <v>232</v>
       </c>
-      <c r="P102" s="125"/>
-      <c r="Q102" s="125"/>
-      <c r="R102" s="126"/>
-      <c r="S102" s="124" t="s">
+      <c r="P102" s="131"/>
+      <c r="Q102" s="131"/>
+      <c r="R102" s="151"/>
+      <c r="S102" s="130" t="s">
         <v>306</v>
       </c>
-      <c r="T102" s="125"/>
-      <c r="U102" s="125"/>
-      <c r="V102" s="125"/>
-      <c r="W102" s="125"/>
-      <c r="X102" s="125"/>
-      <c r="Y102" s="125"/>
-      <c r="Z102" s="125"/>
-      <c r="AA102" s="125"/>
-      <c r="AB102" s="125"/>
-      <c r="AC102" s="125"/>
-      <c r="AD102" s="126"/>
-      <c r="AE102" s="124" t="s">
+      <c r="T102" s="131"/>
+      <c r="U102" s="131"/>
+      <c r="V102" s="131"/>
+      <c r="W102" s="131"/>
+      <c r="X102" s="131"/>
+      <c r="Y102" s="131"/>
+      <c r="Z102" s="131"/>
+      <c r="AA102" s="131"/>
+      <c r="AB102" s="131"/>
+      <c r="AC102" s="131"/>
+      <c r="AD102" s="151"/>
+      <c r="AE102" s="130" t="s">
         <v>307</v>
       </c>
-      <c r="AF102" s="125"/>
-      <c r="AG102" s="125"/>
-      <c r="AH102" s="125"/>
-      <c r="AI102" s="125"/>
-      <c r="AJ102" s="125"/>
-      <c r="AK102" s="125"/>
-      <c r="AL102" s="125"/>
-      <c r="AM102" s="125"/>
-      <c r="AN102" s="125"/>
-      <c r="AO102" s="125"/>
-      <c r="AP102" s="126"/>
-      <c r="AQ102" s="124" t="s">
+      <c r="AF102" s="131"/>
+      <c r="AG102" s="131"/>
+      <c r="AH102" s="131"/>
+      <c r="AI102" s="131"/>
+      <c r="AJ102" s="131"/>
+      <c r="AK102" s="131"/>
+      <c r="AL102" s="131"/>
+      <c r="AM102" s="131"/>
+      <c r="AN102" s="131"/>
+      <c r="AO102" s="131"/>
+      <c r="AP102" s="151"/>
+      <c r="AQ102" s="130" t="s">
         <v>224</v>
       </c>
-      <c r="AR102" s="126"/>
-      <c r="AS102" s="124" t="s">
+      <c r="AR102" s="151"/>
+      <c r="AS102" s="130" t="s">
         <v>234</v>
       </c>
-      <c r="AT102" s="125"/>
-      <c r="AU102" s="125"/>
-      <c r="AV102" s="125"/>
-      <c r="AW102" s="125"/>
-      <c r="AX102" s="125"/>
-      <c r="AY102" s="125"/>
-      <c r="AZ102" s="126"/>
+      <c r="AT102" s="131"/>
+      <c r="AU102" s="131"/>
+      <c r="AV102" s="131"/>
+      <c r="AW102" s="131"/>
+      <c r="AX102" s="131"/>
+      <c r="AY102" s="131"/>
+      <c r="AZ102" s="151"/>
       <c r="BA102" s="42"/>
       <c r="BB102" s="42"/>
       <c r="BC102" s="42"/>
@@ -12792,68 +12853,68 @@
       <c r="B104" s="42"/>
       <c r="C104" s="42"/>
       <c r="D104" s="42"/>
-      <c r="E104" s="184" t="s">
+      <c r="E104" s="133" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="186"/>
-      <c r="G104" s="186"/>
-      <c r="H104" s="186"/>
-      <c r="I104" s="186"/>
-      <c r="J104" s="186"/>
-      <c r="K104" s="185"/>
-      <c r="L104" s="184" t="s">
+      <c r="F104" s="134"/>
+      <c r="G104" s="134"/>
+      <c r="H104" s="134"/>
+      <c r="I104" s="134"/>
+      <c r="J104" s="134"/>
+      <c r="K104" s="135"/>
+      <c r="L104" s="133" t="s">
         <v>226</v>
       </c>
-      <c r="M104" s="186"/>
-      <c r="N104" s="185"/>
-      <c r="O104" s="184" t="s">
+      <c r="M104" s="134"/>
+      <c r="N104" s="135"/>
+      <c r="O104" s="133" t="s">
         <v>227</v>
       </c>
-      <c r="P104" s="186"/>
-      <c r="Q104" s="186"/>
-      <c r="R104" s="185"/>
-      <c r="S104" s="184" t="s">
+      <c r="P104" s="134"/>
+      <c r="Q104" s="134"/>
+      <c r="R104" s="135"/>
+      <c r="S104" s="133" t="s">
         <v>228</v>
       </c>
-      <c r="T104" s="186"/>
-      <c r="U104" s="186"/>
-      <c r="V104" s="186"/>
-      <c r="W104" s="186"/>
-      <c r="X104" s="186"/>
-      <c r="Y104" s="186"/>
-      <c r="Z104" s="186"/>
-      <c r="AA104" s="186"/>
-      <c r="AB104" s="186"/>
-      <c r="AC104" s="186"/>
-      <c r="AD104" s="185"/>
-      <c r="AE104" s="184" t="s">
+      <c r="T104" s="134"/>
+      <c r="U104" s="134"/>
+      <c r="V104" s="134"/>
+      <c r="W104" s="134"/>
+      <c r="X104" s="134"/>
+      <c r="Y104" s="134"/>
+      <c r="Z104" s="134"/>
+      <c r="AA104" s="134"/>
+      <c r="AB104" s="134"/>
+      <c r="AC104" s="134"/>
+      <c r="AD104" s="135"/>
+      <c r="AE104" s="133" t="s">
         <v>228</v>
       </c>
-      <c r="AF104" s="186"/>
-      <c r="AG104" s="186"/>
-      <c r="AH104" s="186"/>
-      <c r="AI104" s="186"/>
-      <c r="AJ104" s="186"/>
-      <c r="AK104" s="186"/>
-      <c r="AL104" s="186"/>
-      <c r="AM104" s="186"/>
-      <c r="AN104" s="186"/>
-      <c r="AO104" s="186"/>
-      <c r="AP104" s="185"/>
-      <c r="AQ104" s="184" t="s">
+      <c r="AF104" s="134"/>
+      <c r="AG104" s="134"/>
+      <c r="AH104" s="134"/>
+      <c r="AI104" s="134"/>
+      <c r="AJ104" s="134"/>
+      <c r="AK104" s="134"/>
+      <c r="AL104" s="134"/>
+      <c r="AM104" s="134"/>
+      <c r="AN104" s="134"/>
+      <c r="AO104" s="134"/>
+      <c r="AP104" s="135"/>
+      <c r="AQ104" s="133" t="s">
         <v>230</v>
       </c>
-      <c r="AR104" s="185"/>
-      <c r="AS104" s="184" t="s">
+      <c r="AR104" s="135"/>
+      <c r="AS104" s="133" t="s">
         <v>229</v>
       </c>
-      <c r="AT104" s="186"/>
-      <c r="AU104" s="186"/>
-      <c r="AV104" s="186"/>
-      <c r="AW104" s="186"/>
-      <c r="AX104" s="186"/>
-      <c r="AY104" s="186"/>
-      <c r="AZ104" s="185"/>
+      <c r="AT104" s="134"/>
+      <c r="AU104" s="134"/>
+      <c r="AV104" s="134"/>
+      <c r="AW104" s="134"/>
+      <c r="AX104" s="134"/>
+      <c r="AY104" s="134"/>
+      <c r="AZ104" s="135"/>
       <c r="BA104" s="42"/>
       <c r="BB104" s="42"/>
       <c r="BC104" s="42"/>
@@ -12939,11 +13000,11 @@
       <c r="I106" s="76"/>
       <c r="J106" s="76"/>
       <c r="K106" s="77"/>
-      <c r="L106" s="154" t="s">
+      <c r="L106" s="136" t="s">
         <v>246</v>
       </c>
-      <c r="M106" s="155"/>
-      <c r="N106" s="156"/>
+      <c r="M106" s="137"/>
+      <c r="N106" s="138"/>
       <c r="O106" s="53"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="50"/>
@@ -12982,16 +13043,16 @@
       <c r="AR106" s="51">
         <v>0</v>
       </c>
-      <c r="AS106" s="120" t="s">
+      <c r="AS106" s="189" t="s">
         <v>231</v>
       </c>
-      <c r="AT106" s="121"/>
-      <c r="AU106" s="121"/>
-      <c r="AV106" s="121"/>
-      <c r="AW106" s="121"/>
-      <c r="AX106" s="121"/>
-      <c r="AY106" s="121"/>
-      <c r="AZ106" s="122"/>
+      <c r="AT106" s="190"/>
+      <c r="AU106" s="190"/>
+      <c r="AV106" s="190"/>
+      <c r="AW106" s="190"/>
+      <c r="AX106" s="190"/>
+      <c r="AY106" s="190"/>
+      <c r="AZ106" s="191"/>
       <c r="BA106" s="50" t="s">
         <v>316</v>
       </c>
@@ -13057,16 +13118,16 @@
       <c r="AR107" s="51">
         <v>1</v>
       </c>
-      <c r="AS107" s="120" t="s">
+      <c r="AS107" s="189" t="s">
         <v>354</v>
       </c>
-      <c r="AT107" s="121"/>
-      <c r="AU107" s="121"/>
-      <c r="AV107" s="121"/>
-      <c r="AW107" s="121"/>
-      <c r="AX107" s="121"/>
-      <c r="AY107" s="121"/>
-      <c r="AZ107" s="122"/>
+      <c r="AT107" s="190"/>
+      <c r="AU107" s="190"/>
+      <c r="AV107" s="190"/>
+      <c r="AW107" s="190"/>
+      <c r="AX107" s="190"/>
+      <c r="AY107" s="190"/>
+      <c r="AZ107" s="191"/>
       <c r="BA107" s="50" t="s">
         <v>298</v>
       </c>
@@ -13134,16 +13195,16 @@
       <c r="AR108" s="51">
         <v>0</v>
       </c>
-      <c r="AS108" s="120" t="s">
+      <c r="AS108" s="189" t="s">
         <v>353</v>
       </c>
-      <c r="AT108" s="121"/>
-      <c r="AU108" s="121"/>
-      <c r="AV108" s="121"/>
-      <c r="AW108" s="121"/>
-      <c r="AX108" s="121"/>
-      <c r="AY108" s="121"/>
-      <c r="AZ108" s="122"/>
+      <c r="AT108" s="190"/>
+      <c r="AU108" s="190"/>
+      <c r="AV108" s="190"/>
+      <c r="AW108" s="190"/>
+      <c r="AX108" s="190"/>
+      <c r="AY108" s="190"/>
+      <c r="AZ108" s="191"/>
       <c r="BA108" s="50" t="s">
         <v>265</v>
       </c>
@@ -13207,16 +13268,16 @@
       <c r="AR109" s="51">
         <v>1</v>
       </c>
-      <c r="AS109" s="120" t="s">
+      <c r="AS109" s="189" t="s">
         <v>233</v>
       </c>
-      <c r="AT109" s="121"/>
-      <c r="AU109" s="121"/>
-      <c r="AV109" s="121"/>
-      <c r="AW109" s="121"/>
-      <c r="AX109" s="121"/>
-      <c r="AY109" s="121"/>
-      <c r="AZ109" s="122"/>
+      <c r="AT109" s="190"/>
+      <c r="AU109" s="190"/>
+      <c r="AV109" s="190"/>
+      <c r="AW109" s="190"/>
+      <c r="AX109" s="190"/>
+      <c r="AY109" s="190"/>
+      <c r="AZ109" s="191"/>
       <c r="BA109" s="50" t="s">
         <v>260</v>
       </c>
@@ -13372,12 +13433,12 @@
       <c r="L112" s="49"/>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
-      <c r="O112" s="145" t="s">
+      <c r="O112" s="177" t="s">
         <v>232</v>
       </c>
-      <c r="P112" s="146"/>
-      <c r="Q112" s="146"/>
-      <c r="R112" s="147"/>
+      <c r="P112" s="178"/>
+      <c r="Q112" s="178"/>
+      <c r="R112" s="179"/>
       <c r="S112" s="50"/>
       <c r="T112" s="50"/>
       <c r="U112" s="50"/>
@@ -13402,20 +13463,20 @@
       <c r="AN112" s="50"/>
       <c r="AO112" s="50"/>
       <c r="AP112" s="50"/>
-      <c r="AQ112" s="140" t="s">
+      <c r="AQ112" s="172" t="s">
         <v>302</v>
       </c>
-      <c r="AR112" s="141"/>
-      <c r="AS112" s="142" t="s">
+      <c r="AR112" s="173"/>
+      <c r="AS112" s="174" t="s">
         <v>299</v>
       </c>
-      <c r="AT112" s="143"/>
-      <c r="AU112" s="143"/>
-      <c r="AV112" s="143"/>
-      <c r="AW112" s="143"/>
-      <c r="AX112" s="143"/>
-      <c r="AY112" s="143"/>
-      <c r="AZ112" s="144"/>
+      <c r="AT112" s="175"/>
+      <c r="AU112" s="175"/>
+      <c r="AV112" s="175"/>
+      <c r="AW112" s="175"/>
+      <c r="AX112" s="175"/>
+      <c r="AY112" s="175"/>
+      <c r="AZ112" s="176"/>
       <c r="BA112" s="42"/>
       <c r="BB112" s="42"/>
       <c r="BC112" s="42"/>
@@ -14616,20 +14677,20 @@
       <c r="AN130" s="42"/>
       <c r="AO130" s="42"/>
       <c r="AP130" s="42"/>
-      <c r="AQ130" s="140" t="s">
+      <c r="AQ130" s="172" t="s">
         <v>304</v>
       </c>
-      <c r="AR130" s="141"/>
-      <c r="AS130" s="142" t="s">
+      <c r="AR130" s="173"/>
+      <c r="AS130" s="174" t="s">
         <v>355</v>
       </c>
-      <c r="AT130" s="143"/>
-      <c r="AU130" s="143"/>
-      <c r="AV130" s="143"/>
-      <c r="AW130" s="143"/>
-      <c r="AX130" s="143"/>
-      <c r="AY130" s="143"/>
-      <c r="AZ130" s="144"/>
+      <c r="AT130" s="175"/>
+      <c r="AU130" s="175"/>
+      <c r="AV130" s="175"/>
+      <c r="AW130" s="175"/>
+      <c r="AX130" s="175"/>
+      <c r="AY130" s="175"/>
+      <c r="AZ130" s="176"/>
       <c r="BA130" s="42"/>
       <c r="BB130" s="42"/>
       <c r="BC130" s="42"/>
@@ -14683,16 +14744,16 @@
       <c r="AP131" s="42"/>
       <c r="AQ131" s="42"/>
       <c r="AR131" s="42"/>
-      <c r="AS131" s="148" t="s">
+      <c r="AS131" s="180" t="s">
         <v>301</v>
       </c>
-      <c r="AT131" s="149"/>
-      <c r="AU131" s="149"/>
-      <c r="AV131" s="149"/>
-      <c r="AW131" s="149"/>
-      <c r="AX131" s="149"/>
-      <c r="AY131" s="149"/>
-      <c r="AZ131" s="150"/>
+      <c r="AT131" s="181"/>
+      <c r="AU131" s="181"/>
+      <c r="AV131" s="181"/>
+      <c r="AW131" s="181"/>
+      <c r="AX131" s="181"/>
+      <c r="AY131" s="181"/>
+      <c r="AZ131" s="182"/>
       <c r="BA131" s="42"/>
       <c r="BB131" s="42"/>
       <c r="BC131" s="42"/>
@@ -14805,20 +14866,20 @@
       <c r="AN133" s="42"/>
       <c r="AO133" s="42"/>
       <c r="AP133" s="42"/>
-      <c r="AQ133" s="140" t="s">
+      <c r="AQ133" s="172" t="s">
         <v>303</v>
       </c>
-      <c r="AR133" s="141"/>
-      <c r="AS133" s="142" t="s">
+      <c r="AR133" s="173"/>
+      <c r="AS133" s="174" t="s">
         <v>305</v>
       </c>
-      <c r="AT133" s="143"/>
-      <c r="AU133" s="143"/>
-      <c r="AV133" s="143"/>
-      <c r="AW133" s="143"/>
-      <c r="AX133" s="143"/>
-      <c r="AY133" s="143"/>
-      <c r="AZ133" s="144"/>
+      <c r="AT133" s="175"/>
+      <c r="AU133" s="175"/>
+      <c r="AV133" s="175"/>
+      <c r="AW133" s="175"/>
+      <c r="AX133" s="175"/>
+      <c r="AY133" s="175"/>
+      <c r="AZ133" s="176"/>
       <c r="BA133" s="42"/>
       <c r="BB133" s="42"/>
       <c r="BC133" s="42"/>
@@ -17441,6 +17502,193 @@
     </row>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="AS109:AZ109"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="S102:AD102"/>
+    <mergeCell ref="AQ102:AR102"/>
+    <mergeCell ref="AS102:AZ102"/>
+    <mergeCell ref="AE102:AP102"/>
+    <mergeCell ref="E102:K102"/>
+    <mergeCell ref="L102:N102"/>
+    <mergeCell ref="O102:R102"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="AS106:AZ106"/>
+    <mergeCell ref="AS107:AZ107"/>
+    <mergeCell ref="AS108:AZ108"/>
+    <mergeCell ref="AV46:AW46"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE30:AF30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="AQ112:AR112"/>
+    <mergeCell ref="AQ130:AR130"/>
+    <mergeCell ref="AQ133:AR133"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="AS112:AZ112"/>
+    <mergeCell ref="O112:R112"/>
+    <mergeCell ref="AS130:AZ130"/>
+    <mergeCell ref="AS131:AZ131"/>
+    <mergeCell ref="AS133:AZ133"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="U99:AB99"/>
+    <mergeCell ref="AC99:AJ99"/>
+    <mergeCell ref="AK99:AR99"/>
+    <mergeCell ref="AS99:AZ99"/>
+    <mergeCell ref="O99:T99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AS95:AZ95"/>
+    <mergeCell ref="AK95:AR95"/>
+    <mergeCell ref="AC95:AJ95"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="AQ104:AR104"/>
+    <mergeCell ref="AS104:AZ104"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="AS97:AZ97"/>
+    <mergeCell ref="AK97:AR97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="O104:R104"/>
+    <mergeCell ref="S104:AD104"/>
+    <mergeCell ref="AE104:AP104"/>
+    <mergeCell ref="AC97:AJ97"/>
+    <mergeCell ref="U97:AB97"/>
+    <mergeCell ref="O97:T97"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="U95:AB95"/>
+    <mergeCell ref="O95:T95"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
     <mergeCell ref="AZ23:BF23"/>
     <mergeCell ref="BB24:BF24"/>
     <mergeCell ref="BD25:BF25"/>
@@ -17465,193 +17713,6 @@
     <mergeCell ref="AT22:AU22"/>
     <mergeCell ref="AV23:AW23"/>
     <mergeCell ref="AX23:AY23"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="U95:AB95"/>
-    <mergeCell ref="O95:T95"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="AQ104:AR104"/>
-    <mergeCell ref="AS104:AZ104"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="AS97:AZ97"/>
-    <mergeCell ref="AK97:AR97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="L104:N104"/>
-    <mergeCell ref="O104:R104"/>
-    <mergeCell ref="S104:AD104"/>
-    <mergeCell ref="AE104:AP104"/>
-    <mergeCell ref="AC97:AJ97"/>
-    <mergeCell ref="U97:AB97"/>
-    <mergeCell ref="O97:T97"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AQ112:AR112"/>
-    <mergeCell ref="AQ130:AR130"/>
-    <mergeCell ref="AQ133:AR133"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="AS112:AZ112"/>
-    <mergeCell ref="O112:R112"/>
-    <mergeCell ref="AS130:AZ130"/>
-    <mergeCell ref="AS131:AZ131"/>
-    <mergeCell ref="AS133:AZ133"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="U99:AB99"/>
-    <mergeCell ref="AC99:AJ99"/>
-    <mergeCell ref="AK99:AR99"/>
-    <mergeCell ref="AS99:AZ99"/>
-    <mergeCell ref="O99:T99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AS95:AZ95"/>
-    <mergeCell ref="AK95:AR95"/>
-    <mergeCell ref="AC95:AJ95"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="AS109:AZ109"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="S102:AD102"/>
-    <mergeCell ref="AQ102:AR102"/>
-    <mergeCell ref="AS102:AZ102"/>
-    <mergeCell ref="AE102:AP102"/>
-    <mergeCell ref="E102:K102"/>
-    <mergeCell ref="L102:N102"/>
-    <mergeCell ref="O102:R102"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="AS106:AZ106"/>
-    <mergeCell ref="AS107:AZ107"/>
-    <mergeCell ref="AS108:AZ108"/>
-    <mergeCell ref="AV46:AW46"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[Slot Doc] Add a list of spare pins on Master and Slave
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFE1393-3DBE-4346-8FA1-C96FC09D4315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D189130-2490-4081-996C-B779A4CFDD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
+    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin mapping" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="427">
   <si>
     <t>Timing Slot EFR32x</t>
   </si>
@@ -2204,13 +2204,45 @@
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2219,62 +2251,17 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2283,81 +2270,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2402,6 +2314,15 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2411,28 +2332,107 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2462,13 +2462,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2247255</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476</xdr:colOff>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2506,13 +2506,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>2200409</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2550,13 +2550,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2616,13 +2616,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2682,13 +2682,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2748,13 +2748,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2814,13 +2814,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>249530</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>173313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>589442</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>116163</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2880,13 +2880,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>281280</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>166963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>621192</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>109813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3510,10 +3510,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,7 +5397,7 @@
       <c r="E35" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="194" t="s">
+      <c r="F35" s="120" t="s">
         <v>379</v>
       </c>
       <c r="G35" s="93" t="s">
@@ -5577,61 +5577,61 @@
       <c r="N38" s="5"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="195" t="s">
+      <c r="A39" s="121" t="s">
         <v>418</v>
       </c>
-      <c r="B39" s="196" t="s">
+      <c r="B39" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="195" t="s">
+      <c r="C39" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="195" t="s">
+      <c r="D39" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="195" t="s">
+      <c r="E39" s="121" t="s">
         <v>129</v>
       </c>
-      <c r="F39" s="195" t="s">
+      <c r="F39" s="121" t="s">
         <v>379</v>
       </c>
-      <c r="G39" s="195" t="s">
+      <c r="G39" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="H39" s="195" t="s">
+      <c r="H39" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="I39" s="195" t="s">
+      <c r="I39" s="121" t="s">
         <v>426</v>
       </c>
       <c r="K39" s="89" t="s">
         <v>388</v>
       </c>
-      <c r="M39" s="195" t="s">
+      <c r="M39" s="121" t="s">
         <v>418</v>
       </c>
-      <c r="N39" s="196" t="s">
+      <c r="N39" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="O39" s="195" t="s">
+      <c r="O39" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="P39" s="195" t="s">
+      <c r="P39" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="Q39" s="195" t="s">
+      <c r="Q39" s="121" t="s">
         <v>129</v>
       </c>
-      <c r="R39" s="195" t="s">
+      <c r="R39" s="121" t="s">
         <v>379</v>
       </c>
-      <c r="S39" s="195" t="s">
+      <c r="S39" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="T39" s="195" t="s">
+      <c r="T39" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="U39" s="195" t="s">
+      <c r="U39" s="121" t="s">
         <v>426</v>
       </c>
       <c r="Y39" s="95" t="s">
@@ -5639,61 +5639,61 @@
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A40" s="195" t="s">
+      <c r="A40" s="121" t="s">
         <v>418</v>
       </c>
-      <c r="B40" s="196" t="s">
+      <c r="B40" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="195" t="s">
+      <c r="C40" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="195" t="s">
+      <c r="D40" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="195" t="s">
+      <c r="E40" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="F40" s="195" t="s">
+      <c r="F40" s="121" t="s">
         <v>379</v>
       </c>
-      <c r="G40" s="195" t="s">
+      <c r="G40" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="H40" s="195" t="s">
+      <c r="H40" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="I40" s="195" t="s">
+      <c r="I40" s="121" t="s">
         <v>426</v>
       </c>
       <c r="K40" s="89" t="s">
         <v>388</v>
       </c>
-      <c r="M40" s="195" t="s">
+      <c r="M40" s="121" t="s">
         <v>418</v>
       </c>
-      <c r="N40" s="196" t="s">
+      <c r="N40" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="O40" s="195" t="s">
+      <c r="O40" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="P40" s="195" t="s">
+      <c r="P40" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="Q40" s="195" t="s">
+      <c r="Q40" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="R40" s="195" t="s">
+      <c r="R40" s="121" t="s">
         <v>379</v>
       </c>
-      <c r="S40" s="195" t="s">
+      <c r="S40" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="T40" s="195" t="s">
+      <c r="T40" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="U40" s="195" t="s">
+      <c r="U40" s="121" t="s">
         <v>426</v>
       </c>
       <c r="Y40" s="95" t="s">
@@ -5704,7 +5704,7 @@
       <c r="A42" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="B42" s="197"/>
+      <c r="B42" s="123"/>
       <c r="C42" s="14" t="s">
         <v>46</v>
       </c>
@@ -5732,7 +5732,7 @@
       <c r="A43" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="B43" s="197"/>
+      <c r="B43" s="123"/>
       <c r="C43" s="14" t="s">
         <v>46</v>
       </c>
@@ -5753,6 +5753,127 @@
         <v>423</v>
       </c>
       <c r="K43" s="90" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B44" s="123"/>
+      <c r="C44" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B45" s="123"/>
+      <c r="C45" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B46" s="123"/>
+      <c r="C46" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I46" s="14"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B47" s="123"/>
+      <c r="C47" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I47" s="14"/>
+      <c r="K47" s="90" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48" s="123"/>
+      <c r="C48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I48" s="14"/>
+      <c r="K48" s="90" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5910,21 +6031,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="192"/>
-      <c r="M3" s="192"/>
-      <c r="N3" s="192"/>
-      <c r="O3" s="192"/>
-      <c r="P3" s="192"/>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="192"/>
-      <c r="S3" s="192"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="127"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="127"/>
+      <c r="Q3" s="127"/>
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -6032,45 +6153,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="185" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="150"/>
-      <c r="K5" s="152" t="s">
+      <c r="F5" s="186"/>
+      <c r="G5" s="186"/>
+      <c r="H5" s="186"/>
+      <c r="I5" s="186"/>
+      <c r="J5" s="187"/>
+      <c r="K5" s="176" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="155"/>
-      <c r="M5" s="155"/>
-      <c r="N5" s="155"/>
-      <c r="O5" s="153"/>
-      <c r="P5" s="152" t="s">
+      <c r="L5" s="193"/>
+      <c r="M5" s="193"/>
+      <c r="N5" s="193"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="176" t="s">
         <v>276</v>
       </c>
-      <c r="Q5" s="153"/>
-      <c r="R5" s="156" t="s">
+      <c r="Q5" s="177"/>
+      <c r="R5" s="178" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="157"/>
-      <c r="T5" s="157"/>
-      <c r="U5" s="157"/>
-      <c r="V5" s="157"/>
-      <c r="W5" s="158"/>
-      <c r="X5" s="152" t="s">
+      <c r="S5" s="179"/>
+      <c r="T5" s="179"/>
+      <c r="U5" s="179"/>
+      <c r="V5" s="179"/>
+      <c r="W5" s="180"/>
+      <c r="X5" s="176" t="s">
         <v>270</v>
       </c>
-      <c r="Y5" s="153"/>
-      <c r="Z5" s="148" t="s">
+      <c r="Y5" s="177"/>
+      <c r="Z5" s="185" t="s">
         <v>339</v>
       </c>
-      <c r="AA5" s="149"/>
-      <c r="AB5" s="149"/>
-      <c r="AC5" s="149"/>
-      <c r="AD5" s="149"/>
-      <c r="AE5" s="150"/>
+      <c r="AA5" s="186"/>
+      <c r="AB5" s="186"/>
+      <c r="AC5" s="186"/>
+      <c r="AD5" s="186"/>
+      <c r="AE5" s="187"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -6105,45 +6226,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="129" t="s">
+      <c r="E6" s="192" t="s">
         <v>395</v>
       </c>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="139" t="s">
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="191" t="s">
         <v>336</v>
       </c>
-      <c r="L6" s="139"/>
-      <c r="M6" s="139"/>
-      <c r="N6" s="139"/>
-      <c r="O6" s="139"/>
-      <c r="P6" s="139" t="s">
+      <c r="L6" s="191"/>
+      <c r="M6" s="191"/>
+      <c r="N6" s="191"/>
+      <c r="O6" s="191"/>
+      <c r="P6" s="191" t="s">
         <v>338</v>
       </c>
-      <c r="Q6" s="139"/>
-      <c r="R6" s="129" t="s">
+      <c r="Q6" s="191"/>
+      <c r="R6" s="192" t="s">
         <v>271</v>
       </c>
-      <c r="S6" s="129"/>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129"/>
-      <c r="X6" s="129" t="s">
+      <c r="S6" s="192"/>
+      <c r="T6" s="192"/>
+      <c r="U6" s="192"/>
+      <c r="V6" s="192"/>
+      <c r="W6" s="192"/>
+      <c r="X6" s="192" t="s">
         <v>338</v>
       </c>
-      <c r="Y6" s="129"/>
-      <c r="Z6" s="129" t="s">
+      <c r="Y6" s="192"/>
+      <c r="Z6" s="192" t="s">
         <v>395</v>
       </c>
-      <c r="AA6" s="129"/>
-      <c r="AB6" s="129"/>
-      <c r="AC6" s="129"/>
-      <c r="AD6" s="129"/>
-      <c r="AE6" s="129"/>
+      <c r="AA6" s="192"/>
+      <c r="AB6" s="192"/>
+      <c r="AC6" s="192"/>
+      <c r="AD6" s="192"/>
+      <c r="AE6" s="192"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -6184,29 +6305,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="154" t="s">
+      <c r="K7" s="184" t="s">
         <v>337</v>
       </c>
-      <c r="L7" s="154"/>
-      <c r="M7" s="154"/>
-      <c r="N7" s="154"/>
-      <c r="O7" s="154"/>
-      <c r="P7" s="154" t="s">
+      <c r="L7" s="184"/>
+      <c r="M7" s="184"/>
+      <c r="N7" s="184"/>
+      <c r="O7" s="184"/>
+      <c r="P7" s="184" t="s">
         <v>337</v>
       </c>
-      <c r="Q7" s="154"/>
-      <c r="R7" s="154" t="s">
+      <c r="Q7" s="184"/>
+      <c r="R7" s="184" t="s">
         <v>278</v>
       </c>
-      <c r="S7" s="154"/>
-      <c r="T7" s="154"/>
-      <c r="U7" s="154"/>
-      <c r="V7" s="154"/>
-      <c r="W7" s="154"/>
-      <c r="X7" s="154" t="s">
+      <c r="S7" s="184"/>
+      <c r="T7" s="184"/>
+      <c r="U7" s="184"/>
+      <c r="V7" s="184"/>
+      <c r="W7" s="184"/>
+      <c r="X7" s="184" t="s">
         <v>337</v>
       </c>
-      <c r="Y7" s="154"/>
+      <c r="Y7" s="184"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -6639,10 +6760,10 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="127" t="s">
+      <c r="E14" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="193"/>
+      <c r="F14" s="132"/>
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
@@ -6667,10 +6788,10 @@
       <c r="AB14" s="108"/>
       <c r="AC14" s="108"/>
       <c r="AD14" s="108"/>
-      <c r="AE14" s="127" t="s">
+      <c r="AE14" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="193"/>
+      <c r="AF14" s="132"/>
       <c r="AG14" s="104"/>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
@@ -6713,67 +6834,67 @@
       <c r="G15" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H15" s="125" t="s">
+      <c r="H15" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="126"/>
-      <c r="J15" s="123" t="s">
+      <c r="I15" s="134"/>
+      <c r="J15" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="124"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="121"/>
-      <c r="N15" s="121"/>
-      <c r="O15" s="121"/>
-      <c r="P15" s="121"/>
-      <c r="Q15" s="121"/>
-      <c r="R15" s="121"/>
-      <c r="S15" s="121"/>
-      <c r="T15" s="121"/>
-      <c r="U15" s="121"/>
-      <c r="V15" s="121"/>
-      <c r="W15" s="121"/>
-      <c r="X15" s="121"/>
-      <c r="Y15" s="121"/>
-      <c r="Z15" s="121"/>
-      <c r="AA15" s="121"/>
-      <c r="AB15" s="121"/>
-      <c r="AC15" s="121"/>
-      <c r="AD15" s="121"/>
-      <c r="AE15" s="121"/>
-      <c r="AF15" s="122"/>
+      <c r="K15" s="136"/>
+      <c r="L15" s="194"/>
+      <c r="M15" s="195"/>
+      <c r="N15" s="195"/>
+      <c r="O15" s="195"/>
+      <c r="P15" s="195"/>
+      <c r="Q15" s="195"/>
+      <c r="R15" s="195"/>
+      <c r="S15" s="195"/>
+      <c r="T15" s="195"/>
+      <c r="U15" s="195"/>
+      <c r="V15" s="195"/>
+      <c r="W15" s="195"/>
+      <c r="X15" s="195"/>
+      <c r="Y15" s="195"/>
+      <c r="Z15" s="195"/>
+      <c r="AA15" s="195"/>
+      <c r="AB15" s="195"/>
+      <c r="AC15" s="195"/>
+      <c r="AD15" s="195"/>
+      <c r="AE15" s="195"/>
+      <c r="AF15" s="196"/>
       <c r="AG15" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="AH15" s="125" t="s">
+      <c r="AH15" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="AI15" s="126"/>
-      <c r="AJ15" s="123" t="s">
+      <c r="AI15" s="134"/>
+      <c r="AJ15" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AK15" s="124"/>
-      <c r="AL15" s="120"/>
-      <c r="AM15" s="121"/>
-      <c r="AN15" s="121"/>
-      <c r="AO15" s="121"/>
-      <c r="AP15" s="121"/>
-      <c r="AQ15" s="121"/>
-      <c r="AR15" s="121"/>
-      <c r="AS15" s="121"/>
-      <c r="AT15" s="121"/>
-      <c r="AU15" s="121"/>
-      <c r="AV15" s="121"/>
-      <c r="AW15" s="121"/>
-      <c r="AX15" s="121"/>
-      <c r="AY15" s="121"/>
-      <c r="AZ15" s="121"/>
-      <c r="BA15" s="121"/>
-      <c r="BB15" s="121"/>
-      <c r="BC15" s="121"/>
-      <c r="BD15" s="121"/>
-      <c r="BE15" s="121"/>
-      <c r="BF15" s="121"/>
+      <c r="AK15" s="136"/>
+      <c r="AL15" s="194"/>
+      <c r="AM15" s="195"/>
+      <c r="AN15" s="195"/>
+      <c r="AO15" s="195"/>
+      <c r="AP15" s="195"/>
+      <c r="AQ15" s="195"/>
+      <c r="AR15" s="195"/>
+      <c r="AS15" s="195"/>
+      <c r="AT15" s="195"/>
+      <c r="AU15" s="195"/>
+      <c r="AV15" s="195"/>
+      <c r="AW15" s="195"/>
+      <c r="AX15" s="195"/>
+      <c r="AY15" s="195"/>
+      <c r="AZ15" s="195"/>
+      <c r="BA15" s="195"/>
+      <c r="BB15" s="195"/>
+      <c r="BC15" s="195"/>
+      <c r="BD15" s="195"/>
+      <c r="BE15" s="195"/>
+      <c r="BF15" s="195"/>
       <c r="BG15" s="103"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -6794,33 +6915,33 @@
         <v>287</v>
       </c>
       <c r="I16" s="110"/>
-      <c r="J16" s="125" t="s">
+      <c r="J16" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="126"/>
-      <c r="L16" s="123" t="s">
+      <c r="K16" s="134"/>
+      <c r="L16" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="M16" s="124"/>
-      <c r="N16" s="120"/>
-      <c r="O16" s="121"/>
-      <c r="P16" s="121"/>
-      <c r="Q16" s="121"/>
-      <c r="R16" s="121"/>
-      <c r="S16" s="121"/>
-      <c r="T16" s="121"/>
-      <c r="U16" s="121"/>
-      <c r="V16" s="121"/>
-      <c r="W16" s="121"/>
-      <c r="X16" s="121"/>
-      <c r="Y16" s="121"/>
-      <c r="Z16" s="121"/>
-      <c r="AA16" s="121"/>
-      <c r="AB16" s="121"/>
-      <c r="AC16" s="121"/>
-      <c r="AD16" s="121"/>
-      <c r="AE16" s="121"/>
-      <c r="AF16" s="122"/>
+      <c r="M16" s="136"/>
+      <c r="N16" s="194"/>
+      <c r="O16" s="195"/>
+      <c r="P16" s="195"/>
+      <c r="Q16" s="195"/>
+      <c r="R16" s="195"/>
+      <c r="S16" s="195"/>
+      <c r="T16" s="195"/>
+      <c r="U16" s="195"/>
+      <c r="V16" s="195"/>
+      <c r="W16" s="195"/>
+      <c r="X16" s="195"/>
+      <c r="Y16" s="195"/>
+      <c r="Z16" s="195"/>
+      <c r="AA16" s="195"/>
+      <c r="AB16" s="195"/>
+      <c r="AC16" s="195"/>
+      <c r="AD16" s="195"/>
+      <c r="AE16" s="195"/>
+      <c r="AF16" s="196"/>
       <c r="AG16" s="106" t="s">
         <v>274</v>
       </c>
@@ -6828,33 +6949,33 @@
         <v>287</v>
       </c>
       <c r="AI16" s="110"/>
-      <c r="AJ16" s="125" t="s">
+      <c r="AJ16" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="AK16" s="126"/>
-      <c r="AL16" s="123" t="s">
+      <c r="AK16" s="134"/>
+      <c r="AL16" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AM16" s="124"/>
-      <c r="AN16" s="120"/>
-      <c r="AO16" s="121"/>
-      <c r="AP16" s="121"/>
-      <c r="AQ16" s="121"/>
-      <c r="AR16" s="121"/>
-      <c r="AS16" s="121"/>
-      <c r="AT16" s="121"/>
-      <c r="AU16" s="121"/>
-      <c r="AV16" s="121"/>
-      <c r="AW16" s="121"/>
-      <c r="AX16" s="121"/>
-      <c r="AY16" s="121"/>
-      <c r="AZ16" s="121"/>
-      <c r="BA16" s="121"/>
-      <c r="BB16" s="121"/>
-      <c r="BC16" s="121"/>
-      <c r="BD16" s="121"/>
-      <c r="BE16" s="121"/>
-      <c r="BF16" s="121"/>
+      <c r="AM16" s="136"/>
+      <c r="AN16" s="194"/>
+      <c r="AO16" s="195"/>
+      <c r="AP16" s="195"/>
+      <c r="AQ16" s="195"/>
+      <c r="AR16" s="195"/>
+      <c r="AS16" s="195"/>
+      <c r="AT16" s="195"/>
+      <c r="AU16" s="195"/>
+      <c r="AV16" s="195"/>
+      <c r="AW16" s="195"/>
+      <c r="AX16" s="195"/>
+      <c r="AY16" s="195"/>
+      <c r="AZ16" s="195"/>
+      <c r="BA16" s="195"/>
+      <c r="BB16" s="195"/>
+      <c r="BC16" s="195"/>
+      <c r="BD16" s="195"/>
+      <c r="BE16" s="195"/>
+      <c r="BF16" s="195"/>
       <c r="BG16" s="103"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -6877,31 +6998,31 @@
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
       <c r="K17" s="110"/>
-      <c r="L17" s="125" t="s">
+      <c r="L17" s="133" t="s">
         <v>281</v>
       </c>
-      <c r="M17" s="126"/>
-      <c r="N17" s="123" t="s">
+      <c r="M17" s="134"/>
+      <c r="N17" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="O17" s="124"/>
-      <c r="P17" s="120"/>
-      <c r="Q17" s="121"/>
-      <c r="R17" s="121"/>
-      <c r="S17" s="121"/>
-      <c r="T17" s="121"/>
-      <c r="U17" s="121"/>
-      <c r="V17" s="121"/>
-      <c r="W17" s="121"/>
-      <c r="X17" s="121"/>
-      <c r="Y17" s="121"/>
-      <c r="Z17" s="121"/>
-      <c r="AA17" s="121"/>
-      <c r="AB17" s="121"/>
-      <c r="AC17" s="121"/>
-      <c r="AD17" s="121"/>
-      <c r="AE17" s="121"/>
-      <c r="AF17" s="122"/>
+      <c r="O17" s="136"/>
+      <c r="P17" s="194"/>
+      <c r="Q17" s="195"/>
+      <c r="R17" s="195"/>
+      <c r="S17" s="195"/>
+      <c r="T17" s="195"/>
+      <c r="U17" s="195"/>
+      <c r="V17" s="195"/>
+      <c r="W17" s="195"/>
+      <c r="X17" s="195"/>
+      <c r="Y17" s="195"/>
+      <c r="Z17" s="195"/>
+      <c r="AA17" s="195"/>
+      <c r="AB17" s="195"/>
+      <c r="AC17" s="195"/>
+      <c r="AD17" s="195"/>
+      <c r="AE17" s="195"/>
+      <c r="AF17" s="196"/>
       <c r="AG17" s="106" t="s">
         <v>274</v>
       </c>
@@ -6911,31 +7032,31 @@
       <c r="AI17" s="111"/>
       <c r="AJ17" s="111"/>
       <c r="AK17" s="110"/>
-      <c r="AL17" s="125" t="s">
+      <c r="AL17" s="133" t="s">
         <v>281</v>
       </c>
-      <c r="AM17" s="126"/>
-      <c r="AN17" s="123" t="s">
+      <c r="AM17" s="134"/>
+      <c r="AN17" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AO17" s="124"/>
-      <c r="AP17" s="120"/>
-      <c r="AQ17" s="121"/>
-      <c r="AR17" s="121"/>
-      <c r="AS17" s="121"/>
-      <c r="AT17" s="121"/>
-      <c r="AU17" s="121"/>
-      <c r="AV17" s="121"/>
-      <c r="AW17" s="121"/>
-      <c r="AX17" s="121"/>
-      <c r="AY17" s="121"/>
-      <c r="AZ17" s="121"/>
-      <c r="BA17" s="121"/>
-      <c r="BB17" s="121"/>
-      <c r="BC17" s="121"/>
-      <c r="BD17" s="121"/>
-      <c r="BE17" s="121"/>
-      <c r="BF17" s="121"/>
+      <c r="AO17" s="136"/>
+      <c r="AP17" s="194"/>
+      <c r="AQ17" s="195"/>
+      <c r="AR17" s="195"/>
+      <c r="AS17" s="195"/>
+      <c r="AT17" s="195"/>
+      <c r="AU17" s="195"/>
+      <c r="AV17" s="195"/>
+      <c r="AW17" s="195"/>
+      <c r="AX17" s="195"/>
+      <c r="AY17" s="195"/>
+      <c r="AZ17" s="195"/>
+      <c r="BA17" s="195"/>
+      <c r="BB17" s="195"/>
+      <c r="BC17" s="195"/>
+      <c r="BD17" s="195"/>
+      <c r="BE17" s="195"/>
+      <c r="BF17" s="195"/>
       <c r="BG17" s="103"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -6960,27 +7081,27 @@
       <c r="K18" s="111"/>
       <c r="L18" s="111"/>
       <c r="M18" s="110"/>
-      <c r="N18" s="127" t="s">
+      <c r="N18" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="O18" s="128"/>
-      <c r="P18" s="120"/>
-      <c r="Q18" s="121"/>
-      <c r="R18" s="121"/>
-      <c r="S18" s="121"/>
-      <c r="T18" s="121"/>
-      <c r="U18" s="121"/>
-      <c r="V18" s="121"/>
-      <c r="W18" s="121"/>
-      <c r="X18" s="121"/>
-      <c r="Y18" s="121"/>
-      <c r="Z18" s="121"/>
-      <c r="AA18" s="121"/>
-      <c r="AB18" s="121"/>
-      <c r="AC18" s="121"/>
-      <c r="AD18" s="121"/>
-      <c r="AE18" s="121"/>
-      <c r="AF18" s="122"/>
+      <c r="O18" s="140"/>
+      <c r="P18" s="194"/>
+      <c r="Q18" s="195"/>
+      <c r="R18" s="195"/>
+      <c r="S18" s="195"/>
+      <c r="T18" s="195"/>
+      <c r="U18" s="195"/>
+      <c r="V18" s="195"/>
+      <c r="W18" s="195"/>
+      <c r="X18" s="195"/>
+      <c r="Y18" s="195"/>
+      <c r="Z18" s="195"/>
+      <c r="AA18" s="195"/>
+      <c r="AB18" s="195"/>
+      <c r="AC18" s="195"/>
+      <c r="AD18" s="195"/>
+      <c r="AE18" s="195"/>
+      <c r="AF18" s="196"/>
       <c r="AG18" s="106" t="s">
         <v>274</v>
       </c>
@@ -6992,27 +7113,27 @@
       <c r="AK18" s="111"/>
       <c r="AL18" s="111"/>
       <c r="AM18" s="110"/>
-      <c r="AN18" s="127" t="s">
+      <c r="AN18" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="AO18" s="128"/>
-      <c r="AP18" s="120"/>
-      <c r="AQ18" s="121"/>
-      <c r="AR18" s="121"/>
-      <c r="AS18" s="121"/>
-      <c r="AT18" s="121"/>
-      <c r="AU18" s="121"/>
-      <c r="AV18" s="121"/>
-      <c r="AW18" s="121"/>
-      <c r="AX18" s="121"/>
-      <c r="AY18" s="121"/>
-      <c r="AZ18" s="121"/>
-      <c r="BA18" s="121"/>
-      <c r="BB18" s="121"/>
-      <c r="BC18" s="121"/>
-      <c r="BD18" s="121"/>
-      <c r="BE18" s="121"/>
-      <c r="BF18" s="121"/>
+      <c r="AO18" s="140"/>
+      <c r="AP18" s="194"/>
+      <c r="AQ18" s="195"/>
+      <c r="AR18" s="195"/>
+      <c r="AS18" s="195"/>
+      <c r="AT18" s="195"/>
+      <c r="AU18" s="195"/>
+      <c r="AV18" s="195"/>
+      <c r="AW18" s="195"/>
+      <c r="AX18" s="195"/>
+      <c r="AY18" s="195"/>
+      <c r="AZ18" s="195"/>
+      <c r="BA18" s="195"/>
+      <c r="BB18" s="195"/>
+      <c r="BC18" s="195"/>
+      <c r="BD18" s="195"/>
+      <c r="BE18" s="195"/>
+      <c r="BF18" s="195"/>
       <c r="BG18" s="103"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -7238,23 +7359,23 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
       <c r="S22" s="110"/>
-      <c r="T22" s="125" t="s">
+      <c r="T22" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="126"/>
-      <c r="V22" s="123" t="s">
+      <c r="U22" s="134"/>
+      <c r="V22" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="W22" s="124"/>
-      <c r="X22" s="120"/>
-      <c r="Y22" s="121"/>
-      <c r="Z22" s="121"/>
-      <c r="AA22" s="121"/>
-      <c r="AB22" s="121"/>
-      <c r="AC22" s="121"/>
-      <c r="AD22" s="121"/>
-      <c r="AE22" s="121"/>
-      <c r="AF22" s="122"/>
+      <c r="W22" s="136"/>
+      <c r="X22" s="194"/>
+      <c r="Y22" s="195"/>
+      <c r="Z22" s="195"/>
+      <c r="AA22" s="195"/>
+      <c r="AB22" s="195"/>
+      <c r="AC22" s="195"/>
+      <c r="AD22" s="195"/>
+      <c r="AE22" s="195"/>
+      <c r="AF22" s="196"/>
       <c r="AG22" s="106" t="s">
         <v>274</v>
       </c>
@@ -7272,23 +7393,23 @@
       <c r="AQ22" s="111"/>
       <c r="AR22" s="111"/>
       <c r="AS22" s="110"/>
-      <c r="AT22" s="125" t="s">
+      <c r="AT22" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="AU22" s="126"/>
-      <c r="AV22" s="123" t="s">
+      <c r="AU22" s="134"/>
+      <c r="AV22" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AW22" s="124"/>
-      <c r="AX22" s="120"/>
-      <c r="AY22" s="121"/>
-      <c r="AZ22" s="121"/>
-      <c r="BA22" s="121"/>
-      <c r="BB22" s="121"/>
-      <c r="BC22" s="121"/>
-      <c r="BD22" s="121"/>
-      <c r="BE22" s="121"/>
-      <c r="BF22" s="121"/>
+      <c r="AW22" s="136"/>
+      <c r="AX22" s="194"/>
+      <c r="AY22" s="195"/>
+      <c r="AZ22" s="195"/>
+      <c r="BA22" s="195"/>
+      <c r="BB22" s="195"/>
+      <c r="BC22" s="195"/>
+      <c r="BD22" s="195"/>
+      <c r="BE22" s="195"/>
+      <c r="BF22" s="195"/>
       <c r="BG22" s="103"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -7321,21 +7442,21 @@
       <c r="S23" s="111"/>
       <c r="T23" s="111"/>
       <c r="U23" s="110"/>
-      <c r="V23" s="125" t="s">
+      <c r="V23" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="W23" s="126"/>
-      <c r="X23" s="123" t="s">
+      <c r="W23" s="134"/>
+      <c r="X23" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="Y23" s="124"/>
-      <c r="Z23" s="120"/>
-      <c r="AA23" s="121"/>
-      <c r="AB23" s="121"/>
-      <c r="AC23" s="121"/>
-      <c r="AD23" s="121"/>
-      <c r="AE23" s="121"/>
-      <c r="AF23" s="122"/>
+      <c r="Y23" s="136"/>
+      <c r="Z23" s="194"/>
+      <c r="AA23" s="195"/>
+      <c r="AB23" s="195"/>
+      <c r="AC23" s="195"/>
+      <c r="AD23" s="195"/>
+      <c r="AE23" s="195"/>
+      <c r="AF23" s="196"/>
       <c r="AG23" s="106" t="s">
         <v>274</v>
       </c>
@@ -7355,21 +7476,21 @@
       <c r="AS23" s="111"/>
       <c r="AT23" s="111"/>
       <c r="AU23" s="110"/>
-      <c r="AV23" s="125" t="s">
+      <c r="AV23" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="AW23" s="126"/>
-      <c r="AX23" s="123" t="s">
+      <c r="AW23" s="134"/>
+      <c r="AX23" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AY23" s="124"/>
-      <c r="AZ23" s="120"/>
-      <c r="BA23" s="121"/>
-      <c r="BB23" s="121"/>
-      <c r="BC23" s="121"/>
-      <c r="BD23" s="121"/>
-      <c r="BE23" s="121"/>
-      <c r="BF23" s="121"/>
+      <c r="AY23" s="136"/>
+      <c r="AZ23" s="194"/>
+      <c r="BA23" s="195"/>
+      <c r="BB23" s="195"/>
+      <c r="BC23" s="195"/>
+      <c r="BD23" s="195"/>
+      <c r="BE23" s="195"/>
+      <c r="BF23" s="195"/>
       <c r="BG23" s="103"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -7404,19 +7525,19 @@
       <c r="U24" s="111"/>
       <c r="V24" s="111"/>
       <c r="W24" s="110"/>
-      <c r="X24" s="125" t="s">
+      <c r="X24" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="Y24" s="126"/>
-      <c r="Z24" s="123" t="s">
+      <c r="Y24" s="134"/>
+      <c r="Z24" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AA24" s="124"/>
-      <c r="AB24" s="120"/>
-      <c r="AC24" s="121"/>
-      <c r="AD24" s="121"/>
-      <c r="AE24" s="121"/>
-      <c r="AF24" s="122"/>
+      <c r="AA24" s="136"/>
+      <c r="AB24" s="194"/>
+      <c r="AC24" s="195"/>
+      <c r="AD24" s="195"/>
+      <c r="AE24" s="195"/>
+      <c r="AF24" s="196"/>
       <c r="AG24" s="106" t="s">
         <v>274</v>
       </c>
@@ -7438,19 +7559,19 @@
       <c r="AU24" s="111"/>
       <c r="AV24" s="111"/>
       <c r="AW24" s="110"/>
-      <c r="AX24" s="125" t="s">
+      <c r="AX24" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="AY24" s="126"/>
-      <c r="AZ24" s="123" t="s">
+      <c r="AY24" s="134"/>
+      <c r="AZ24" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="BA24" s="124"/>
-      <c r="BB24" s="120"/>
-      <c r="BC24" s="121"/>
-      <c r="BD24" s="121"/>
-      <c r="BE24" s="121"/>
-      <c r="BF24" s="121"/>
+      <c r="BA24" s="136"/>
+      <c r="BB24" s="194"/>
+      <c r="BC24" s="195"/>
+      <c r="BD24" s="195"/>
+      <c r="BE24" s="195"/>
+      <c r="BF24" s="195"/>
       <c r="BG24" s="103"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -7487,17 +7608,17 @@
       <c r="W25" s="111"/>
       <c r="X25" s="111"/>
       <c r="Y25" s="110"/>
-      <c r="Z25" s="127" t="s">
+      <c r="Z25" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="AA25" s="128"/>
-      <c r="AB25" s="123" t="s">
+      <c r="AA25" s="140"/>
+      <c r="AB25" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AC25" s="124"/>
-      <c r="AD25" s="120"/>
-      <c r="AE25" s="121"/>
-      <c r="AF25" s="122"/>
+      <c r="AC25" s="136"/>
+      <c r="AD25" s="194"/>
+      <c r="AE25" s="195"/>
+      <c r="AF25" s="196"/>
       <c r="AG25" s="106" t="s">
         <v>274</v>
       </c>
@@ -7521,17 +7642,17 @@
       <c r="AW25" s="111"/>
       <c r="AX25" s="111"/>
       <c r="AY25" s="110"/>
-      <c r="AZ25" s="127" t="s">
+      <c r="AZ25" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="BA25" s="128"/>
-      <c r="BB25" s="123" t="s">
+      <c r="BA25" s="140"/>
+      <c r="BB25" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="BC25" s="124"/>
-      <c r="BD25" s="120"/>
-      <c r="BE25" s="121"/>
-      <c r="BF25" s="121"/>
+      <c r="BC25" s="136"/>
+      <c r="BD25" s="194"/>
+      <c r="BE25" s="195"/>
+      <c r="BF25" s="195"/>
       <c r="BG25" s="103"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -7789,29 +7910,29 @@
         <v>318</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="170" t="s">
+      <c r="E30" s="137" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="171"/>
+      <c r="F30" s="138"/>
       <c r="G30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="170" t="s">
+      <c r="H30" s="137" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="171"/>
-      <c r="J30" s="170" t="s">
+      <c r="I30" s="138"/>
+      <c r="J30" s="137" t="s">
         <v>280</v>
       </c>
-      <c r="K30" s="171"/>
-      <c r="L30" s="170" t="s">
+      <c r="K30" s="138"/>
+      <c r="L30" s="137" t="s">
         <v>281</v>
       </c>
-      <c r="M30" s="171"/>
-      <c r="N30" s="170" t="s">
+      <c r="M30" s="138"/>
+      <c r="N30" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="O30" s="171"/>
+      <c r="O30" s="138"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>239</v>
@@ -7820,50 +7941,50 @@
         <v>239</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="170" t="s">
+      <c r="T30" s="137" t="s">
         <v>283</v>
       </c>
-      <c r="U30" s="171"/>
-      <c r="V30" s="170" t="s">
+      <c r="U30" s="138"/>
+      <c r="V30" s="137" t="s">
         <v>284</v>
       </c>
-      <c r="W30" s="171"/>
-      <c r="X30" s="170" t="s">
+      <c r="W30" s="138"/>
+      <c r="X30" s="137" t="s">
         <v>285</v>
       </c>
-      <c r="Y30" s="171"/>
-      <c r="Z30" s="170" t="s">
+      <c r="Y30" s="138"/>
+      <c r="Z30" s="137" t="s">
         <v>286</v>
       </c>
-      <c r="AA30" s="171"/>
-      <c r="AB30" s="144" t="s">
+      <c r="AA30" s="138"/>
+      <c r="AB30" s="141" t="s">
         <v>297</v>
       </c>
-      <c r="AC30" s="145"/>
-      <c r="AD30" s="146"/>
-      <c r="AE30" s="170" t="s">
+      <c r="AC30" s="142"/>
+      <c r="AD30" s="143"/>
+      <c r="AE30" s="137" t="s">
         <v>273</v>
       </c>
-      <c r="AF30" s="171"/>
+      <c r="AF30" s="138"/>
       <c r="AG30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="AH30" s="170" t="s">
+      <c r="AH30" s="137" t="s">
         <v>279</v>
       </c>
-      <c r="AI30" s="171"/>
-      <c r="AJ30" s="170" t="s">
+      <c r="AI30" s="138"/>
+      <c r="AJ30" s="137" t="s">
         <v>280</v>
       </c>
-      <c r="AK30" s="171"/>
-      <c r="AL30" s="170" t="s">
+      <c r="AK30" s="138"/>
+      <c r="AL30" s="137" t="s">
         <v>281</v>
       </c>
-      <c r="AM30" s="171"/>
-      <c r="AN30" s="170" t="s">
+      <c r="AM30" s="138"/>
+      <c r="AN30" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="AO30" s="171"/>
+      <c r="AO30" s="138"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>239</v>
@@ -7872,27 +7993,27 @@
         <v>239</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="170" t="s">
+      <c r="AT30" s="137" t="s">
         <v>283</v>
       </c>
-      <c r="AU30" s="171"/>
-      <c r="AV30" s="170" t="s">
+      <c r="AU30" s="138"/>
+      <c r="AV30" s="137" t="s">
         <v>284</v>
       </c>
-      <c r="AW30" s="171"/>
-      <c r="AX30" s="170" t="s">
+      <c r="AW30" s="138"/>
+      <c r="AX30" s="137" t="s">
         <v>285</v>
       </c>
-      <c r="AY30" s="171"/>
-      <c r="AZ30" s="170" t="s">
+      <c r="AY30" s="138"/>
+      <c r="AZ30" s="137" t="s">
         <v>286</v>
       </c>
-      <c r="BA30" s="171"/>
-      <c r="BB30" s="144" t="s">
+      <c r="BA30" s="138"/>
+      <c r="BB30" s="141" t="s">
         <v>297</v>
       </c>
-      <c r="BC30" s="145"/>
-      <c r="BD30" s="146"/>
+      <c r="BC30" s="142"/>
+      <c r="BD30" s="143"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -7904,10 +8025,10 @@
         <v>317</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="147" t="s">
+      <c r="E31" s="139" t="s">
         <v>323</v>
       </c>
-      <c r="F31" s="147"/>
+      <c r="F31" s="139"/>
       <c r="G31" s="22" t="s">
         <v>324</v>
       </c>
@@ -7934,10 +8055,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="147" t="s">
+      <c r="AE31" s="139" t="s">
         <v>323</v>
       </c>
-      <c r="AF31" s="147"/>
+      <c r="AF31" s="139"/>
       <c r="AG31" s="22" t="s">
         <v>324</v>
       </c>
@@ -8061,14 +8182,14 @@
       <c r="Q33" s="168"/>
       <c r="R33" s="168"/>
       <c r="S33" s="169"/>
-      <c r="T33" s="170" t="s">
+      <c r="T33" s="137" t="s">
         <v>275</v>
       </c>
-      <c r="U33" s="171"/>
-      <c r="V33" s="144" t="s">
+      <c r="U33" s="138"/>
+      <c r="V33" s="141" t="s">
         <v>297</v>
       </c>
-      <c r="W33" s="146"/>
+      <c r="W33" s="143"/>
       <c r="X33" s="167" t="s">
         <v>319</v>
       </c>
@@ -8099,14 +8220,14 @@
       <c r="AQ33" s="168"/>
       <c r="AR33" s="168"/>
       <c r="AS33" s="169"/>
-      <c r="AT33" s="170" t="s">
+      <c r="AT33" s="137" t="s">
         <v>275</v>
       </c>
-      <c r="AU33" s="171"/>
-      <c r="AV33" s="144" t="s">
+      <c r="AU33" s="138"/>
+      <c r="AV33" s="141" t="s">
         <v>297</v>
       </c>
-      <c r="AW33" s="146"/>
+      <c r="AW33" s="143"/>
       <c r="AX33" s="167" t="s">
         <v>319</v>
       </c>
@@ -8127,10 +8248,10 @@
         <v>317</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="147" t="s">
+      <c r="E34" s="139" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="147"/>
+      <c r="F34" s="139"/>
       <c r="G34" s="22" t="s">
         <v>321</v>
       </c>
@@ -8146,10 +8267,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="147" t="s">
+      <c r="T34" s="139" t="s">
         <v>323</v>
       </c>
-      <c r="U34" s="147"/>
+      <c r="U34" s="139"/>
       <c r="V34" s="22" t="s">
         <v>325</v>
       </c>
@@ -8178,10 +8299,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="147" t="s">
+      <c r="AT34" s="139" t="s">
         <v>323</v>
       </c>
-      <c r="AU34" s="147"/>
+      <c r="AU34" s="139"/>
       <c r="AV34" s="22" t="s">
         <v>320</v>
       </c>
@@ -8452,33 +8573,33 @@
         <v>326</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="162" t="s">
+      <c r="E39" s="170" t="s">
         <v>273</v>
       </c>
-      <c r="F39" s="163"/>
-      <c r="G39" s="165" t="s">
+      <c r="F39" s="171"/>
+      <c r="G39" s="172" t="s">
         <v>273</v>
       </c>
-      <c r="H39" s="166"/>
+      <c r="H39" s="173"/>
       <c r="I39" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="J39" s="127" t="s">
+      <c r="J39" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="K39" s="128"/>
-      <c r="L39" s="127" t="s">
+      <c r="K39" s="140"/>
+      <c r="L39" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="M39" s="128"/>
-      <c r="N39" s="127" t="s">
+      <c r="M39" s="140"/>
+      <c r="N39" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="O39" s="128"/>
-      <c r="P39" s="127" t="s">
+      <c r="O39" s="140"/>
+      <c r="P39" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="Q39" s="128"/>
+      <c r="Q39" s="140"/>
       <c r="R39" s="103"/>
       <c r="S39" s="103" t="s">
         <v>239</v>
@@ -8487,50 +8608,50 @@
         <v>239</v>
       </c>
       <c r="U39" s="103"/>
-      <c r="V39" s="127" t="s">
+      <c r="V39" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="W39" s="128"/>
-      <c r="X39" s="127" t="s">
+      <c r="W39" s="140"/>
+      <c r="X39" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="Y39" s="128"/>
-      <c r="Z39" s="127" t="s">
+      <c r="Y39" s="140"/>
+      <c r="Z39" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="AA39" s="128"/>
-      <c r="AB39" s="127" t="s">
+      <c r="AA39" s="140"/>
+      <c r="AB39" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="AC39" s="128"/>
-      <c r="AD39" s="123" t="s">
+      <c r="AC39" s="140"/>
+      <c r="AD39" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AE39" s="164"/>
-      <c r="AF39" s="124"/>
-      <c r="AG39" s="127" t="s">
+      <c r="AE39" s="175"/>
+      <c r="AF39" s="136"/>
+      <c r="AG39" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="AH39" s="128"/>
+      <c r="AH39" s="140"/>
       <c r="AI39" s="112" t="s">
         <v>319</v>
       </c>
-      <c r="AJ39" s="127" t="s">
+      <c r="AJ39" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="AK39" s="128"/>
-      <c r="AL39" s="127" t="s">
+      <c r="AK39" s="140"/>
+      <c r="AL39" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="AM39" s="128"/>
-      <c r="AN39" s="127" t="s">
+      <c r="AM39" s="140"/>
+      <c r="AN39" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="AO39" s="128"/>
-      <c r="AP39" s="127" t="s">
+      <c r="AO39" s="140"/>
+      <c r="AP39" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="AQ39" s="128"/>
+      <c r="AQ39" s="140"/>
       <c r="AR39" s="103"/>
       <c r="AS39" s="103" t="s">
         <v>239</v>
@@ -8559,14 +8680,14 @@
         <v>351</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="140" t="s">
+      <c r="E40" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="140"/>
-      <c r="G40" s="140" t="s">
+      <c r="F40" s="174"/>
+      <c r="G40" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="H40" s="140"/>
+      <c r="H40" s="174"/>
       <c r="I40" s="113" t="s">
         <v>324</v>
       </c>
@@ -8593,10 +8714,10 @@
       <c r="AD40" s="103"/>
       <c r="AE40" s="103"/>
       <c r="AF40" s="103"/>
-      <c r="AG40" s="140" t="s">
+      <c r="AG40" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="AH40" s="140"/>
+      <c r="AH40" s="174"/>
       <c r="AI40" s="113" t="s">
         <v>328</v>
       </c>
@@ -8632,27 +8753,27 @@
         <v>327</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="127" t="s">
+      <c r="E41" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="128"/>
+      <c r="F41" s="140"/>
       <c r="G41" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="H41" s="127" t="s">
+      <c r="H41" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="I41" s="128"/>
-      <c r="J41" s="127" t="s">
+      <c r="I41" s="140"/>
+      <c r="J41" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="K41" s="128"/>
-      <c r="L41" s="162"/>
-      <c r="M41" s="163"/>
-      <c r="N41" s="165" t="s">
+      <c r="K41" s="140"/>
+      <c r="L41" s="170"/>
+      <c r="M41" s="171"/>
+      <c r="N41" s="172" t="s">
         <v>282</v>
       </c>
-      <c r="O41" s="166"/>
+      <c r="O41" s="173"/>
       <c r="P41" s="103"/>
       <c r="Q41" s="103" t="s">
         <v>239</v>
@@ -8661,50 +8782,50 @@
         <v>239</v>
       </c>
       <c r="S41" s="103"/>
-      <c r="T41" s="127" t="s">
+      <c r="T41" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="U41" s="128"/>
-      <c r="V41" s="127" t="s">
+      <c r="U41" s="140"/>
+      <c r="V41" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="W41" s="128"/>
-      <c r="X41" s="127" t="s">
+      <c r="W41" s="140"/>
+      <c r="X41" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="Y41" s="128"/>
-      <c r="Z41" s="127" t="s">
+      <c r="Y41" s="140"/>
+      <c r="Z41" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="AA41" s="128"/>
-      <c r="AB41" s="123" t="s">
+      <c r="AA41" s="140"/>
+      <c r="AB41" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AC41" s="164"/>
-      <c r="AD41" s="124"/>
-      <c r="AE41" s="127" t="s">
+      <c r="AC41" s="175"/>
+      <c r="AD41" s="136"/>
+      <c r="AE41" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="AF41" s="128"/>
+      <c r="AF41" s="140"/>
       <c r="AG41" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="AH41" s="127" t="s">
+      <c r="AH41" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="AI41" s="128"/>
-      <c r="AJ41" s="127" t="s">
+      <c r="AI41" s="140"/>
+      <c r="AJ41" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="AK41" s="128"/>
-      <c r="AL41" s="127" t="s">
+      <c r="AK41" s="140"/>
+      <c r="AL41" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="AM41" s="128"/>
-      <c r="AN41" s="127" t="s">
+      <c r="AM41" s="140"/>
+      <c r="AN41" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="AO41" s="128"/>
+      <c r="AO41" s="140"/>
       <c r="AP41" s="103"/>
       <c r="AQ41" s="103" t="s">
         <v>239</v>
@@ -8713,27 +8834,27 @@
         <v>239</v>
       </c>
       <c r="AS41" s="103"/>
-      <c r="AT41" s="127" t="s">
+      <c r="AT41" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="AU41" s="128"/>
-      <c r="AV41" s="127" t="s">
+      <c r="AU41" s="140"/>
+      <c r="AV41" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="AW41" s="128"/>
-      <c r="AX41" s="127" t="s">
+      <c r="AW41" s="140"/>
+      <c r="AX41" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="AY41" s="128"/>
-      <c r="AZ41" s="127" t="s">
+      <c r="AY41" s="140"/>
+      <c r="AZ41" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="BA41" s="128"/>
-      <c r="BB41" s="123" t="s">
+      <c r="BA41" s="140"/>
+      <c r="BB41" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="BC41" s="164"/>
-      <c r="BD41" s="124"/>
+      <c r="BC41" s="175"/>
+      <c r="BD41" s="136"/>
       <c r="BE41" s="103"/>
       <c r="BF41" s="103"/>
       <c r="BG41" s="103"/>
@@ -8745,10 +8866,10 @@
         <v>352</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="140" t="s">
+      <c r="E42" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="140"/>
+      <c r="F42" s="174"/>
       <c r="G42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8775,10 +8896,10 @@
       <c r="AB42" s="103"/>
       <c r="AC42" s="103"/>
       <c r="AD42" s="103"/>
-      <c r="AE42" s="140" t="s">
+      <c r="AE42" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="AF42" s="140"/>
+      <c r="AF42" s="174"/>
       <c r="AG42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8888,75 +9009,75 @@
       <c r="G44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="159" t="s">
+      <c r="H44" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="I44" s="160"/>
-      <c r="J44" s="160"/>
-      <c r="K44" s="160"/>
-      <c r="L44" s="160"/>
-      <c r="M44" s="160"/>
-      <c r="N44" s="160"/>
-      <c r="O44" s="160"/>
-      <c r="P44" s="160"/>
-      <c r="Q44" s="160"/>
-      <c r="R44" s="160"/>
-      <c r="S44" s="161"/>
-      <c r="T44" s="162" t="s">
+      <c r="I44" s="182"/>
+      <c r="J44" s="182"/>
+      <c r="K44" s="182"/>
+      <c r="L44" s="182"/>
+      <c r="M44" s="182"/>
+      <c r="N44" s="182"/>
+      <c r="O44" s="182"/>
+      <c r="P44" s="182"/>
+      <c r="Q44" s="182"/>
+      <c r="R44" s="182"/>
+      <c r="S44" s="183"/>
+      <c r="T44" s="170" t="s">
         <v>275</v>
       </c>
-      <c r="U44" s="163"/>
-      <c r="V44" s="123" t="s">
+      <c r="U44" s="171"/>
+      <c r="V44" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="W44" s="124"/>
-      <c r="X44" s="159" t="s">
+      <c r="W44" s="136"/>
+      <c r="X44" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="Y44" s="160"/>
-      <c r="Z44" s="160"/>
-      <c r="AA44" s="160"/>
-      <c r="AB44" s="160"/>
-      <c r="AC44" s="160"/>
-      <c r="AD44" s="160"/>
-      <c r="AE44" s="161"/>
+      <c r="Y44" s="182"/>
+      <c r="Z44" s="182"/>
+      <c r="AA44" s="182"/>
+      <c r="AB44" s="182"/>
+      <c r="AC44" s="182"/>
+      <c r="AD44" s="182"/>
+      <c r="AE44" s="183"/>
       <c r="AF44" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH44" s="159" t="s">
+      <c r="AH44" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="AI44" s="160"/>
-      <c r="AJ44" s="160"/>
-      <c r="AK44" s="160"/>
-      <c r="AL44" s="160"/>
-      <c r="AM44" s="160"/>
-      <c r="AN44" s="160"/>
-      <c r="AO44" s="160"/>
-      <c r="AP44" s="160"/>
-      <c r="AQ44" s="160"/>
-      <c r="AR44" s="160"/>
-      <c r="AS44" s="161"/>
-      <c r="AT44" s="127" t="s">
+      <c r="AI44" s="182"/>
+      <c r="AJ44" s="182"/>
+      <c r="AK44" s="182"/>
+      <c r="AL44" s="182"/>
+      <c r="AM44" s="182"/>
+      <c r="AN44" s="182"/>
+      <c r="AO44" s="182"/>
+      <c r="AP44" s="182"/>
+      <c r="AQ44" s="182"/>
+      <c r="AR44" s="182"/>
+      <c r="AS44" s="183"/>
+      <c r="AT44" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="AU44" s="128"/>
-      <c r="AV44" s="123" t="s">
+      <c r="AU44" s="140"/>
+      <c r="AV44" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AW44" s="124"/>
-      <c r="AX44" s="159" t="s">
+      <c r="AW44" s="136"/>
+      <c r="AX44" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="AY44" s="160"/>
-      <c r="AZ44" s="160"/>
-      <c r="BA44" s="160"/>
-      <c r="BB44" s="160"/>
-      <c r="BC44" s="160"/>
-      <c r="BD44" s="161"/>
+      <c r="AY44" s="182"/>
+      <c r="AZ44" s="182"/>
+      <c r="BA44" s="182"/>
+      <c r="BB44" s="182"/>
+      <c r="BC44" s="182"/>
+      <c r="BD44" s="183"/>
       <c r="BE44" s="103"/>
       <c r="BF44" s="103"/>
       <c r="BG44" s="103"/>
@@ -8968,10 +9089,10 @@
         <v>352</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="140" t="s">
+      <c r="E45" s="174" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="140"/>
+      <c r="F45" s="174"/>
       <c r="G45" s="113" t="s">
         <v>321</v>
       </c>
@@ -8987,10 +9108,10 @@
       <c r="Q45" s="116"/>
       <c r="R45" s="116"/>
       <c r="S45" s="103"/>
-      <c r="T45" s="140" t="s">
+      <c r="T45" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="U45" s="140"/>
+      <c r="U45" s="174"/>
       <c r="V45" s="113" t="s">
         <v>325</v>
       </c>
@@ -9019,10 +9140,10 @@
       <c r="AQ45" s="116"/>
       <c r="AR45" s="116"/>
       <c r="AS45" s="103"/>
-      <c r="AT45" s="140" t="s">
+      <c r="AT45" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="AU45" s="140"/>
+      <c r="AU45" s="174"/>
       <c r="AV45" s="113" t="s">
         <v>320</v>
       </c>
@@ -9051,70 +9172,70 @@
       <c r="F46" s="117" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="159" t="s">
+      <c r="G46" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="H46" s="160"/>
-      <c r="I46" s="160"/>
-      <c r="J46" s="160"/>
-      <c r="K46" s="160"/>
-      <c r="L46" s="160"/>
-      <c r="M46" s="160"/>
-      <c r="N46" s="160"/>
-      <c r="O46" s="160"/>
-      <c r="P46" s="160"/>
-      <c r="Q46" s="160"/>
-      <c r="R46" s="160"/>
-      <c r="S46" s="160"/>
-      <c r="T46" s="160"/>
-      <c r="U46" s="160"/>
-      <c r="V46" s="160"/>
-      <c r="W46" s="160"/>
-      <c r="X46" s="160"/>
-      <c r="Y46" s="160"/>
-      <c r="Z46" s="160"/>
-      <c r="AA46" s="160"/>
-      <c r="AB46" s="160"/>
-      <c r="AC46" s="160"/>
-      <c r="AD46" s="160"/>
-      <c r="AE46" s="161"/>
+      <c r="H46" s="182"/>
+      <c r="I46" s="182"/>
+      <c r="J46" s="182"/>
+      <c r="K46" s="182"/>
+      <c r="L46" s="182"/>
+      <c r="M46" s="182"/>
+      <c r="N46" s="182"/>
+      <c r="O46" s="182"/>
+      <c r="P46" s="182"/>
+      <c r="Q46" s="182"/>
+      <c r="R46" s="182"/>
+      <c r="S46" s="182"/>
+      <c r="T46" s="182"/>
+      <c r="U46" s="182"/>
+      <c r="V46" s="182"/>
+      <c r="W46" s="182"/>
+      <c r="X46" s="182"/>
+      <c r="Y46" s="182"/>
+      <c r="Z46" s="182"/>
+      <c r="AA46" s="182"/>
+      <c r="AB46" s="182"/>
+      <c r="AC46" s="182"/>
+      <c r="AD46" s="182"/>
+      <c r="AE46" s="183"/>
       <c r="AF46" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG46" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH46" s="159" t="s">
+      <c r="AH46" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="AI46" s="160"/>
-      <c r="AJ46" s="160"/>
-      <c r="AK46" s="160"/>
-      <c r="AL46" s="160"/>
-      <c r="AM46" s="160"/>
-      <c r="AN46" s="160"/>
-      <c r="AO46" s="160"/>
-      <c r="AP46" s="160"/>
-      <c r="AQ46" s="160"/>
-      <c r="AR46" s="160"/>
-      <c r="AS46" s="161"/>
-      <c r="AT46" s="127" t="s">
+      <c r="AI46" s="182"/>
+      <c r="AJ46" s="182"/>
+      <c r="AK46" s="182"/>
+      <c r="AL46" s="182"/>
+      <c r="AM46" s="182"/>
+      <c r="AN46" s="182"/>
+      <c r="AO46" s="182"/>
+      <c r="AP46" s="182"/>
+      <c r="AQ46" s="182"/>
+      <c r="AR46" s="182"/>
+      <c r="AS46" s="183"/>
+      <c r="AT46" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="AU46" s="128"/>
-      <c r="AV46" s="123" t="s">
+      <c r="AU46" s="140"/>
+      <c r="AV46" s="135" t="s">
         <v>297</v>
       </c>
-      <c r="AW46" s="124"/>
-      <c r="AX46" s="159" t="s">
+      <c r="AW46" s="136"/>
+      <c r="AX46" s="181" t="s">
         <v>319</v>
       </c>
-      <c r="AY46" s="160"/>
-      <c r="AZ46" s="160"/>
-      <c r="BA46" s="160"/>
-      <c r="BB46" s="160"/>
-      <c r="BC46" s="160"/>
-      <c r="BD46" s="161"/>
+      <c r="AY46" s="182"/>
+      <c r="AZ46" s="182"/>
+      <c r="BA46" s="182"/>
+      <c r="BB46" s="182"/>
+      <c r="BC46" s="182"/>
+      <c r="BD46" s="183"/>
       <c r="BE46" s="103"/>
       <c r="BF46" s="103"/>
       <c r="BG46" s="103"/>
@@ -9171,10 +9292,10 @@
       <c r="AQ47" s="116"/>
       <c r="AR47" s="116"/>
       <c r="AS47" s="103"/>
-      <c r="AT47" s="140" t="s">
+      <c r="AT47" s="174" t="s">
         <v>323</v>
       </c>
-      <c r="AU47" s="140"/>
+      <c r="AU47" s="174"/>
       <c r="AV47" s="113" t="s">
         <v>320</v>
       </c>
@@ -9565,20 +9686,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="130" t="s">
+      <c r="E54" s="128" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="131"/>
-      <c r="I54" s="131"/>
-      <c r="J54" s="131"/>
-      <c r="K54" s="151"/>
-      <c r="L54" s="130" t="s">
+      <c r="F54" s="129"/>
+      <c r="G54" s="129"/>
+      <c r="H54" s="129"/>
+      <c r="I54" s="129"/>
+      <c r="J54" s="129"/>
+      <c r="K54" s="130"/>
+      <c r="L54" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="131"/>
-      <c r="N54" s="132"/>
+      <c r="M54" s="129"/>
+      <c r="N54" s="197"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -9699,20 +9820,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="133" t="s">
+      <c r="E56" s="188" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="134"/>
-      <c r="G56" s="134"/>
-      <c r="H56" s="134"/>
-      <c r="I56" s="134"/>
-      <c r="J56" s="134"/>
-      <c r="K56" s="135"/>
-      <c r="L56" s="133" t="s">
+      <c r="F56" s="190"/>
+      <c r="G56" s="190"/>
+      <c r="H56" s="190"/>
+      <c r="I56" s="190"/>
+      <c r="J56" s="190"/>
+      <c r="K56" s="189"/>
+      <c r="L56" s="188" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="134"/>
-      <c r="N56" s="135"/>
+      <c r="M56" s="190"/>
+      <c r="N56" s="189"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -12184,68 +12305,68 @@
         <v>364</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="130" t="s">
+      <c r="E95" s="128" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="131"/>
-      <c r="G95" s="131"/>
-      <c r="H95" s="131"/>
-      <c r="I95" s="131"/>
-      <c r="J95" s="131"/>
-      <c r="K95" s="151"/>
-      <c r="L95" s="130" t="s">
+      <c r="F95" s="129"/>
+      <c r="G95" s="129"/>
+      <c r="H95" s="129"/>
+      <c r="I95" s="129"/>
+      <c r="J95" s="129"/>
+      <c r="K95" s="130"/>
+      <c r="L95" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="131"/>
-      <c r="N95" s="151"/>
-      <c r="O95" s="141" t="s">
+      <c r="M95" s="129"/>
+      <c r="N95" s="130"/>
+      <c r="O95" s="164" t="s">
         <v>260</v>
       </c>
-      <c r="P95" s="142"/>
-      <c r="Q95" s="142"/>
-      <c r="R95" s="142"/>
-      <c r="S95" s="142"/>
-      <c r="T95" s="143"/>
-      <c r="U95" s="141" t="s">
+      <c r="P95" s="165"/>
+      <c r="Q95" s="165"/>
+      <c r="R95" s="165"/>
+      <c r="S95" s="165"/>
+      <c r="T95" s="166"/>
+      <c r="U95" s="164" t="s">
         <v>260</v>
       </c>
-      <c r="V95" s="142"/>
-      <c r="W95" s="142"/>
-      <c r="X95" s="142"/>
-      <c r="Y95" s="142"/>
-      <c r="Z95" s="142"/>
-      <c r="AA95" s="142"/>
-      <c r="AB95" s="143"/>
-      <c r="AC95" s="141" t="s">
+      <c r="V95" s="165"/>
+      <c r="W95" s="165"/>
+      <c r="X95" s="165"/>
+      <c r="Y95" s="165"/>
+      <c r="Z95" s="165"/>
+      <c r="AA95" s="165"/>
+      <c r="AB95" s="166"/>
+      <c r="AC95" s="164" t="s">
         <v>260</v>
       </c>
-      <c r="AD95" s="142"/>
-      <c r="AE95" s="142"/>
-      <c r="AF95" s="142"/>
-      <c r="AG95" s="142"/>
-      <c r="AH95" s="142"/>
-      <c r="AI95" s="142"/>
-      <c r="AJ95" s="143"/>
-      <c r="AK95" s="141" t="s">
+      <c r="AD95" s="165"/>
+      <c r="AE95" s="165"/>
+      <c r="AF95" s="165"/>
+      <c r="AG95" s="165"/>
+      <c r="AH95" s="165"/>
+      <c r="AI95" s="165"/>
+      <c r="AJ95" s="166"/>
+      <c r="AK95" s="164" t="s">
         <v>260</v>
       </c>
-      <c r="AL95" s="142"/>
-      <c r="AM95" s="142"/>
-      <c r="AN95" s="142"/>
-      <c r="AO95" s="142"/>
-      <c r="AP95" s="142"/>
-      <c r="AQ95" s="142"/>
-      <c r="AR95" s="143"/>
-      <c r="AS95" s="186" t="s">
+      <c r="AL95" s="165"/>
+      <c r="AM95" s="165"/>
+      <c r="AN95" s="165"/>
+      <c r="AO95" s="165"/>
+      <c r="AP95" s="165"/>
+      <c r="AQ95" s="165"/>
+      <c r="AR95" s="166"/>
+      <c r="AS95" s="161" t="s">
         <v>356</v>
       </c>
-      <c r="AT95" s="187"/>
-      <c r="AU95" s="187"/>
-      <c r="AV95" s="187"/>
-      <c r="AW95" s="187"/>
-      <c r="AX95" s="187"/>
-      <c r="AY95" s="187"/>
-      <c r="AZ95" s="188"/>
+      <c r="AT95" s="162"/>
+      <c r="AU95" s="162"/>
+      <c r="AV95" s="162"/>
+      <c r="AW95" s="162"/>
+      <c r="AX95" s="162"/>
+      <c r="AY95" s="162"/>
+      <c r="AZ95" s="163"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -12350,68 +12471,68 @@
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="133" t="s">
+      <c r="E97" s="188" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="134"/>
-      <c r="G97" s="134"/>
-      <c r="H97" s="134"/>
-      <c r="I97" s="134"/>
-      <c r="J97" s="134"/>
-      <c r="K97" s="135"/>
-      <c r="L97" s="133" t="s">
+      <c r="F97" s="190"/>
+      <c r="G97" s="190"/>
+      <c r="H97" s="190"/>
+      <c r="I97" s="190"/>
+      <c r="J97" s="190"/>
+      <c r="K97" s="189"/>
+      <c r="L97" s="188" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="134"/>
-      <c r="N97" s="134"/>
-      <c r="O97" s="133" t="s">
+      <c r="M97" s="190"/>
+      <c r="N97" s="190"/>
+      <c r="O97" s="188" t="s">
         <v>272</v>
       </c>
-      <c r="P97" s="134"/>
-      <c r="Q97" s="134"/>
-      <c r="R97" s="134"/>
-      <c r="S97" s="134"/>
-      <c r="T97" s="135"/>
-      <c r="U97" s="133" t="s">
+      <c r="P97" s="190"/>
+      <c r="Q97" s="190"/>
+      <c r="R97" s="190"/>
+      <c r="S97" s="190"/>
+      <c r="T97" s="189"/>
+      <c r="U97" s="188" t="s">
         <v>229</v>
       </c>
-      <c r="V97" s="134"/>
-      <c r="W97" s="134"/>
-      <c r="X97" s="134"/>
-      <c r="Y97" s="134"/>
-      <c r="Z97" s="134"/>
-      <c r="AA97" s="134"/>
-      <c r="AB97" s="135"/>
-      <c r="AC97" s="133" t="s">
+      <c r="V97" s="190"/>
+      <c r="W97" s="190"/>
+      <c r="X97" s="190"/>
+      <c r="Y97" s="190"/>
+      <c r="Z97" s="190"/>
+      <c r="AA97" s="190"/>
+      <c r="AB97" s="189"/>
+      <c r="AC97" s="188" t="s">
         <v>229</v>
       </c>
-      <c r="AD97" s="134"/>
-      <c r="AE97" s="134"/>
-      <c r="AF97" s="134"/>
-      <c r="AG97" s="134"/>
-      <c r="AH97" s="134"/>
-      <c r="AI97" s="134"/>
-      <c r="AJ97" s="135"/>
-      <c r="AK97" s="133" t="s">
+      <c r="AD97" s="190"/>
+      <c r="AE97" s="190"/>
+      <c r="AF97" s="190"/>
+      <c r="AG97" s="190"/>
+      <c r="AH97" s="190"/>
+      <c r="AI97" s="190"/>
+      <c r="AJ97" s="189"/>
+      <c r="AK97" s="188" t="s">
         <v>229</v>
       </c>
-      <c r="AL97" s="134"/>
-      <c r="AM97" s="134"/>
-      <c r="AN97" s="134"/>
-      <c r="AO97" s="134"/>
-      <c r="AP97" s="134"/>
-      <c r="AQ97" s="134"/>
-      <c r="AR97" s="135"/>
-      <c r="AS97" s="134" t="s">
+      <c r="AL97" s="190"/>
+      <c r="AM97" s="190"/>
+      <c r="AN97" s="190"/>
+      <c r="AO97" s="190"/>
+      <c r="AP97" s="190"/>
+      <c r="AQ97" s="190"/>
+      <c r="AR97" s="189"/>
+      <c r="AS97" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="AT97" s="134"/>
-      <c r="AU97" s="134"/>
-      <c r="AV97" s="134"/>
-      <c r="AW97" s="134"/>
-      <c r="AX97" s="134"/>
-      <c r="AY97" s="134"/>
-      <c r="AZ97" s="135"/>
+      <c r="AT97" s="190"/>
+      <c r="AU97" s="190"/>
+      <c r="AV97" s="190"/>
+      <c r="AW97" s="190"/>
+      <c r="AX97" s="190"/>
+      <c r="AY97" s="190"/>
+      <c r="AZ97" s="189"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -12486,68 +12607,68 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="183" t="s">
+      <c r="E99" s="155" t="s">
         <v>402</v>
       </c>
-      <c r="F99" s="184"/>
-      <c r="G99" s="184"/>
-      <c r="H99" s="184"/>
-      <c r="I99" s="184"/>
-      <c r="J99" s="184"/>
-      <c r="K99" s="185"/>
-      <c r="L99" s="136" t="s">
+      <c r="F99" s="156"/>
+      <c r="G99" s="156"/>
+      <c r="H99" s="156"/>
+      <c r="I99" s="156"/>
+      <c r="J99" s="156"/>
+      <c r="K99" s="157"/>
+      <c r="L99" s="158" t="s">
         <v>246</v>
       </c>
-      <c r="M99" s="137"/>
-      <c r="N99" s="138"/>
-      <c r="O99" s="180" t="s">
+      <c r="M99" s="159"/>
+      <c r="N99" s="160"/>
+      <c r="O99" s="152" t="s">
         <v>235</v>
       </c>
-      <c r="P99" s="181"/>
-      <c r="Q99" s="181"/>
-      <c r="R99" s="181"/>
-      <c r="S99" s="181"/>
-      <c r="T99" s="182"/>
-      <c r="U99" s="180" t="s">
+      <c r="P99" s="153"/>
+      <c r="Q99" s="153"/>
+      <c r="R99" s="153"/>
+      <c r="S99" s="153"/>
+      <c r="T99" s="154"/>
+      <c r="U99" s="152" t="s">
         <v>235</v>
       </c>
-      <c r="V99" s="181"/>
-      <c r="W99" s="181"/>
-      <c r="X99" s="181"/>
-      <c r="Y99" s="181"/>
-      <c r="Z99" s="181"/>
-      <c r="AA99" s="181"/>
-      <c r="AB99" s="182"/>
-      <c r="AC99" s="180" t="s">
+      <c r="V99" s="153"/>
+      <c r="W99" s="153"/>
+      <c r="X99" s="153"/>
+      <c r="Y99" s="153"/>
+      <c r="Z99" s="153"/>
+      <c r="AA99" s="153"/>
+      <c r="AB99" s="154"/>
+      <c r="AC99" s="152" t="s">
         <v>235</v>
       </c>
-      <c r="AD99" s="181"/>
-      <c r="AE99" s="181"/>
-      <c r="AF99" s="181"/>
-      <c r="AG99" s="181"/>
-      <c r="AH99" s="181"/>
-      <c r="AI99" s="181"/>
-      <c r="AJ99" s="182"/>
-      <c r="AK99" s="180" t="s">
+      <c r="AD99" s="153"/>
+      <c r="AE99" s="153"/>
+      <c r="AF99" s="153"/>
+      <c r="AG99" s="153"/>
+      <c r="AH99" s="153"/>
+      <c r="AI99" s="153"/>
+      <c r="AJ99" s="154"/>
+      <c r="AK99" s="152" t="s">
         <v>235</v>
       </c>
-      <c r="AL99" s="181"/>
-      <c r="AM99" s="181"/>
-      <c r="AN99" s="181"/>
-      <c r="AO99" s="181"/>
-      <c r="AP99" s="181"/>
-      <c r="AQ99" s="181"/>
-      <c r="AR99" s="182"/>
-      <c r="AS99" s="180" t="s">
+      <c r="AL99" s="153"/>
+      <c r="AM99" s="153"/>
+      <c r="AN99" s="153"/>
+      <c r="AO99" s="153"/>
+      <c r="AP99" s="153"/>
+      <c r="AQ99" s="153"/>
+      <c r="AR99" s="154"/>
+      <c r="AS99" s="152" t="s">
         <v>301</v>
       </c>
-      <c r="AT99" s="181"/>
-      <c r="AU99" s="181"/>
-      <c r="AV99" s="181"/>
-      <c r="AW99" s="181"/>
-      <c r="AX99" s="181"/>
-      <c r="AY99" s="181"/>
-      <c r="AZ99" s="182"/>
+      <c r="AT99" s="153"/>
+      <c r="AU99" s="153"/>
+      <c r="AV99" s="153"/>
+      <c r="AW99" s="153"/>
+      <c r="AX99" s="153"/>
+      <c r="AY99" s="153"/>
+      <c r="AZ99" s="154"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -12689,68 +12810,68 @@
         <v>367</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="130" t="s">
+      <c r="E102" s="128" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="131"/>
-      <c r="G102" s="131"/>
-      <c r="H102" s="131"/>
-      <c r="I102" s="131"/>
-      <c r="J102" s="131"/>
-      <c r="K102" s="151"/>
-      <c r="L102" s="130" t="s">
+      <c r="F102" s="129"/>
+      <c r="G102" s="129"/>
+      <c r="H102" s="129"/>
+      <c r="I102" s="129"/>
+      <c r="J102" s="129"/>
+      <c r="K102" s="130"/>
+      <c r="L102" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="M102" s="131"/>
-      <c r="N102" s="151"/>
-      <c r="O102" s="130" t="s">
+      <c r="M102" s="129"/>
+      <c r="N102" s="130"/>
+      <c r="O102" s="128" t="s">
         <v>232</v>
       </c>
-      <c r="P102" s="131"/>
-      <c r="Q102" s="131"/>
-      <c r="R102" s="151"/>
-      <c r="S102" s="130" t="s">
+      <c r="P102" s="129"/>
+      <c r="Q102" s="129"/>
+      <c r="R102" s="130"/>
+      <c r="S102" s="128" t="s">
         <v>306</v>
       </c>
-      <c r="T102" s="131"/>
-      <c r="U102" s="131"/>
-      <c r="V102" s="131"/>
-      <c r="W102" s="131"/>
-      <c r="X102" s="131"/>
-      <c r="Y102" s="131"/>
-      <c r="Z102" s="131"/>
-      <c r="AA102" s="131"/>
-      <c r="AB102" s="131"/>
-      <c r="AC102" s="131"/>
-      <c r="AD102" s="151"/>
-      <c r="AE102" s="130" t="s">
+      <c r="T102" s="129"/>
+      <c r="U102" s="129"/>
+      <c r="V102" s="129"/>
+      <c r="W102" s="129"/>
+      <c r="X102" s="129"/>
+      <c r="Y102" s="129"/>
+      <c r="Z102" s="129"/>
+      <c r="AA102" s="129"/>
+      <c r="AB102" s="129"/>
+      <c r="AC102" s="129"/>
+      <c r="AD102" s="130"/>
+      <c r="AE102" s="128" t="s">
         <v>307</v>
       </c>
-      <c r="AF102" s="131"/>
-      <c r="AG102" s="131"/>
-      <c r="AH102" s="131"/>
-      <c r="AI102" s="131"/>
-      <c r="AJ102" s="131"/>
-      <c r="AK102" s="131"/>
-      <c r="AL102" s="131"/>
-      <c r="AM102" s="131"/>
-      <c r="AN102" s="131"/>
-      <c r="AO102" s="131"/>
-      <c r="AP102" s="151"/>
-      <c r="AQ102" s="130" t="s">
+      <c r="AF102" s="129"/>
+      <c r="AG102" s="129"/>
+      <c r="AH102" s="129"/>
+      <c r="AI102" s="129"/>
+      <c r="AJ102" s="129"/>
+      <c r="AK102" s="129"/>
+      <c r="AL102" s="129"/>
+      <c r="AM102" s="129"/>
+      <c r="AN102" s="129"/>
+      <c r="AO102" s="129"/>
+      <c r="AP102" s="130"/>
+      <c r="AQ102" s="128" t="s">
         <v>224</v>
       </c>
-      <c r="AR102" s="151"/>
-      <c r="AS102" s="130" t="s">
+      <c r="AR102" s="130"/>
+      <c r="AS102" s="128" t="s">
         <v>234</v>
       </c>
-      <c r="AT102" s="131"/>
-      <c r="AU102" s="131"/>
-      <c r="AV102" s="131"/>
-      <c r="AW102" s="131"/>
-      <c r="AX102" s="131"/>
-      <c r="AY102" s="131"/>
-      <c r="AZ102" s="151"/>
+      <c r="AT102" s="129"/>
+      <c r="AU102" s="129"/>
+      <c r="AV102" s="129"/>
+      <c r="AW102" s="129"/>
+      <c r="AX102" s="129"/>
+      <c r="AY102" s="129"/>
+      <c r="AZ102" s="130"/>
       <c r="BA102" s="42"/>
       <c r="BB102" s="42"/>
       <c r="BC102" s="42"/>
@@ -12853,68 +12974,68 @@
       <c r="B104" s="42"/>
       <c r="C104" s="42"/>
       <c r="D104" s="42"/>
-      <c r="E104" s="133" t="s">
+      <c r="E104" s="188" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="134"/>
-      <c r="G104" s="134"/>
-      <c r="H104" s="134"/>
-      <c r="I104" s="134"/>
-      <c r="J104" s="134"/>
-      <c r="K104" s="135"/>
-      <c r="L104" s="133" t="s">
+      <c r="F104" s="190"/>
+      <c r="G104" s="190"/>
+      <c r="H104" s="190"/>
+      <c r="I104" s="190"/>
+      <c r="J104" s="190"/>
+      <c r="K104" s="189"/>
+      <c r="L104" s="188" t="s">
         <v>226</v>
       </c>
-      <c r="M104" s="134"/>
-      <c r="N104" s="135"/>
-      <c r="O104" s="133" t="s">
+      <c r="M104" s="190"/>
+      <c r="N104" s="189"/>
+      <c r="O104" s="188" t="s">
         <v>227</v>
       </c>
-      <c r="P104" s="134"/>
-      <c r="Q104" s="134"/>
-      <c r="R104" s="135"/>
-      <c r="S104" s="133" t="s">
+      <c r="P104" s="190"/>
+      <c r="Q104" s="190"/>
+      <c r="R104" s="189"/>
+      <c r="S104" s="188" t="s">
         <v>228</v>
       </c>
-      <c r="T104" s="134"/>
-      <c r="U104" s="134"/>
-      <c r="V104" s="134"/>
-      <c r="W104" s="134"/>
-      <c r="X104" s="134"/>
-      <c r="Y104" s="134"/>
-      <c r="Z104" s="134"/>
-      <c r="AA104" s="134"/>
-      <c r="AB104" s="134"/>
-      <c r="AC104" s="134"/>
-      <c r="AD104" s="135"/>
-      <c r="AE104" s="133" t="s">
+      <c r="T104" s="190"/>
+      <c r="U104" s="190"/>
+      <c r="V104" s="190"/>
+      <c r="W104" s="190"/>
+      <c r="X104" s="190"/>
+      <c r="Y104" s="190"/>
+      <c r="Z104" s="190"/>
+      <c r="AA104" s="190"/>
+      <c r="AB104" s="190"/>
+      <c r="AC104" s="190"/>
+      <c r="AD104" s="189"/>
+      <c r="AE104" s="188" t="s">
         <v>228</v>
       </c>
-      <c r="AF104" s="134"/>
-      <c r="AG104" s="134"/>
-      <c r="AH104" s="134"/>
-      <c r="AI104" s="134"/>
-      <c r="AJ104" s="134"/>
-      <c r="AK104" s="134"/>
-      <c r="AL104" s="134"/>
-      <c r="AM104" s="134"/>
-      <c r="AN104" s="134"/>
-      <c r="AO104" s="134"/>
-      <c r="AP104" s="135"/>
-      <c r="AQ104" s="133" t="s">
+      <c r="AF104" s="190"/>
+      <c r="AG104" s="190"/>
+      <c r="AH104" s="190"/>
+      <c r="AI104" s="190"/>
+      <c r="AJ104" s="190"/>
+      <c r="AK104" s="190"/>
+      <c r="AL104" s="190"/>
+      <c r="AM104" s="190"/>
+      <c r="AN104" s="190"/>
+      <c r="AO104" s="190"/>
+      <c r="AP104" s="189"/>
+      <c r="AQ104" s="188" t="s">
         <v>230</v>
       </c>
-      <c r="AR104" s="135"/>
-      <c r="AS104" s="133" t="s">
+      <c r="AR104" s="189"/>
+      <c r="AS104" s="188" t="s">
         <v>229</v>
       </c>
-      <c r="AT104" s="134"/>
-      <c r="AU104" s="134"/>
-      <c r="AV104" s="134"/>
-      <c r="AW104" s="134"/>
-      <c r="AX104" s="134"/>
-      <c r="AY104" s="134"/>
-      <c r="AZ104" s="135"/>
+      <c r="AT104" s="190"/>
+      <c r="AU104" s="190"/>
+      <c r="AV104" s="190"/>
+      <c r="AW104" s="190"/>
+      <c r="AX104" s="190"/>
+      <c r="AY104" s="190"/>
+      <c r="AZ104" s="189"/>
       <c r="BA104" s="42"/>
       <c r="BB104" s="42"/>
       <c r="BC104" s="42"/>
@@ -13000,11 +13121,11 @@
       <c r="I106" s="76"/>
       <c r="J106" s="76"/>
       <c r="K106" s="77"/>
-      <c r="L106" s="136" t="s">
+      <c r="L106" s="158" t="s">
         <v>246</v>
       </c>
-      <c r="M106" s="137"/>
-      <c r="N106" s="138"/>
+      <c r="M106" s="159"/>
+      <c r="N106" s="160"/>
       <c r="O106" s="53"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="50"/>
@@ -13043,16 +13164,16 @@
       <c r="AR106" s="51">
         <v>0</v>
       </c>
-      <c r="AS106" s="189" t="s">
+      <c r="AS106" s="124" t="s">
         <v>231</v>
       </c>
-      <c r="AT106" s="190"/>
-      <c r="AU106" s="190"/>
-      <c r="AV106" s="190"/>
-      <c r="AW106" s="190"/>
-      <c r="AX106" s="190"/>
-      <c r="AY106" s="190"/>
-      <c r="AZ106" s="191"/>
+      <c r="AT106" s="125"/>
+      <c r="AU106" s="125"/>
+      <c r="AV106" s="125"/>
+      <c r="AW106" s="125"/>
+      <c r="AX106" s="125"/>
+      <c r="AY106" s="125"/>
+      <c r="AZ106" s="126"/>
       <c r="BA106" s="50" t="s">
         <v>316</v>
       </c>
@@ -13118,16 +13239,16 @@
       <c r="AR107" s="51">
         <v>1</v>
       </c>
-      <c r="AS107" s="189" t="s">
+      <c r="AS107" s="124" t="s">
         <v>354</v>
       </c>
-      <c r="AT107" s="190"/>
-      <c r="AU107" s="190"/>
-      <c r="AV107" s="190"/>
-      <c r="AW107" s="190"/>
-      <c r="AX107" s="190"/>
-      <c r="AY107" s="190"/>
-      <c r="AZ107" s="191"/>
+      <c r="AT107" s="125"/>
+      <c r="AU107" s="125"/>
+      <c r="AV107" s="125"/>
+      <c r="AW107" s="125"/>
+      <c r="AX107" s="125"/>
+      <c r="AY107" s="125"/>
+      <c r="AZ107" s="126"/>
       <c r="BA107" s="50" t="s">
         <v>298</v>
       </c>
@@ -13195,16 +13316,16 @@
       <c r="AR108" s="51">
         <v>0</v>
       </c>
-      <c r="AS108" s="189" t="s">
+      <c r="AS108" s="124" t="s">
         <v>353</v>
       </c>
-      <c r="AT108" s="190"/>
-      <c r="AU108" s="190"/>
-      <c r="AV108" s="190"/>
-      <c r="AW108" s="190"/>
-      <c r="AX108" s="190"/>
-      <c r="AY108" s="190"/>
-      <c r="AZ108" s="191"/>
+      <c r="AT108" s="125"/>
+      <c r="AU108" s="125"/>
+      <c r="AV108" s="125"/>
+      <c r="AW108" s="125"/>
+      <c r="AX108" s="125"/>
+      <c r="AY108" s="125"/>
+      <c r="AZ108" s="126"/>
       <c r="BA108" s="50" t="s">
         <v>265</v>
       </c>
@@ -13268,16 +13389,16 @@
       <c r="AR109" s="51">
         <v>1</v>
       </c>
-      <c r="AS109" s="189" t="s">
+      <c r="AS109" s="124" t="s">
         <v>233</v>
       </c>
-      <c r="AT109" s="190"/>
-      <c r="AU109" s="190"/>
-      <c r="AV109" s="190"/>
-      <c r="AW109" s="190"/>
-      <c r="AX109" s="190"/>
-      <c r="AY109" s="190"/>
-      <c r="AZ109" s="191"/>
+      <c r="AT109" s="125"/>
+      <c r="AU109" s="125"/>
+      <c r="AV109" s="125"/>
+      <c r="AW109" s="125"/>
+      <c r="AX109" s="125"/>
+      <c r="AY109" s="125"/>
+      <c r="AZ109" s="126"/>
       <c r="BA109" s="50" t="s">
         <v>260</v>
       </c>
@@ -13433,12 +13554,12 @@
       <c r="L112" s="49"/>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
-      <c r="O112" s="177" t="s">
+      <c r="O112" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="P112" s="178"/>
-      <c r="Q112" s="178"/>
-      <c r="R112" s="179"/>
+      <c r="P112" s="150"/>
+      <c r="Q112" s="150"/>
+      <c r="R112" s="151"/>
       <c r="S112" s="50"/>
       <c r="T112" s="50"/>
       <c r="U112" s="50"/>
@@ -13463,20 +13584,20 @@
       <c r="AN112" s="50"/>
       <c r="AO112" s="50"/>
       <c r="AP112" s="50"/>
-      <c r="AQ112" s="172" t="s">
+      <c r="AQ112" s="144" t="s">
         <v>302</v>
       </c>
-      <c r="AR112" s="173"/>
-      <c r="AS112" s="174" t="s">
+      <c r="AR112" s="145"/>
+      <c r="AS112" s="146" t="s">
         <v>299</v>
       </c>
-      <c r="AT112" s="175"/>
-      <c r="AU112" s="175"/>
-      <c r="AV112" s="175"/>
-      <c r="AW112" s="175"/>
-      <c r="AX112" s="175"/>
-      <c r="AY112" s="175"/>
-      <c r="AZ112" s="176"/>
+      <c r="AT112" s="147"/>
+      <c r="AU112" s="147"/>
+      <c r="AV112" s="147"/>
+      <c r="AW112" s="147"/>
+      <c r="AX112" s="147"/>
+      <c r="AY112" s="147"/>
+      <c r="AZ112" s="148"/>
       <c r="BA112" s="42"/>
       <c r="BB112" s="42"/>
       <c r="BC112" s="42"/>
@@ -14677,20 +14798,20 @@
       <c r="AN130" s="42"/>
       <c r="AO130" s="42"/>
       <c r="AP130" s="42"/>
-      <c r="AQ130" s="172" t="s">
+      <c r="AQ130" s="144" t="s">
         <v>304</v>
       </c>
-      <c r="AR130" s="173"/>
-      <c r="AS130" s="174" t="s">
+      <c r="AR130" s="145"/>
+      <c r="AS130" s="146" t="s">
         <v>355</v>
       </c>
-      <c r="AT130" s="175"/>
-      <c r="AU130" s="175"/>
-      <c r="AV130" s="175"/>
-      <c r="AW130" s="175"/>
-      <c r="AX130" s="175"/>
-      <c r="AY130" s="175"/>
-      <c r="AZ130" s="176"/>
+      <c r="AT130" s="147"/>
+      <c r="AU130" s="147"/>
+      <c r="AV130" s="147"/>
+      <c r="AW130" s="147"/>
+      <c r="AX130" s="147"/>
+      <c r="AY130" s="147"/>
+      <c r="AZ130" s="148"/>
       <c r="BA130" s="42"/>
       <c r="BB130" s="42"/>
       <c r="BC130" s="42"/>
@@ -14744,16 +14865,16 @@
       <c r="AP131" s="42"/>
       <c r="AQ131" s="42"/>
       <c r="AR131" s="42"/>
-      <c r="AS131" s="180" t="s">
+      <c r="AS131" s="152" t="s">
         <v>301</v>
       </c>
-      <c r="AT131" s="181"/>
-      <c r="AU131" s="181"/>
-      <c r="AV131" s="181"/>
-      <c r="AW131" s="181"/>
-      <c r="AX131" s="181"/>
-      <c r="AY131" s="181"/>
-      <c r="AZ131" s="182"/>
+      <c r="AT131" s="153"/>
+      <c r="AU131" s="153"/>
+      <c r="AV131" s="153"/>
+      <c r="AW131" s="153"/>
+      <c r="AX131" s="153"/>
+      <c r="AY131" s="153"/>
+      <c r="AZ131" s="154"/>
       <c r="BA131" s="42"/>
       <c r="BB131" s="42"/>
       <c r="BC131" s="42"/>
@@ -14866,20 +14987,20 @@
       <c r="AN133" s="42"/>
       <c r="AO133" s="42"/>
       <c r="AP133" s="42"/>
-      <c r="AQ133" s="172" t="s">
+      <c r="AQ133" s="144" t="s">
         <v>303</v>
       </c>
-      <c r="AR133" s="173"/>
-      <c r="AS133" s="174" t="s">
+      <c r="AR133" s="145"/>
+      <c r="AS133" s="146" t="s">
         <v>305</v>
       </c>
-      <c r="AT133" s="175"/>
-      <c r="AU133" s="175"/>
-      <c r="AV133" s="175"/>
-      <c r="AW133" s="175"/>
-      <c r="AX133" s="175"/>
-      <c r="AY133" s="175"/>
-      <c r="AZ133" s="176"/>
+      <c r="AT133" s="147"/>
+      <c r="AU133" s="147"/>
+      <c r="AV133" s="147"/>
+      <c r="AW133" s="147"/>
+      <c r="AX133" s="147"/>
+      <c r="AY133" s="147"/>
+      <c r="AZ133" s="148"/>
       <c r="BA133" s="42"/>
       <c r="BB133" s="42"/>
       <c r="BC133" s="42"/>
@@ -17502,6 +17623,193 @@
     </row>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="AZ23:BF23"/>
+    <mergeCell ref="BB24:BF24"/>
+    <mergeCell ref="BD25:BF25"/>
+    <mergeCell ref="AD25:AF25"/>
+    <mergeCell ref="L15:AF15"/>
+    <mergeCell ref="N16:AF16"/>
+    <mergeCell ref="P17:AF17"/>
+    <mergeCell ref="P18:AF18"/>
+    <mergeCell ref="AL15:BF15"/>
+    <mergeCell ref="AN16:BF16"/>
+    <mergeCell ref="AP17:BF17"/>
+    <mergeCell ref="AP18:BF18"/>
+    <mergeCell ref="AX22:BF22"/>
+    <mergeCell ref="AJ15:AK15"/>
+    <mergeCell ref="AV22:AW22"/>
+    <mergeCell ref="AH15:AI15"/>
+    <mergeCell ref="AJ16:AK16"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AT22:AU22"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AX23:AY23"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="U95:AB95"/>
+    <mergeCell ref="O95:T95"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="AQ104:AR104"/>
+    <mergeCell ref="AS104:AZ104"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="AS97:AZ97"/>
+    <mergeCell ref="AK97:AR97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="O104:R104"/>
+    <mergeCell ref="S104:AD104"/>
+    <mergeCell ref="AE104:AP104"/>
+    <mergeCell ref="AC97:AJ97"/>
+    <mergeCell ref="U97:AB97"/>
+    <mergeCell ref="O97:T97"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AQ112:AR112"/>
+    <mergeCell ref="AQ130:AR130"/>
+    <mergeCell ref="AQ133:AR133"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="AS112:AZ112"/>
+    <mergeCell ref="O112:R112"/>
+    <mergeCell ref="AS130:AZ130"/>
+    <mergeCell ref="AS131:AZ131"/>
+    <mergeCell ref="AS133:AZ133"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="U99:AB99"/>
+    <mergeCell ref="AC99:AJ99"/>
+    <mergeCell ref="AK99:AR99"/>
+    <mergeCell ref="AS99:AZ99"/>
+    <mergeCell ref="O99:T99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AS95:AZ95"/>
+    <mergeCell ref="AK95:AR95"/>
+    <mergeCell ref="AC95:AJ95"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
     <mergeCell ref="AS109:AZ109"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="S102:AD102"/>
@@ -17526,193 +17834,6 @@
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="Z30:AA30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="AQ112:AR112"/>
-    <mergeCell ref="AQ130:AR130"/>
-    <mergeCell ref="AQ133:AR133"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="AS112:AZ112"/>
-    <mergeCell ref="O112:R112"/>
-    <mergeCell ref="AS130:AZ130"/>
-    <mergeCell ref="AS131:AZ131"/>
-    <mergeCell ref="AS133:AZ133"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="U99:AB99"/>
-    <mergeCell ref="AC99:AJ99"/>
-    <mergeCell ref="AK99:AR99"/>
-    <mergeCell ref="AS99:AZ99"/>
-    <mergeCell ref="O99:T99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AS95:AZ95"/>
-    <mergeCell ref="AK95:AR95"/>
-    <mergeCell ref="AC95:AJ95"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AQ104:AR104"/>
-    <mergeCell ref="AS104:AZ104"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="AS97:AZ97"/>
-    <mergeCell ref="AK97:AR97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="L104:N104"/>
-    <mergeCell ref="O104:R104"/>
-    <mergeCell ref="S104:AD104"/>
-    <mergeCell ref="AE104:AP104"/>
-    <mergeCell ref="AC97:AJ97"/>
-    <mergeCell ref="U97:AB97"/>
-    <mergeCell ref="O97:T97"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="U95:AB95"/>
-    <mergeCell ref="O95:T95"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="AZ23:BF23"/>
-    <mergeCell ref="BB24:BF24"/>
-    <mergeCell ref="BD25:BF25"/>
-    <mergeCell ref="AD25:AF25"/>
-    <mergeCell ref="L15:AF15"/>
-    <mergeCell ref="N16:AF16"/>
-    <mergeCell ref="P17:AF17"/>
-    <mergeCell ref="P18:AF18"/>
-    <mergeCell ref="AL15:BF15"/>
-    <mergeCell ref="AN16:BF16"/>
-    <mergeCell ref="AP17:BF17"/>
-    <mergeCell ref="AP18:BF18"/>
-    <mergeCell ref="AX22:BF22"/>
-    <mergeCell ref="AJ15:AK15"/>
-    <mergeCell ref="AV22:AW22"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AT22:AU22"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AX23:AY23"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[Slot Doc] EN_CS_FLASH on PA07
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D189130-2490-4081-996C-B779A4CFDD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7751CAEB-8A01-4864-9692-FF1280975DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="426">
   <si>
     <t>Timing Slot EFR32x</t>
   </si>
@@ -1342,9 +1342,6 @@
   </si>
   <si>
     <t>P21/F8</t>
-  </si>
-  <si>
-    <t>VCOM RTS</t>
   </si>
   <si>
     <t>VCOM CTS</t>
@@ -1969,7 +1966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2212,16 +2209,34 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2230,38 +2245,41 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2270,6 +2288,81 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2314,15 +2407,6 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2332,107 +2416,24 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2462,13 +2463,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>476</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2506,13 +2507,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>2200409</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2550,13 +2551,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2616,13 +2617,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2682,13 +2683,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2748,13 +2749,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2814,13 +2815,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>249530</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>173313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>589442</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>116163</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2880,13 +2881,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>281280</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>166963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>621192</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>109813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3510,10 +3511,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE48"/>
+  <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4269,7 +4270,7 @@
         <v>62</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K15" s="89" t="s">
         <v>388</v>
@@ -4299,7 +4300,7 @@
         <v>62</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="Y15" s="95" t="s">
         <v>389</v>
@@ -5237,33 +5238,33 @@
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A32" s="118" t="s">
+      <c r="A32" s="198" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="119" t="s">
+      <c r="B32" s="199" t="s">
         <v>403</v>
       </c>
-      <c r="C32" s="118" t="s">
+      <c r="C32" s="198" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="118" t="s">
-        <v>113</v>
-      </c>
-      <c r="E32" s="118" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" s="118"/>
-      <c r="G32" s="118" t="s">
+      <c r="D32" s="198" t="s">
+        <v>420</v>
+      </c>
+      <c r="E32" s="198" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="198"/>
+      <c r="G32" s="198" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="118" t="s">
+      <c r="H32" s="198" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="118" t="s">
+      <c r="I32" s="198" t="s">
         <v>405</v>
       </c>
-      <c r="K32" s="89" t="s">
-        <v>388</v>
+      <c r="K32" s="90" t="s">
+        <v>387</v>
       </c>
       <c r="M32" s="118" t="s">
         <v>103</v>
@@ -5444,7 +5445,7 @@
         <v>391</v>
       </c>
       <c r="Y35" s="98" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
@@ -5507,7 +5508,7 @@
       </c>
       <c r="V36" s="96"/>
       <c r="Y36" s="98" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
@@ -5570,7 +5571,7 @@
       </c>
       <c r="V37" s="96"/>
       <c r="Y37" s="98" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
@@ -5602,7 +5603,7 @@
         <v>391</v>
       </c>
       <c r="I39" s="121" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K39" s="89" t="s">
         <v>388</v>
@@ -5632,7 +5633,7 @@
         <v>391</v>
       </c>
       <c r="U39" s="121" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Y39" s="95" t="s">
         <v>389</v>
@@ -5664,7 +5665,7 @@
         <v>391</v>
       </c>
       <c r="I40" s="121" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K40" s="89" t="s">
         <v>388</v>
@@ -5694,7 +5695,7 @@
         <v>391</v>
       </c>
       <c r="U40" s="121" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Y40" s="95" t="s">
         <v>389</v>
@@ -5709,10 +5710,10 @@
         <v>46</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="14" t="s">
@@ -5737,24 +5738,19 @@
         <v>46</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>421</v>
+        <v>118</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14" t="s">
         <v>62</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="K43" s="90" t="s">
-        <v>387</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="I43" s="14"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
@@ -5765,10 +5761,10 @@
         <v>46</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="14" t="s">
@@ -5785,13 +5781,13 @@
       </c>
       <c r="B45" s="123"/>
       <c r="C45" s="14" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="14" t="s">
@@ -5808,13 +5804,13 @@
       </c>
       <c r="B46" s="123"/>
       <c r="C46" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="14" t="s">
@@ -5824,6 +5820,9 @@
         <v>46</v>
       </c>
       <c r="I46" s="14"/>
+      <c r="K46" s="90" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
@@ -5831,13 +5830,13 @@
       </c>
       <c r="B47" s="123"/>
       <c r="C47" s="14" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="F47" s="14"/>
       <c r="G47" s="14" t="s">
@@ -5848,32 +5847,6 @@
       </c>
       <c r="I47" s="14"/>
       <c r="K47" s="90" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="B48" s="123"/>
-      <c r="C48" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I48" s="14"/>
-      <c r="K48" s="90" t="s">
         <v>387</v>
       </c>
     </row>
@@ -6031,21 +6004,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
-      <c r="S3" s="127"/>
+      <c r="E3" s="196"/>
+      <c r="F3" s="196"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="196"/>
+      <c r="J3" s="196"/>
+      <c r="K3" s="196"/>
+      <c r="L3" s="196"/>
+      <c r="M3" s="196"/>
+      <c r="N3" s="196"/>
+      <c r="O3" s="196"/>
+      <c r="P3" s="196"/>
+      <c r="Q3" s="196"/>
+      <c r="R3" s="196"/>
+      <c r="S3" s="196"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -6153,45 +6126,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="185" t="s">
+      <c r="E5" s="152" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="186"/>
-      <c r="G5" s="186"/>
-      <c r="H5" s="186"/>
-      <c r="I5" s="186"/>
-      <c r="J5" s="187"/>
-      <c r="K5" s="176" t="s">
+      <c r="F5" s="153"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="156" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="193"/>
-      <c r="M5" s="193"/>
-      <c r="N5" s="193"/>
-      <c r="O5" s="177"/>
-      <c r="P5" s="176" t="s">
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="157"/>
+      <c r="P5" s="156" t="s">
         <v>276</v>
       </c>
-      <c r="Q5" s="177"/>
-      <c r="R5" s="178" t="s">
+      <c r="Q5" s="157"/>
+      <c r="R5" s="160" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="179"/>
-      <c r="T5" s="179"/>
-      <c r="U5" s="179"/>
-      <c r="V5" s="179"/>
-      <c r="W5" s="180"/>
-      <c r="X5" s="176" t="s">
+      <c r="S5" s="161"/>
+      <c r="T5" s="161"/>
+      <c r="U5" s="161"/>
+      <c r="V5" s="161"/>
+      <c r="W5" s="162"/>
+      <c r="X5" s="156" t="s">
         <v>270</v>
       </c>
-      <c r="Y5" s="177"/>
-      <c r="Z5" s="185" t="s">
+      <c r="Y5" s="157"/>
+      <c r="Z5" s="152" t="s">
         <v>339</v>
       </c>
-      <c r="AA5" s="186"/>
-      <c r="AB5" s="186"/>
-      <c r="AC5" s="186"/>
-      <c r="AD5" s="186"/>
-      <c r="AE5" s="187"/>
+      <c r="AA5" s="153"/>
+      <c r="AB5" s="153"/>
+      <c r="AC5" s="153"/>
+      <c r="AD5" s="153"/>
+      <c r="AE5" s="154"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -6226,45 +6199,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="192" t="s">
+      <c r="E6" s="133" t="s">
         <v>395</v>
       </c>
-      <c r="F6" s="192"/>
-      <c r="G6" s="192"/>
-      <c r="H6" s="192"/>
-      <c r="I6" s="192"/>
-      <c r="J6" s="192"/>
-      <c r="K6" s="191" t="s">
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
+      <c r="K6" s="143" t="s">
         <v>336</v>
       </c>
-      <c r="L6" s="191"/>
-      <c r="M6" s="191"/>
-      <c r="N6" s="191"/>
-      <c r="O6" s="191"/>
-      <c r="P6" s="191" t="s">
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143" t="s">
         <v>338</v>
       </c>
-      <c r="Q6" s="191"/>
-      <c r="R6" s="192" t="s">
+      <c r="Q6" s="143"/>
+      <c r="R6" s="133" t="s">
         <v>271</v>
       </c>
-      <c r="S6" s="192"/>
-      <c r="T6" s="192"/>
-      <c r="U6" s="192"/>
-      <c r="V6" s="192"/>
-      <c r="W6" s="192"/>
-      <c r="X6" s="192" t="s">
+      <c r="S6" s="133"/>
+      <c r="T6" s="133"/>
+      <c r="U6" s="133"/>
+      <c r="V6" s="133"/>
+      <c r="W6" s="133"/>
+      <c r="X6" s="133" t="s">
         <v>338</v>
       </c>
-      <c r="Y6" s="192"/>
-      <c r="Z6" s="192" t="s">
+      <c r="Y6" s="133"/>
+      <c r="Z6" s="133" t="s">
         <v>395</v>
       </c>
-      <c r="AA6" s="192"/>
-      <c r="AB6" s="192"/>
-      <c r="AC6" s="192"/>
-      <c r="AD6" s="192"/>
-      <c r="AE6" s="192"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="133"/>
+      <c r="AC6" s="133"/>
+      <c r="AD6" s="133"/>
+      <c r="AE6" s="133"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -6305,29 +6278,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="184" t="s">
+      <c r="K7" s="158" t="s">
         <v>337</v>
       </c>
-      <c r="L7" s="184"/>
-      <c r="M7" s="184"/>
-      <c r="N7" s="184"/>
-      <c r="O7" s="184"/>
-      <c r="P7" s="184" t="s">
+      <c r="L7" s="158"/>
+      <c r="M7" s="158"/>
+      <c r="N7" s="158"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="158" t="s">
         <v>337</v>
       </c>
-      <c r="Q7" s="184"/>
-      <c r="R7" s="184" t="s">
+      <c r="Q7" s="158"/>
+      <c r="R7" s="158" t="s">
         <v>278</v>
       </c>
-      <c r="S7" s="184"/>
-      <c r="T7" s="184"/>
-      <c r="U7" s="184"/>
-      <c r="V7" s="184"/>
-      <c r="W7" s="184"/>
-      <c r="X7" s="184" t="s">
+      <c r="S7" s="158"/>
+      <c r="T7" s="158"/>
+      <c r="U7" s="158"/>
+      <c r="V7" s="158"/>
+      <c r="W7" s="158"/>
+      <c r="X7" s="158" t="s">
         <v>337</v>
       </c>
-      <c r="Y7" s="184"/>
+      <c r="Y7" s="158"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -6763,7 +6736,7 @@
       <c r="E14" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="132"/>
+      <c r="F14" s="197"/>
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
@@ -6791,7 +6764,7 @@
       <c r="AE14" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="132"/>
+      <c r="AF14" s="197"/>
       <c r="AG14" s="104"/>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
@@ -6834,67 +6807,67 @@
       <c r="G15" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H15" s="133" t="s">
+      <c r="H15" s="129" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="134"/>
-      <c r="J15" s="135" t="s">
+      <c r="I15" s="130"/>
+      <c r="J15" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="136"/>
-      <c r="L15" s="194"/>
-      <c r="M15" s="195"/>
-      <c r="N15" s="195"/>
-      <c r="O15" s="195"/>
-      <c r="P15" s="195"/>
-      <c r="Q15" s="195"/>
-      <c r="R15" s="195"/>
-      <c r="S15" s="195"/>
-      <c r="T15" s="195"/>
-      <c r="U15" s="195"/>
-      <c r="V15" s="195"/>
-      <c r="W15" s="195"/>
-      <c r="X15" s="195"/>
-      <c r="Y15" s="195"/>
-      <c r="Z15" s="195"/>
-      <c r="AA15" s="195"/>
-      <c r="AB15" s="195"/>
-      <c r="AC15" s="195"/>
-      <c r="AD15" s="195"/>
-      <c r="AE15" s="195"/>
-      <c r="AF15" s="196"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="125"/>
+      <c r="N15" s="125"/>
+      <c r="O15" s="125"/>
+      <c r="P15" s="125"/>
+      <c r="Q15" s="125"/>
+      <c r="R15" s="125"/>
+      <c r="S15" s="125"/>
+      <c r="T15" s="125"/>
+      <c r="U15" s="125"/>
+      <c r="V15" s="125"/>
+      <c r="W15" s="125"/>
+      <c r="X15" s="125"/>
+      <c r="Y15" s="125"/>
+      <c r="Z15" s="125"/>
+      <c r="AA15" s="125"/>
+      <c r="AB15" s="125"/>
+      <c r="AC15" s="125"/>
+      <c r="AD15" s="125"/>
+      <c r="AE15" s="125"/>
+      <c r="AF15" s="126"/>
       <c r="AG15" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="AH15" s="133" t="s">
+      <c r="AH15" s="129" t="s">
         <v>279</v>
       </c>
-      <c r="AI15" s="134"/>
-      <c r="AJ15" s="135" t="s">
+      <c r="AI15" s="130"/>
+      <c r="AJ15" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AK15" s="136"/>
-      <c r="AL15" s="194"/>
-      <c r="AM15" s="195"/>
-      <c r="AN15" s="195"/>
-      <c r="AO15" s="195"/>
-      <c r="AP15" s="195"/>
-      <c r="AQ15" s="195"/>
-      <c r="AR15" s="195"/>
-      <c r="AS15" s="195"/>
-      <c r="AT15" s="195"/>
-      <c r="AU15" s="195"/>
-      <c r="AV15" s="195"/>
-      <c r="AW15" s="195"/>
-      <c r="AX15" s="195"/>
-      <c r="AY15" s="195"/>
-      <c r="AZ15" s="195"/>
-      <c r="BA15" s="195"/>
-      <c r="BB15" s="195"/>
-      <c r="BC15" s="195"/>
-      <c r="BD15" s="195"/>
-      <c r="BE15" s="195"/>
-      <c r="BF15" s="195"/>
+      <c r="AK15" s="128"/>
+      <c r="AL15" s="124"/>
+      <c r="AM15" s="125"/>
+      <c r="AN15" s="125"/>
+      <c r="AO15" s="125"/>
+      <c r="AP15" s="125"/>
+      <c r="AQ15" s="125"/>
+      <c r="AR15" s="125"/>
+      <c r="AS15" s="125"/>
+      <c r="AT15" s="125"/>
+      <c r="AU15" s="125"/>
+      <c r="AV15" s="125"/>
+      <c r="AW15" s="125"/>
+      <c r="AX15" s="125"/>
+      <c r="AY15" s="125"/>
+      <c r="AZ15" s="125"/>
+      <c r="BA15" s="125"/>
+      <c r="BB15" s="125"/>
+      <c r="BC15" s="125"/>
+      <c r="BD15" s="125"/>
+      <c r="BE15" s="125"/>
+      <c r="BF15" s="125"/>
       <c r="BG15" s="103"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -6915,33 +6888,33 @@
         <v>287</v>
       </c>
       <c r="I16" s="110"/>
-      <c r="J16" s="133" t="s">
+      <c r="J16" s="129" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="134"/>
-      <c r="L16" s="135" t="s">
+      <c r="K16" s="130"/>
+      <c r="L16" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="M16" s="136"/>
-      <c r="N16" s="194"/>
-      <c r="O16" s="195"/>
-      <c r="P16" s="195"/>
-      <c r="Q16" s="195"/>
-      <c r="R16" s="195"/>
-      <c r="S16" s="195"/>
-      <c r="T16" s="195"/>
-      <c r="U16" s="195"/>
-      <c r="V16" s="195"/>
-      <c r="W16" s="195"/>
-      <c r="X16" s="195"/>
-      <c r="Y16" s="195"/>
-      <c r="Z16" s="195"/>
-      <c r="AA16" s="195"/>
-      <c r="AB16" s="195"/>
-      <c r="AC16" s="195"/>
-      <c r="AD16" s="195"/>
-      <c r="AE16" s="195"/>
-      <c r="AF16" s="196"/>
+      <c r="M16" s="128"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="125"/>
+      <c r="P16" s="125"/>
+      <c r="Q16" s="125"/>
+      <c r="R16" s="125"/>
+      <c r="S16" s="125"/>
+      <c r="T16" s="125"/>
+      <c r="U16" s="125"/>
+      <c r="V16" s="125"/>
+      <c r="W16" s="125"/>
+      <c r="X16" s="125"/>
+      <c r="Y16" s="125"/>
+      <c r="Z16" s="125"/>
+      <c r="AA16" s="125"/>
+      <c r="AB16" s="125"/>
+      <c r="AC16" s="125"/>
+      <c r="AD16" s="125"/>
+      <c r="AE16" s="125"/>
+      <c r="AF16" s="126"/>
       <c r="AG16" s="106" t="s">
         <v>274</v>
       </c>
@@ -6949,33 +6922,33 @@
         <v>287</v>
       </c>
       <c r="AI16" s="110"/>
-      <c r="AJ16" s="133" t="s">
+      <c r="AJ16" s="129" t="s">
         <v>280</v>
       </c>
-      <c r="AK16" s="134"/>
-      <c r="AL16" s="135" t="s">
+      <c r="AK16" s="130"/>
+      <c r="AL16" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AM16" s="136"/>
-      <c r="AN16" s="194"/>
-      <c r="AO16" s="195"/>
-      <c r="AP16" s="195"/>
-      <c r="AQ16" s="195"/>
-      <c r="AR16" s="195"/>
-      <c r="AS16" s="195"/>
-      <c r="AT16" s="195"/>
-      <c r="AU16" s="195"/>
-      <c r="AV16" s="195"/>
-      <c r="AW16" s="195"/>
-      <c r="AX16" s="195"/>
-      <c r="AY16" s="195"/>
-      <c r="AZ16" s="195"/>
-      <c r="BA16" s="195"/>
-      <c r="BB16" s="195"/>
-      <c r="BC16" s="195"/>
-      <c r="BD16" s="195"/>
-      <c r="BE16" s="195"/>
-      <c r="BF16" s="195"/>
+      <c r="AM16" s="128"/>
+      <c r="AN16" s="124"/>
+      <c r="AO16" s="125"/>
+      <c r="AP16" s="125"/>
+      <c r="AQ16" s="125"/>
+      <c r="AR16" s="125"/>
+      <c r="AS16" s="125"/>
+      <c r="AT16" s="125"/>
+      <c r="AU16" s="125"/>
+      <c r="AV16" s="125"/>
+      <c r="AW16" s="125"/>
+      <c r="AX16" s="125"/>
+      <c r="AY16" s="125"/>
+      <c r="AZ16" s="125"/>
+      <c r="BA16" s="125"/>
+      <c r="BB16" s="125"/>
+      <c r="BC16" s="125"/>
+      <c r="BD16" s="125"/>
+      <c r="BE16" s="125"/>
+      <c r="BF16" s="125"/>
       <c r="BG16" s="103"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -6998,31 +6971,31 @@
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
       <c r="K17" s="110"/>
-      <c r="L17" s="133" t="s">
+      <c r="L17" s="129" t="s">
         <v>281</v>
       </c>
-      <c r="M17" s="134"/>
-      <c r="N17" s="135" t="s">
+      <c r="M17" s="130"/>
+      <c r="N17" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="O17" s="136"/>
-      <c r="P17" s="194"/>
-      <c r="Q17" s="195"/>
-      <c r="R17" s="195"/>
-      <c r="S17" s="195"/>
-      <c r="T17" s="195"/>
-      <c r="U17" s="195"/>
-      <c r="V17" s="195"/>
-      <c r="W17" s="195"/>
-      <c r="X17" s="195"/>
-      <c r="Y17" s="195"/>
-      <c r="Z17" s="195"/>
-      <c r="AA17" s="195"/>
-      <c r="AB17" s="195"/>
-      <c r="AC17" s="195"/>
-      <c r="AD17" s="195"/>
-      <c r="AE17" s="195"/>
-      <c r="AF17" s="196"/>
+      <c r="O17" s="128"/>
+      <c r="P17" s="124"/>
+      <c r="Q17" s="125"/>
+      <c r="R17" s="125"/>
+      <c r="S17" s="125"/>
+      <c r="T17" s="125"/>
+      <c r="U17" s="125"/>
+      <c r="V17" s="125"/>
+      <c r="W17" s="125"/>
+      <c r="X17" s="125"/>
+      <c r="Y17" s="125"/>
+      <c r="Z17" s="125"/>
+      <c r="AA17" s="125"/>
+      <c r="AB17" s="125"/>
+      <c r="AC17" s="125"/>
+      <c r="AD17" s="125"/>
+      <c r="AE17" s="125"/>
+      <c r="AF17" s="126"/>
       <c r="AG17" s="106" t="s">
         <v>274</v>
       </c>
@@ -7032,31 +7005,31 @@
       <c r="AI17" s="111"/>
       <c r="AJ17" s="111"/>
       <c r="AK17" s="110"/>
-      <c r="AL17" s="133" t="s">
+      <c r="AL17" s="129" t="s">
         <v>281</v>
       </c>
-      <c r="AM17" s="134"/>
-      <c r="AN17" s="135" t="s">
+      <c r="AM17" s="130"/>
+      <c r="AN17" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AO17" s="136"/>
-      <c r="AP17" s="194"/>
-      <c r="AQ17" s="195"/>
-      <c r="AR17" s="195"/>
-      <c r="AS17" s="195"/>
-      <c r="AT17" s="195"/>
-      <c r="AU17" s="195"/>
-      <c r="AV17" s="195"/>
-      <c r="AW17" s="195"/>
-      <c r="AX17" s="195"/>
-      <c r="AY17" s="195"/>
-      <c r="AZ17" s="195"/>
-      <c r="BA17" s="195"/>
-      <c r="BB17" s="195"/>
-      <c r="BC17" s="195"/>
-      <c r="BD17" s="195"/>
-      <c r="BE17" s="195"/>
-      <c r="BF17" s="195"/>
+      <c r="AO17" s="128"/>
+      <c r="AP17" s="124"/>
+      <c r="AQ17" s="125"/>
+      <c r="AR17" s="125"/>
+      <c r="AS17" s="125"/>
+      <c r="AT17" s="125"/>
+      <c r="AU17" s="125"/>
+      <c r="AV17" s="125"/>
+      <c r="AW17" s="125"/>
+      <c r="AX17" s="125"/>
+      <c r="AY17" s="125"/>
+      <c r="AZ17" s="125"/>
+      <c r="BA17" s="125"/>
+      <c r="BB17" s="125"/>
+      <c r="BC17" s="125"/>
+      <c r="BD17" s="125"/>
+      <c r="BE17" s="125"/>
+      <c r="BF17" s="125"/>
       <c r="BG17" s="103"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -7084,24 +7057,24 @@
       <c r="N18" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="O18" s="140"/>
-      <c r="P18" s="194"/>
-      <c r="Q18" s="195"/>
-      <c r="R18" s="195"/>
-      <c r="S18" s="195"/>
-      <c r="T18" s="195"/>
-      <c r="U18" s="195"/>
-      <c r="V18" s="195"/>
-      <c r="W18" s="195"/>
-      <c r="X18" s="195"/>
-      <c r="Y18" s="195"/>
-      <c r="Z18" s="195"/>
-      <c r="AA18" s="195"/>
-      <c r="AB18" s="195"/>
-      <c r="AC18" s="195"/>
-      <c r="AD18" s="195"/>
-      <c r="AE18" s="195"/>
-      <c r="AF18" s="196"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="124"/>
+      <c r="Q18" s="125"/>
+      <c r="R18" s="125"/>
+      <c r="S18" s="125"/>
+      <c r="T18" s="125"/>
+      <c r="U18" s="125"/>
+      <c r="V18" s="125"/>
+      <c r="W18" s="125"/>
+      <c r="X18" s="125"/>
+      <c r="Y18" s="125"/>
+      <c r="Z18" s="125"/>
+      <c r="AA18" s="125"/>
+      <c r="AB18" s="125"/>
+      <c r="AC18" s="125"/>
+      <c r="AD18" s="125"/>
+      <c r="AE18" s="125"/>
+      <c r="AF18" s="126"/>
       <c r="AG18" s="106" t="s">
         <v>274</v>
       </c>
@@ -7116,24 +7089,24 @@
       <c r="AN18" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="AO18" s="140"/>
-      <c r="AP18" s="194"/>
-      <c r="AQ18" s="195"/>
-      <c r="AR18" s="195"/>
-      <c r="AS18" s="195"/>
-      <c r="AT18" s="195"/>
-      <c r="AU18" s="195"/>
-      <c r="AV18" s="195"/>
-      <c r="AW18" s="195"/>
-      <c r="AX18" s="195"/>
-      <c r="AY18" s="195"/>
-      <c r="AZ18" s="195"/>
-      <c r="BA18" s="195"/>
-      <c r="BB18" s="195"/>
-      <c r="BC18" s="195"/>
-      <c r="BD18" s="195"/>
-      <c r="BE18" s="195"/>
-      <c r="BF18" s="195"/>
+      <c r="AO18" s="132"/>
+      <c r="AP18" s="124"/>
+      <c r="AQ18" s="125"/>
+      <c r="AR18" s="125"/>
+      <c r="AS18" s="125"/>
+      <c r="AT18" s="125"/>
+      <c r="AU18" s="125"/>
+      <c r="AV18" s="125"/>
+      <c r="AW18" s="125"/>
+      <c r="AX18" s="125"/>
+      <c r="AY18" s="125"/>
+      <c r="AZ18" s="125"/>
+      <c r="BA18" s="125"/>
+      <c r="BB18" s="125"/>
+      <c r="BC18" s="125"/>
+      <c r="BD18" s="125"/>
+      <c r="BE18" s="125"/>
+      <c r="BF18" s="125"/>
       <c r="BG18" s="103"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -7359,23 +7332,23 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
       <c r="S22" s="110"/>
-      <c r="T22" s="133" t="s">
+      <c r="T22" s="129" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="134"/>
-      <c r="V22" s="135" t="s">
+      <c r="U22" s="130"/>
+      <c r="V22" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="W22" s="136"/>
-      <c r="X22" s="194"/>
-      <c r="Y22" s="195"/>
-      <c r="Z22" s="195"/>
-      <c r="AA22" s="195"/>
-      <c r="AB22" s="195"/>
-      <c r="AC22" s="195"/>
-      <c r="AD22" s="195"/>
-      <c r="AE22" s="195"/>
-      <c r="AF22" s="196"/>
+      <c r="W22" s="128"/>
+      <c r="X22" s="124"/>
+      <c r="Y22" s="125"/>
+      <c r="Z22" s="125"/>
+      <c r="AA22" s="125"/>
+      <c r="AB22" s="125"/>
+      <c r="AC22" s="125"/>
+      <c r="AD22" s="125"/>
+      <c r="AE22" s="125"/>
+      <c r="AF22" s="126"/>
       <c r="AG22" s="106" t="s">
         <v>274</v>
       </c>
@@ -7393,23 +7366,23 @@
       <c r="AQ22" s="111"/>
       <c r="AR22" s="111"/>
       <c r="AS22" s="110"/>
-      <c r="AT22" s="133" t="s">
+      <c r="AT22" s="129" t="s">
         <v>283</v>
       </c>
-      <c r="AU22" s="134"/>
-      <c r="AV22" s="135" t="s">
+      <c r="AU22" s="130"/>
+      <c r="AV22" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AW22" s="136"/>
-      <c r="AX22" s="194"/>
-      <c r="AY22" s="195"/>
-      <c r="AZ22" s="195"/>
-      <c r="BA22" s="195"/>
-      <c r="BB22" s="195"/>
-      <c r="BC22" s="195"/>
-      <c r="BD22" s="195"/>
-      <c r="BE22" s="195"/>
-      <c r="BF22" s="195"/>
+      <c r="AW22" s="128"/>
+      <c r="AX22" s="124"/>
+      <c r="AY22" s="125"/>
+      <c r="AZ22" s="125"/>
+      <c r="BA22" s="125"/>
+      <c r="BB22" s="125"/>
+      <c r="BC22" s="125"/>
+      <c r="BD22" s="125"/>
+      <c r="BE22" s="125"/>
+      <c r="BF22" s="125"/>
       <c r="BG22" s="103"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -7442,21 +7415,21 @@
       <c r="S23" s="111"/>
       <c r="T23" s="111"/>
       <c r="U23" s="110"/>
-      <c r="V23" s="133" t="s">
+      <c r="V23" s="129" t="s">
         <v>284</v>
       </c>
-      <c r="W23" s="134"/>
-      <c r="X23" s="135" t="s">
+      <c r="W23" s="130"/>
+      <c r="X23" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="Y23" s="136"/>
-      <c r="Z23" s="194"/>
-      <c r="AA23" s="195"/>
-      <c r="AB23" s="195"/>
-      <c r="AC23" s="195"/>
-      <c r="AD23" s="195"/>
-      <c r="AE23" s="195"/>
-      <c r="AF23" s="196"/>
+      <c r="Y23" s="128"/>
+      <c r="Z23" s="124"/>
+      <c r="AA23" s="125"/>
+      <c r="AB23" s="125"/>
+      <c r="AC23" s="125"/>
+      <c r="AD23" s="125"/>
+      <c r="AE23" s="125"/>
+      <c r="AF23" s="126"/>
       <c r="AG23" s="106" t="s">
         <v>274</v>
       </c>
@@ -7476,21 +7449,21 @@
       <c r="AS23" s="111"/>
       <c r="AT23" s="111"/>
       <c r="AU23" s="110"/>
-      <c r="AV23" s="133" t="s">
+      <c r="AV23" s="129" t="s">
         <v>284</v>
       </c>
-      <c r="AW23" s="134"/>
-      <c r="AX23" s="135" t="s">
+      <c r="AW23" s="130"/>
+      <c r="AX23" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AY23" s="136"/>
-      <c r="AZ23" s="194"/>
-      <c r="BA23" s="195"/>
-      <c r="BB23" s="195"/>
-      <c r="BC23" s="195"/>
-      <c r="BD23" s="195"/>
-      <c r="BE23" s="195"/>
-      <c r="BF23" s="195"/>
+      <c r="AY23" s="128"/>
+      <c r="AZ23" s="124"/>
+      <c r="BA23" s="125"/>
+      <c r="BB23" s="125"/>
+      <c r="BC23" s="125"/>
+      <c r="BD23" s="125"/>
+      <c r="BE23" s="125"/>
+      <c r="BF23" s="125"/>
       <c r="BG23" s="103"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -7525,19 +7498,19 @@
       <c r="U24" s="111"/>
       <c r="V24" s="111"/>
       <c r="W24" s="110"/>
-      <c r="X24" s="133" t="s">
+      <c r="X24" s="129" t="s">
         <v>285</v>
       </c>
-      <c r="Y24" s="134"/>
-      <c r="Z24" s="135" t="s">
+      <c r="Y24" s="130"/>
+      <c r="Z24" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AA24" s="136"/>
-      <c r="AB24" s="194"/>
-      <c r="AC24" s="195"/>
-      <c r="AD24" s="195"/>
-      <c r="AE24" s="195"/>
-      <c r="AF24" s="196"/>
+      <c r="AA24" s="128"/>
+      <c r="AB24" s="124"/>
+      <c r="AC24" s="125"/>
+      <c r="AD24" s="125"/>
+      <c r="AE24" s="125"/>
+      <c r="AF24" s="126"/>
       <c r="AG24" s="106" t="s">
         <v>274</v>
       </c>
@@ -7559,19 +7532,19 @@
       <c r="AU24" s="111"/>
       <c r="AV24" s="111"/>
       <c r="AW24" s="110"/>
-      <c r="AX24" s="133" t="s">
+      <c r="AX24" s="129" t="s">
         <v>285</v>
       </c>
-      <c r="AY24" s="134"/>
-      <c r="AZ24" s="135" t="s">
+      <c r="AY24" s="130"/>
+      <c r="AZ24" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="BA24" s="136"/>
-      <c r="BB24" s="194"/>
-      <c r="BC24" s="195"/>
-      <c r="BD24" s="195"/>
-      <c r="BE24" s="195"/>
-      <c r="BF24" s="195"/>
+      <c r="BA24" s="128"/>
+      <c r="BB24" s="124"/>
+      <c r="BC24" s="125"/>
+      <c r="BD24" s="125"/>
+      <c r="BE24" s="125"/>
+      <c r="BF24" s="125"/>
       <c r="BG24" s="103"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -7611,14 +7584,14 @@
       <c r="Z25" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="AA25" s="140"/>
-      <c r="AB25" s="135" t="s">
+      <c r="AA25" s="132"/>
+      <c r="AB25" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AC25" s="136"/>
-      <c r="AD25" s="194"/>
-      <c r="AE25" s="195"/>
-      <c r="AF25" s="196"/>
+      <c r="AC25" s="128"/>
+      <c r="AD25" s="124"/>
+      <c r="AE25" s="125"/>
+      <c r="AF25" s="126"/>
       <c r="AG25" s="106" t="s">
         <v>274</v>
       </c>
@@ -7645,14 +7618,14 @@
       <c r="AZ25" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="BA25" s="140"/>
-      <c r="BB25" s="135" t="s">
+      <c r="BA25" s="132"/>
+      <c r="BB25" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="BC25" s="136"/>
-      <c r="BD25" s="194"/>
-      <c r="BE25" s="195"/>
-      <c r="BF25" s="195"/>
+      <c r="BC25" s="128"/>
+      <c r="BD25" s="124"/>
+      <c r="BE25" s="125"/>
+      <c r="BF25" s="125"/>
       <c r="BG25" s="103"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -7910,29 +7883,29 @@
         <v>318</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="137" t="s">
+      <c r="E30" s="174" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="138"/>
+      <c r="F30" s="175"/>
       <c r="G30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="137" t="s">
+      <c r="H30" s="174" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="138"/>
-      <c r="J30" s="137" t="s">
+      <c r="I30" s="175"/>
+      <c r="J30" s="174" t="s">
         <v>280</v>
       </c>
-      <c r="K30" s="138"/>
-      <c r="L30" s="137" t="s">
+      <c r="K30" s="175"/>
+      <c r="L30" s="174" t="s">
         <v>281</v>
       </c>
-      <c r="M30" s="138"/>
-      <c r="N30" s="137" t="s">
+      <c r="M30" s="175"/>
+      <c r="N30" s="174" t="s">
         <v>282</v>
       </c>
-      <c r="O30" s="138"/>
+      <c r="O30" s="175"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>239</v>
@@ -7941,50 +7914,50 @@
         <v>239</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="137" t="s">
+      <c r="T30" s="174" t="s">
         <v>283</v>
       </c>
-      <c r="U30" s="138"/>
-      <c r="V30" s="137" t="s">
+      <c r="U30" s="175"/>
+      <c r="V30" s="174" t="s">
         <v>284</v>
       </c>
-      <c r="W30" s="138"/>
-      <c r="X30" s="137" t="s">
+      <c r="W30" s="175"/>
+      <c r="X30" s="174" t="s">
         <v>285</v>
       </c>
-      <c r="Y30" s="138"/>
-      <c r="Z30" s="137" t="s">
+      <c r="Y30" s="175"/>
+      <c r="Z30" s="174" t="s">
         <v>286</v>
       </c>
-      <c r="AA30" s="138"/>
-      <c r="AB30" s="141" t="s">
+      <c r="AA30" s="175"/>
+      <c r="AB30" s="148" t="s">
         <v>297</v>
       </c>
-      <c r="AC30" s="142"/>
-      <c r="AD30" s="143"/>
-      <c r="AE30" s="137" t="s">
+      <c r="AC30" s="149"/>
+      <c r="AD30" s="150"/>
+      <c r="AE30" s="174" t="s">
         <v>273</v>
       </c>
-      <c r="AF30" s="138"/>
+      <c r="AF30" s="175"/>
       <c r="AG30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="AH30" s="137" t="s">
+      <c r="AH30" s="174" t="s">
         <v>279</v>
       </c>
-      <c r="AI30" s="138"/>
-      <c r="AJ30" s="137" t="s">
+      <c r="AI30" s="175"/>
+      <c r="AJ30" s="174" t="s">
         <v>280</v>
       </c>
-      <c r="AK30" s="138"/>
-      <c r="AL30" s="137" t="s">
+      <c r="AK30" s="175"/>
+      <c r="AL30" s="174" t="s">
         <v>281</v>
       </c>
-      <c r="AM30" s="138"/>
-      <c r="AN30" s="137" t="s">
+      <c r="AM30" s="175"/>
+      <c r="AN30" s="174" t="s">
         <v>282</v>
       </c>
-      <c r="AO30" s="138"/>
+      <c r="AO30" s="175"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>239</v>
@@ -7993,27 +7966,27 @@
         <v>239</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="137" t="s">
+      <c r="AT30" s="174" t="s">
         <v>283</v>
       </c>
-      <c r="AU30" s="138"/>
-      <c r="AV30" s="137" t="s">
+      <c r="AU30" s="175"/>
+      <c r="AV30" s="174" t="s">
         <v>284</v>
       </c>
-      <c r="AW30" s="138"/>
-      <c r="AX30" s="137" t="s">
+      <c r="AW30" s="175"/>
+      <c r="AX30" s="174" t="s">
         <v>285</v>
       </c>
-      <c r="AY30" s="138"/>
-      <c r="AZ30" s="137" t="s">
+      <c r="AY30" s="175"/>
+      <c r="AZ30" s="174" t="s">
         <v>286</v>
       </c>
-      <c r="BA30" s="138"/>
-      <c r="BB30" s="141" t="s">
+      <c r="BA30" s="175"/>
+      <c r="BB30" s="148" t="s">
         <v>297</v>
       </c>
-      <c r="BC30" s="142"/>
-      <c r="BD30" s="143"/>
+      <c r="BC30" s="149"/>
+      <c r="BD30" s="150"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -8025,10 +7998,10 @@
         <v>317</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="139" t="s">
+      <c r="E31" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="F31" s="139"/>
+      <c r="F31" s="151"/>
       <c r="G31" s="22" t="s">
         <v>324</v>
       </c>
@@ -8055,10 +8028,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="139" t="s">
+      <c r="AE31" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="AF31" s="139"/>
+      <c r="AF31" s="151"/>
       <c r="AG31" s="22" t="s">
         <v>324</v>
       </c>
@@ -8168,75 +8141,75 @@
       <c r="G33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="H33" s="167" t="s">
+      <c r="H33" s="171" t="s">
         <v>319</v>
       </c>
-      <c r="I33" s="168"/>
-      <c r="J33" s="168"/>
-      <c r="K33" s="168"/>
-      <c r="L33" s="168"/>
-      <c r="M33" s="168"/>
-      <c r="N33" s="168"/>
-      <c r="O33" s="168"/>
-      <c r="P33" s="168"/>
-      <c r="Q33" s="168"/>
-      <c r="R33" s="168"/>
-      <c r="S33" s="169"/>
-      <c r="T33" s="137" t="s">
+      <c r="I33" s="172"/>
+      <c r="J33" s="172"/>
+      <c r="K33" s="172"/>
+      <c r="L33" s="172"/>
+      <c r="M33" s="172"/>
+      <c r="N33" s="172"/>
+      <c r="O33" s="172"/>
+      <c r="P33" s="172"/>
+      <c r="Q33" s="172"/>
+      <c r="R33" s="172"/>
+      <c r="S33" s="173"/>
+      <c r="T33" s="174" t="s">
         <v>275</v>
       </c>
-      <c r="U33" s="138"/>
-      <c r="V33" s="141" t="s">
+      <c r="U33" s="175"/>
+      <c r="V33" s="148" t="s">
         <v>297</v>
       </c>
-      <c r="W33" s="143"/>
-      <c r="X33" s="167" t="s">
+      <c r="W33" s="150"/>
+      <c r="X33" s="171" t="s">
         <v>319</v>
       </c>
-      <c r="Y33" s="168"/>
-      <c r="Z33" s="168"/>
-      <c r="AA33" s="168"/>
-      <c r="AB33" s="168"/>
-      <c r="AC33" s="168"/>
-      <c r="AD33" s="168"/>
-      <c r="AE33" s="169"/>
+      <c r="Y33" s="172"/>
+      <c r="Z33" s="172"/>
+      <c r="AA33" s="172"/>
+      <c r="AB33" s="172"/>
+      <c r="AC33" s="172"/>
+      <c r="AD33" s="172"/>
+      <c r="AE33" s="173"/>
       <c r="AF33" s="24" t="s">
         <v>273</v>
       </c>
       <c r="AG33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="AH33" s="167" t="s">
+      <c r="AH33" s="171" t="s">
         <v>319</v>
       </c>
-      <c r="AI33" s="168"/>
-      <c r="AJ33" s="168"/>
-      <c r="AK33" s="168"/>
-      <c r="AL33" s="168"/>
-      <c r="AM33" s="168"/>
-      <c r="AN33" s="168"/>
-      <c r="AO33" s="168"/>
-      <c r="AP33" s="168"/>
-      <c r="AQ33" s="168"/>
-      <c r="AR33" s="168"/>
-      <c r="AS33" s="169"/>
-      <c r="AT33" s="137" t="s">
+      <c r="AI33" s="172"/>
+      <c r="AJ33" s="172"/>
+      <c r="AK33" s="172"/>
+      <c r="AL33" s="172"/>
+      <c r="AM33" s="172"/>
+      <c r="AN33" s="172"/>
+      <c r="AO33" s="172"/>
+      <c r="AP33" s="172"/>
+      <c r="AQ33" s="172"/>
+      <c r="AR33" s="172"/>
+      <c r="AS33" s="173"/>
+      <c r="AT33" s="174" t="s">
         <v>275</v>
       </c>
-      <c r="AU33" s="138"/>
-      <c r="AV33" s="141" t="s">
+      <c r="AU33" s="175"/>
+      <c r="AV33" s="148" t="s">
         <v>297</v>
       </c>
-      <c r="AW33" s="143"/>
-      <c r="AX33" s="167" t="s">
+      <c r="AW33" s="150"/>
+      <c r="AX33" s="171" t="s">
         <v>319</v>
       </c>
-      <c r="AY33" s="168"/>
-      <c r="AZ33" s="168"/>
-      <c r="BA33" s="168"/>
-      <c r="BB33" s="168"/>
-      <c r="BC33" s="168"/>
-      <c r="BD33" s="169"/>
+      <c r="AY33" s="172"/>
+      <c r="AZ33" s="172"/>
+      <c r="BA33" s="172"/>
+      <c r="BB33" s="172"/>
+      <c r="BC33" s="172"/>
+      <c r="BD33" s="173"/>
       <c r="BE33" s="7"/>
       <c r="BF33" s="7"/>
       <c r="BG33" s="7"/>
@@ -8248,10 +8221,10 @@
         <v>317</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="139" t="s">
+      <c r="E34" s="151" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="139"/>
+      <c r="F34" s="151"/>
       <c r="G34" s="22" t="s">
         <v>321</v>
       </c>
@@ -8267,10 +8240,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="139" t="s">
+      <c r="T34" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="U34" s="139"/>
+      <c r="U34" s="151"/>
       <c r="V34" s="22" t="s">
         <v>325</v>
       </c>
@@ -8299,10 +8272,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="139" t="s">
+      <c r="AT34" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="AU34" s="139"/>
+      <c r="AU34" s="151"/>
       <c r="AV34" s="22" t="s">
         <v>320</v>
       </c>
@@ -8573,33 +8546,33 @@
         <v>326</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="170" t="s">
+      <c r="E39" s="166" t="s">
         <v>273</v>
       </c>
-      <c r="F39" s="171"/>
-      <c r="G39" s="172" t="s">
+      <c r="F39" s="167"/>
+      <c r="G39" s="169" t="s">
         <v>273</v>
       </c>
-      <c r="H39" s="173"/>
+      <c r="H39" s="170"/>
       <c r="I39" s="100" t="s">
         <v>319</v>
       </c>
       <c r="J39" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="K39" s="140"/>
+      <c r="K39" s="132"/>
       <c r="L39" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="M39" s="140"/>
+      <c r="M39" s="132"/>
       <c r="N39" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="O39" s="140"/>
+      <c r="O39" s="132"/>
       <c r="P39" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="Q39" s="140"/>
+      <c r="Q39" s="132"/>
       <c r="R39" s="103"/>
       <c r="S39" s="103" t="s">
         <v>239</v>
@@ -8611,47 +8584,47 @@
       <c r="V39" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="W39" s="140"/>
+      <c r="W39" s="132"/>
       <c r="X39" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="Y39" s="140"/>
+      <c r="Y39" s="132"/>
       <c r="Z39" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="AA39" s="140"/>
+      <c r="AA39" s="132"/>
       <c r="AB39" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="AC39" s="140"/>
-      <c r="AD39" s="135" t="s">
+      <c r="AC39" s="132"/>
+      <c r="AD39" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AE39" s="175"/>
-      <c r="AF39" s="136"/>
+      <c r="AE39" s="168"/>
+      <c r="AF39" s="128"/>
       <c r="AG39" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="AH39" s="140"/>
+      <c r="AH39" s="132"/>
       <c r="AI39" s="112" t="s">
         <v>319</v>
       </c>
       <c r="AJ39" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="AK39" s="140"/>
+      <c r="AK39" s="132"/>
       <c r="AL39" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="AM39" s="140"/>
+      <c r="AM39" s="132"/>
       <c r="AN39" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="AO39" s="140"/>
+      <c r="AO39" s="132"/>
       <c r="AP39" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="AQ39" s="140"/>
+      <c r="AQ39" s="132"/>
       <c r="AR39" s="103"/>
       <c r="AS39" s="103" t="s">
         <v>239</v>
@@ -8680,14 +8653,14 @@
         <v>351</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="174" t="s">
+      <c r="E40" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="174"/>
-      <c r="G40" s="174" t="s">
+      <c r="F40" s="144"/>
+      <c r="G40" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="H40" s="174"/>
+      <c r="H40" s="144"/>
       <c r="I40" s="113" t="s">
         <v>324</v>
       </c>
@@ -8714,10 +8687,10 @@
       <c r="AD40" s="103"/>
       <c r="AE40" s="103"/>
       <c r="AF40" s="103"/>
-      <c r="AG40" s="174" t="s">
+      <c r="AG40" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="AH40" s="174"/>
+      <c r="AH40" s="144"/>
       <c r="AI40" s="113" t="s">
         <v>328</v>
       </c>
@@ -8756,24 +8729,24 @@
       <c r="E41" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="140"/>
+      <c r="F41" s="132"/>
       <c r="G41" s="100" t="s">
         <v>319</v>
       </c>
       <c r="H41" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="I41" s="140"/>
+      <c r="I41" s="132"/>
       <c r="J41" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="K41" s="140"/>
-      <c r="L41" s="170"/>
-      <c r="M41" s="171"/>
-      <c r="N41" s="172" t="s">
+      <c r="K41" s="132"/>
+      <c r="L41" s="166"/>
+      <c r="M41" s="167"/>
+      <c r="N41" s="169" t="s">
         <v>282</v>
       </c>
-      <c r="O41" s="173"/>
+      <c r="O41" s="170"/>
       <c r="P41" s="103"/>
       <c r="Q41" s="103" t="s">
         <v>239</v>
@@ -8785,47 +8758,47 @@
       <c r="T41" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="U41" s="140"/>
+      <c r="U41" s="132"/>
       <c r="V41" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="W41" s="140"/>
+      <c r="W41" s="132"/>
       <c r="X41" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="Y41" s="140"/>
+      <c r="Y41" s="132"/>
       <c r="Z41" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="AA41" s="140"/>
-      <c r="AB41" s="135" t="s">
+      <c r="AA41" s="132"/>
+      <c r="AB41" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AC41" s="175"/>
-      <c r="AD41" s="136"/>
+      <c r="AC41" s="168"/>
+      <c r="AD41" s="128"/>
       <c r="AE41" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="AF41" s="140"/>
+      <c r="AF41" s="132"/>
       <c r="AG41" s="100" t="s">
         <v>319</v>
       </c>
       <c r="AH41" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="AI41" s="140"/>
+      <c r="AI41" s="132"/>
       <c r="AJ41" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="AK41" s="140"/>
+      <c r="AK41" s="132"/>
       <c r="AL41" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="AM41" s="140"/>
+      <c r="AM41" s="132"/>
       <c r="AN41" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="AO41" s="140"/>
+      <c r="AO41" s="132"/>
       <c r="AP41" s="103"/>
       <c r="AQ41" s="103" t="s">
         <v>239</v>
@@ -8837,24 +8810,24 @@
       <c r="AT41" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="AU41" s="140"/>
+      <c r="AU41" s="132"/>
       <c r="AV41" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="AW41" s="140"/>
+      <c r="AW41" s="132"/>
       <c r="AX41" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="AY41" s="140"/>
+      <c r="AY41" s="132"/>
       <c r="AZ41" s="131" t="s">
         <v>286</v>
       </c>
-      <c r="BA41" s="140"/>
-      <c r="BB41" s="135" t="s">
+      <c r="BA41" s="132"/>
+      <c r="BB41" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="BC41" s="175"/>
-      <c r="BD41" s="136"/>
+      <c r="BC41" s="168"/>
+      <c r="BD41" s="128"/>
       <c r="BE41" s="103"/>
       <c r="BF41" s="103"/>
       <c r="BG41" s="103"/>
@@ -8866,10 +8839,10 @@
         <v>352</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="174" t="s">
+      <c r="E42" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="174"/>
+      <c r="F42" s="144"/>
       <c r="G42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8896,10 +8869,10 @@
       <c r="AB42" s="103"/>
       <c r="AC42" s="103"/>
       <c r="AD42" s="103"/>
-      <c r="AE42" s="174" t="s">
+      <c r="AE42" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="AF42" s="174"/>
+      <c r="AF42" s="144"/>
       <c r="AG42" s="113" t="s">
         <v>324</v>
       </c>
@@ -9009,75 +8982,75 @@
       <c r="G44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="181" t="s">
+      <c r="H44" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="I44" s="182"/>
-      <c r="J44" s="182"/>
-      <c r="K44" s="182"/>
-      <c r="L44" s="182"/>
-      <c r="M44" s="182"/>
-      <c r="N44" s="182"/>
-      <c r="O44" s="182"/>
-      <c r="P44" s="182"/>
-      <c r="Q44" s="182"/>
-      <c r="R44" s="182"/>
-      <c r="S44" s="183"/>
-      <c r="T44" s="170" t="s">
+      <c r="I44" s="164"/>
+      <c r="J44" s="164"/>
+      <c r="K44" s="164"/>
+      <c r="L44" s="164"/>
+      <c r="M44" s="164"/>
+      <c r="N44" s="164"/>
+      <c r="O44" s="164"/>
+      <c r="P44" s="164"/>
+      <c r="Q44" s="164"/>
+      <c r="R44" s="164"/>
+      <c r="S44" s="165"/>
+      <c r="T44" s="166" t="s">
         <v>275</v>
       </c>
-      <c r="U44" s="171"/>
-      <c r="V44" s="135" t="s">
+      <c r="U44" s="167"/>
+      <c r="V44" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="W44" s="136"/>
-      <c r="X44" s="181" t="s">
+      <c r="W44" s="128"/>
+      <c r="X44" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="Y44" s="182"/>
-      <c r="Z44" s="182"/>
-      <c r="AA44" s="182"/>
-      <c r="AB44" s="182"/>
-      <c r="AC44" s="182"/>
-      <c r="AD44" s="182"/>
-      <c r="AE44" s="183"/>
+      <c r="Y44" s="164"/>
+      <c r="Z44" s="164"/>
+      <c r="AA44" s="164"/>
+      <c r="AB44" s="164"/>
+      <c r="AC44" s="164"/>
+      <c r="AD44" s="164"/>
+      <c r="AE44" s="165"/>
       <c r="AF44" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH44" s="181" t="s">
+      <c r="AH44" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="AI44" s="182"/>
-      <c r="AJ44" s="182"/>
-      <c r="AK44" s="182"/>
-      <c r="AL44" s="182"/>
-      <c r="AM44" s="182"/>
-      <c r="AN44" s="182"/>
-      <c r="AO44" s="182"/>
-      <c r="AP44" s="182"/>
-      <c r="AQ44" s="182"/>
-      <c r="AR44" s="182"/>
-      <c r="AS44" s="183"/>
+      <c r="AI44" s="164"/>
+      <c r="AJ44" s="164"/>
+      <c r="AK44" s="164"/>
+      <c r="AL44" s="164"/>
+      <c r="AM44" s="164"/>
+      <c r="AN44" s="164"/>
+      <c r="AO44" s="164"/>
+      <c r="AP44" s="164"/>
+      <c r="AQ44" s="164"/>
+      <c r="AR44" s="164"/>
+      <c r="AS44" s="165"/>
       <c r="AT44" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="AU44" s="140"/>
-      <c r="AV44" s="135" t="s">
+      <c r="AU44" s="132"/>
+      <c r="AV44" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AW44" s="136"/>
-      <c r="AX44" s="181" t="s">
+      <c r="AW44" s="128"/>
+      <c r="AX44" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="AY44" s="182"/>
-      <c r="AZ44" s="182"/>
-      <c r="BA44" s="182"/>
-      <c r="BB44" s="182"/>
-      <c r="BC44" s="182"/>
-      <c r="BD44" s="183"/>
+      <c r="AY44" s="164"/>
+      <c r="AZ44" s="164"/>
+      <c r="BA44" s="164"/>
+      <c r="BB44" s="164"/>
+      <c r="BC44" s="164"/>
+      <c r="BD44" s="165"/>
       <c r="BE44" s="103"/>
       <c r="BF44" s="103"/>
       <c r="BG44" s="103"/>
@@ -9089,10 +9062,10 @@
         <v>352</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="174" t="s">
+      <c r="E45" s="144" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="174"/>
+      <c r="F45" s="144"/>
       <c r="G45" s="113" t="s">
         <v>321</v>
       </c>
@@ -9108,10 +9081,10 @@
       <c r="Q45" s="116"/>
       <c r="R45" s="116"/>
       <c r="S45" s="103"/>
-      <c r="T45" s="174" t="s">
+      <c r="T45" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="U45" s="174"/>
+      <c r="U45" s="144"/>
       <c r="V45" s="113" t="s">
         <v>325</v>
       </c>
@@ -9140,10 +9113,10 @@
       <c r="AQ45" s="116"/>
       <c r="AR45" s="116"/>
       <c r="AS45" s="103"/>
-      <c r="AT45" s="174" t="s">
+      <c r="AT45" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="AU45" s="174"/>
+      <c r="AU45" s="144"/>
       <c r="AV45" s="113" t="s">
         <v>320</v>
       </c>
@@ -9172,70 +9145,70 @@
       <c r="F46" s="117" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="181" t="s">
+      <c r="G46" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="H46" s="182"/>
-      <c r="I46" s="182"/>
-      <c r="J46" s="182"/>
-      <c r="K46" s="182"/>
-      <c r="L46" s="182"/>
-      <c r="M46" s="182"/>
-      <c r="N46" s="182"/>
-      <c r="O46" s="182"/>
-      <c r="P46" s="182"/>
-      <c r="Q46" s="182"/>
-      <c r="R46" s="182"/>
-      <c r="S46" s="182"/>
-      <c r="T46" s="182"/>
-      <c r="U46" s="182"/>
-      <c r="V46" s="182"/>
-      <c r="W46" s="182"/>
-      <c r="X46" s="182"/>
-      <c r="Y46" s="182"/>
-      <c r="Z46" s="182"/>
-      <c r="AA46" s="182"/>
-      <c r="AB46" s="182"/>
-      <c r="AC46" s="182"/>
-      <c r="AD46" s="182"/>
-      <c r="AE46" s="183"/>
+      <c r="H46" s="164"/>
+      <c r="I46" s="164"/>
+      <c r="J46" s="164"/>
+      <c r="K46" s="164"/>
+      <c r="L46" s="164"/>
+      <c r="M46" s="164"/>
+      <c r="N46" s="164"/>
+      <c r="O46" s="164"/>
+      <c r="P46" s="164"/>
+      <c r="Q46" s="164"/>
+      <c r="R46" s="164"/>
+      <c r="S46" s="164"/>
+      <c r="T46" s="164"/>
+      <c r="U46" s="164"/>
+      <c r="V46" s="164"/>
+      <c r="W46" s="164"/>
+      <c r="X46" s="164"/>
+      <c r="Y46" s="164"/>
+      <c r="Z46" s="164"/>
+      <c r="AA46" s="164"/>
+      <c r="AB46" s="164"/>
+      <c r="AC46" s="164"/>
+      <c r="AD46" s="164"/>
+      <c r="AE46" s="165"/>
       <c r="AF46" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG46" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH46" s="181" t="s">
+      <c r="AH46" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="AI46" s="182"/>
-      <c r="AJ46" s="182"/>
-      <c r="AK46" s="182"/>
-      <c r="AL46" s="182"/>
-      <c r="AM46" s="182"/>
-      <c r="AN46" s="182"/>
-      <c r="AO46" s="182"/>
-      <c r="AP46" s="182"/>
-      <c r="AQ46" s="182"/>
-      <c r="AR46" s="182"/>
-      <c r="AS46" s="183"/>
+      <c r="AI46" s="164"/>
+      <c r="AJ46" s="164"/>
+      <c r="AK46" s="164"/>
+      <c r="AL46" s="164"/>
+      <c r="AM46" s="164"/>
+      <c r="AN46" s="164"/>
+      <c r="AO46" s="164"/>
+      <c r="AP46" s="164"/>
+      <c r="AQ46" s="164"/>
+      <c r="AR46" s="164"/>
+      <c r="AS46" s="165"/>
       <c r="AT46" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="AU46" s="140"/>
-      <c r="AV46" s="135" t="s">
+      <c r="AU46" s="132"/>
+      <c r="AV46" s="127" t="s">
         <v>297</v>
       </c>
-      <c r="AW46" s="136"/>
-      <c r="AX46" s="181" t="s">
+      <c r="AW46" s="128"/>
+      <c r="AX46" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="AY46" s="182"/>
-      <c r="AZ46" s="182"/>
-      <c r="BA46" s="182"/>
-      <c r="BB46" s="182"/>
-      <c r="BC46" s="182"/>
-      <c r="BD46" s="183"/>
+      <c r="AY46" s="164"/>
+      <c r="AZ46" s="164"/>
+      <c r="BA46" s="164"/>
+      <c r="BB46" s="164"/>
+      <c r="BC46" s="164"/>
+      <c r="BD46" s="165"/>
       <c r="BE46" s="103"/>
       <c r="BF46" s="103"/>
       <c r="BG46" s="103"/>
@@ -9292,10 +9265,10 @@
       <c r="AQ47" s="116"/>
       <c r="AR47" s="116"/>
       <c r="AS47" s="103"/>
-      <c r="AT47" s="174" t="s">
+      <c r="AT47" s="144" t="s">
         <v>323</v>
       </c>
-      <c r="AU47" s="174"/>
+      <c r="AU47" s="144"/>
       <c r="AV47" s="113" t="s">
         <v>320</v>
       </c>
@@ -9686,20 +9659,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="128" t="s">
+      <c r="E54" s="134" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="129"/>
-      <c r="G54" s="129"/>
-      <c r="H54" s="129"/>
-      <c r="I54" s="129"/>
-      <c r="J54" s="129"/>
-      <c r="K54" s="130"/>
-      <c r="L54" s="128" t="s">
+      <c r="F54" s="135"/>
+      <c r="G54" s="135"/>
+      <c r="H54" s="135"/>
+      <c r="I54" s="135"/>
+      <c r="J54" s="135"/>
+      <c r="K54" s="155"/>
+      <c r="L54" s="134" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="129"/>
-      <c r="N54" s="197"/>
+      <c r="M54" s="135"/>
+      <c r="N54" s="136"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -9820,20 +9793,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="188" t="s">
+      <c r="E56" s="137" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="190"/>
-      <c r="G56" s="190"/>
-      <c r="H56" s="190"/>
-      <c r="I56" s="190"/>
-      <c r="J56" s="190"/>
-      <c r="K56" s="189"/>
-      <c r="L56" s="188" t="s">
+      <c r="F56" s="138"/>
+      <c r="G56" s="138"/>
+      <c r="H56" s="138"/>
+      <c r="I56" s="138"/>
+      <c r="J56" s="138"/>
+      <c r="K56" s="139"/>
+      <c r="L56" s="137" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="190"/>
-      <c r="N56" s="189"/>
+      <c r="M56" s="138"/>
+      <c r="N56" s="139"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -12305,68 +12278,68 @@
         <v>364</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="128" t="s">
+      <c r="E95" s="134" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="129"/>
-      <c r="G95" s="129"/>
-      <c r="H95" s="129"/>
-      <c r="I95" s="129"/>
-      <c r="J95" s="129"/>
-      <c r="K95" s="130"/>
-      <c r="L95" s="128" t="s">
+      <c r="F95" s="135"/>
+      <c r="G95" s="135"/>
+      <c r="H95" s="135"/>
+      <c r="I95" s="135"/>
+      <c r="J95" s="135"/>
+      <c r="K95" s="155"/>
+      <c r="L95" s="134" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="129"/>
-      <c r="N95" s="130"/>
-      <c r="O95" s="164" t="s">
+      <c r="M95" s="135"/>
+      <c r="N95" s="155"/>
+      <c r="O95" s="145" t="s">
         <v>260</v>
       </c>
-      <c r="P95" s="165"/>
-      <c r="Q95" s="165"/>
-      <c r="R95" s="165"/>
-      <c r="S95" s="165"/>
-      <c r="T95" s="166"/>
-      <c r="U95" s="164" t="s">
+      <c r="P95" s="146"/>
+      <c r="Q95" s="146"/>
+      <c r="R95" s="146"/>
+      <c r="S95" s="146"/>
+      <c r="T95" s="147"/>
+      <c r="U95" s="145" t="s">
         <v>260</v>
       </c>
-      <c r="V95" s="165"/>
-      <c r="W95" s="165"/>
-      <c r="X95" s="165"/>
-      <c r="Y95" s="165"/>
-      <c r="Z95" s="165"/>
-      <c r="AA95" s="165"/>
-      <c r="AB95" s="166"/>
-      <c r="AC95" s="164" t="s">
+      <c r="V95" s="146"/>
+      <c r="W95" s="146"/>
+      <c r="X95" s="146"/>
+      <c r="Y95" s="146"/>
+      <c r="Z95" s="146"/>
+      <c r="AA95" s="146"/>
+      <c r="AB95" s="147"/>
+      <c r="AC95" s="145" t="s">
         <v>260</v>
       </c>
-      <c r="AD95" s="165"/>
-      <c r="AE95" s="165"/>
-      <c r="AF95" s="165"/>
-      <c r="AG95" s="165"/>
-      <c r="AH95" s="165"/>
-      <c r="AI95" s="165"/>
-      <c r="AJ95" s="166"/>
-      <c r="AK95" s="164" t="s">
+      <c r="AD95" s="146"/>
+      <c r="AE95" s="146"/>
+      <c r="AF95" s="146"/>
+      <c r="AG95" s="146"/>
+      <c r="AH95" s="146"/>
+      <c r="AI95" s="146"/>
+      <c r="AJ95" s="147"/>
+      <c r="AK95" s="145" t="s">
         <v>260</v>
       </c>
-      <c r="AL95" s="165"/>
-      <c r="AM95" s="165"/>
-      <c r="AN95" s="165"/>
-      <c r="AO95" s="165"/>
-      <c r="AP95" s="165"/>
-      <c r="AQ95" s="165"/>
-      <c r="AR95" s="166"/>
-      <c r="AS95" s="161" t="s">
+      <c r="AL95" s="146"/>
+      <c r="AM95" s="146"/>
+      <c r="AN95" s="146"/>
+      <c r="AO95" s="146"/>
+      <c r="AP95" s="146"/>
+      <c r="AQ95" s="146"/>
+      <c r="AR95" s="147"/>
+      <c r="AS95" s="190" t="s">
         <v>356</v>
       </c>
-      <c r="AT95" s="162"/>
-      <c r="AU95" s="162"/>
-      <c r="AV95" s="162"/>
-      <c r="AW95" s="162"/>
-      <c r="AX95" s="162"/>
-      <c r="AY95" s="162"/>
-      <c r="AZ95" s="163"/>
+      <c r="AT95" s="191"/>
+      <c r="AU95" s="191"/>
+      <c r="AV95" s="191"/>
+      <c r="AW95" s="191"/>
+      <c r="AX95" s="191"/>
+      <c r="AY95" s="191"/>
+      <c r="AZ95" s="192"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -12471,68 +12444,68 @@
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="188" t="s">
+      <c r="E97" s="137" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="190"/>
-      <c r="G97" s="190"/>
-      <c r="H97" s="190"/>
-      <c r="I97" s="190"/>
-      <c r="J97" s="190"/>
-      <c r="K97" s="189"/>
-      <c r="L97" s="188" t="s">
+      <c r="F97" s="138"/>
+      <c r="G97" s="138"/>
+      <c r="H97" s="138"/>
+      <c r="I97" s="138"/>
+      <c r="J97" s="138"/>
+      <c r="K97" s="139"/>
+      <c r="L97" s="137" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="190"/>
-      <c r="N97" s="190"/>
-      <c r="O97" s="188" t="s">
+      <c r="M97" s="138"/>
+      <c r="N97" s="138"/>
+      <c r="O97" s="137" t="s">
         <v>272</v>
       </c>
-      <c r="P97" s="190"/>
-      <c r="Q97" s="190"/>
-      <c r="R97" s="190"/>
-      <c r="S97" s="190"/>
-      <c r="T97" s="189"/>
-      <c r="U97" s="188" t="s">
+      <c r="P97" s="138"/>
+      <c r="Q97" s="138"/>
+      <c r="R97" s="138"/>
+      <c r="S97" s="138"/>
+      <c r="T97" s="139"/>
+      <c r="U97" s="137" t="s">
         <v>229</v>
       </c>
-      <c r="V97" s="190"/>
-      <c r="W97" s="190"/>
-      <c r="X97" s="190"/>
-      <c r="Y97" s="190"/>
-      <c r="Z97" s="190"/>
-      <c r="AA97" s="190"/>
-      <c r="AB97" s="189"/>
-      <c r="AC97" s="188" t="s">
+      <c r="V97" s="138"/>
+      <c r="W97" s="138"/>
+      <c r="X97" s="138"/>
+      <c r="Y97" s="138"/>
+      <c r="Z97" s="138"/>
+      <c r="AA97" s="138"/>
+      <c r="AB97" s="139"/>
+      <c r="AC97" s="137" t="s">
         <v>229</v>
       </c>
-      <c r="AD97" s="190"/>
-      <c r="AE97" s="190"/>
-      <c r="AF97" s="190"/>
-      <c r="AG97" s="190"/>
-      <c r="AH97" s="190"/>
-      <c r="AI97" s="190"/>
-      <c r="AJ97" s="189"/>
-      <c r="AK97" s="188" t="s">
+      <c r="AD97" s="138"/>
+      <c r="AE97" s="138"/>
+      <c r="AF97" s="138"/>
+      <c r="AG97" s="138"/>
+      <c r="AH97" s="138"/>
+      <c r="AI97" s="138"/>
+      <c r="AJ97" s="139"/>
+      <c r="AK97" s="137" t="s">
         <v>229</v>
       </c>
-      <c r="AL97" s="190"/>
-      <c r="AM97" s="190"/>
-      <c r="AN97" s="190"/>
-      <c r="AO97" s="190"/>
-      <c r="AP97" s="190"/>
-      <c r="AQ97" s="190"/>
-      <c r="AR97" s="189"/>
-      <c r="AS97" s="190" t="s">
+      <c r="AL97" s="138"/>
+      <c r="AM97" s="138"/>
+      <c r="AN97" s="138"/>
+      <c r="AO97" s="138"/>
+      <c r="AP97" s="138"/>
+      <c r="AQ97" s="138"/>
+      <c r="AR97" s="139"/>
+      <c r="AS97" s="138" t="s">
         <v>229</v>
       </c>
-      <c r="AT97" s="190"/>
-      <c r="AU97" s="190"/>
-      <c r="AV97" s="190"/>
-      <c r="AW97" s="190"/>
-      <c r="AX97" s="190"/>
-      <c r="AY97" s="190"/>
-      <c r="AZ97" s="189"/>
+      <c r="AT97" s="138"/>
+      <c r="AU97" s="138"/>
+      <c r="AV97" s="138"/>
+      <c r="AW97" s="138"/>
+      <c r="AX97" s="138"/>
+      <c r="AY97" s="138"/>
+      <c r="AZ97" s="139"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -12607,68 +12580,68 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="155" t="s">
+      <c r="E99" s="187" t="s">
         <v>402</v>
       </c>
-      <c r="F99" s="156"/>
-      <c r="G99" s="156"/>
-      <c r="H99" s="156"/>
-      <c r="I99" s="156"/>
-      <c r="J99" s="156"/>
-      <c r="K99" s="157"/>
-      <c r="L99" s="158" t="s">
+      <c r="F99" s="188"/>
+      <c r="G99" s="188"/>
+      <c r="H99" s="188"/>
+      <c r="I99" s="188"/>
+      <c r="J99" s="188"/>
+      <c r="K99" s="189"/>
+      <c r="L99" s="140" t="s">
         <v>246</v>
       </c>
-      <c r="M99" s="159"/>
-      <c r="N99" s="160"/>
-      <c r="O99" s="152" t="s">
+      <c r="M99" s="141"/>
+      <c r="N99" s="142"/>
+      <c r="O99" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="P99" s="153"/>
-      <c r="Q99" s="153"/>
-      <c r="R99" s="153"/>
-      <c r="S99" s="153"/>
-      <c r="T99" s="154"/>
-      <c r="U99" s="152" t="s">
+      <c r="P99" s="185"/>
+      <c r="Q99" s="185"/>
+      <c r="R99" s="185"/>
+      <c r="S99" s="185"/>
+      <c r="T99" s="186"/>
+      <c r="U99" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="V99" s="153"/>
-      <c r="W99" s="153"/>
-      <c r="X99" s="153"/>
-      <c r="Y99" s="153"/>
-      <c r="Z99" s="153"/>
-      <c r="AA99" s="153"/>
-      <c r="AB99" s="154"/>
-      <c r="AC99" s="152" t="s">
+      <c r="V99" s="185"/>
+      <c r="W99" s="185"/>
+      <c r="X99" s="185"/>
+      <c r="Y99" s="185"/>
+      <c r="Z99" s="185"/>
+      <c r="AA99" s="185"/>
+      <c r="AB99" s="186"/>
+      <c r="AC99" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="AD99" s="153"/>
-      <c r="AE99" s="153"/>
-      <c r="AF99" s="153"/>
-      <c r="AG99" s="153"/>
-      <c r="AH99" s="153"/>
-      <c r="AI99" s="153"/>
-      <c r="AJ99" s="154"/>
-      <c r="AK99" s="152" t="s">
+      <c r="AD99" s="185"/>
+      <c r="AE99" s="185"/>
+      <c r="AF99" s="185"/>
+      <c r="AG99" s="185"/>
+      <c r="AH99" s="185"/>
+      <c r="AI99" s="185"/>
+      <c r="AJ99" s="186"/>
+      <c r="AK99" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="AL99" s="153"/>
-      <c r="AM99" s="153"/>
-      <c r="AN99" s="153"/>
-      <c r="AO99" s="153"/>
-      <c r="AP99" s="153"/>
-      <c r="AQ99" s="153"/>
-      <c r="AR99" s="154"/>
-      <c r="AS99" s="152" t="s">
+      <c r="AL99" s="185"/>
+      <c r="AM99" s="185"/>
+      <c r="AN99" s="185"/>
+      <c r="AO99" s="185"/>
+      <c r="AP99" s="185"/>
+      <c r="AQ99" s="185"/>
+      <c r="AR99" s="186"/>
+      <c r="AS99" s="184" t="s">
         <v>301</v>
       </c>
-      <c r="AT99" s="153"/>
-      <c r="AU99" s="153"/>
-      <c r="AV99" s="153"/>
-      <c r="AW99" s="153"/>
-      <c r="AX99" s="153"/>
-      <c r="AY99" s="153"/>
-      <c r="AZ99" s="154"/>
+      <c r="AT99" s="185"/>
+      <c r="AU99" s="185"/>
+      <c r="AV99" s="185"/>
+      <c r="AW99" s="185"/>
+      <c r="AX99" s="185"/>
+      <c r="AY99" s="185"/>
+      <c r="AZ99" s="186"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -12810,68 +12783,68 @@
         <v>367</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="128" t="s">
+      <c r="E102" s="134" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="129"/>
-      <c r="G102" s="129"/>
-      <c r="H102" s="129"/>
-      <c r="I102" s="129"/>
-      <c r="J102" s="129"/>
-      <c r="K102" s="130"/>
-      <c r="L102" s="128" t="s">
+      <c r="F102" s="135"/>
+      <c r="G102" s="135"/>
+      <c r="H102" s="135"/>
+      <c r="I102" s="135"/>
+      <c r="J102" s="135"/>
+      <c r="K102" s="155"/>
+      <c r="L102" s="134" t="s">
         <v>223</v>
       </c>
-      <c r="M102" s="129"/>
-      <c r="N102" s="130"/>
-      <c r="O102" s="128" t="s">
+      <c r="M102" s="135"/>
+      <c r="N102" s="155"/>
+      <c r="O102" s="134" t="s">
         <v>232</v>
       </c>
-      <c r="P102" s="129"/>
-      <c r="Q102" s="129"/>
-      <c r="R102" s="130"/>
-      <c r="S102" s="128" t="s">
+      <c r="P102" s="135"/>
+      <c r="Q102" s="135"/>
+      <c r="R102" s="155"/>
+      <c r="S102" s="134" t="s">
         <v>306</v>
       </c>
-      <c r="T102" s="129"/>
-      <c r="U102" s="129"/>
-      <c r="V102" s="129"/>
-      <c r="W102" s="129"/>
-      <c r="X102" s="129"/>
-      <c r="Y102" s="129"/>
-      <c r="Z102" s="129"/>
-      <c r="AA102" s="129"/>
-      <c r="AB102" s="129"/>
-      <c r="AC102" s="129"/>
-      <c r="AD102" s="130"/>
-      <c r="AE102" s="128" t="s">
+      <c r="T102" s="135"/>
+      <c r="U102" s="135"/>
+      <c r="V102" s="135"/>
+      <c r="W102" s="135"/>
+      <c r="X102" s="135"/>
+      <c r="Y102" s="135"/>
+      <c r="Z102" s="135"/>
+      <c r="AA102" s="135"/>
+      <c r="AB102" s="135"/>
+      <c r="AC102" s="135"/>
+      <c r="AD102" s="155"/>
+      <c r="AE102" s="134" t="s">
         <v>307</v>
       </c>
-      <c r="AF102" s="129"/>
-      <c r="AG102" s="129"/>
-      <c r="AH102" s="129"/>
-      <c r="AI102" s="129"/>
-      <c r="AJ102" s="129"/>
-      <c r="AK102" s="129"/>
-      <c r="AL102" s="129"/>
-      <c r="AM102" s="129"/>
-      <c r="AN102" s="129"/>
-      <c r="AO102" s="129"/>
-      <c r="AP102" s="130"/>
-      <c r="AQ102" s="128" t="s">
+      <c r="AF102" s="135"/>
+      <c r="AG102" s="135"/>
+      <c r="AH102" s="135"/>
+      <c r="AI102" s="135"/>
+      <c r="AJ102" s="135"/>
+      <c r="AK102" s="135"/>
+      <c r="AL102" s="135"/>
+      <c r="AM102" s="135"/>
+      <c r="AN102" s="135"/>
+      <c r="AO102" s="135"/>
+      <c r="AP102" s="155"/>
+      <c r="AQ102" s="134" t="s">
         <v>224</v>
       </c>
-      <c r="AR102" s="130"/>
-      <c r="AS102" s="128" t="s">
+      <c r="AR102" s="155"/>
+      <c r="AS102" s="134" t="s">
         <v>234</v>
       </c>
-      <c r="AT102" s="129"/>
-      <c r="AU102" s="129"/>
-      <c r="AV102" s="129"/>
-      <c r="AW102" s="129"/>
-      <c r="AX102" s="129"/>
-      <c r="AY102" s="129"/>
-      <c r="AZ102" s="130"/>
+      <c r="AT102" s="135"/>
+      <c r="AU102" s="135"/>
+      <c r="AV102" s="135"/>
+      <c r="AW102" s="135"/>
+      <c r="AX102" s="135"/>
+      <c r="AY102" s="135"/>
+      <c r="AZ102" s="155"/>
       <c r="BA102" s="42"/>
       <c r="BB102" s="42"/>
       <c r="BC102" s="42"/>
@@ -12974,68 +12947,68 @@
       <c r="B104" s="42"/>
       <c r="C104" s="42"/>
       <c r="D104" s="42"/>
-      <c r="E104" s="188" t="s">
+      <c r="E104" s="137" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="190"/>
-      <c r="G104" s="190"/>
-      <c r="H104" s="190"/>
-      <c r="I104" s="190"/>
-      <c r="J104" s="190"/>
-      <c r="K104" s="189"/>
-      <c r="L104" s="188" t="s">
+      <c r="F104" s="138"/>
+      <c r="G104" s="138"/>
+      <c r="H104" s="138"/>
+      <c r="I104" s="138"/>
+      <c r="J104" s="138"/>
+      <c r="K104" s="139"/>
+      <c r="L104" s="137" t="s">
         <v>226</v>
       </c>
-      <c r="M104" s="190"/>
-      <c r="N104" s="189"/>
-      <c r="O104" s="188" t="s">
+      <c r="M104" s="138"/>
+      <c r="N104" s="139"/>
+      <c r="O104" s="137" t="s">
         <v>227</v>
       </c>
-      <c r="P104" s="190"/>
-      <c r="Q104" s="190"/>
-      <c r="R104" s="189"/>
-      <c r="S104" s="188" t="s">
+      <c r="P104" s="138"/>
+      <c r="Q104" s="138"/>
+      <c r="R104" s="139"/>
+      <c r="S104" s="137" t="s">
         <v>228</v>
       </c>
-      <c r="T104" s="190"/>
-      <c r="U104" s="190"/>
-      <c r="V104" s="190"/>
-      <c r="W104" s="190"/>
-      <c r="X104" s="190"/>
-      <c r="Y104" s="190"/>
-      <c r="Z104" s="190"/>
-      <c r="AA104" s="190"/>
-      <c r="AB104" s="190"/>
-      <c r="AC104" s="190"/>
-      <c r="AD104" s="189"/>
-      <c r="AE104" s="188" t="s">
+      <c r="T104" s="138"/>
+      <c r="U104" s="138"/>
+      <c r="V104" s="138"/>
+      <c r="W104" s="138"/>
+      <c r="X104" s="138"/>
+      <c r="Y104" s="138"/>
+      <c r="Z104" s="138"/>
+      <c r="AA104" s="138"/>
+      <c r="AB104" s="138"/>
+      <c r="AC104" s="138"/>
+      <c r="AD104" s="139"/>
+      <c r="AE104" s="137" t="s">
         <v>228</v>
       </c>
-      <c r="AF104" s="190"/>
-      <c r="AG104" s="190"/>
-      <c r="AH104" s="190"/>
-      <c r="AI104" s="190"/>
-      <c r="AJ104" s="190"/>
-      <c r="AK104" s="190"/>
-      <c r="AL104" s="190"/>
-      <c r="AM104" s="190"/>
-      <c r="AN104" s="190"/>
-      <c r="AO104" s="190"/>
-      <c r="AP104" s="189"/>
-      <c r="AQ104" s="188" t="s">
+      <c r="AF104" s="138"/>
+      <c r="AG104" s="138"/>
+      <c r="AH104" s="138"/>
+      <c r="AI104" s="138"/>
+      <c r="AJ104" s="138"/>
+      <c r="AK104" s="138"/>
+      <c r="AL104" s="138"/>
+      <c r="AM104" s="138"/>
+      <c r="AN104" s="138"/>
+      <c r="AO104" s="138"/>
+      <c r="AP104" s="139"/>
+      <c r="AQ104" s="137" t="s">
         <v>230</v>
       </c>
-      <c r="AR104" s="189"/>
-      <c r="AS104" s="188" t="s">
+      <c r="AR104" s="139"/>
+      <c r="AS104" s="137" t="s">
         <v>229</v>
       </c>
-      <c r="AT104" s="190"/>
-      <c r="AU104" s="190"/>
-      <c r="AV104" s="190"/>
-      <c r="AW104" s="190"/>
-      <c r="AX104" s="190"/>
-      <c r="AY104" s="190"/>
-      <c r="AZ104" s="189"/>
+      <c r="AT104" s="138"/>
+      <c r="AU104" s="138"/>
+      <c r="AV104" s="138"/>
+      <c r="AW104" s="138"/>
+      <c r="AX104" s="138"/>
+      <c r="AY104" s="138"/>
+      <c r="AZ104" s="139"/>
       <c r="BA104" s="42"/>
       <c r="BB104" s="42"/>
       <c r="BC104" s="42"/>
@@ -13121,11 +13094,11 @@
       <c r="I106" s="76"/>
       <c r="J106" s="76"/>
       <c r="K106" s="77"/>
-      <c r="L106" s="158" t="s">
+      <c r="L106" s="140" t="s">
         <v>246</v>
       </c>
-      <c r="M106" s="159"/>
-      <c r="N106" s="160"/>
+      <c r="M106" s="141"/>
+      <c r="N106" s="142"/>
       <c r="O106" s="53"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="50"/>
@@ -13164,16 +13137,16 @@
       <c r="AR106" s="51">
         <v>0</v>
       </c>
-      <c r="AS106" s="124" t="s">
+      <c r="AS106" s="193" t="s">
         <v>231</v>
       </c>
-      <c r="AT106" s="125"/>
-      <c r="AU106" s="125"/>
-      <c r="AV106" s="125"/>
-      <c r="AW106" s="125"/>
-      <c r="AX106" s="125"/>
-      <c r="AY106" s="125"/>
-      <c r="AZ106" s="126"/>
+      <c r="AT106" s="194"/>
+      <c r="AU106" s="194"/>
+      <c r="AV106" s="194"/>
+      <c r="AW106" s="194"/>
+      <c r="AX106" s="194"/>
+      <c r="AY106" s="194"/>
+      <c r="AZ106" s="195"/>
       <c r="BA106" s="50" t="s">
         <v>316</v>
       </c>
@@ -13239,16 +13212,16 @@
       <c r="AR107" s="51">
         <v>1</v>
       </c>
-      <c r="AS107" s="124" t="s">
+      <c r="AS107" s="193" t="s">
         <v>354</v>
       </c>
-      <c r="AT107" s="125"/>
-      <c r="AU107" s="125"/>
-      <c r="AV107" s="125"/>
-      <c r="AW107" s="125"/>
-      <c r="AX107" s="125"/>
-      <c r="AY107" s="125"/>
-      <c r="AZ107" s="126"/>
+      <c r="AT107" s="194"/>
+      <c r="AU107" s="194"/>
+      <c r="AV107" s="194"/>
+      <c r="AW107" s="194"/>
+      <c r="AX107" s="194"/>
+      <c r="AY107" s="194"/>
+      <c r="AZ107" s="195"/>
       <c r="BA107" s="50" t="s">
         <v>298</v>
       </c>
@@ -13316,16 +13289,16 @@
       <c r="AR108" s="51">
         <v>0</v>
       </c>
-      <c r="AS108" s="124" t="s">
+      <c r="AS108" s="193" t="s">
         <v>353</v>
       </c>
-      <c r="AT108" s="125"/>
-      <c r="AU108" s="125"/>
-      <c r="AV108" s="125"/>
-      <c r="AW108" s="125"/>
-      <c r="AX108" s="125"/>
-      <c r="AY108" s="125"/>
-      <c r="AZ108" s="126"/>
+      <c r="AT108" s="194"/>
+      <c r="AU108" s="194"/>
+      <c r="AV108" s="194"/>
+      <c r="AW108" s="194"/>
+      <c r="AX108" s="194"/>
+      <c r="AY108" s="194"/>
+      <c r="AZ108" s="195"/>
       <c r="BA108" s="50" t="s">
         <v>265</v>
       </c>
@@ -13389,16 +13362,16 @@
       <c r="AR109" s="51">
         <v>1</v>
       </c>
-      <c r="AS109" s="124" t="s">
+      <c r="AS109" s="193" t="s">
         <v>233</v>
       </c>
-      <c r="AT109" s="125"/>
-      <c r="AU109" s="125"/>
-      <c r="AV109" s="125"/>
-      <c r="AW109" s="125"/>
-      <c r="AX109" s="125"/>
-      <c r="AY109" s="125"/>
-      <c r="AZ109" s="126"/>
+      <c r="AT109" s="194"/>
+      <c r="AU109" s="194"/>
+      <c r="AV109" s="194"/>
+      <c r="AW109" s="194"/>
+      <c r="AX109" s="194"/>
+      <c r="AY109" s="194"/>
+      <c r="AZ109" s="195"/>
       <c r="BA109" s="50" t="s">
         <v>260</v>
       </c>
@@ -13554,12 +13527,12 @@
       <c r="L112" s="49"/>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
-      <c r="O112" s="149" t="s">
+      <c r="O112" s="181" t="s">
         <v>232</v>
       </c>
-      <c r="P112" s="150"/>
-      <c r="Q112" s="150"/>
-      <c r="R112" s="151"/>
+      <c r="P112" s="182"/>
+      <c r="Q112" s="182"/>
+      <c r="R112" s="183"/>
       <c r="S112" s="50"/>
       <c r="T112" s="50"/>
       <c r="U112" s="50"/>
@@ -13584,20 +13557,20 @@
       <c r="AN112" s="50"/>
       <c r="AO112" s="50"/>
       <c r="AP112" s="50"/>
-      <c r="AQ112" s="144" t="s">
+      <c r="AQ112" s="176" t="s">
         <v>302</v>
       </c>
-      <c r="AR112" s="145"/>
-      <c r="AS112" s="146" t="s">
+      <c r="AR112" s="177"/>
+      <c r="AS112" s="178" t="s">
         <v>299</v>
       </c>
-      <c r="AT112" s="147"/>
-      <c r="AU112" s="147"/>
-      <c r="AV112" s="147"/>
-      <c r="AW112" s="147"/>
-      <c r="AX112" s="147"/>
-      <c r="AY112" s="147"/>
-      <c r="AZ112" s="148"/>
+      <c r="AT112" s="179"/>
+      <c r="AU112" s="179"/>
+      <c r="AV112" s="179"/>
+      <c r="AW112" s="179"/>
+      <c r="AX112" s="179"/>
+      <c r="AY112" s="179"/>
+      <c r="AZ112" s="180"/>
       <c r="BA112" s="42"/>
       <c r="BB112" s="42"/>
       <c r="BC112" s="42"/>
@@ -14798,20 +14771,20 @@
       <c r="AN130" s="42"/>
       <c r="AO130" s="42"/>
       <c r="AP130" s="42"/>
-      <c r="AQ130" s="144" t="s">
+      <c r="AQ130" s="176" t="s">
         <v>304</v>
       </c>
-      <c r="AR130" s="145"/>
-      <c r="AS130" s="146" t="s">
+      <c r="AR130" s="177"/>
+      <c r="AS130" s="178" t="s">
         <v>355</v>
       </c>
-      <c r="AT130" s="147"/>
-      <c r="AU130" s="147"/>
-      <c r="AV130" s="147"/>
-      <c r="AW130" s="147"/>
-      <c r="AX130" s="147"/>
-      <c r="AY130" s="147"/>
-      <c r="AZ130" s="148"/>
+      <c r="AT130" s="179"/>
+      <c r="AU130" s="179"/>
+      <c r="AV130" s="179"/>
+      <c r="AW130" s="179"/>
+      <c r="AX130" s="179"/>
+      <c r="AY130" s="179"/>
+      <c r="AZ130" s="180"/>
       <c r="BA130" s="42"/>
       <c r="BB130" s="42"/>
       <c r="BC130" s="42"/>
@@ -14865,16 +14838,16 @@
       <c r="AP131" s="42"/>
       <c r="AQ131" s="42"/>
       <c r="AR131" s="42"/>
-      <c r="AS131" s="152" t="s">
+      <c r="AS131" s="184" t="s">
         <v>301</v>
       </c>
-      <c r="AT131" s="153"/>
-      <c r="AU131" s="153"/>
-      <c r="AV131" s="153"/>
-      <c r="AW131" s="153"/>
-      <c r="AX131" s="153"/>
-      <c r="AY131" s="153"/>
-      <c r="AZ131" s="154"/>
+      <c r="AT131" s="185"/>
+      <c r="AU131" s="185"/>
+      <c r="AV131" s="185"/>
+      <c r="AW131" s="185"/>
+      <c r="AX131" s="185"/>
+      <c r="AY131" s="185"/>
+      <c r="AZ131" s="186"/>
       <c r="BA131" s="42"/>
       <c r="BB131" s="42"/>
       <c r="BC131" s="42"/>
@@ -14987,20 +14960,20 @@
       <c r="AN133" s="42"/>
       <c r="AO133" s="42"/>
       <c r="AP133" s="42"/>
-      <c r="AQ133" s="144" t="s">
+      <c r="AQ133" s="176" t="s">
         <v>303</v>
       </c>
-      <c r="AR133" s="145"/>
-      <c r="AS133" s="146" t="s">
+      <c r="AR133" s="177"/>
+      <c r="AS133" s="178" t="s">
         <v>305</v>
       </c>
-      <c r="AT133" s="147"/>
-      <c r="AU133" s="147"/>
-      <c r="AV133" s="147"/>
-      <c r="AW133" s="147"/>
-      <c r="AX133" s="147"/>
-      <c r="AY133" s="147"/>
-      <c r="AZ133" s="148"/>
+      <c r="AT133" s="179"/>
+      <c r="AU133" s="179"/>
+      <c r="AV133" s="179"/>
+      <c r="AW133" s="179"/>
+      <c r="AX133" s="179"/>
+      <c r="AY133" s="179"/>
+      <c r="AZ133" s="180"/>
       <c r="BA133" s="42"/>
       <c r="BB133" s="42"/>
       <c r="BC133" s="42"/>
@@ -17623,6 +17596,193 @@
     </row>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="AS109:AZ109"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="S102:AD102"/>
+    <mergeCell ref="AQ102:AR102"/>
+    <mergeCell ref="AS102:AZ102"/>
+    <mergeCell ref="AE102:AP102"/>
+    <mergeCell ref="E102:K102"/>
+    <mergeCell ref="L102:N102"/>
+    <mergeCell ref="O102:R102"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="AS106:AZ106"/>
+    <mergeCell ref="AS107:AZ107"/>
+    <mergeCell ref="AS108:AZ108"/>
+    <mergeCell ref="AV46:AW46"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE30:AF30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="AQ112:AR112"/>
+    <mergeCell ref="AQ130:AR130"/>
+    <mergeCell ref="AQ133:AR133"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="AS112:AZ112"/>
+    <mergeCell ref="O112:R112"/>
+    <mergeCell ref="AS130:AZ130"/>
+    <mergeCell ref="AS131:AZ131"/>
+    <mergeCell ref="AS133:AZ133"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="U99:AB99"/>
+    <mergeCell ref="AC99:AJ99"/>
+    <mergeCell ref="AK99:AR99"/>
+    <mergeCell ref="AS99:AZ99"/>
+    <mergeCell ref="O99:T99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AS95:AZ95"/>
+    <mergeCell ref="AK95:AR95"/>
+    <mergeCell ref="AC95:AJ95"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="AQ104:AR104"/>
+    <mergeCell ref="AS104:AZ104"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="AS97:AZ97"/>
+    <mergeCell ref="AK97:AR97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="O104:R104"/>
+    <mergeCell ref="S104:AD104"/>
+    <mergeCell ref="AE104:AP104"/>
+    <mergeCell ref="AC97:AJ97"/>
+    <mergeCell ref="U97:AB97"/>
+    <mergeCell ref="O97:T97"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="U95:AB95"/>
+    <mergeCell ref="O95:T95"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
     <mergeCell ref="AZ23:BF23"/>
     <mergeCell ref="BB24:BF24"/>
     <mergeCell ref="BD25:BF25"/>
@@ -17647,193 +17807,6 @@
     <mergeCell ref="AT22:AU22"/>
     <mergeCell ref="AV23:AW23"/>
     <mergeCell ref="AX23:AY23"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="U95:AB95"/>
-    <mergeCell ref="O95:T95"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="AQ104:AR104"/>
-    <mergeCell ref="AS104:AZ104"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="AS97:AZ97"/>
-    <mergeCell ref="AK97:AR97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="L104:N104"/>
-    <mergeCell ref="O104:R104"/>
-    <mergeCell ref="S104:AD104"/>
-    <mergeCell ref="AE104:AP104"/>
-    <mergeCell ref="AC97:AJ97"/>
-    <mergeCell ref="U97:AB97"/>
-    <mergeCell ref="O97:T97"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AQ112:AR112"/>
-    <mergeCell ref="AQ130:AR130"/>
-    <mergeCell ref="AQ133:AR133"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="AS112:AZ112"/>
-    <mergeCell ref="O112:R112"/>
-    <mergeCell ref="AS130:AZ130"/>
-    <mergeCell ref="AS131:AZ131"/>
-    <mergeCell ref="AS133:AZ133"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="U99:AB99"/>
-    <mergeCell ref="AC99:AJ99"/>
-    <mergeCell ref="AK99:AR99"/>
-    <mergeCell ref="AS99:AZ99"/>
-    <mergeCell ref="O99:T99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AS95:AZ95"/>
-    <mergeCell ref="AK95:AR95"/>
-    <mergeCell ref="AC95:AJ95"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="AS109:AZ109"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="S102:AD102"/>
-    <mergeCell ref="AQ102:AR102"/>
-    <mergeCell ref="AS102:AZ102"/>
-    <mergeCell ref="AE102:AP102"/>
-    <mergeCell ref="E102:K102"/>
-    <mergeCell ref="L102:N102"/>
-    <mergeCell ref="O102:R102"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="AS106:AZ106"/>
-    <mergeCell ref="AS107:AZ107"/>
-    <mergeCell ref="AS108:AZ108"/>
-    <mergeCell ref="AV46:AW46"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[Slot Doc] Update spare pin for Master
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7751CAEB-8A01-4864-9692-FF1280975DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2FBC9E-B247-4CA3-ADA4-208A965559BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="426">
   <si>
     <t>Timing Slot EFR32x</t>
   </si>
@@ -2209,13 +2209,41 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2224,62 +2252,17 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2288,81 +2271,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2407,6 +2315,15 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2416,24 +2333,107 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2463,13 +2463,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>476</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2507,13 +2507,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>2200409</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2551,13 +2551,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2617,13 +2617,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2683,13 +2683,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2749,13 +2749,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2815,13 +2815,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>249530</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>173313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>589442</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>116163</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2881,13 +2881,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>281280</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>166963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>621192</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>109813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3511,10 +3511,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE47"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5238,29 +5238,29 @@
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A32" s="198" t="s">
+      <c r="A32" s="124" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="199" t="s">
+      <c r="B32" s="125" t="s">
         <v>403</v>
       </c>
-      <c r="C32" s="198" t="s">
+      <c r="C32" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="198" t="s">
+      <c r="D32" s="124" t="s">
         <v>420</v>
       </c>
-      <c r="E32" s="198" t="s">
+      <c r="E32" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="198"/>
-      <c r="G32" s="198" t="s">
+      <c r="F32" s="124"/>
+      <c r="G32" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="198" t="s">
+      <c r="H32" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="198" t="s">
+      <c r="I32" s="124" t="s">
         <v>405</v>
       </c>
       <c r="K32" s="90" t="s">
@@ -5830,15 +5830,17 @@
       </c>
       <c r="B47" s="123"/>
       <c r="C47" s="14" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F47" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>379</v>
+      </c>
       <c r="G47" s="14" t="s">
         <v>62</v>
       </c>
@@ -5846,7 +5848,30 @@
         <v>46</v>
       </c>
       <c r="I47" s="14"/>
-      <c r="K47" s="90" t="s">
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48" s="123"/>
+      <c r="C48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I48" s="14"/>
+      <c r="K48" s="90" t="s">
         <v>387</v>
       </c>
     </row>
@@ -6004,21 +6029,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="196"/>
-      <c r="O3" s="196"/>
-      <c r="P3" s="196"/>
-      <c r="Q3" s="196"/>
-      <c r="R3" s="196"/>
-      <c r="S3" s="196"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="129"/>
+      <c r="Q3" s="129"/>
+      <c r="R3" s="129"/>
+      <c r="S3" s="129"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -6126,45 +6151,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="152" t="s">
+      <c r="E5" s="187" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="156" t="s">
+      <c r="F5" s="188"/>
+      <c r="G5" s="188"/>
+      <c r="H5" s="188"/>
+      <c r="I5" s="188"/>
+      <c r="J5" s="189"/>
+      <c r="K5" s="178" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="157"/>
-      <c r="P5" s="156" t="s">
+      <c r="L5" s="195"/>
+      <c r="M5" s="195"/>
+      <c r="N5" s="195"/>
+      <c r="O5" s="179"/>
+      <c r="P5" s="178" t="s">
         <v>276</v>
       </c>
-      <c r="Q5" s="157"/>
-      <c r="R5" s="160" t="s">
+      <c r="Q5" s="179"/>
+      <c r="R5" s="180" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="161"/>
-      <c r="T5" s="161"/>
-      <c r="U5" s="161"/>
-      <c r="V5" s="161"/>
-      <c r="W5" s="162"/>
-      <c r="X5" s="156" t="s">
+      <c r="S5" s="181"/>
+      <c r="T5" s="181"/>
+      <c r="U5" s="181"/>
+      <c r="V5" s="181"/>
+      <c r="W5" s="182"/>
+      <c r="X5" s="178" t="s">
         <v>270</v>
       </c>
-      <c r="Y5" s="157"/>
-      <c r="Z5" s="152" t="s">
+      <c r="Y5" s="179"/>
+      <c r="Z5" s="187" t="s">
         <v>339</v>
       </c>
-      <c r="AA5" s="153"/>
-      <c r="AB5" s="153"/>
-      <c r="AC5" s="153"/>
-      <c r="AD5" s="153"/>
-      <c r="AE5" s="154"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="188"/>
+      <c r="AC5" s="188"/>
+      <c r="AD5" s="188"/>
+      <c r="AE5" s="189"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -6199,45 +6224,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="133" t="s">
+      <c r="E6" s="194" t="s">
         <v>395</v>
       </c>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
-      <c r="K6" s="143" t="s">
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="194"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="194"/>
+      <c r="K6" s="193" t="s">
         <v>336</v>
       </c>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="143"/>
-      <c r="P6" s="143" t="s">
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
+      <c r="P6" s="193" t="s">
         <v>338</v>
       </c>
-      <c r="Q6" s="143"/>
-      <c r="R6" s="133" t="s">
+      <c r="Q6" s="193"/>
+      <c r="R6" s="194" t="s">
         <v>271</v>
       </c>
-      <c r="S6" s="133"/>
-      <c r="T6" s="133"/>
-      <c r="U6" s="133"/>
-      <c r="V6" s="133"/>
-      <c r="W6" s="133"/>
-      <c r="X6" s="133" t="s">
+      <c r="S6" s="194"/>
+      <c r="T6" s="194"/>
+      <c r="U6" s="194"/>
+      <c r="V6" s="194"/>
+      <c r="W6" s="194"/>
+      <c r="X6" s="194" t="s">
         <v>338</v>
       </c>
-      <c r="Y6" s="133"/>
-      <c r="Z6" s="133" t="s">
+      <c r="Y6" s="194"/>
+      <c r="Z6" s="194" t="s">
         <v>395</v>
       </c>
-      <c r="AA6" s="133"/>
-      <c r="AB6" s="133"/>
-      <c r="AC6" s="133"/>
-      <c r="AD6" s="133"/>
-      <c r="AE6" s="133"/>
+      <c r="AA6" s="194"/>
+      <c r="AB6" s="194"/>
+      <c r="AC6" s="194"/>
+      <c r="AD6" s="194"/>
+      <c r="AE6" s="194"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -6278,29 +6303,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="158" t="s">
+      <c r="K7" s="186" t="s">
         <v>337</v>
       </c>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="158"/>
-      <c r="P7" s="158" t="s">
+      <c r="L7" s="186"/>
+      <c r="M7" s="186"/>
+      <c r="N7" s="186"/>
+      <c r="O7" s="186"/>
+      <c r="P7" s="186" t="s">
         <v>337</v>
       </c>
-      <c r="Q7" s="158"/>
-      <c r="R7" s="158" t="s">
+      <c r="Q7" s="186"/>
+      <c r="R7" s="186" t="s">
         <v>278</v>
       </c>
-      <c r="S7" s="158"/>
-      <c r="T7" s="158"/>
-      <c r="U7" s="158"/>
-      <c r="V7" s="158"/>
-      <c r="W7" s="158"/>
-      <c r="X7" s="158" t="s">
+      <c r="S7" s="186"/>
+      <c r="T7" s="186"/>
+      <c r="U7" s="186"/>
+      <c r="V7" s="186"/>
+      <c r="W7" s="186"/>
+      <c r="X7" s="186" t="s">
         <v>337</v>
       </c>
-      <c r="Y7" s="158"/>
+      <c r="Y7" s="186"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -6733,10 +6758,10 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="131" t="s">
+      <c r="E14" s="133" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="197"/>
+      <c r="F14" s="134"/>
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
@@ -6761,10 +6786,10 @@
       <c r="AB14" s="108"/>
       <c r="AC14" s="108"/>
       <c r="AD14" s="108"/>
-      <c r="AE14" s="131" t="s">
+      <c r="AE14" s="133" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="197"/>
+      <c r="AF14" s="134"/>
       <c r="AG14" s="104"/>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
@@ -6807,67 +6832,67 @@
       <c r="G15" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H15" s="129" t="s">
+      <c r="H15" s="135" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="130"/>
-      <c r="J15" s="127" t="s">
+      <c r="I15" s="136"/>
+      <c r="J15" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="128"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="125"/>
-      <c r="N15" s="125"/>
-      <c r="O15" s="125"/>
-      <c r="P15" s="125"/>
-      <c r="Q15" s="125"/>
-      <c r="R15" s="125"/>
-      <c r="S15" s="125"/>
-      <c r="T15" s="125"/>
-      <c r="U15" s="125"/>
-      <c r="V15" s="125"/>
-      <c r="W15" s="125"/>
-      <c r="X15" s="125"/>
-      <c r="Y15" s="125"/>
-      <c r="Z15" s="125"/>
-      <c r="AA15" s="125"/>
-      <c r="AB15" s="125"/>
-      <c r="AC15" s="125"/>
-      <c r="AD15" s="125"/>
-      <c r="AE15" s="125"/>
-      <c r="AF15" s="126"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="196"/>
+      <c r="M15" s="197"/>
+      <c r="N15" s="197"/>
+      <c r="O15" s="197"/>
+      <c r="P15" s="197"/>
+      <c r="Q15" s="197"/>
+      <c r="R15" s="197"/>
+      <c r="S15" s="197"/>
+      <c r="T15" s="197"/>
+      <c r="U15" s="197"/>
+      <c r="V15" s="197"/>
+      <c r="W15" s="197"/>
+      <c r="X15" s="197"/>
+      <c r="Y15" s="197"/>
+      <c r="Z15" s="197"/>
+      <c r="AA15" s="197"/>
+      <c r="AB15" s="197"/>
+      <c r="AC15" s="197"/>
+      <c r="AD15" s="197"/>
+      <c r="AE15" s="197"/>
+      <c r="AF15" s="198"/>
       <c r="AG15" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="AH15" s="129" t="s">
+      <c r="AH15" s="135" t="s">
         <v>279</v>
       </c>
-      <c r="AI15" s="130"/>
-      <c r="AJ15" s="127" t="s">
+      <c r="AI15" s="136"/>
+      <c r="AJ15" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AK15" s="128"/>
-      <c r="AL15" s="124"/>
-      <c r="AM15" s="125"/>
-      <c r="AN15" s="125"/>
-      <c r="AO15" s="125"/>
-      <c r="AP15" s="125"/>
-      <c r="AQ15" s="125"/>
-      <c r="AR15" s="125"/>
-      <c r="AS15" s="125"/>
-      <c r="AT15" s="125"/>
-      <c r="AU15" s="125"/>
-      <c r="AV15" s="125"/>
-      <c r="AW15" s="125"/>
-      <c r="AX15" s="125"/>
-      <c r="AY15" s="125"/>
-      <c r="AZ15" s="125"/>
-      <c r="BA15" s="125"/>
-      <c r="BB15" s="125"/>
-      <c r="BC15" s="125"/>
-      <c r="BD15" s="125"/>
-      <c r="BE15" s="125"/>
-      <c r="BF15" s="125"/>
+      <c r="AK15" s="138"/>
+      <c r="AL15" s="196"/>
+      <c r="AM15" s="197"/>
+      <c r="AN15" s="197"/>
+      <c r="AO15" s="197"/>
+      <c r="AP15" s="197"/>
+      <c r="AQ15" s="197"/>
+      <c r="AR15" s="197"/>
+      <c r="AS15" s="197"/>
+      <c r="AT15" s="197"/>
+      <c r="AU15" s="197"/>
+      <c r="AV15" s="197"/>
+      <c r="AW15" s="197"/>
+      <c r="AX15" s="197"/>
+      <c r="AY15" s="197"/>
+      <c r="AZ15" s="197"/>
+      <c r="BA15" s="197"/>
+      <c r="BB15" s="197"/>
+      <c r="BC15" s="197"/>
+      <c r="BD15" s="197"/>
+      <c r="BE15" s="197"/>
+      <c r="BF15" s="197"/>
       <c r="BG15" s="103"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -6888,33 +6913,33 @@
         <v>287</v>
       </c>
       <c r="I16" s="110"/>
-      <c r="J16" s="129" t="s">
+      <c r="J16" s="135" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="130"/>
-      <c r="L16" s="127" t="s">
+      <c r="K16" s="136"/>
+      <c r="L16" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="M16" s="128"/>
-      <c r="N16" s="124"/>
-      <c r="O16" s="125"/>
-      <c r="P16" s="125"/>
-      <c r="Q16" s="125"/>
-      <c r="R16" s="125"/>
-      <c r="S16" s="125"/>
-      <c r="T16" s="125"/>
-      <c r="U16" s="125"/>
-      <c r="V16" s="125"/>
-      <c r="W16" s="125"/>
-      <c r="X16" s="125"/>
-      <c r="Y16" s="125"/>
-      <c r="Z16" s="125"/>
-      <c r="AA16" s="125"/>
-      <c r="AB16" s="125"/>
-      <c r="AC16" s="125"/>
-      <c r="AD16" s="125"/>
-      <c r="AE16" s="125"/>
-      <c r="AF16" s="126"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="196"/>
+      <c r="O16" s="197"/>
+      <c r="P16" s="197"/>
+      <c r="Q16" s="197"/>
+      <c r="R16" s="197"/>
+      <c r="S16" s="197"/>
+      <c r="T16" s="197"/>
+      <c r="U16" s="197"/>
+      <c r="V16" s="197"/>
+      <c r="W16" s="197"/>
+      <c r="X16" s="197"/>
+      <c r="Y16" s="197"/>
+      <c r="Z16" s="197"/>
+      <c r="AA16" s="197"/>
+      <c r="AB16" s="197"/>
+      <c r="AC16" s="197"/>
+      <c r="AD16" s="197"/>
+      <c r="AE16" s="197"/>
+      <c r="AF16" s="198"/>
       <c r="AG16" s="106" t="s">
         <v>274</v>
       </c>
@@ -6922,33 +6947,33 @@
         <v>287</v>
       </c>
       <c r="AI16" s="110"/>
-      <c r="AJ16" s="129" t="s">
+      <c r="AJ16" s="135" t="s">
         <v>280</v>
       </c>
-      <c r="AK16" s="130"/>
-      <c r="AL16" s="127" t="s">
+      <c r="AK16" s="136"/>
+      <c r="AL16" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AM16" s="128"/>
-      <c r="AN16" s="124"/>
-      <c r="AO16" s="125"/>
-      <c r="AP16" s="125"/>
-      <c r="AQ16" s="125"/>
-      <c r="AR16" s="125"/>
-      <c r="AS16" s="125"/>
-      <c r="AT16" s="125"/>
-      <c r="AU16" s="125"/>
-      <c r="AV16" s="125"/>
-      <c r="AW16" s="125"/>
-      <c r="AX16" s="125"/>
-      <c r="AY16" s="125"/>
-      <c r="AZ16" s="125"/>
-      <c r="BA16" s="125"/>
-      <c r="BB16" s="125"/>
-      <c r="BC16" s="125"/>
-      <c r="BD16" s="125"/>
-      <c r="BE16" s="125"/>
-      <c r="BF16" s="125"/>
+      <c r="AM16" s="138"/>
+      <c r="AN16" s="196"/>
+      <c r="AO16" s="197"/>
+      <c r="AP16" s="197"/>
+      <c r="AQ16" s="197"/>
+      <c r="AR16" s="197"/>
+      <c r="AS16" s="197"/>
+      <c r="AT16" s="197"/>
+      <c r="AU16" s="197"/>
+      <c r="AV16" s="197"/>
+      <c r="AW16" s="197"/>
+      <c r="AX16" s="197"/>
+      <c r="AY16" s="197"/>
+      <c r="AZ16" s="197"/>
+      <c r="BA16" s="197"/>
+      <c r="BB16" s="197"/>
+      <c r="BC16" s="197"/>
+      <c r="BD16" s="197"/>
+      <c r="BE16" s="197"/>
+      <c r="BF16" s="197"/>
       <c r="BG16" s="103"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -6971,31 +6996,31 @@
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
       <c r="K17" s="110"/>
-      <c r="L17" s="129" t="s">
+      <c r="L17" s="135" t="s">
         <v>281</v>
       </c>
-      <c r="M17" s="130"/>
-      <c r="N17" s="127" t="s">
+      <c r="M17" s="136"/>
+      <c r="N17" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="O17" s="128"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="125"/>
-      <c r="R17" s="125"/>
-      <c r="S17" s="125"/>
-      <c r="T17" s="125"/>
-      <c r="U17" s="125"/>
-      <c r="V17" s="125"/>
-      <c r="W17" s="125"/>
-      <c r="X17" s="125"/>
-      <c r="Y17" s="125"/>
-      <c r="Z17" s="125"/>
-      <c r="AA17" s="125"/>
-      <c r="AB17" s="125"/>
-      <c r="AC17" s="125"/>
-      <c r="AD17" s="125"/>
-      <c r="AE17" s="125"/>
-      <c r="AF17" s="126"/>
+      <c r="O17" s="138"/>
+      <c r="P17" s="196"/>
+      <c r="Q17" s="197"/>
+      <c r="R17" s="197"/>
+      <c r="S17" s="197"/>
+      <c r="T17" s="197"/>
+      <c r="U17" s="197"/>
+      <c r="V17" s="197"/>
+      <c r="W17" s="197"/>
+      <c r="X17" s="197"/>
+      <c r="Y17" s="197"/>
+      <c r="Z17" s="197"/>
+      <c r="AA17" s="197"/>
+      <c r="AB17" s="197"/>
+      <c r="AC17" s="197"/>
+      <c r="AD17" s="197"/>
+      <c r="AE17" s="197"/>
+      <c r="AF17" s="198"/>
       <c r="AG17" s="106" t="s">
         <v>274</v>
       </c>
@@ -7005,31 +7030,31 @@
       <c r="AI17" s="111"/>
       <c r="AJ17" s="111"/>
       <c r="AK17" s="110"/>
-      <c r="AL17" s="129" t="s">
+      <c r="AL17" s="135" t="s">
         <v>281</v>
       </c>
-      <c r="AM17" s="130"/>
-      <c r="AN17" s="127" t="s">
+      <c r="AM17" s="136"/>
+      <c r="AN17" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AO17" s="128"/>
-      <c r="AP17" s="124"/>
-      <c r="AQ17" s="125"/>
-      <c r="AR17" s="125"/>
-      <c r="AS17" s="125"/>
-      <c r="AT17" s="125"/>
-      <c r="AU17" s="125"/>
-      <c r="AV17" s="125"/>
-      <c r="AW17" s="125"/>
-      <c r="AX17" s="125"/>
-      <c r="AY17" s="125"/>
-      <c r="AZ17" s="125"/>
-      <c r="BA17" s="125"/>
-      <c r="BB17" s="125"/>
-      <c r="BC17" s="125"/>
-      <c r="BD17" s="125"/>
-      <c r="BE17" s="125"/>
-      <c r="BF17" s="125"/>
+      <c r="AO17" s="138"/>
+      <c r="AP17" s="196"/>
+      <c r="AQ17" s="197"/>
+      <c r="AR17" s="197"/>
+      <c r="AS17" s="197"/>
+      <c r="AT17" s="197"/>
+      <c r="AU17" s="197"/>
+      <c r="AV17" s="197"/>
+      <c r="AW17" s="197"/>
+      <c r="AX17" s="197"/>
+      <c r="AY17" s="197"/>
+      <c r="AZ17" s="197"/>
+      <c r="BA17" s="197"/>
+      <c r="BB17" s="197"/>
+      <c r="BC17" s="197"/>
+      <c r="BD17" s="197"/>
+      <c r="BE17" s="197"/>
+      <c r="BF17" s="197"/>
       <c r="BG17" s="103"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -7054,27 +7079,27 @@
       <c r="K18" s="111"/>
       <c r="L18" s="111"/>
       <c r="M18" s="110"/>
-      <c r="N18" s="131" t="s">
+      <c r="N18" s="133" t="s">
         <v>282</v>
       </c>
-      <c r="O18" s="132"/>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="125"/>
-      <c r="S18" s="125"/>
-      <c r="T18" s="125"/>
-      <c r="U18" s="125"/>
-      <c r="V18" s="125"/>
-      <c r="W18" s="125"/>
-      <c r="X18" s="125"/>
-      <c r="Y18" s="125"/>
-      <c r="Z18" s="125"/>
-      <c r="AA18" s="125"/>
-      <c r="AB18" s="125"/>
-      <c r="AC18" s="125"/>
-      <c r="AD18" s="125"/>
-      <c r="AE18" s="125"/>
-      <c r="AF18" s="126"/>
+      <c r="O18" s="142"/>
+      <c r="P18" s="196"/>
+      <c r="Q18" s="197"/>
+      <c r="R18" s="197"/>
+      <c r="S18" s="197"/>
+      <c r="T18" s="197"/>
+      <c r="U18" s="197"/>
+      <c r="V18" s="197"/>
+      <c r="W18" s="197"/>
+      <c r="X18" s="197"/>
+      <c r="Y18" s="197"/>
+      <c r="Z18" s="197"/>
+      <c r="AA18" s="197"/>
+      <c r="AB18" s="197"/>
+      <c r="AC18" s="197"/>
+      <c r="AD18" s="197"/>
+      <c r="AE18" s="197"/>
+      <c r="AF18" s="198"/>
       <c r="AG18" s="106" t="s">
         <v>274</v>
       </c>
@@ -7086,27 +7111,27 @@
       <c r="AK18" s="111"/>
       <c r="AL18" s="111"/>
       <c r="AM18" s="110"/>
-      <c r="AN18" s="131" t="s">
+      <c r="AN18" s="133" t="s">
         <v>282</v>
       </c>
-      <c r="AO18" s="132"/>
-      <c r="AP18" s="124"/>
-      <c r="AQ18" s="125"/>
-      <c r="AR18" s="125"/>
-      <c r="AS18" s="125"/>
-      <c r="AT18" s="125"/>
-      <c r="AU18" s="125"/>
-      <c r="AV18" s="125"/>
-      <c r="AW18" s="125"/>
-      <c r="AX18" s="125"/>
-      <c r="AY18" s="125"/>
-      <c r="AZ18" s="125"/>
-      <c r="BA18" s="125"/>
-      <c r="BB18" s="125"/>
-      <c r="BC18" s="125"/>
-      <c r="BD18" s="125"/>
-      <c r="BE18" s="125"/>
-      <c r="BF18" s="125"/>
+      <c r="AO18" s="142"/>
+      <c r="AP18" s="196"/>
+      <c r="AQ18" s="197"/>
+      <c r="AR18" s="197"/>
+      <c r="AS18" s="197"/>
+      <c r="AT18" s="197"/>
+      <c r="AU18" s="197"/>
+      <c r="AV18" s="197"/>
+      <c r="AW18" s="197"/>
+      <c r="AX18" s="197"/>
+      <c r="AY18" s="197"/>
+      <c r="AZ18" s="197"/>
+      <c r="BA18" s="197"/>
+      <c r="BB18" s="197"/>
+      <c r="BC18" s="197"/>
+      <c r="BD18" s="197"/>
+      <c r="BE18" s="197"/>
+      <c r="BF18" s="197"/>
       <c r="BG18" s="103"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -7332,23 +7357,23 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
       <c r="S22" s="110"/>
-      <c r="T22" s="129" t="s">
+      <c r="T22" s="135" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="130"/>
-      <c r="V22" s="127" t="s">
+      <c r="U22" s="136"/>
+      <c r="V22" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="W22" s="128"/>
-      <c r="X22" s="124"/>
-      <c r="Y22" s="125"/>
-      <c r="Z22" s="125"/>
-      <c r="AA22" s="125"/>
-      <c r="AB22" s="125"/>
-      <c r="AC22" s="125"/>
-      <c r="AD22" s="125"/>
-      <c r="AE22" s="125"/>
-      <c r="AF22" s="126"/>
+      <c r="W22" s="138"/>
+      <c r="X22" s="196"/>
+      <c r="Y22" s="197"/>
+      <c r="Z22" s="197"/>
+      <c r="AA22" s="197"/>
+      <c r="AB22" s="197"/>
+      <c r="AC22" s="197"/>
+      <c r="AD22" s="197"/>
+      <c r="AE22" s="197"/>
+      <c r="AF22" s="198"/>
       <c r="AG22" s="106" t="s">
         <v>274</v>
       </c>
@@ -7366,23 +7391,23 @@
       <c r="AQ22" s="111"/>
       <c r="AR22" s="111"/>
       <c r="AS22" s="110"/>
-      <c r="AT22" s="129" t="s">
+      <c r="AT22" s="135" t="s">
         <v>283</v>
       </c>
-      <c r="AU22" s="130"/>
-      <c r="AV22" s="127" t="s">
+      <c r="AU22" s="136"/>
+      <c r="AV22" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AW22" s="128"/>
-      <c r="AX22" s="124"/>
-      <c r="AY22" s="125"/>
-      <c r="AZ22" s="125"/>
-      <c r="BA22" s="125"/>
-      <c r="BB22" s="125"/>
-      <c r="BC22" s="125"/>
-      <c r="BD22" s="125"/>
-      <c r="BE22" s="125"/>
-      <c r="BF22" s="125"/>
+      <c r="AW22" s="138"/>
+      <c r="AX22" s="196"/>
+      <c r="AY22" s="197"/>
+      <c r="AZ22" s="197"/>
+      <c r="BA22" s="197"/>
+      <c r="BB22" s="197"/>
+      <c r="BC22" s="197"/>
+      <c r="BD22" s="197"/>
+      <c r="BE22" s="197"/>
+      <c r="BF22" s="197"/>
       <c r="BG22" s="103"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -7415,21 +7440,21 @@
       <c r="S23" s="111"/>
       <c r="T23" s="111"/>
       <c r="U23" s="110"/>
-      <c r="V23" s="129" t="s">
+      <c r="V23" s="135" t="s">
         <v>284</v>
       </c>
-      <c r="W23" s="130"/>
-      <c r="X23" s="127" t="s">
+      <c r="W23" s="136"/>
+      <c r="X23" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="Y23" s="128"/>
-      <c r="Z23" s="124"/>
-      <c r="AA23" s="125"/>
-      <c r="AB23" s="125"/>
-      <c r="AC23" s="125"/>
-      <c r="AD23" s="125"/>
-      <c r="AE23" s="125"/>
-      <c r="AF23" s="126"/>
+      <c r="Y23" s="138"/>
+      <c r="Z23" s="196"/>
+      <c r="AA23" s="197"/>
+      <c r="AB23" s="197"/>
+      <c r="AC23" s="197"/>
+      <c r="AD23" s="197"/>
+      <c r="AE23" s="197"/>
+      <c r="AF23" s="198"/>
       <c r="AG23" s="106" t="s">
         <v>274</v>
       </c>
@@ -7449,21 +7474,21 @@
       <c r="AS23" s="111"/>
       <c r="AT23" s="111"/>
       <c r="AU23" s="110"/>
-      <c r="AV23" s="129" t="s">
+      <c r="AV23" s="135" t="s">
         <v>284</v>
       </c>
-      <c r="AW23" s="130"/>
-      <c r="AX23" s="127" t="s">
+      <c r="AW23" s="136"/>
+      <c r="AX23" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AY23" s="128"/>
-      <c r="AZ23" s="124"/>
-      <c r="BA23" s="125"/>
-      <c r="BB23" s="125"/>
-      <c r="BC23" s="125"/>
-      <c r="BD23" s="125"/>
-      <c r="BE23" s="125"/>
-      <c r="BF23" s="125"/>
+      <c r="AY23" s="138"/>
+      <c r="AZ23" s="196"/>
+      <c r="BA23" s="197"/>
+      <c r="BB23" s="197"/>
+      <c r="BC23" s="197"/>
+      <c r="BD23" s="197"/>
+      <c r="BE23" s="197"/>
+      <c r="BF23" s="197"/>
       <c r="BG23" s="103"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -7498,19 +7523,19 @@
       <c r="U24" s="111"/>
       <c r="V24" s="111"/>
       <c r="W24" s="110"/>
-      <c r="X24" s="129" t="s">
+      <c r="X24" s="135" t="s">
         <v>285</v>
       </c>
-      <c r="Y24" s="130"/>
-      <c r="Z24" s="127" t="s">
+      <c r="Y24" s="136"/>
+      <c r="Z24" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AA24" s="128"/>
-      <c r="AB24" s="124"/>
-      <c r="AC24" s="125"/>
-      <c r="AD24" s="125"/>
-      <c r="AE24" s="125"/>
-      <c r="AF24" s="126"/>
+      <c r="AA24" s="138"/>
+      <c r="AB24" s="196"/>
+      <c r="AC24" s="197"/>
+      <c r="AD24" s="197"/>
+      <c r="AE24" s="197"/>
+      <c r="AF24" s="198"/>
       <c r="AG24" s="106" t="s">
         <v>274</v>
       </c>
@@ -7532,19 +7557,19 @@
       <c r="AU24" s="111"/>
       <c r="AV24" s="111"/>
       <c r="AW24" s="110"/>
-      <c r="AX24" s="129" t="s">
+      <c r="AX24" s="135" t="s">
         <v>285</v>
       </c>
-      <c r="AY24" s="130"/>
-      <c r="AZ24" s="127" t="s">
+      <c r="AY24" s="136"/>
+      <c r="AZ24" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="BA24" s="128"/>
-      <c r="BB24" s="124"/>
-      <c r="BC24" s="125"/>
-      <c r="BD24" s="125"/>
-      <c r="BE24" s="125"/>
-      <c r="BF24" s="125"/>
+      <c r="BA24" s="138"/>
+      <c r="BB24" s="196"/>
+      <c r="BC24" s="197"/>
+      <c r="BD24" s="197"/>
+      <c r="BE24" s="197"/>
+      <c r="BF24" s="197"/>
       <c r="BG24" s="103"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -7581,17 +7606,17 @@
       <c r="W25" s="111"/>
       <c r="X25" s="111"/>
       <c r="Y25" s="110"/>
-      <c r="Z25" s="131" t="s">
+      <c r="Z25" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="AA25" s="132"/>
-      <c r="AB25" s="127" t="s">
+      <c r="AA25" s="142"/>
+      <c r="AB25" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AC25" s="128"/>
-      <c r="AD25" s="124"/>
-      <c r="AE25" s="125"/>
-      <c r="AF25" s="126"/>
+      <c r="AC25" s="138"/>
+      <c r="AD25" s="196"/>
+      <c r="AE25" s="197"/>
+      <c r="AF25" s="198"/>
       <c r="AG25" s="106" t="s">
         <v>274</v>
       </c>
@@ -7615,17 +7640,17 @@
       <c r="AW25" s="111"/>
       <c r="AX25" s="111"/>
       <c r="AY25" s="110"/>
-      <c r="AZ25" s="131" t="s">
+      <c r="AZ25" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="BA25" s="132"/>
-      <c r="BB25" s="127" t="s">
+      <c r="BA25" s="142"/>
+      <c r="BB25" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="BC25" s="128"/>
-      <c r="BD25" s="124"/>
-      <c r="BE25" s="125"/>
-      <c r="BF25" s="125"/>
+      <c r="BC25" s="138"/>
+      <c r="BD25" s="196"/>
+      <c r="BE25" s="197"/>
+      <c r="BF25" s="197"/>
       <c r="BG25" s="103"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -7883,29 +7908,29 @@
         <v>318</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="174" t="s">
+      <c r="E30" s="139" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="175"/>
+      <c r="F30" s="140"/>
       <c r="G30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="174" t="s">
+      <c r="H30" s="139" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="175"/>
-      <c r="J30" s="174" t="s">
+      <c r="I30" s="140"/>
+      <c r="J30" s="139" t="s">
         <v>280</v>
       </c>
-      <c r="K30" s="175"/>
-      <c r="L30" s="174" t="s">
+      <c r="K30" s="140"/>
+      <c r="L30" s="139" t="s">
         <v>281</v>
       </c>
-      <c r="M30" s="175"/>
-      <c r="N30" s="174" t="s">
+      <c r="M30" s="140"/>
+      <c r="N30" s="139" t="s">
         <v>282</v>
       </c>
-      <c r="O30" s="175"/>
+      <c r="O30" s="140"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>239</v>
@@ -7914,50 +7939,50 @@
         <v>239</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="174" t="s">
+      <c r="T30" s="139" t="s">
         <v>283</v>
       </c>
-      <c r="U30" s="175"/>
-      <c r="V30" s="174" t="s">
+      <c r="U30" s="140"/>
+      <c r="V30" s="139" t="s">
         <v>284</v>
       </c>
-      <c r="W30" s="175"/>
-      <c r="X30" s="174" t="s">
+      <c r="W30" s="140"/>
+      <c r="X30" s="139" t="s">
         <v>285</v>
       </c>
-      <c r="Y30" s="175"/>
-      <c r="Z30" s="174" t="s">
+      <c r="Y30" s="140"/>
+      <c r="Z30" s="139" t="s">
         <v>286</v>
       </c>
-      <c r="AA30" s="175"/>
-      <c r="AB30" s="148" t="s">
+      <c r="AA30" s="140"/>
+      <c r="AB30" s="143" t="s">
         <v>297</v>
       </c>
-      <c r="AC30" s="149"/>
-      <c r="AD30" s="150"/>
-      <c r="AE30" s="174" t="s">
+      <c r="AC30" s="144"/>
+      <c r="AD30" s="145"/>
+      <c r="AE30" s="139" t="s">
         <v>273</v>
       </c>
-      <c r="AF30" s="175"/>
+      <c r="AF30" s="140"/>
       <c r="AG30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="AH30" s="174" t="s">
+      <c r="AH30" s="139" t="s">
         <v>279</v>
       </c>
-      <c r="AI30" s="175"/>
-      <c r="AJ30" s="174" t="s">
+      <c r="AI30" s="140"/>
+      <c r="AJ30" s="139" t="s">
         <v>280</v>
       </c>
-      <c r="AK30" s="175"/>
-      <c r="AL30" s="174" t="s">
+      <c r="AK30" s="140"/>
+      <c r="AL30" s="139" t="s">
         <v>281</v>
       </c>
-      <c r="AM30" s="175"/>
-      <c r="AN30" s="174" t="s">
+      <c r="AM30" s="140"/>
+      <c r="AN30" s="139" t="s">
         <v>282</v>
       </c>
-      <c r="AO30" s="175"/>
+      <c r="AO30" s="140"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>239</v>
@@ -7966,27 +7991,27 @@
         <v>239</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="174" t="s">
+      <c r="AT30" s="139" t="s">
         <v>283</v>
       </c>
-      <c r="AU30" s="175"/>
-      <c r="AV30" s="174" t="s">
+      <c r="AU30" s="140"/>
+      <c r="AV30" s="139" t="s">
         <v>284</v>
       </c>
-      <c r="AW30" s="175"/>
-      <c r="AX30" s="174" t="s">
+      <c r="AW30" s="140"/>
+      <c r="AX30" s="139" t="s">
         <v>285</v>
       </c>
-      <c r="AY30" s="175"/>
-      <c r="AZ30" s="174" t="s">
+      <c r="AY30" s="140"/>
+      <c r="AZ30" s="139" t="s">
         <v>286</v>
       </c>
-      <c r="BA30" s="175"/>
-      <c r="BB30" s="148" t="s">
+      <c r="BA30" s="140"/>
+      <c r="BB30" s="143" t="s">
         <v>297</v>
       </c>
-      <c r="BC30" s="149"/>
-      <c r="BD30" s="150"/>
+      <c r="BC30" s="144"/>
+      <c r="BD30" s="145"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -7998,10 +8023,10 @@
         <v>317</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="151" t="s">
+      <c r="E31" s="141" t="s">
         <v>323</v>
       </c>
-      <c r="F31" s="151"/>
+      <c r="F31" s="141"/>
       <c r="G31" s="22" t="s">
         <v>324</v>
       </c>
@@ -8028,10 +8053,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="151" t="s">
+      <c r="AE31" s="141" t="s">
         <v>323</v>
       </c>
-      <c r="AF31" s="151"/>
+      <c r="AF31" s="141"/>
       <c r="AG31" s="22" t="s">
         <v>324</v>
       </c>
@@ -8141,75 +8166,75 @@
       <c r="G33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="H33" s="171" t="s">
+      <c r="H33" s="169" t="s">
         <v>319</v>
       </c>
-      <c r="I33" s="172"/>
-      <c r="J33" s="172"/>
-      <c r="K33" s="172"/>
-      <c r="L33" s="172"/>
-      <c r="M33" s="172"/>
-      <c r="N33" s="172"/>
-      <c r="O33" s="172"/>
-      <c r="P33" s="172"/>
-      <c r="Q33" s="172"/>
-      <c r="R33" s="172"/>
-      <c r="S33" s="173"/>
-      <c r="T33" s="174" t="s">
+      <c r="I33" s="170"/>
+      <c r="J33" s="170"/>
+      <c r="K33" s="170"/>
+      <c r="L33" s="170"/>
+      <c r="M33" s="170"/>
+      <c r="N33" s="170"/>
+      <c r="O33" s="170"/>
+      <c r="P33" s="170"/>
+      <c r="Q33" s="170"/>
+      <c r="R33" s="170"/>
+      <c r="S33" s="171"/>
+      <c r="T33" s="139" t="s">
         <v>275</v>
       </c>
-      <c r="U33" s="175"/>
-      <c r="V33" s="148" t="s">
+      <c r="U33" s="140"/>
+      <c r="V33" s="143" t="s">
         <v>297</v>
       </c>
-      <c r="W33" s="150"/>
-      <c r="X33" s="171" t="s">
+      <c r="W33" s="145"/>
+      <c r="X33" s="169" t="s">
         <v>319</v>
       </c>
-      <c r="Y33" s="172"/>
-      <c r="Z33" s="172"/>
-      <c r="AA33" s="172"/>
-      <c r="AB33" s="172"/>
-      <c r="AC33" s="172"/>
-      <c r="AD33" s="172"/>
-      <c r="AE33" s="173"/>
+      <c r="Y33" s="170"/>
+      <c r="Z33" s="170"/>
+      <c r="AA33" s="170"/>
+      <c r="AB33" s="170"/>
+      <c r="AC33" s="170"/>
+      <c r="AD33" s="170"/>
+      <c r="AE33" s="171"/>
       <c r="AF33" s="24" t="s">
         <v>273</v>
       </c>
       <c r="AG33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="AH33" s="171" t="s">
+      <c r="AH33" s="169" t="s">
         <v>319</v>
       </c>
-      <c r="AI33" s="172"/>
-      <c r="AJ33" s="172"/>
-      <c r="AK33" s="172"/>
-      <c r="AL33" s="172"/>
-      <c r="AM33" s="172"/>
-      <c r="AN33" s="172"/>
-      <c r="AO33" s="172"/>
-      <c r="AP33" s="172"/>
-      <c r="AQ33" s="172"/>
-      <c r="AR33" s="172"/>
-      <c r="AS33" s="173"/>
-      <c r="AT33" s="174" t="s">
+      <c r="AI33" s="170"/>
+      <c r="AJ33" s="170"/>
+      <c r="AK33" s="170"/>
+      <c r="AL33" s="170"/>
+      <c r="AM33" s="170"/>
+      <c r="AN33" s="170"/>
+      <c r="AO33" s="170"/>
+      <c r="AP33" s="170"/>
+      <c r="AQ33" s="170"/>
+      <c r="AR33" s="170"/>
+      <c r="AS33" s="171"/>
+      <c r="AT33" s="139" t="s">
         <v>275</v>
       </c>
-      <c r="AU33" s="175"/>
-      <c r="AV33" s="148" t="s">
+      <c r="AU33" s="140"/>
+      <c r="AV33" s="143" t="s">
         <v>297</v>
       </c>
-      <c r="AW33" s="150"/>
-      <c r="AX33" s="171" t="s">
+      <c r="AW33" s="145"/>
+      <c r="AX33" s="169" t="s">
         <v>319</v>
       </c>
-      <c r="AY33" s="172"/>
-      <c r="AZ33" s="172"/>
-      <c r="BA33" s="172"/>
-      <c r="BB33" s="172"/>
-      <c r="BC33" s="172"/>
-      <c r="BD33" s="173"/>
+      <c r="AY33" s="170"/>
+      <c r="AZ33" s="170"/>
+      <c r="BA33" s="170"/>
+      <c r="BB33" s="170"/>
+      <c r="BC33" s="170"/>
+      <c r="BD33" s="171"/>
       <c r="BE33" s="7"/>
       <c r="BF33" s="7"/>
       <c r="BG33" s="7"/>
@@ -8221,10 +8246,10 @@
         <v>317</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="151" t="s">
+      <c r="E34" s="141" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="151"/>
+      <c r="F34" s="141"/>
       <c r="G34" s="22" t="s">
         <v>321</v>
       </c>
@@ -8240,10 +8265,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="151" t="s">
+      <c r="T34" s="141" t="s">
         <v>323</v>
       </c>
-      <c r="U34" s="151"/>
+      <c r="U34" s="141"/>
       <c r="V34" s="22" t="s">
         <v>325</v>
       </c>
@@ -8272,10 +8297,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="151" t="s">
+      <c r="AT34" s="141" t="s">
         <v>323</v>
       </c>
-      <c r="AU34" s="151"/>
+      <c r="AU34" s="141"/>
       <c r="AV34" s="22" t="s">
         <v>320</v>
       </c>
@@ -8546,33 +8571,33 @@
         <v>326</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="166" t="s">
+      <c r="E39" s="172" t="s">
         <v>273</v>
       </c>
-      <c r="F39" s="167"/>
-      <c r="G39" s="169" t="s">
+      <c r="F39" s="173"/>
+      <c r="G39" s="174" t="s">
         <v>273</v>
       </c>
-      <c r="H39" s="170"/>
+      <c r="H39" s="175"/>
       <c r="I39" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="J39" s="131" t="s">
+      <c r="J39" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="K39" s="132"/>
-      <c r="L39" s="131" t="s">
+      <c r="K39" s="142"/>
+      <c r="L39" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="M39" s="132"/>
-      <c r="N39" s="131" t="s">
+      <c r="M39" s="142"/>
+      <c r="N39" s="133" t="s">
         <v>281</v>
       </c>
-      <c r="O39" s="132"/>
-      <c r="P39" s="131" t="s">
+      <c r="O39" s="142"/>
+      <c r="P39" s="133" t="s">
         <v>282</v>
       </c>
-      <c r="Q39" s="132"/>
+      <c r="Q39" s="142"/>
       <c r="R39" s="103"/>
       <c r="S39" s="103" t="s">
         <v>239</v>
@@ -8581,50 +8606,50 @@
         <v>239</v>
       </c>
       <c r="U39" s="103"/>
-      <c r="V39" s="131" t="s">
+      <c r="V39" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="W39" s="132"/>
-      <c r="X39" s="131" t="s">
+      <c r="W39" s="142"/>
+      <c r="X39" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="Y39" s="132"/>
-      <c r="Z39" s="131" t="s">
+      <c r="Y39" s="142"/>
+      <c r="Z39" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="AA39" s="132"/>
-      <c r="AB39" s="131" t="s">
+      <c r="AA39" s="142"/>
+      <c r="AB39" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="AC39" s="132"/>
-      <c r="AD39" s="127" t="s">
+      <c r="AC39" s="142"/>
+      <c r="AD39" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AE39" s="168"/>
-      <c r="AF39" s="128"/>
-      <c r="AG39" s="131" t="s">
+      <c r="AE39" s="177"/>
+      <c r="AF39" s="138"/>
+      <c r="AG39" s="133" t="s">
         <v>273</v>
       </c>
-      <c r="AH39" s="132"/>
+      <c r="AH39" s="142"/>
       <c r="AI39" s="112" t="s">
         <v>319</v>
       </c>
-      <c r="AJ39" s="131" t="s">
+      <c r="AJ39" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="AK39" s="132"/>
-      <c r="AL39" s="131" t="s">
+      <c r="AK39" s="142"/>
+      <c r="AL39" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="AM39" s="132"/>
-      <c r="AN39" s="131" t="s">
+      <c r="AM39" s="142"/>
+      <c r="AN39" s="133" t="s">
         <v>281</v>
       </c>
-      <c r="AO39" s="132"/>
-      <c r="AP39" s="131" t="s">
+      <c r="AO39" s="142"/>
+      <c r="AP39" s="133" t="s">
         <v>282</v>
       </c>
-      <c r="AQ39" s="132"/>
+      <c r="AQ39" s="142"/>
       <c r="AR39" s="103"/>
       <c r="AS39" s="103" t="s">
         <v>239</v>
@@ -8653,14 +8678,14 @@
         <v>351</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="144" t="s">
+      <c r="E40" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="144"/>
-      <c r="G40" s="144" t="s">
+      <c r="F40" s="176"/>
+      <c r="G40" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="H40" s="144"/>
+      <c r="H40" s="176"/>
       <c r="I40" s="113" t="s">
         <v>324</v>
       </c>
@@ -8687,10 +8712,10 @@
       <c r="AD40" s="103"/>
       <c r="AE40" s="103"/>
       <c r="AF40" s="103"/>
-      <c r="AG40" s="144" t="s">
+      <c r="AG40" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="AH40" s="144"/>
+      <c r="AH40" s="176"/>
       <c r="AI40" s="113" t="s">
         <v>328</v>
       </c>
@@ -8726,27 +8751,27 @@
         <v>327</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="131" t="s">
+      <c r="E41" s="133" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="132"/>
+      <c r="F41" s="142"/>
       <c r="G41" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="H41" s="131" t="s">
+      <c r="H41" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="I41" s="132"/>
-      <c r="J41" s="131" t="s">
+      <c r="I41" s="142"/>
+      <c r="J41" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="K41" s="132"/>
-      <c r="L41" s="166"/>
-      <c r="M41" s="167"/>
-      <c r="N41" s="169" t="s">
+      <c r="K41" s="142"/>
+      <c r="L41" s="172"/>
+      <c r="M41" s="173"/>
+      <c r="N41" s="174" t="s">
         <v>282</v>
       </c>
-      <c r="O41" s="170"/>
+      <c r="O41" s="175"/>
       <c r="P41" s="103"/>
       <c r="Q41" s="103" t="s">
         <v>239</v>
@@ -8755,50 +8780,50 @@
         <v>239</v>
       </c>
       <c r="S41" s="103"/>
-      <c r="T41" s="131" t="s">
+      <c r="T41" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="U41" s="132"/>
-      <c r="V41" s="131" t="s">
+      <c r="U41" s="142"/>
+      <c r="V41" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="W41" s="132"/>
-      <c r="X41" s="131" t="s">
+      <c r="W41" s="142"/>
+      <c r="X41" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="Y41" s="132"/>
-      <c r="Z41" s="131" t="s">
+      <c r="Y41" s="142"/>
+      <c r="Z41" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="AA41" s="132"/>
-      <c r="AB41" s="127" t="s">
+      <c r="AA41" s="142"/>
+      <c r="AB41" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AC41" s="168"/>
-      <c r="AD41" s="128"/>
-      <c r="AE41" s="131" t="s">
+      <c r="AC41" s="177"/>
+      <c r="AD41" s="138"/>
+      <c r="AE41" s="133" t="s">
         <v>273</v>
       </c>
-      <c r="AF41" s="132"/>
+      <c r="AF41" s="142"/>
       <c r="AG41" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="AH41" s="131" t="s">
+      <c r="AH41" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="AI41" s="132"/>
-      <c r="AJ41" s="131" t="s">
+      <c r="AI41" s="142"/>
+      <c r="AJ41" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="AK41" s="132"/>
-      <c r="AL41" s="131" t="s">
+      <c r="AK41" s="142"/>
+      <c r="AL41" s="133" t="s">
         <v>281</v>
       </c>
-      <c r="AM41" s="132"/>
-      <c r="AN41" s="131" t="s">
+      <c r="AM41" s="142"/>
+      <c r="AN41" s="133" t="s">
         <v>282</v>
       </c>
-      <c r="AO41" s="132"/>
+      <c r="AO41" s="142"/>
       <c r="AP41" s="103"/>
       <c r="AQ41" s="103" t="s">
         <v>239</v>
@@ -8807,27 +8832,27 @@
         <v>239</v>
       </c>
       <c r="AS41" s="103"/>
-      <c r="AT41" s="131" t="s">
+      <c r="AT41" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="AU41" s="132"/>
-      <c r="AV41" s="131" t="s">
+      <c r="AU41" s="142"/>
+      <c r="AV41" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="AW41" s="132"/>
-      <c r="AX41" s="131" t="s">
+      <c r="AW41" s="142"/>
+      <c r="AX41" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="AY41" s="132"/>
-      <c r="AZ41" s="131" t="s">
+      <c r="AY41" s="142"/>
+      <c r="AZ41" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="BA41" s="132"/>
-      <c r="BB41" s="127" t="s">
+      <c r="BA41" s="142"/>
+      <c r="BB41" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="BC41" s="168"/>
-      <c r="BD41" s="128"/>
+      <c r="BC41" s="177"/>
+      <c r="BD41" s="138"/>
       <c r="BE41" s="103"/>
       <c r="BF41" s="103"/>
       <c r="BG41" s="103"/>
@@ -8839,10 +8864,10 @@
         <v>352</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="144" t="s">
+      <c r="E42" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="144"/>
+      <c r="F42" s="176"/>
       <c r="G42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8869,10 +8894,10 @@
       <c r="AB42" s="103"/>
       <c r="AC42" s="103"/>
       <c r="AD42" s="103"/>
-      <c r="AE42" s="144" t="s">
+      <c r="AE42" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="AF42" s="144"/>
+      <c r="AF42" s="176"/>
       <c r="AG42" s="113" t="s">
         <v>324</v>
       </c>
@@ -8982,75 +9007,75 @@
       <c r="G44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="163" t="s">
+      <c r="H44" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="I44" s="164"/>
-      <c r="J44" s="164"/>
-      <c r="K44" s="164"/>
-      <c r="L44" s="164"/>
-      <c r="M44" s="164"/>
-      <c r="N44" s="164"/>
-      <c r="O44" s="164"/>
-      <c r="P44" s="164"/>
-      <c r="Q44" s="164"/>
-      <c r="R44" s="164"/>
-      <c r="S44" s="165"/>
-      <c r="T44" s="166" t="s">
+      <c r="I44" s="184"/>
+      <c r="J44" s="184"/>
+      <c r="K44" s="184"/>
+      <c r="L44" s="184"/>
+      <c r="M44" s="184"/>
+      <c r="N44" s="184"/>
+      <c r="O44" s="184"/>
+      <c r="P44" s="184"/>
+      <c r="Q44" s="184"/>
+      <c r="R44" s="184"/>
+      <c r="S44" s="185"/>
+      <c r="T44" s="172" t="s">
         <v>275</v>
       </c>
-      <c r="U44" s="167"/>
-      <c r="V44" s="127" t="s">
+      <c r="U44" s="173"/>
+      <c r="V44" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="W44" s="128"/>
-      <c r="X44" s="163" t="s">
+      <c r="W44" s="138"/>
+      <c r="X44" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="Y44" s="164"/>
-      <c r="Z44" s="164"/>
-      <c r="AA44" s="164"/>
-      <c r="AB44" s="164"/>
-      <c r="AC44" s="164"/>
-      <c r="AD44" s="164"/>
-      <c r="AE44" s="165"/>
+      <c r="Y44" s="184"/>
+      <c r="Z44" s="184"/>
+      <c r="AA44" s="184"/>
+      <c r="AB44" s="184"/>
+      <c r="AC44" s="184"/>
+      <c r="AD44" s="184"/>
+      <c r="AE44" s="185"/>
       <c r="AF44" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH44" s="163" t="s">
+      <c r="AH44" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="AI44" s="164"/>
-      <c r="AJ44" s="164"/>
-      <c r="AK44" s="164"/>
-      <c r="AL44" s="164"/>
-      <c r="AM44" s="164"/>
-      <c r="AN44" s="164"/>
-      <c r="AO44" s="164"/>
-      <c r="AP44" s="164"/>
-      <c r="AQ44" s="164"/>
-      <c r="AR44" s="164"/>
-      <c r="AS44" s="165"/>
-      <c r="AT44" s="131" t="s">
+      <c r="AI44" s="184"/>
+      <c r="AJ44" s="184"/>
+      <c r="AK44" s="184"/>
+      <c r="AL44" s="184"/>
+      <c r="AM44" s="184"/>
+      <c r="AN44" s="184"/>
+      <c r="AO44" s="184"/>
+      <c r="AP44" s="184"/>
+      <c r="AQ44" s="184"/>
+      <c r="AR44" s="184"/>
+      <c r="AS44" s="185"/>
+      <c r="AT44" s="133" t="s">
         <v>275</v>
       </c>
-      <c r="AU44" s="132"/>
-      <c r="AV44" s="127" t="s">
+      <c r="AU44" s="142"/>
+      <c r="AV44" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AW44" s="128"/>
-      <c r="AX44" s="163" t="s">
+      <c r="AW44" s="138"/>
+      <c r="AX44" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="AY44" s="164"/>
-      <c r="AZ44" s="164"/>
-      <c r="BA44" s="164"/>
-      <c r="BB44" s="164"/>
-      <c r="BC44" s="164"/>
-      <c r="BD44" s="165"/>
+      <c r="AY44" s="184"/>
+      <c r="AZ44" s="184"/>
+      <c r="BA44" s="184"/>
+      <c r="BB44" s="184"/>
+      <c r="BC44" s="184"/>
+      <c r="BD44" s="185"/>
       <c r="BE44" s="103"/>
       <c r="BF44" s="103"/>
       <c r="BG44" s="103"/>
@@ -9062,10 +9087,10 @@
         <v>352</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="144" t="s">
+      <c r="E45" s="176" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="144"/>
+      <c r="F45" s="176"/>
       <c r="G45" s="113" t="s">
         <v>321</v>
       </c>
@@ -9081,10 +9106,10 @@
       <c r="Q45" s="116"/>
       <c r="R45" s="116"/>
       <c r="S45" s="103"/>
-      <c r="T45" s="144" t="s">
+      <c r="T45" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="U45" s="144"/>
+      <c r="U45" s="176"/>
       <c r="V45" s="113" t="s">
         <v>325</v>
       </c>
@@ -9113,10 +9138,10 @@
       <c r="AQ45" s="116"/>
       <c r="AR45" s="116"/>
       <c r="AS45" s="103"/>
-      <c r="AT45" s="144" t="s">
+      <c r="AT45" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="AU45" s="144"/>
+      <c r="AU45" s="176"/>
       <c r="AV45" s="113" t="s">
         <v>320</v>
       </c>
@@ -9145,70 +9170,70 @@
       <c r="F46" s="117" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="163" t="s">
+      <c r="G46" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="H46" s="164"/>
-      <c r="I46" s="164"/>
-      <c r="J46" s="164"/>
-      <c r="K46" s="164"/>
-      <c r="L46" s="164"/>
-      <c r="M46" s="164"/>
-      <c r="N46" s="164"/>
-      <c r="O46" s="164"/>
-      <c r="P46" s="164"/>
-      <c r="Q46" s="164"/>
-      <c r="R46" s="164"/>
-      <c r="S46" s="164"/>
-      <c r="T46" s="164"/>
-      <c r="U46" s="164"/>
-      <c r="V46" s="164"/>
-      <c r="W46" s="164"/>
-      <c r="X46" s="164"/>
-      <c r="Y46" s="164"/>
-      <c r="Z46" s="164"/>
-      <c r="AA46" s="164"/>
-      <c r="AB46" s="164"/>
-      <c r="AC46" s="164"/>
-      <c r="AD46" s="164"/>
-      <c r="AE46" s="165"/>
+      <c r="H46" s="184"/>
+      <c r="I46" s="184"/>
+      <c r="J46" s="184"/>
+      <c r="K46" s="184"/>
+      <c r="L46" s="184"/>
+      <c r="M46" s="184"/>
+      <c r="N46" s="184"/>
+      <c r="O46" s="184"/>
+      <c r="P46" s="184"/>
+      <c r="Q46" s="184"/>
+      <c r="R46" s="184"/>
+      <c r="S46" s="184"/>
+      <c r="T46" s="184"/>
+      <c r="U46" s="184"/>
+      <c r="V46" s="184"/>
+      <c r="W46" s="184"/>
+      <c r="X46" s="184"/>
+      <c r="Y46" s="184"/>
+      <c r="Z46" s="184"/>
+      <c r="AA46" s="184"/>
+      <c r="AB46" s="184"/>
+      <c r="AC46" s="184"/>
+      <c r="AD46" s="184"/>
+      <c r="AE46" s="185"/>
       <c r="AF46" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG46" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH46" s="163" t="s">
+      <c r="AH46" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="AI46" s="164"/>
-      <c r="AJ46" s="164"/>
-      <c r="AK46" s="164"/>
-      <c r="AL46" s="164"/>
-      <c r="AM46" s="164"/>
-      <c r="AN46" s="164"/>
-      <c r="AO46" s="164"/>
-      <c r="AP46" s="164"/>
-      <c r="AQ46" s="164"/>
-      <c r="AR46" s="164"/>
-      <c r="AS46" s="165"/>
-      <c r="AT46" s="131" t="s">
+      <c r="AI46" s="184"/>
+      <c r="AJ46" s="184"/>
+      <c r="AK46" s="184"/>
+      <c r="AL46" s="184"/>
+      <c r="AM46" s="184"/>
+      <c r="AN46" s="184"/>
+      <c r="AO46" s="184"/>
+      <c r="AP46" s="184"/>
+      <c r="AQ46" s="184"/>
+      <c r="AR46" s="184"/>
+      <c r="AS46" s="185"/>
+      <c r="AT46" s="133" t="s">
         <v>275</v>
       </c>
-      <c r="AU46" s="132"/>
-      <c r="AV46" s="127" t="s">
+      <c r="AU46" s="142"/>
+      <c r="AV46" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="AW46" s="128"/>
-      <c r="AX46" s="163" t="s">
+      <c r="AW46" s="138"/>
+      <c r="AX46" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="AY46" s="164"/>
-      <c r="AZ46" s="164"/>
-      <c r="BA46" s="164"/>
-      <c r="BB46" s="164"/>
-      <c r="BC46" s="164"/>
-      <c r="BD46" s="165"/>
+      <c r="AY46" s="184"/>
+      <c r="AZ46" s="184"/>
+      <c r="BA46" s="184"/>
+      <c r="BB46" s="184"/>
+      <c r="BC46" s="184"/>
+      <c r="BD46" s="185"/>
       <c r="BE46" s="103"/>
       <c r="BF46" s="103"/>
       <c r="BG46" s="103"/>
@@ -9265,10 +9290,10 @@
       <c r="AQ47" s="116"/>
       <c r="AR47" s="116"/>
       <c r="AS47" s="103"/>
-      <c r="AT47" s="144" t="s">
+      <c r="AT47" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="AU47" s="144"/>
+      <c r="AU47" s="176"/>
       <c r="AV47" s="113" t="s">
         <v>320</v>
       </c>
@@ -9659,20 +9684,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="134" t="s">
+      <c r="E54" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="135"/>
-      <c r="G54" s="135"/>
-      <c r="H54" s="135"/>
-      <c r="I54" s="135"/>
-      <c r="J54" s="135"/>
-      <c r="K54" s="155"/>
-      <c r="L54" s="134" t="s">
+      <c r="F54" s="131"/>
+      <c r="G54" s="131"/>
+      <c r="H54" s="131"/>
+      <c r="I54" s="131"/>
+      <c r="J54" s="131"/>
+      <c r="K54" s="132"/>
+      <c r="L54" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="135"/>
-      <c r="N54" s="136"/>
+      <c r="M54" s="131"/>
+      <c r="N54" s="199"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -9793,20 +9818,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="137" t="s">
+      <c r="E56" s="190" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="138"/>
-      <c r="G56" s="138"/>
-      <c r="H56" s="138"/>
-      <c r="I56" s="138"/>
-      <c r="J56" s="138"/>
-      <c r="K56" s="139"/>
-      <c r="L56" s="137" t="s">
+      <c r="F56" s="192"/>
+      <c r="G56" s="192"/>
+      <c r="H56" s="192"/>
+      <c r="I56" s="192"/>
+      <c r="J56" s="192"/>
+      <c r="K56" s="191"/>
+      <c r="L56" s="190" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="138"/>
-      <c r="N56" s="139"/>
+      <c r="M56" s="192"/>
+      <c r="N56" s="191"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -12278,68 +12303,68 @@
         <v>364</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="134" t="s">
+      <c r="E95" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="135"/>
-      <c r="G95" s="135"/>
-      <c r="H95" s="135"/>
-      <c r="I95" s="135"/>
-      <c r="J95" s="135"/>
-      <c r="K95" s="155"/>
-      <c r="L95" s="134" t="s">
+      <c r="F95" s="131"/>
+      <c r="G95" s="131"/>
+      <c r="H95" s="131"/>
+      <c r="I95" s="131"/>
+      <c r="J95" s="131"/>
+      <c r="K95" s="132"/>
+      <c r="L95" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="135"/>
-      <c r="N95" s="155"/>
-      <c r="O95" s="145" t="s">
+      <c r="M95" s="131"/>
+      <c r="N95" s="132"/>
+      <c r="O95" s="166" t="s">
         <v>260</v>
       </c>
-      <c r="P95" s="146"/>
-      <c r="Q95" s="146"/>
-      <c r="R95" s="146"/>
-      <c r="S95" s="146"/>
-      <c r="T95" s="147"/>
-      <c r="U95" s="145" t="s">
+      <c r="P95" s="167"/>
+      <c r="Q95" s="167"/>
+      <c r="R95" s="167"/>
+      <c r="S95" s="167"/>
+      <c r="T95" s="168"/>
+      <c r="U95" s="166" t="s">
         <v>260</v>
       </c>
-      <c r="V95" s="146"/>
-      <c r="W95" s="146"/>
-      <c r="X95" s="146"/>
-      <c r="Y95" s="146"/>
-      <c r="Z95" s="146"/>
-      <c r="AA95" s="146"/>
-      <c r="AB95" s="147"/>
-      <c r="AC95" s="145" t="s">
+      <c r="V95" s="167"/>
+      <c r="W95" s="167"/>
+      <c r="X95" s="167"/>
+      <c r="Y95" s="167"/>
+      <c r="Z95" s="167"/>
+      <c r="AA95" s="167"/>
+      <c r="AB95" s="168"/>
+      <c r="AC95" s="166" t="s">
         <v>260</v>
       </c>
-      <c r="AD95" s="146"/>
-      <c r="AE95" s="146"/>
-      <c r="AF95" s="146"/>
-      <c r="AG95" s="146"/>
-      <c r="AH95" s="146"/>
-      <c r="AI95" s="146"/>
-      <c r="AJ95" s="147"/>
-      <c r="AK95" s="145" t="s">
+      <c r="AD95" s="167"/>
+      <c r="AE95" s="167"/>
+      <c r="AF95" s="167"/>
+      <c r="AG95" s="167"/>
+      <c r="AH95" s="167"/>
+      <c r="AI95" s="167"/>
+      <c r="AJ95" s="168"/>
+      <c r="AK95" s="166" t="s">
         <v>260</v>
       </c>
-      <c r="AL95" s="146"/>
-      <c r="AM95" s="146"/>
-      <c r="AN95" s="146"/>
-      <c r="AO95" s="146"/>
-      <c r="AP95" s="146"/>
-      <c r="AQ95" s="146"/>
-      <c r="AR95" s="147"/>
-      <c r="AS95" s="190" t="s">
+      <c r="AL95" s="167"/>
+      <c r="AM95" s="167"/>
+      <c r="AN95" s="167"/>
+      <c r="AO95" s="167"/>
+      <c r="AP95" s="167"/>
+      <c r="AQ95" s="167"/>
+      <c r="AR95" s="168"/>
+      <c r="AS95" s="163" t="s">
         <v>356</v>
       </c>
-      <c r="AT95" s="191"/>
-      <c r="AU95" s="191"/>
-      <c r="AV95" s="191"/>
-      <c r="AW95" s="191"/>
-      <c r="AX95" s="191"/>
-      <c r="AY95" s="191"/>
-      <c r="AZ95" s="192"/>
+      <c r="AT95" s="164"/>
+      <c r="AU95" s="164"/>
+      <c r="AV95" s="164"/>
+      <c r="AW95" s="164"/>
+      <c r="AX95" s="164"/>
+      <c r="AY95" s="164"/>
+      <c r="AZ95" s="165"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -12444,68 +12469,68 @@
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="137" t="s">
+      <c r="E97" s="190" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="138"/>
-      <c r="G97" s="138"/>
-      <c r="H97" s="138"/>
-      <c r="I97" s="138"/>
-      <c r="J97" s="138"/>
-      <c r="K97" s="139"/>
-      <c r="L97" s="137" t="s">
+      <c r="F97" s="192"/>
+      <c r="G97" s="192"/>
+      <c r="H97" s="192"/>
+      <c r="I97" s="192"/>
+      <c r="J97" s="192"/>
+      <c r="K97" s="191"/>
+      <c r="L97" s="190" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="138"/>
-      <c r="N97" s="138"/>
-      <c r="O97" s="137" t="s">
+      <c r="M97" s="192"/>
+      <c r="N97" s="192"/>
+      <c r="O97" s="190" t="s">
         <v>272</v>
       </c>
-      <c r="P97" s="138"/>
-      <c r="Q97" s="138"/>
-      <c r="R97" s="138"/>
-      <c r="S97" s="138"/>
-      <c r="T97" s="139"/>
-      <c r="U97" s="137" t="s">
+      <c r="P97" s="192"/>
+      <c r="Q97" s="192"/>
+      <c r="R97" s="192"/>
+      <c r="S97" s="192"/>
+      <c r="T97" s="191"/>
+      <c r="U97" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="V97" s="138"/>
-      <c r="W97" s="138"/>
-      <c r="X97" s="138"/>
-      <c r="Y97" s="138"/>
-      <c r="Z97" s="138"/>
-      <c r="AA97" s="138"/>
-      <c r="AB97" s="139"/>
-      <c r="AC97" s="137" t="s">
+      <c r="V97" s="192"/>
+      <c r="W97" s="192"/>
+      <c r="X97" s="192"/>
+      <c r="Y97" s="192"/>
+      <c r="Z97" s="192"/>
+      <c r="AA97" s="192"/>
+      <c r="AB97" s="191"/>
+      <c r="AC97" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="AD97" s="138"/>
-      <c r="AE97" s="138"/>
-      <c r="AF97" s="138"/>
-      <c r="AG97" s="138"/>
-      <c r="AH97" s="138"/>
-      <c r="AI97" s="138"/>
-      <c r="AJ97" s="139"/>
-      <c r="AK97" s="137" t="s">
+      <c r="AD97" s="192"/>
+      <c r="AE97" s="192"/>
+      <c r="AF97" s="192"/>
+      <c r="AG97" s="192"/>
+      <c r="AH97" s="192"/>
+      <c r="AI97" s="192"/>
+      <c r="AJ97" s="191"/>
+      <c r="AK97" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="AL97" s="138"/>
-      <c r="AM97" s="138"/>
-      <c r="AN97" s="138"/>
-      <c r="AO97" s="138"/>
-      <c r="AP97" s="138"/>
-      <c r="AQ97" s="138"/>
-      <c r="AR97" s="139"/>
-      <c r="AS97" s="138" t="s">
+      <c r="AL97" s="192"/>
+      <c r="AM97" s="192"/>
+      <c r="AN97" s="192"/>
+      <c r="AO97" s="192"/>
+      <c r="AP97" s="192"/>
+      <c r="AQ97" s="192"/>
+      <c r="AR97" s="191"/>
+      <c r="AS97" s="192" t="s">
         <v>229</v>
       </c>
-      <c r="AT97" s="138"/>
-      <c r="AU97" s="138"/>
-      <c r="AV97" s="138"/>
-      <c r="AW97" s="138"/>
-      <c r="AX97" s="138"/>
-      <c r="AY97" s="138"/>
-      <c r="AZ97" s="139"/>
+      <c r="AT97" s="192"/>
+      <c r="AU97" s="192"/>
+      <c r="AV97" s="192"/>
+      <c r="AW97" s="192"/>
+      <c r="AX97" s="192"/>
+      <c r="AY97" s="192"/>
+      <c r="AZ97" s="191"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -12580,68 +12605,68 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="187" t="s">
+      <c r="E99" s="157" t="s">
         <v>402</v>
       </c>
-      <c r="F99" s="188"/>
-      <c r="G99" s="188"/>
-      <c r="H99" s="188"/>
-      <c r="I99" s="188"/>
-      <c r="J99" s="188"/>
-      <c r="K99" s="189"/>
-      <c r="L99" s="140" t="s">
+      <c r="F99" s="158"/>
+      <c r="G99" s="158"/>
+      <c r="H99" s="158"/>
+      <c r="I99" s="158"/>
+      <c r="J99" s="158"/>
+      <c r="K99" s="159"/>
+      <c r="L99" s="160" t="s">
         <v>246</v>
       </c>
-      <c r="M99" s="141"/>
-      <c r="N99" s="142"/>
-      <c r="O99" s="184" t="s">
+      <c r="M99" s="161"/>
+      <c r="N99" s="162"/>
+      <c r="O99" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="P99" s="185"/>
-      <c r="Q99" s="185"/>
-      <c r="R99" s="185"/>
-      <c r="S99" s="185"/>
-      <c r="T99" s="186"/>
-      <c r="U99" s="184" t="s">
+      <c r="P99" s="155"/>
+      <c r="Q99" s="155"/>
+      <c r="R99" s="155"/>
+      <c r="S99" s="155"/>
+      <c r="T99" s="156"/>
+      <c r="U99" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="V99" s="185"/>
-      <c r="W99" s="185"/>
-      <c r="X99" s="185"/>
-      <c r="Y99" s="185"/>
-      <c r="Z99" s="185"/>
-      <c r="AA99" s="185"/>
-      <c r="AB99" s="186"/>
-      <c r="AC99" s="184" t="s">
+      <c r="V99" s="155"/>
+      <c r="W99" s="155"/>
+      <c r="X99" s="155"/>
+      <c r="Y99" s="155"/>
+      <c r="Z99" s="155"/>
+      <c r="AA99" s="155"/>
+      <c r="AB99" s="156"/>
+      <c r="AC99" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="AD99" s="185"/>
-      <c r="AE99" s="185"/>
-      <c r="AF99" s="185"/>
-      <c r="AG99" s="185"/>
-      <c r="AH99" s="185"/>
-      <c r="AI99" s="185"/>
-      <c r="AJ99" s="186"/>
-      <c r="AK99" s="184" t="s">
+      <c r="AD99" s="155"/>
+      <c r="AE99" s="155"/>
+      <c r="AF99" s="155"/>
+      <c r="AG99" s="155"/>
+      <c r="AH99" s="155"/>
+      <c r="AI99" s="155"/>
+      <c r="AJ99" s="156"/>
+      <c r="AK99" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="AL99" s="185"/>
-      <c r="AM99" s="185"/>
-      <c r="AN99" s="185"/>
-      <c r="AO99" s="185"/>
-      <c r="AP99" s="185"/>
-      <c r="AQ99" s="185"/>
-      <c r="AR99" s="186"/>
-      <c r="AS99" s="184" t="s">
+      <c r="AL99" s="155"/>
+      <c r="AM99" s="155"/>
+      <c r="AN99" s="155"/>
+      <c r="AO99" s="155"/>
+      <c r="AP99" s="155"/>
+      <c r="AQ99" s="155"/>
+      <c r="AR99" s="156"/>
+      <c r="AS99" s="154" t="s">
         <v>301</v>
       </c>
-      <c r="AT99" s="185"/>
-      <c r="AU99" s="185"/>
-      <c r="AV99" s="185"/>
-      <c r="AW99" s="185"/>
-      <c r="AX99" s="185"/>
-      <c r="AY99" s="185"/>
-      <c r="AZ99" s="186"/>
+      <c r="AT99" s="155"/>
+      <c r="AU99" s="155"/>
+      <c r="AV99" s="155"/>
+      <c r="AW99" s="155"/>
+      <c r="AX99" s="155"/>
+      <c r="AY99" s="155"/>
+      <c r="AZ99" s="156"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -12783,68 +12808,68 @@
         <v>367</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="134" t="s">
+      <c r="E102" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="135"/>
-      <c r="G102" s="135"/>
-      <c r="H102" s="135"/>
-      <c r="I102" s="135"/>
-      <c r="J102" s="135"/>
-      <c r="K102" s="155"/>
-      <c r="L102" s="134" t="s">
+      <c r="F102" s="131"/>
+      <c r="G102" s="131"/>
+      <c r="H102" s="131"/>
+      <c r="I102" s="131"/>
+      <c r="J102" s="131"/>
+      <c r="K102" s="132"/>
+      <c r="L102" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="M102" s="135"/>
-      <c r="N102" s="155"/>
-      <c r="O102" s="134" t="s">
+      <c r="M102" s="131"/>
+      <c r="N102" s="132"/>
+      <c r="O102" s="130" t="s">
         <v>232</v>
       </c>
-      <c r="P102" s="135"/>
-      <c r="Q102" s="135"/>
-      <c r="R102" s="155"/>
-      <c r="S102" s="134" t="s">
+      <c r="P102" s="131"/>
+      <c r="Q102" s="131"/>
+      <c r="R102" s="132"/>
+      <c r="S102" s="130" t="s">
         <v>306</v>
       </c>
-      <c r="T102" s="135"/>
-      <c r="U102" s="135"/>
-      <c r="V102" s="135"/>
-      <c r="W102" s="135"/>
-      <c r="X102" s="135"/>
-      <c r="Y102" s="135"/>
-      <c r="Z102" s="135"/>
-      <c r="AA102" s="135"/>
-      <c r="AB102" s="135"/>
-      <c r="AC102" s="135"/>
-      <c r="AD102" s="155"/>
-      <c r="AE102" s="134" t="s">
+      <c r="T102" s="131"/>
+      <c r="U102" s="131"/>
+      <c r="V102" s="131"/>
+      <c r="W102" s="131"/>
+      <c r="X102" s="131"/>
+      <c r="Y102" s="131"/>
+      <c r="Z102" s="131"/>
+      <c r="AA102" s="131"/>
+      <c r="AB102" s="131"/>
+      <c r="AC102" s="131"/>
+      <c r="AD102" s="132"/>
+      <c r="AE102" s="130" t="s">
         <v>307</v>
       </c>
-      <c r="AF102" s="135"/>
-      <c r="AG102" s="135"/>
-      <c r="AH102" s="135"/>
-      <c r="AI102" s="135"/>
-      <c r="AJ102" s="135"/>
-      <c r="AK102" s="135"/>
-      <c r="AL102" s="135"/>
-      <c r="AM102" s="135"/>
-      <c r="AN102" s="135"/>
-      <c r="AO102" s="135"/>
-      <c r="AP102" s="155"/>
-      <c r="AQ102" s="134" t="s">
+      <c r="AF102" s="131"/>
+      <c r="AG102" s="131"/>
+      <c r="AH102" s="131"/>
+      <c r="AI102" s="131"/>
+      <c r="AJ102" s="131"/>
+      <c r="AK102" s="131"/>
+      <c r="AL102" s="131"/>
+      <c r="AM102" s="131"/>
+      <c r="AN102" s="131"/>
+      <c r="AO102" s="131"/>
+      <c r="AP102" s="132"/>
+      <c r="AQ102" s="130" t="s">
         <v>224</v>
       </c>
-      <c r="AR102" s="155"/>
-      <c r="AS102" s="134" t="s">
+      <c r="AR102" s="132"/>
+      <c r="AS102" s="130" t="s">
         <v>234</v>
       </c>
-      <c r="AT102" s="135"/>
-      <c r="AU102" s="135"/>
-      <c r="AV102" s="135"/>
-      <c r="AW102" s="135"/>
-      <c r="AX102" s="135"/>
-      <c r="AY102" s="135"/>
-      <c r="AZ102" s="155"/>
+      <c r="AT102" s="131"/>
+      <c r="AU102" s="131"/>
+      <c r="AV102" s="131"/>
+      <c r="AW102" s="131"/>
+      <c r="AX102" s="131"/>
+      <c r="AY102" s="131"/>
+      <c r="AZ102" s="132"/>
       <c r="BA102" s="42"/>
       <c r="BB102" s="42"/>
       <c r="BC102" s="42"/>
@@ -12947,68 +12972,68 @@
       <c r="B104" s="42"/>
       <c r="C104" s="42"/>
       <c r="D104" s="42"/>
-      <c r="E104" s="137" t="s">
+      <c r="E104" s="190" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="138"/>
-      <c r="G104" s="138"/>
-      <c r="H104" s="138"/>
-      <c r="I104" s="138"/>
-      <c r="J104" s="138"/>
-      <c r="K104" s="139"/>
-      <c r="L104" s="137" t="s">
+      <c r="F104" s="192"/>
+      <c r="G104" s="192"/>
+      <c r="H104" s="192"/>
+      <c r="I104" s="192"/>
+      <c r="J104" s="192"/>
+      <c r="K104" s="191"/>
+      <c r="L104" s="190" t="s">
         <v>226</v>
       </c>
-      <c r="M104" s="138"/>
-      <c r="N104" s="139"/>
-      <c r="O104" s="137" t="s">
+      <c r="M104" s="192"/>
+      <c r="N104" s="191"/>
+      <c r="O104" s="190" t="s">
         <v>227</v>
       </c>
-      <c r="P104" s="138"/>
-      <c r="Q104" s="138"/>
-      <c r="R104" s="139"/>
-      <c r="S104" s="137" t="s">
+      <c r="P104" s="192"/>
+      <c r="Q104" s="192"/>
+      <c r="R104" s="191"/>
+      <c r="S104" s="190" t="s">
         <v>228</v>
       </c>
-      <c r="T104" s="138"/>
-      <c r="U104" s="138"/>
-      <c r="V104" s="138"/>
-      <c r="W104" s="138"/>
-      <c r="X104" s="138"/>
-      <c r="Y104" s="138"/>
-      <c r="Z104" s="138"/>
-      <c r="AA104" s="138"/>
-      <c r="AB104" s="138"/>
-      <c r="AC104" s="138"/>
-      <c r="AD104" s="139"/>
-      <c r="AE104" s="137" t="s">
+      <c r="T104" s="192"/>
+      <c r="U104" s="192"/>
+      <c r="V104" s="192"/>
+      <c r="W104" s="192"/>
+      <c r="X104" s="192"/>
+      <c r="Y104" s="192"/>
+      <c r="Z104" s="192"/>
+      <c r="AA104" s="192"/>
+      <c r="AB104" s="192"/>
+      <c r="AC104" s="192"/>
+      <c r="AD104" s="191"/>
+      <c r="AE104" s="190" t="s">
         <v>228</v>
       </c>
-      <c r="AF104" s="138"/>
-      <c r="AG104" s="138"/>
-      <c r="AH104" s="138"/>
-      <c r="AI104" s="138"/>
-      <c r="AJ104" s="138"/>
-      <c r="AK104" s="138"/>
-      <c r="AL104" s="138"/>
-      <c r="AM104" s="138"/>
-      <c r="AN104" s="138"/>
-      <c r="AO104" s="138"/>
-      <c r="AP104" s="139"/>
-      <c r="AQ104" s="137" t="s">
+      <c r="AF104" s="192"/>
+      <c r="AG104" s="192"/>
+      <c r="AH104" s="192"/>
+      <c r="AI104" s="192"/>
+      <c r="AJ104" s="192"/>
+      <c r="AK104" s="192"/>
+      <c r="AL104" s="192"/>
+      <c r="AM104" s="192"/>
+      <c r="AN104" s="192"/>
+      <c r="AO104" s="192"/>
+      <c r="AP104" s="191"/>
+      <c r="AQ104" s="190" t="s">
         <v>230</v>
       </c>
-      <c r="AR104" s="139"/>
-      <c r="AS104" s="137" t="s">
+      <c r="AR104" s="191"/>
+      <c r="AS104" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="AT104" s="138"/>
-      <c r="AU104" s="138"/>
-      <c r="AV104" s="138"/>
-      <c r="AW104" s="138"/>
-      <c r="AX104" s="138"/>
-      <c r="AY104" s="138"/>
-      <c r="AZ104" s="139"/>
+      <c r="AT104" s="192"/>
+      <c r="AU104" s="192"/>
+      <c r="AV104" s="192"/>
+      <c r="AW104" s="192"/>
+      <c r="AX104" s="192"/>
+      <c r="AY104" s="192"/>
+      <c r="AZ104" s="191"/>
       <c r="BA104" s="42"/>
       <c r="BB104" s="42"/>
       <c r="BC104" s="42"/>
@@ -13094,11 +13119,11 @@
       <c r="I106" s="76"/>
       <c r="J106" s="76"/>
       <c r="K106" s="77"/>
-      <c r="L106" s="140" t="s">
+      <c r="L106" s="160" t="s">
         <v>246</v>
       </c>
-      <c r="M106" s="141"/>
-      <c r="N106" s="142"/>
+      <c r="M106" s="161"/>
+      <c r="N106" s="162"/>
       <c r="O106" s="53"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="50"/>
@@ -13137,16 +13162,16 @@
       <c r="AR106" s="51">
         <v>0</v>
       </c>
-      <c r="AS106" s="193" t="s">
+      <c r="AS106" s="126" t="s">
         <v>231</v>
       </c>
-      <c r="AT106" s="194"/>
-      <c r="AU106" s="194"/>
-      <c r="AV106" s="194"/>
-      <c r="AW106" s="194"/>
-      <c r="AX106" s="194"/>
-      <c r="AY106" s="194"/>
-      <c r="AZ106" s="195"/>
+      <c r="AT106" s="127"/>
+      <c r="AU106" s="127"/>
+      <c r="AV106" s="127"/>
+      <c r="AW106" s="127"/>
+      <c r="AX106" s="127"/>
+      <c r="AY106" s="127"/>
+      <c r="AZ106" s="128"/>
       <c r="BA106" s="50" t="s">
         <v>316</v>
       </c>
@@ -13212,16 +13237,16 @@
       <c r="AR107" s="51">
         <v>1</v>
       </c>
-      <c r="AS107" s="193" t="s">
+      <c r="AS107" s="126" t="s">
         <v>354</v>
       </c>
-      <c r="AT107" s="194"/>
-      <c r="AU107" s="194"/>
-      <c r="AV107" s="194"/>
-      <c r="AW107" s="194"/>
-      <c r="AX107" s="194"/>
-      <c r="AY107" s="194"/>
-      <c r="AZ107" s="195"/>
+      <c r="AT107" s="127"/>
+      <c r="AU107" s="127"/>
+      <c r="AV107" s="127"/>
+      <c r="AW107" s="127"/>
+      <c r="AX107" s="127"/>
+      <c r="AY107" s="127"/>
+      <c r="AZ107" s="128"/>
       <c r="BA107" s="50" t="s">
         <v>298</v>
       </c>
@@ -13289,16 +13314,16 @@
       <c r="AR108" s="51">
         <v>0</v>
       </c>
-      <c r="AS108" s="193" t="s">
+      <c r="AS108" s="126" t="s">
         <v>353</v>
       </c>
-      <c r="AT108" s="194"/>
-      <c r="AU108" s="194"/>
-      <c r="AV108" s="194"/>
-      <c r="AW108" s="194"/>
-      <c r="AX108" s="194"/>
-      <c r="AY108" s="194"/>
-      <c r="AZ108" s="195"/>
+      <c r="AT108" s="127"/>
+      <c r="AU108" s="127"/>
+      <c r="AV108" s="127"/>
+      <c r="AW108" s="127"/>
+      <c r="AX108" s="127"/>
+      <c r="AY108" s="127"/>
+      <c r="AZ108" s="128"/>
       <c r="BA108" s="50" t="s">
         <v>265</v>
       </c>
@@ -13362,16 +13387,16 @@
       <c r="AR109" s="51">
         <v>1</v>
       </c>
-      <c r="AS109" s="193" t="s">
+      <c r="AS109" s="126" t="s">
         <v>233</v>
       </c>
-      <c r="AT109" s="194"/>
-      <c r="AU109" s="194"/>
-      <c r="AV109" s="194"/>
-      <c r="AW109" s="194"/>
-      <c r="AX109" s="194"/>
-      <c r="AY109" s="194"/>
-      <c r="AZ109" s="195"/>
+      <c r="AT109" s="127"/>
+      <c r="AU109" s="127"/>
+      <c r="AV109" s="127"/>
+      <c r="AW109" s="127"/>
+      <c r="AX109" s="127"/>
+      <c r="AY109" s="127"/>
+      <c r="AZ109" s="128"/>
       <c r="BA109" s="50" t="s">
         <v>260</v>
       </c>
@@ -13527,12 +13552,12 @@
       <c r="L112" s="49"/>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
-      <c r="O112" s="181" t="s">
+      <c r="O112" s="151" t="s">
         <v>232</v>
       </c>
-      <c r="P112" s="182"/>
-      <c r="Q112" s="182"/>
-      <c r="R112" s="183"/>
+      <c r="P112" s="152"/>
+      <c r="Q112" s="152"/>
+      <c r="R112" s="153"/>
       <c r="S112" s="50"/>
       <c r="T112" s="50"/>
       <c r="U112" s="50"/>
@@ -13557,20 +13582,20 @@
       <c r="AN112" s="50"/>
       <c r="AO112" s="50"/>
       <c r="AP112" s="50"/>
-      <c r="AQ112" s="176" t="s">
+      <c r="AQ112" s="146" t="s">
         <v>302</v>
       </c>
-      <c r="AR112" s="177"/>
-      <c r="AS112" s="178" t="s">
+      <c r="AR112" s="147"/>
+      <c r="AS112" s="148" t="s">
         <v>299</v>
       </c>
-      <c r="AT112" s="179"/>
-      <c r="AU112" s="179"/>
-      <c r="AV112" s="179"/>
-      <c r="AW112" s="179"/>
-      <c r="AX112" s="179"/>
-      <c r="AY112" s="179"/>
-      <c r="AZ112" s="180"/>
+      <c r="AT112" s="149"/>
+      <c r="AU112" s="149"/>
+      <c r="AV112" s="149"/>
+      <c r="AW112" s="149"/>
+      <c r="AX112" s="149"/>
+      <c r="AY112" s="149"/>
+      <c r="AZ112" s="150"/>
       <c r="BA112" s="42"/>
       <c r="BB112" s="42"/>
       <c r="BC112" s="42"/>
@@ -14771,20 +14796,20 @@
       <c r="AN130" s="42"/>
       <c r="AO130" s="42"/>
       <c r="AP130" s="42"/>
-      <c r="AQ130" s="176" t="s">
+      <c r="AQ130" s="146" t="s">
         <v>304</v>
       </c>
-      <c r="AR130" s="177"/>
-      <c r="AS130" s="178" t="s">
+      <c r="AR130" s="147"/>
+      <c r="AS130" s="148" t="s">
         <v>355</v>
       </c>
-      <c r="AT130" s="179"/>
-      <c r="AU130" s="179"/>
-      <c r="AV130" s="179"/>
-      <c r="AW130" s="179"/>
-      <c r="AX130" s="179"/>
-      <c r="AY130" s="179"/>
-      <c r="AZ130" s="180"/>
+      <c r="AT130" s="149"/>
+      <c r="AU130" s="149"/>
+      <c r="AV130" s="149"/>
+      <c r="AW130" s="149"/>
+      <c r="AX130" s="149"/>
+      <c r="AY130" s="149"/>
+      <c r="AZ130" s="150"/>
       <c r="BA130" s="42"/>
       <c r="BB130" s="42"/>
       <c r="BC130" s="42"/>
@@ -14838,16 +14863,16 @@
       <c r="AP131" s="42"/>
       <c r="AQ131" s="42"/>
       <c r="AR131" s="42"/>
-      <c r="AS131" s="184" t="s">
+      <c r="AS131" s="154" t="s">
         <v>301</v>
       </c>
-      <c r="AT131" s="185"/>
-      <c r="AU131" s="185"/>
-      <c r="AV131" s="185"/>
-      <c r="AW131" s="185"/>
-      <c r="AX131" s="185"/>
-      <c r="AY131" s="185"/>
-      <c r="AZ131" s="186"/>
+      <c r="AT131" s="155"/>
+      <c r="AU131" s="155"/>
+      <c r="AV131" s="155"/>
+      <c r="AW131" s="155"/>
+      <c r="AX131" s="155"/>
+      <c r="AY131" s="155"/>
+      <c r="AZ131" s="156"/>
       <c r="BA131" s="42"/>
       <c r="BB131" s="42"/>
       <c r="BC131" s="42"/>
@@ -14960,20 +14985,20 @@
       <c r="AN133" s="42"/>
       <c r="AO133" s="42"/>
       <c r="AP133" s="42"/>
-      <c r="AQ133" s="176" t="s">
+      <c r="AQ133" s="146" t="s">
         <v>303</v>
       </c>
-      <c r="AR133" s="177"/>
-      <c r="AS133" s="178" t="s">
+      <c r="AR133" s="147"/>
+      <c r="AS133" s="148" t="s">
         <v>305</v>
       </c>
-      <c r="AT133" s="179"/>
-      <c r="AU133" s="179"/>
-      <c r="AV133" s="179"/>
-      <c r="AW133" s="179"/>
-      <c r="AX133" s="179"/>
-      <c r="AY133" s="179"/>
-      <c r="AZ133" s="180"/>
+      <c r="AT133" s="149"/>
+      <c r="AU133" s="149"/>
+      <c r="AV133" s="149"/>
+      <c r="AW133" s="149"/>
+      <c r="AX133" s="149"/>
+      <c r="AY133" s="149"/>
+      <c r="AZ133" s="150"/>
       <c r="BA133" s="42"/>
       <c r="BB133" s="42"/>
       <c r="BC133" s="42"/>
@@ -17596,6 +17621,193 @@
     </row>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="AZ23:BF23"/>
+    <mergeCell ref="BB24:BF24"/>
+    <mergeCell ref="BD25:BF25"/>
+    <mergeCell ref="AD25:AF25"/>
+    <mergeCell ref="L15:AF15"/>
+    <mergeCell ref="N16:AF16"/>
+    <mergeCell ref="P17:AF17"/>
+    <mergeCell ref="P18:AF18"/>
+    <mergeCell ref="AL15:BF15"/>
+    <mergeCell ref="AN16:BF16"/>
+    <mergeCell ref="AP17:BF17"/>
+    <mergeCell ref="AP18:BF18"/>
+    <mergeCell ref="AX22:BF22"/>
+    <mergeCell ref="AJ15:AK15"/>
+    <mergeCell ref="AV22:AW22"/>
+    <mergeCell ref="AH15:AI15"/>
+    <mergeCell ref="AJ16:AK16"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AT22:AU22"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AX23:AY23"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="U95:AB95"/>
+    <mergeCell ref="O95:T95"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="AQ104:AR104"/>
+    <mergeCell ref="AS104:AZ104"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="AS97:AZ97"/>
+    <mergeCell ref="AK97:AR97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="O104:R104"/>
+    <mergeCell ref="S104:AD104"/>
+    <mergeCell ref="AE104:AP104"/>
+    <mergeCell ref="AC97:AJ97"/>
+    <mergeCell ref="U97:AB97"/>
+    <mergeCell ref="O97:T97"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AQ112:AR112"/>
+    <mergeCell ref="AQ130:AR130"/>
+    <mergeCell ref="AQ133:AR133"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="AS112:AZ112"/>
+    <mergeCell ref="O112:R112"/>
+    <mergeCell ref="AS130:AZ130"/>
+    <mergeCell ref="AS131:AZ131"/>
+    <mergeCell ref="AS133:AZ133"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="U99:AB99"/>
+    <mergeCell ref="AC99:AJ99"/>
+    <mergeCell ref="AK99:AR99"/>
+    <mergeCell ref="AS99:AZ99"/>
+    <mergeCell ref="O99:T99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AS95:AZ95"/>
+    <mergeCell ref="AK95:AR95"/>
+    <mergeCell ref="AC95:AJ95"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
     <mergeCell ref="AS109:AZ109"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="S102:AD102"/>
@@ -17620,193 +17832,6 @@
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="Z30:AA30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="AQ112:AR112"/>
-    <mergeCell ref="AQ130:AR130"/>
-    <mergeCell ref="AQ133:AR133"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="AS112:AZ112"/>
-    <mergeCell ref="O112:R112"/>
-    <mergeCell ref="AS130:AZ130"/>
-    <mergeCell ref="AS131:AZ131"/>
-    <mergeCell ref="AS133:AZ133"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="U99:AB99"/>
-    <mergeCell ref="AC99:AJ99"/>
-    <mergeCell ref="AK99:AR99"/>
-    <mergeCell ref="AS99:AZ99"/>
-    <mergeCell ref="O99:T99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AS95:AZ95"/>
-    <mergeCell ref="AK95:AR95"/>
-    <mergeCell ref="AC95:AJ95"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AQ104:AR104"/>
-    <mergeCell ref="AS104:AZ104"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="AS97:AZ97"/>
-    <mergeCell ref="AK97:AR97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="L104:N104"/>
-    <mergeCell ref="O104:R104"/>
-    <mergeCell ref="S104:AD104"/>
-    <mergeCell ref="AE104:AP104"/>
-    <mergeCell ref="AC97:AJ97"/>
-    <mergeCell ref="U97:AB97"/>
-    <mergeCell ref="O97:T97"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="U95:AB95"/>
-    <mergeCell ref="O95:T95"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="AZ23:BF23"/>
-    <mergeCell ref="BB24:BF24"/>
-    <mergeCell ref="BD25:BF25"/>
-    <mergeCell ref="AD25:AF25"/>
-    <mergeCell ref="L15:AF15"/>
-    <mergeCell ref="N16:AF16"/>
-    <mergeCell ref="P17:AF17"/>
-    <mergeCell ref="P18:AF18"/>
-    <mergeCell ref="AL15:BF15"/>
-    <mergeCell ref="AN16:BF16"/>
-    <mergeCell ref="AP17:BF17"/>
-    <mergeCell ref="AP18:BF18"/>
-    <mergeCell ref="AX22:BF22"/>
-    <mergeCell ref="AJ15:AK15"/>
-    <mergeCell ref="AV22:AW22"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AT22:AU22"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AX23:AY23"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[Slot Doc] Add device code in pin mapping for project
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40003728-477F-4164-9446-2FDFF334A45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1BB6B0-E119-4281-8180-EEE24AE2E3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
@@ -1390,9 +1390,6 @@
     <t>CS_CPU</t>
   </si>
   <si>
-    <t>Pin Mapping SLAVE (QFN 32 pin)</t>
-  </si>
-  <si>
     <t>4,5,6</t>
   </si>
   <si>
@@ -1423,13 +1420,16 @@
     <t>No LED#3/Debug Dout#3</t>
   </si>
   <si>
-    <t>Pin Mapping MASTER (QFN 32 pin)</t>
-  </si>
-  <si>
     <t>Pin Mapping MASTER/SLAVE EFR32xG22 (BRD4182A - QFN 40 pin)</t>
   </si>
   <si>
-    <t>Pin Mapping MASTER/SLAVE EFR32xG22 (BRD4183A - QFN 32 pin)</t>
+    <t>Pin Mapping MASTER (EFR32MG22C224F512IM40 - QFN 32 pin)</t>
+  </si>
+  <si>
+    <t>Pin Mapping SLAVE (EFR32MG22C224F512IM40 - QFN 32 pin)</t>
+  </si>
+  <si>
+    <t>Pin Mapping SLAVE EFR32xG22 (BRD4183A - QFN 32 pin)</t>
   </si>
 </sst>
 </file>
@@ -2297,13 +2297,57 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2312,62 +2356,17 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2376,81 +2375,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2495,6 +2419,15 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2504,41 +2437,108 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3617,7 +3617,7 @@
   </sheetPr>
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -3644,7 +3644,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="M1" s="17" t="s">
         <v>450</v>
@@ -4675,59 +4675,59 @@
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A20" s="200" t="s">
+      <c r="A20" s="126" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="201">
+      <c r="B20" s="127">
         <v>1</v>
       </c>
-      <c r="C20" s="200" t="s">
+      <c r="C20" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="200" t="s">
+      <c r="D20" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="202" t="s">
+      <c r="E20" s="128" t="s">
         <v>115</v>
       </c>
-      <c r="F20" s="200" t="s">
+      <c r="F20" s="126" t="s">
         <v>379</v>
       </c>
-      <c r="G20" s="200" t="s">
+      <c r="G20" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="202" t="s">
+      <c r="H20" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="I20" s="200" t="s">
+      <c r="I20" s="126" t="s">
         <v>119</v>
       </c>
       <c r="K20" s="90" t="s">
         <v>387</v>
       </c>
-      <c r="M20" s="202" t="s">
+      <c r="M20" s="128" t="s">
         <v>114</v>
       </c>
-      <c r="N20" s="203">
+      <c r="N20" s="129">
         <v>1</v>
       </c>
-      <c r="O20" s="202" t="s">
+      <c r="O20" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="P20" s="202" t="s">
+      <c r="P20" s="128" t="s">
         <v>117</v>
       </c>
-      <c r="Q20" s="202" t="s">
+      <c r="Q20" s="128" t="s">
         <v>115</v>
       </c>
-      <c r="R20" s="202"/>
-      <c r="S20" s="202" t="s">
+      <c r="R20" s="128"/>
+      <c r="S20" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="T20" s="202" t="s">
+      <c r="T20" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="U20" s="202" t="s">
+      <c r="U20" s="128" t="s">
         <v>119</v>
       </c>
       <c r="V20" s="96"/>
@@ -6081,7 +6081,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,7 +6106,7 @@
         <v>448</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="J1" s="5"/>
     </row>
@@ -6146,7 +6146,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C4" s="97" t="s">
         <v>46</v>
@@ -6155,7 +6155,7 @@
       <c r="E4" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="G4" s="206"/>
+      <c r="G4" s="132"/>
       <c r="I4" s="9" t="s">
         <v>59</v>
       </c>
@@ -6175,11 +6175,11 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="87"/>
-      <c r="B5" s="204"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="96"/>
       <c r="D5" s="87"/>
       <c r="E5" s="87"/>
-      <c r="G5" s="206"/>
+      <c r="G5" s="132"/>
       <c r="I5" s="9" t="s">
         <v>59</v>
       </c>
@@ -6199,11 +6199,11 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="87"/>
-      <c r="B6" s="204"/>
-      <c r="C6" s="205"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="131"/>
       <c r="D6" s="87"/>
       <c r="E6" s="87"/>
-      <c r="G6" s="206"/>
+      <c r="G6" s="132"/>
       <c r="I6" s="9" t="s">
         <v>59</v>
       </c>
@@ -6223,14 +6223,14 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="87"/>
-      <c r="B7" s="204"/>
-      <c r="C7" s="205"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="131"/>
       <c r="D7" s="87"/>
       <c r="E7" s="87"/>
-      <c r="G7" s="206"/>
+      <c r="G7" s="132"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K7" s="97"/>
       <c r="L7" s="9"/>
@@ -6256,9 +6256,9 @@
         <v>379</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>444</v>
-      </c>
-      <c r="G9" s="206"/>
+        <v>443</v>
+      </c>
+      <c r="G9" s="132"/>
       <c r="I9" s="9" t="s">
         <v>67</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>379</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6289,15 +6289,15 @@
         <v>379</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="G10" s="206"/>
-      <c r="I10" s="207"/>
-      <c r="J10" s="208"/>
-      <c r="K10" s="207"/>
-      <c r="L10" s="207"/>
+        <v>444</v>
+      </c>
+      <c r="G10" s="132"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="134"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
       <c r="M10" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N10" s="96"/>
     </row>
@@ -6320,7 +6320,7 @@
       <c r="E12" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="G12" s="206"/>
+      <c r="G12" s="132"/>
       <c r="I12" s="9" t="s">
         <v>131</v>
       </c>
@@ -6353,7 +6353,7 @@
       <c r="E13" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="G13" s="206"/>
+      <c r="G13" s="132"/>
       <c r="I13" s="9" t="s">
         <v>131</v>
       </c>
@@ -6384,9 +6384,9 @@
         <v>379</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>446</v>
-      </c>
-      <c r="G14" s="206"/>
+        <v>445</v>
+      </c>
+      <c r="G14" s="132"/>
       <c r="I14" s="9" t="s">
         <v>131</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>379</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6412,9 +6412,9 @@
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>440</v>
-      </c>
-      <c r="G16" s="206"/>
+        <v>439</v>
+      </c>
+      <c r="G16" s="132"/>
       <c r="I16" s="9" t="s">
         <v>77</v>
       </c>
@@ -6438,9 +6438,9 @@
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>441</v>
-      </c>
-      <c r="G18" s="206"/>
+        <v>440</v>
+      </c>
+      <c r="G18" s="132"/>
       <c r="I18" s="9" t="s">
         <v>114</v>
       </c>
@@ -6476,7 +6476,7 @@
       <c r="E20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="206"/>
+      <c r="G20" s="132"/>
       <c r="I20" s="9" t="s">
         <v>82</v>
       </c>
@@ -6509,7 +6509,7 @@
       <c r="E21" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="206"/>
+      <c r="G21" s="132"/>
       <c r="I21" s="9" t="s">
         <v>82</v>
       </c>
@@ -6545,7 +6545,7 @@
       <c r="E23" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="G23" s="206"/>
+      <c r="G23" s="132"/>
       <c r="I23" s="7" t="s">
         <v>99</v>
       </c>
@@ -6578,7 +6578,7 @@
       <c r="E24" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="G24" s="206"/>
+      <c r="G24" s="132"/>
       <c r="I24" s="7" t="s">
         <v>99</v>
       </c>
@@ -6611,7 +6611,7 @@
       <c r="E25" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="G25" s="206"/>
+      <c r="G25" s="132"/>
       <c r="I25" s="7" t="s">
         <v>99</v>
       </c>
@@ -6644,7 +6644,7 @@
       <c r="E26" s="124" t="s">
         <v>435</v>
       </c>
-      <c r="G26" s="206"/>
+      <c r="G26" s="132"/>
       <c r="I26" s="124" t="s">
         <v>103</v>
       </c>
@@ -6664,11 +6664,11 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="87"/>
-      <c r="B27" s="204"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="87"/>
       <c r="D27" s="87"/>
       <c r="E27" s="87"/>
-      <c r="G27" s="206"/>
+      <c r="G27" s="132"/>
       <c r="I27" s="7" t="s">
         <v>103</v>
       </c>
@@ -6705,13 +6705,13 @@
       <c r="E29" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="206"/>
-      <c r="I29" s="207"/>
-      <c r="J29" s="208"/>
-      <c r="K29" s="207"/>
-      <c r="L29" s="207"/>
-      <c r="M29" s="209" t="s">
-        <v>443</v>
+      <c r="G29" s="132"/>
+      <c r="I29" s="133"/>
+      <c r="J29" s="134"/>
+      <c r="K29" s="133"/>
+      <c r="L29" s="133"/>
+      <c r="M29" s="135" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -6730,11 +6730,11 @@
       <c r="E30" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G30" s="206"/>
+      <c r="G30" s="132"/>
       <c r="I30" s="14"/>
       <c r="J30" s="123"/>
-      <c r="K30" s="207"/>
-      <c r="L30" s="207"/>
+      <c r="K30" s="133"/>
+      <c r="L30" s="133"/>
       <c r="M30" s="14"/>
       <c r="N30" s="96"/>
     </row>
@@ -6754,11 +6754,11 @@
       <c r="E31" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G31" s="206"/>
+      <c r="G31" s="132"/>
       <c r="I31" s="14"/>
       <c r="J31" s="123"/>
-      <c r="K31" s="207"/>
-      <c r="L31" s="207"/>
+      <c r="K31" s="133"/>
+      <c r="L31" s="133"/>
       <c r="M31" s="14"/>
       <c r="N31" s="96"/>
     </row>
@@ -6781,7 +6781,7 @@
       <c r="E33" s="121" t="s">
         <v>423</v>
       </c>
-      <c r="G33" s="206"/>
+      <c r="G33" s="132"/>
       <c r="I33" s="121" t="s">
         <v>416</v>
       </c>
@@ -6814,7 +6814,7 @@
       <c r="E34" s="121" t="s">
         <v>423</v>
       </c>
-      <c r="G34" s="206"/>
+      <c r="G34" s="132"/>
       <c r="I34" s="121" t="s">
         <v>416</v>
       </c>
@@ -7030,21 +7030,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
-      <c r="J3" s="198"/>
-      <c r="K3" s="198"/>
-      <c r="L3" s="198"/>
-      <c r="M3" s="198"/>
-      <c r="N3" s="198"/>
-      <c r="O3" s="198"/>
-      <c r="P3" s="198"/>
-      <c r="Q3" s="198"/>
-      <c r="R3" s="198"/>
-      <c r="S3" s="198"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -7152,45 +7152,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="154" t="s">
+      <c r="E5" s="197" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="155"/>
-      <c r="G5" s="155"/>
-      <c r="H5" s="155"/>
-      <c r="I5" s="155"/>
-      <c r="J5" s="156"/>
-      <c r="K5" s="158" t="s">
+      <c r="F5" s="198"/>
+      <c r="G5" s="198"/>
+      <c r="H5" s="198"/>
+      <c r="I5" s="198"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="188" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="161"/>
-      <c r="M5" s="161"/>
-      <c r="N5" s="161"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="158" t="s">
+      <c r="L5" s="205"/>
+      <c r="M5" s="205"/>
+      <c r="N5" s="205"/>
+      <c r="O5" s="189"/>
+      <c r="P5" s="188" t="s">
         <v>276</v>
       </c>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="162" t="s">
+      <c r="Q5" s="189"/>
+      <c r="R5" s="190" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="163"/>
-      <c r="T5" s="163"/>
-      <c r="U5" s="163"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="164"/>
-      <c r="X5" s="158" t="s">
+      <c r="S5" s="191"/>
+      <c r="T5" s="191"/>
+      <c r="U5" s="191"/>
+      <c r="V5" s="191"/>
+      <c r="W5" s="192"/>
+      <c r="X5" s="188" t="s">
         <v>270</v>
       </c>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="154" t="s">
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="197" t="s">
         <v>339</v>
       </c>
-      <c r="AA5" s="155"/>
-      <c r="AB5" s="155"/>
-      <c r="AC5" s="155"/>
-      <c r="AD5" s="155"/>
-      <c r="AE5" s="156"/>
+      <c r="AA5" s="198"/>
+      <c r="AB5" s="198"/>
+      <c r="AC5" s="198"/>
+      <c r="AD5" s="198"/>
+      <c r="AE5" s="199"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -7225,45 +7225,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="135" t="s">
+      <c r="E6" s="204" t="s">
         <v>395</v>
       </c>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="145" t="s">
+      <c r="F6" s="204"/>
+      <c r="G6" s="204"/>
+      <c r="H6" s="204"/>
+      <c r="I6" s="204"/>
+      <c r="J6" s="204"/>
+      <c r="K6" s="203" t="s">
         <v>336</v>
       </c>
-      <c r="L6" s="145"/>
-      <c r="M6" s="145"/>
-      <c r="N6" s="145"/>
-      <c r="O6" s="145"/>
-      <c r="P6" s="145" t="s">
+      <c r="L6" s="203"/>
+      <c r="M6" s="203"/>
+      <c r="N6" s="203"/>
+      <c r="O6" s="203"/>
+      <c r="P6" s="203" t="s">
         <v>338</v>
       </c>
-      <c r="Q6" s="145"/>
-      <c r="R6" s="135" t="s">
+      <c r="Q6" s="203"/>
+      <c r="R6" s="204" t="s">
         <v>271</v>
       </c>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135" t="s">
+      <c r="S6" s="204"/>
+      <c r="T6" s="204"/>
+      <c r="U6" s="204"/>
+      <c r="V6" s="204"/>
+      <c r="W6" s="204"/>
+      <c r="X6" s="204" t="s">
         <v>338</v>
       </c>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135" t="s">
+      <c r="Y6" s="204"/>
+      <c r="Z6" s="204" t="s">
         <v>395</v>
       </c>
-      <c r="AA6" s="135"/>
-      <c r="AB6" s="135"/>
-      <c r="AC6" s="135"/>
-      <c r="AD6" s="135"/>
-      <c r="AE6" s="135"/>
+      <c r="AA6" s="204"/>
+      <c r="AB6" s="204"/>
+      <c r="AC6" s="204"/>
+      <c r="AD6" s="204"/>
+      <c r="AE6" s="204"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -7304,29 +7304,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="160" t="s">
+      <c r="K7" s="196" t="s">
         <v>337</v>
       </c>
-      <c r="L7" s="160"/>
-      <c r="M7" s="160"/>
-      <c r="N7" s="160"/>
-      <c r="O7" s="160"/>
-      <c r="P7" s="160" t="s">
+      <c r="L7" s="196"/>
+      <c r="M7" s="196"/>
+      <c r="N7" s="196"/>
+      <c r="O7" s="196"/>
+      <c r="P7" s="196" t="s">
         <v>337</v>
       </c>
-      <c r="Q7" s="160"/>
-      <c r="R7" s="160" t="s">
+      <c r="Q7" s="196"/>
+      <c r="R7" s="196" t="s">
         <v>278</v>
       </c>
-      <c r="S7" s="160"/>
-      <c r="T7" s="160"/>
-      <c r="U7" s="160"/>
-      <c r="V7" s="160"/>
-      <c r="W7" s="160"/>
-      <c r="X7" s="160" t="s">
+      <c r="S7" s="196"/>
+      <c r="T7" s="196"/>
+      <c r="U7" s="196"/>
+      <c r="V7" s="196"/>
+      <c r="W7" s="196"/>
+      <c r="X7" s="196" t="s">
         <v>337</v>
       </c>
-      <c r="Y7" s="160"/>
+      <c r="Y7" s="196"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -7759,10 +7759,10 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="133" t="s">
+      <c r="E14" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="199"/>
+      <c r="F14" s="144"/>
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
@@ -7787,10 +7787,10 @@
       <c r="AB14" s="108"/>
       <c r="AC14" s="108"/>
       <c r="AD14" s="108"/>
-      <c r="AE14" s="133" t="s">
+      <c r="AE14" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="199"/>
+      <c r="AF14" s="144"/>
       <c r="AG14" s="104"/>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
@@ -7833,67 +7833,67 @@
       <c r="G15" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H15" s="131" t="s">
+      <c r="H15" s="145" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="132"/>
-      <c r="J15" s="129" t="s">
+      <c r="I15" s="146"/>
+      <c r="J15" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="130"/>
-      <c r="L15" s="126"/>
-      <c r="M15" s="127"/>
-      <c r="N15" s="127"/>
-      <c r="O15" s="127"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-      <c r="S15" s="127"/>
-      <c r="T15" s="127"/>
-      <c r="U15" s="127"/>
-      <c r="V15" s="127"/>
-      <c r="W15" s="127"/>
-      <c r="X15" s="127"/>
-      <c r="Y15" s="127"/>
-      <c r="Z15" s="127"/>
-      <c r="AA15" s="127"/>
-      <c r="AB15" s="127"/>
-      <c r="AC15" s="127"/>
-      <c r="AD15" s="127"/>
-      <c r="AE15" s="127"/>
-      <c r="AF15" s="128"/>
+      <c r="K15" s="148"/>
+      <c r="L15" s="206"/>
+      <c r="M15" s="207"/>
+      <c r="N15" s="207"/>
+      <c r="O15" s="207"/>
+      <c r="P15" s="207"/>
+      <c r="Q15" s="207"/>
+      <c r="R15" s="207"/>
+      <c r="S15" s="207"/>
+      <c r="T15" s="207"/>
+      <c r="U15" s="207"/>
+      <c r="V15" s="207"/>
+      <c r="W15" s="207"/>
+      <c r="X15" s="207"/>
+      <c r="Y15" s="207"/>
+      <c r="Z15" s="207"/>
+      <c r="AA15" s="207"/>
+      <c r="AB15" s="207"/>
+      <c r="AC15" s="207"/>
+      <c r="AD15" s="207"/>
+      <c r="AE15" s="207"/>
+      <c r="AF15" s="208"/>
       <c r="AG15" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="AH15" s="131" t="s">
+      <c r="AH15" s="145" t="s">
         <v>279</v>
       </c>
-      <c r="AI15" s="132"/>
-      <c r="AJ15" s="129" t="s">
+      <c r="AI15" s="146"/>
+      <c r="AJ15" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AK15" s="130"/>
-      <c r="AL15" s="126"/>
-      <c r="AM15" s="127"/>
-      <c r="AN15" s="127"/>
-      <c r="AO15" s="127"/>
-      <c r="AP15" s="127"/>
-      <c r="AQ15" s="127"/>
-      <c r="AR15" s="127"/>
-      <c r="AS15" s="127"/>
-      <c r="AT15" s="127"/>
-      <c r="AU15" s="127"/>
-      <c r="AV15" s="127"/>
-      <c r="AW15" s="127"/>
-      <c r="AX15" s="127"/>
-      <c r="AY15" s="127"/>
-      <c r="AZ15" s="127"/>
-      <c r="BA15" s="127"/>
-      <c r="BB15" s="127"/>
-      <c r="BC15" s="127"/>
-      <c r="BD15" s="127"/>
-      <c r="BE15" s="127"/>
-      <c r="BF15" s="127"/>
+      <c r="AK15" s="148"/>
+      <c r="AL15" s="206"/>
+      <c r="AM15" s="207"/>
+      <c r="AN15" s="207"/>
+      <c r="AO15" s="207"/>
+      <c r="AP15" s="207"/>
+      <c r="AQ15" s="207"/>
+      <c r="AR15" s="207"/>
+      <c r="AS15" s="207"/>
+      <c r="AT15" s="207"/>
+      <c r="AU15" s="207"/>
+      <c r="AV15" s="207"/>
+      <c r="AW15" s="207"/>
+      <c r="AX15" s="207"/>
+      <c r="AY15" s="207"/>
+      <c r="AZ15" s="207"/>
+      <c r="BA15" s="207"/>
+      <c r="BB15" s="207"/>
+      <c r="BC15" s="207"/>
+      <c r="BD15" s="207"/>
+      <c r="BE15" s="207"/>
+      <c r="BF15" s="207"/>
       <c r="BG15" s="103"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -7914,33 +7914,33 @@
         <v>287</v>
       </c>
       <c r="I16" s="110"/>
-      <c r="J16" s="131" t="s">
+      <c r="J16" s="145" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="132"/>
-      <c r="L16" s="129" t="s">
+      <c r="K16" s="146"/>
+      <c r="L16" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="M16" s="130"/>
-      <c r="N16" s="126"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="127"/>
-      <c r="R16" s="127"/>
-      <c r="S16" s="127"/>
-      <c r="T16" s="127"/>
-      <c r="U16" s="127"/>
-      <c r="V16" s="127"/>
-      <c r="W16" s="127"/>
-      <c r="X16" s="127"/>
-      <c r="Y16" s="127"/>
-      <c r="Z16" s="127"/>
-      <c r="AA16" s="127"/>
-      <c r="AB16" s="127"/>
-      <c r="AC16" s="127"/>
-      <c r="AD16" s="127"/>
-      <c r="AE16" s="127"/>
-      <c r="AF16" s="128"/>
+      <c r="M16" s="148"/>
+      <c r="N16" s="206"/>
+      <c r="O16" s="207"/>
+      <c r="P16" s="207"/>
+      <c r="Q16" s="207"/>
+      <c r="R16" s="207"/>
+      <c r="S16" s="207"/>
+      <c r="T16" s="207"/>
+      <c r="U16" s="207"/>
+      <c r="V16" s="207"/>
+      <c r="W16" s="207"/>
+      <c r="X16" s="207"/>
+      <c r="Y16" s="207"/>
+      <c r="Z16" s="207"/>
+      <c r="AA16" s="207"/>
+      <c r="AB16" s="207"/>
+      <c r="AC16" s="207"/>
+      <c r="AD16" s="207"/>
+      <c r="AE16" s="207"/>
+      <c r="AF16" s="208"/>
       <c r="AG16" s="106" t="s">
         <v>274</v>
       </c>
@@ -7948,33 +7948,33 @@
         <v>287</v>
       </c>
       <c r="AI16" s="110"/>
-      <c r="AJ16" s="131" t="s">
+      <c r="AJ16" s="145" t="s">
         <v>280</v>
       </c>
-      <c r="AK16" s="132"/>
-      <c r="AL16" s="129" t="s">
+      <c r="AK16" s="146"/>
+      <c r="AL16" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AM16" s="130"/>
-      <c r="AN16" s="126"/>
-      <c r="AO16" s="127"/>
-      <c r="AP16" s="127"/>
-      <c r="AQ16" s="127"/>
-      <c r="AR16" s="127"/>
-      <c r="AS16" s="127"/>
-      <c r="AT16" s="127"/>
-      <c r="AU16" s="127"/>
-      <c r="AV16" s="127"/>
-      <c r="AW16" s="127"/>
-      <c r="AX16" s="127"/>
-      <c r="AY16" s="127"/>
-      <c r="AZ16" s="127"/>
-      <c r="BA16" s="127"/>
-      <c r="BB16" s="127"/>
-      <c r="BC16" s="127"/>
-      <c r="BD16" s="127"/>
-      <c r="BE16" s="127"/>
-      <c r="BF16" s="127"/>
+      <c r="AM16" s="148"/>
+      <c r="AN16" s="206"/>
+      <c r="AO16" s="207"/>
+      <c r="AP16" s="207"/>
+      <c r="AQ16" s="207"/>
+      <c r="AR16" s="207"/>
+      <c r="AS16" s="207"/>
+      <c r="AT16" s="207"/>
+      <c r="AU16" s="207"/>
+      <c r="AV16" s="207"/>
+      <c r="AW16" s="207"/>
+      <c r="AX16" s="207"/>
+      <c r="AY16" s="207"/>
+      <c r="AZ16" s="207"/>
+      <c r="BA16" s="207"/>
+      <c r="BB16" s="207"/>
+      <c r="BC16" s="207"/>
+      <c r="BD16" s="207"/>
+      <c r="BE16" s="207"/>
+      <c r="BF16" s="207"/>
       <c r="BG16" s="103"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -7997,31 +7997,31 @@
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
       <c r="K17" s="110"/>
-      <c r="L17" s="131" t="s">
+      <c r="L17" s="145" t="s">
         <v>281</v>
       </c>
-      <c r="M17" s="132"/>
-      <c r="N17" s="129" t="s">
+      <c r="M17" s="146"/>
+      <c r="N17" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="O17" s="130"/>
-      <c r="P17" s="126"/>
-      <c r="Q17" s="127"/>
-      <c r="R17" s="127"/>
-      <c r="S17" s="127"/>
-      <c r="T17" s="127"/>
-      <c r="U17" s="127"/>
-      <c r="V17" s="127"/>
-      <c r="W17" s="127"/>
-      <c r="X17" s="127"/>
-      <c r="Y17" s="127"/>
-      <c r="Z17" s="127"/>
-      <c r="AA17" s="127"/>
-      <c r="AB17" s="127"/>
-      <c r="AC17" s="127"/>
-      <c r="AD17" s="127"/>
-      <c r="AE17" s="127"/>
-      <c r="AF17" s="128"/>
+      <c r="O17" s="148"/>
+      <c r="P17" s="206"/>
+      <c r="Q17" s="207"/>
+      <c r="R17" s="207"/>
+      <c r="S17" s="207"/>
+      <c r="T17" s="207"/>
+      <c r="U17" s="207"/>
+      <c r="V17" s="207"/>
+      <c r="W17" s="207"/>
+      <c r="X17" s="207"/>
+      <c r="Y17" s="207"/>
+      <c r="Z17" s="207"/>
+      <c r="AA17" s="207"/>
+      <c r="AB17" s="207"/>
+      <c r="AC17" s="207"/>
+      <c r="AD17" s="207"/>
+      <c r="AE17" s="207"/>
+      <c r="AF17" s="208"/>
       <c r="AG17" s="106" t="s">
         <v>274</v>
       </c>
@@ -8031,31 +8031,31 @@
       <c r="AI17" s="111"/>
       <c r="AJ17" s="111"/>
       <c r="AK17" s="110"/>
-      <c r="AL17" s="131" t="s">
+      <c r="AL17" s="145" t="s">
         <v>281</v>
       </c>
-      <c r="AM17" s="132"/>
-      <c r="AN17" s="129" t="s">
+      <c r="AM17" s="146"/>
+      <c r="AN17" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AO17" s="130"/>
-      <c r="AP17" s="126"/>
-      <c r="AQ17" s="127"/>
-      <c r="AR17" s="127"/>
-      <c r="AS17" s="127"/>
-      <c r="AT17" s="127"/>
-      <c r="AU17" s="127"/>
-      <c r="AV17" s="127"/>
-      <c r="AW17" s="127"/>
-      <c r="AX17" s="127"/>
-      <c r="AY17" s="127"/>
-      <c r="AZ17" s="127"/>
-      <c r="BA17" s="127"/>
-      <c r="BB17" s="127"/>
-      <c r="BC17" s="127"/>
-      <c r="BD17" s="127"/>
-      <c r="BE17" s="127"/>
-      <c r="BF17" s="127"/>
+      <c r="AO17" s="148"/>
+      <c r="AP17" s="206"/>
+      <c r="AQ17" s="207"/>
+      <c r="AR17" s="207"/>
+      <c r="AS17" s="207"/>
+      <c r="AT17" s="207"/>
+      <c r="AU17" s="207"/>
+      <c r="AV17" s="207"/>
+      <c r="AW17" s="207"/>
+      <c r="AX17" s="207"/>
+      <c r="AY17" s="207"/>
+      <c r="AZ17" s="207"/>
+      <c r="BA17" s="207"/>
+      <c r="BB17" s="207"/>
+      <c r="BC17" s="207"/>
+      <c r="BD17" s="207"/>
+      <c r="BE17" s="207"/>
+      <c r="BF17" s="207"/>
       <c r="BG17" s="103"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -8080,27 +8080,27 @@
       <c r="K18" s="111"/>
       <c r="L18" s="111"/>
       <c r="M18" s="110"/>
-      <c r="N18" s="133" t="s">
+      <c r="N18" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="O18" s="134"/>
-      <c r="P18" s="126"/>
-      <c r="Q18" s="127"/>
-      <c r="R18" s="127"/>
-      <c r="S18" s="127"/>
-      <c r="T18" s="127"/>
-      <c r="U18" s="127"/>
-      <c r="V18" s="127"/>
-      <c r="W18" s="127"/>
-      <c r="X18" s="127"/>
-      <c r="Y18" s="127"/>
-      <c r="Z18" s="127"/>
-      <c r="AA18" s="127"/>
-      <c r="AB18" s="127"/>
-      <c r="AC18" s="127"/>
-      <c r="AD18" s="127"/>
-      <c r="AE18" s="127"/>
-      <c r="AF18" s="128"/>
+      <c r="O18" s="152"/>
+      <c r="P18" s="206"/>
+      <c r="Q18" s="207"/>
+      <c r="R18" s="207"/>
+      <c r="S18" s="207"/>
+      <c r="T18" s="207"/>
+      <c r="U18" s="207"/>
+      <c r="V18" s="207"/>
+      <c r="W18" s="207"/>
+      <c r="X18" s="207"/>
+      <c r="Y18" s="207"/>
+      <c r="Z18" s="207"/>
+      <c r="AA18" s="207"/>
+      <c r="AB18" s="207"/>
+      <c r="AC18" s="207"/>
+      <c r="AD18" s="207"/>
+      <c r="AE18" s="207"/>
+      <c r="AF18" s="208"/>
       <c r="AG18" s="106" t="s">
         <v>274</v>
       </c>
@@ -8112,27 +8112,27 @@
       <c r="AK18" s="111"/>
       <c r="AL18" s="111"/>
       <c r="AM18" s="110"/>
-      <c r="AN18" s="133" t="s">
+      <c r="AN18" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="AO18" s="134"/>
-      <c r="AP18" s="126"/>
-      <c r="AQ18" s="127"/>
-      <c r="AR18" s="127"/>
-      <c r="AS18" s="127"/>
-      <c r="AT18" s="127"/>
-      <c r="AU18" s="127"/>
-      <c r="AV18" s="127"/>
-      <c r="AW18" s="127"/>
-      <c r="AX18" s="127"/>
-      <c r="AY18" s="127"/>
-      <c r="AZ18" s="127"/>
-      <c r="BA18" s="127"/>
-      <c r="BB18" s="127"/>
-      <c r="BC18" s="127"/>
-      <c r="BD18" s="127"/>
-      <c r="BE18" s="127"/>
-      <c r="BF18" s="127"/>
+      <c r="AO18" s="152"/>
+      <c r="AP18" s="206"/>
+      <c r="AQ18" s="207"/>
+      <c r="AR18" s="207"/>
+      <c r="AS18" s="207"/>
+      <c r="AT18" s="207"/>
+      <c r="AU18" s="207"/>
+      <c r="AV18" s="207"/>
+      <c r="AW18" s="207"/>
+      <c r="AX18" s="207"/>
+      <c r="AY18" s="207"/>
+      <c r="AZ18" s="207"/>
+      <c r="BA18" s="207"/>
+      <c r="BB18" s="207"/>
+      <c r="BC18" s="207"/>
+      <c r="BD18" s="207"/>
+      <c r="BE18" s="207"/>
+      <c r="BF18" s="207"/>
       <c r="BG18" s="103"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -8358,23 +8358,23 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
       <c r="S22" s="110"/>
-      <c r="T22" s="131" t="s">
+      <c r="T22" s="145" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="132"/>
-      <c r="V22" s="129" t="s">
+      <c r="U22" s="146"/>
+      <c r="V22" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="W22" s="130"/>
-      <c r="X22" s="126"/>
-      <c r="Y22" s="127"/>
-      <c r="Z22" s="127"/>
-      <c r="AA22" s="127"/>
-      <c r="AB22" s="127"/>
-      <c r="AC22" s="127"/>
-      <c r="AD22" s="127"/>
-      <c r="AE22" s="127"/>
-      <c r="AF22" s="128"/>
+      <c r="W22" s="148"/>
+      <c r="X22" s="206"/>
+      <c r="Y22" s="207"/>
+      <c r="Z22" s="207"/>
+      <c r="AA22" s="207"/>
+      <c r="AB22" s="207"/>
+      <c r="AC22" s="207"/>
+      <c r="AD22" s="207"/>
+      <c r="AE22" s="207"/>
+      <c r="AF22" s="208"/>
       <c r="AG22" s="106" t="s">
         <v>274</v>
       </c>
@@ -8392,23 +8392,23 @@
       <c r="AQ22" s="111"/>
       <c r="AR22" s="111"/>
       <c r="AS22" s="110"/>
-      <c r="AT22" s="131" t="s">
+      <c r="AT22" s="145" t="s">
         <v>283</v>
       </c>
-      <c r="AU22" s="132"/>
-      <c r="AV22" s="129" t="s">
+      <c r="AU22" s="146"/>
+      <c r="AV22" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AW22" s="130"/>
-      <c r="AX22" s="126"/>
-      <c r="AY22" s="127"/>
-      <c r="AZ22" s="127"/>
-      <c r="BA22" s="127"/>
-      <c r="BB22" s="127"/>
-      <c r="BC22" s="127"/>
-      <c r="BD22" s="127"/>
-      <c r="BE22" s="127"/>
-      <c r="BF22" s="127"/>
+      <c r="AW22" s="148"/>
+      <c r="AX22" s="206"/>
+      <c r="AY22" s="207"/>
+      <c r="AZ22" s="207"/>
+      <c r="BA22" s="207"/>
+      <c r="BB22" s="207"/>
+      <c r="BC22" s="207"/>
+      <c r="BD22" s="207"/>
+      <c r="BE22" s="207"/>
+      <c r="BF22" s="207"/>
       <c r="BG22" s="103"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -8441,21 +8441,21 @@
       <c r="S23" s="111"/>
       <c r="T23" s="111"/>
       <c r="U23" s="110"/>
-      <c r="V23" s="131" t="s">
+      <c r="V23" s="145" t="s">
         <v>284</v>
       </c>
-      <c r="W23" s="132"/>
-      <c r="X23" s="129" t="s">
+      <c r="W23" s="146"/>
+      <c r="X23" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="Y23" s="130"/>
-      <c r="Z23" s="126"/>
-      <c r="AA23" s="127"/>
-      <c r="AB23" s="127"/>
-      <c r="AC23" s="127"/>
-      <c r="AD23" s="127"/>
-      <c r="AE23" s="127"/>
-      <c r="AF23" s="128"/>
+      <c r="Y23" s="148"/>
+      <c r="Z23" s="206"/>
+      <c r="AA23" s="207"/>
+      <c r="AB23" s="207"/>
+      <c r="AC23" s="207"/>
+      <c r="AD23" s="207"/>
+      <c r="AE23" s="207"/>
+      <c r="AF23" s="208"/>
       <c r="AG23" s="106" t="s">
         <v>274</v>
       </c>
@@ -8475,21 +8475,21 @@
       <c r="AS23" s="111"/>
       <c r="AT23" s="111"/>
       <c r="AU23" s="110"/>
-      <c r="AV23" s="131" t="s">
+      <c r="AV23" s="145" t="s">
         <v>284</v>
       </c>
-      <c r="AW23" s="132"/>
-      <c r="AX23" s="129" t="s">
+      <c r="AW23" s="146"/>
+      <c r="AX23" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AY23" s="130"/>
-      <c r="AZ23" s="126"/>
-      <c r="BA23" s="127"/>
-      <c r="BB23" s="127"/>
-      <c r="BC23" s="127"/>
-      <c r="BD23" s="127"/>
-      <c r="BE23" s="127"/>
-      <c r="BF23" s="127"/>
+      <c r="AY23" s="148"/>
+      <c r="AZ23" s="206"/>
+      <c r="BA23" s="207"/>
+      <c r="BB23" s="207"/>
+      <c r="BC23" s="207"/>
+      <c r="BD23" s="207"/>
+      <c r="BE23" s="207"/>
+      <c r="BF23" s="207"/>
       <c r="BG23" s="103"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -8524,19 +8524,19 @@
       <c r="U24" s="111"/>
       <c r="V24" s="111"/>
       <c r="W24" s="110"/>
-      <c r="X24" s="131" t="s">
+      <c r="X24" s="145" t="s">
         <v>285</v>
       </c>
-      <c r="Y24" s="132"/>
-      <c r="Z24" s="129" t="s">
+      <c r="Y24" s="146"/>
+      <c r="Z24" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AA24" s="130"/>
-      <c r="AB24" s="126"/>
-      <c r="AC24" s="127"/>
-      <c r="AD24" s="127"/>
-      <c r="AE24" s="127"/>
-      <c r="AF24" s="128"/>
+      <c r="AA24" s="148"/>
+      <c r="AB24" s="206"/>
+      <c r="AC24" s="207"/>
+      <c r="AD24" s="207"/>
+      <c r="AE24" s="207"/>
+      <c r="AF24" s="208"/>
       <c r="AG24" s="106" t="s">
         <v>274</v>
       </c>
@@ -8558,19 +8558,19 @@
       <c r="AU24" s="111"/>
       <c r="AV24" s="111"/>
       <c r="AW24" s="110"/>
-      <c r="AX24" s="131" t="s">
+      <c r="AX24" s="145" t="s">
         <v>285</v>
       </c>
-      <c r="AY24" s="132"/>
-      <c r="AZ24" s="129" t="s">
+      <c r="AY24" s="146"/>
+      <c r="AZ24" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="BA24" s="130"/>
-      <c r="BB24" s="126"/>
-      <c r="BC24" s="127"/>
-      <c r="BD24" s="127"/>
-      <c r="BE24" s="127"/>
-      <c r="BF24" s="127"/>
+      <c r="BA24" s="148"/>
+      <c r="BB24" s="206"/>
+      <c r="BC24" s="207"/>
+      <c r="BD24" s="207"/>
+      <c r="BE24" s="207"/>
+      <c r="BF24" s="207"/>
       <c r="BG24" s="103"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -8607,17 +8607,17 @@
       <c r="W25" s="111"/>
       <c r="X25" s="111"/>
       <c r="Y25" s="110"/>
-      <c r="Z25" s="133" t="s">
+      <c r="Z25" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="AA25" s="134"/>
-      <c r="AB25" s="129" t="s">
+      <c r="AA25" s="152"/>
+      <c r="AB25" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AC25" s="130"/>
-      <c r="AD25" s="126"/>
-      <c r="AE25" s="127"/>
-      <c r="AF25" s="128"/>
+      <c r="AC25" s="148"/>
+      <c r="AD25" s="206"/>
+      <c r="AE25" s="207"/>
+      <c r="AF25" s="208"/>
       <c r="AG25" s="106" t="s">
         <v>274</v>
       </c>
@@ -8641,17 +8641,17 @@
       <c r="AW25" s="111"/>
       <c r="AX25" s="111"/>
       <c r="AY25" s="110"/>
-      <c r="AZ25" s="133" t="s">
+      <c r="AZ25" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="BA25" s="134"/>
-      <c r="BB25" s="129" t="s">
+      <c r="BA25" s="152"/>
+      <c r="BB25" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="BC25" s="130"/>
-      <c r="BD25" s="126"/>
-      <c r="BE25" s="127"/>
-      <c r="BF25" s="127"/>
+      <c r="BC25" s="148"/>
+      <c r="BD25" s="206"/>
+      <c r="BE25" s="207"/>
+      <c r="BF25" s="207"/>
       <c r="BG25" s="103"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -8909,29 +8909,29 @@
         <v>318</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="176" t="s">
+      <c r="E30" s="149" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="177"/>
+      <c r="F30" s="150"/>
       <c r="G30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="176" t="s">
+      <c r="H30" s="149" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="177"/>
-      <c r="J30" s="176" t="s">
+      <c r="I30" s="150"/>
+      <c r="J30" s="149" t="s">
         <v>280</v>
       </c>
-      <c r="K30" s="177"/>
-      <c r="L30" s="176" t="s">
+      <c r="K30" s="150"/>
+      <c r="L30" s="149" t="s">
         <v>281</v>
       </c>
-      <c r="M30" s="177"/>
-      <c r="N30" s="176" t="s">
+      <c r="M30" s="150"/>
+      <c r="N30" s="149" t="s">
         <v>282</v>
       </c>
-      <c r="O30" s="177"/>
+      <c r="O30" s="150"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>239</v>
@@ -8940,50 +8940,50 @@
         <v>239</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="176" t="s">
+      <c r="T30" s="149" t="s">
         <v>283</v>
       </c>
-      <c r="U30" s="177"/>
-      <c r="V30" s="176" t="s">
+      <c r="U30" s="150"/>
+      <c r="V30" s="149" t="s">
         <v>284</v>
       </c>
-      <c r="W30" s="177"/>
-      <c r="X30" s="176" t="s">
+      <c r="W30" s="150"/>
+      <c r="X30" s="149" t="s">
         <v>285</v>
       </c>
-      <c r="Y30" s="177"/>
-      <c r="Z30" s="176" t="s">
+      <c r="Y30" s="150"/>
+      <c r="Z30" s="149" t="s">
         <v>286</v>
       </c>
-      <c r="AA30" s="177"/>
-      <c r="AB30" s="150" t="s">
+      <c r="AA30" s="150"/>
+      <c r="AB30" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="AC30" s="151"/>
-      <c r="AD30" s="152"/>
-      <c r="AE30" s="176" t="s">
+      <c r="AC30" s="154"/>
+      <c r="AD30" s="155"/>
+      <c r="AE30" s="149" t="s">
         <v>273</v>
       </c>
-      <c r="AF30" s="177"/>
+      <c r="AF30" s="150"/>
       <c r="AG30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="AH30" s="176" t="s">
+      <c r="AH30" s="149" t="s">
         <v>279</v>
       </c>
-      <c r="AI30" s="177"/>
-      <c r="AJ30" s="176" t="s">
+      <c r="AI30" s="150"/>
+      <c r="AJ30" s="149" t="s">
         <v>280</v>
       </c>
-      <c r="AK30" s="177"/>
-      <c r="AL30" s="176" t="s">
+      <c r="AK30" s="150"/>
+      <c r="AL30" s="149" t="s">
         <v>281</v>
       </c>
-      <c r="AM30" s="177"/>
-      <c r="AN30" s="176" t="s">
+      <c r="AM30" s="150"/>
+      <c r="AN30" s="149" t="s">
         <v>282</v>
       </c>
-      <c r="AO30" s="177"/>
+      <c r="AO30" s="150"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>239</v>
@@ -8992,27 +8992,27 @@
         <v>239</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="176" t="s">
+      <c r="AT30" s="149" t="s">
         <v>283</v>
       </c>
-      <c r="AU30" s="177"/>
-      <c r="AV30" s="176" t="s">
+      <c r="AU30" s="150"/>
+      <c r="AV30" s="149" t="s">
         <v>284</v>
       </c>
-      <c r="AW30" s="177"/>
-      <c r="AX30" s="176" t="s">
+      <c r="AW30" s="150"/>
+      <c r="AX30" s="149" t="s">
         <v>285</v>
       </c>
-      <c r="AY30" s="177"/>
-      <c r="AZ30" s="176" t="s">
+      <c r="AY30" s="150"/>
+      <c r="AZ30" s="149" t="s">
         <v>286</v>
       </c>
-      <c r="BA30" s="177"/>
-      <c r="BB30" s="150" t="s">
+      <c r="BA30" s="150"/>
+      <c r="BB30" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="BC30" s="151"/>
-      <c r="BD30" s="152"/>
+      <c r="BC30" s="154"/>
+      <c r="BD30" s="155"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -9024,10 +9024,10 @@
         <v>317</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="153" t="s">
+      <c r="E31" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="F31" s="153"/>
+      <c r="F31" s="151"/>
       <c r="G31" s="22" t="s">
         <v>324</v>
       </c>
@@ -9054,10 +9054,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="153" t="s">
+      <c r="AE31" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="AF31" s="153"/>
+      <c r="AF31" s="151"/>
       <c r="AG31" s="22" t="s">
         <v>324</v>
       </c>
@@ -9167,75 +9167,75 @@
       <c r="G33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="H33" s="173" t="s">
+      <c r="H33" s="179" t="s">
         <v>319</v>
       </c>
-      <c r="I33" s="174"/>
-      <c r="J33" s="174"/>
-      <c r="K33" s="174"/>
-      <c r="L33" s="174"/>
-      <c r="M33" s="174"/>
-      <c r="N33" s="174"/>
-      <c r="O33" s="174"/>
-      <c r="P33" s="174"/>
-      <c r="Q33" s="174"/>
-      <c r="R33" s="174"/>
-      <c r="S33" s="175"/>
-      <c r="T33" s="176" t="s">
+      <c r="I33" s="180"/>
+      <c r="J33" s="180"/>
+      <c r="K33" s="180"/>
+      <c r="L33" s="180"/>
+      <c r="M33" s="180"/>
+      <c r="N33" s="180"/>
+      <c r="O33" s="180"/>
+      <c r="P33" s="180"/>
+      <c r="Q33" s="180"/>
+      <c r="R33" s="180"/>
+      <c r="S33" s="181"/>
+      <c r="T33" s="149" t="s">
         <v>275</v>
       </c>
-      <c r="U33" s="177"/>
-      <c r="V33" s="150" t="s">
+      <c r="U33" s="150"/>
+      <c r="V33" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="W33" s="152"/>
-      <c r="X33" s="173" t="s">
+      <c r="W33" s="155"/>
+      <c r="X33" s="179" t="s">
         <v>319</v>
       </c>
-      <c r="Y33" s="174"/>
-      <c r="Z33" s="174"/>
-      <c r="AA33" s="174"/>
-      <c r="AB33" s="174"/>
-      <c r="AC33" s="174"/>
-      <c r="AD33" s="174"/>
-      <c r="AE33" s="175"/>
+      <c r="Y33" s="180"/>
+      <c r="Z33" s="180"/>
+      <c r="AA33" s="180"/>
+      <c r="AB33" s="180"/>
+      <c r="AC33" s="180"/>
+      <c r="AD33" s="180"/>
+      <c r="AE33" s="181"/>
       <c r="AF33" s="24" t="s">
         <v>273</v>
       </c>
       <c r="AG33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="AH33" s="173" t="s">
+      <c r="AH33" s="179" t="s">
         <v>319</v>
       </c>
-      <c r="AI33" s="174"/>
-      <c r="AJ33" s="174"/>
-      <c r="AK33" s="174"/>
-      <c r="AL33" s="174"/>
-      <c r="AM33" s="174"/>
-      <c r="AN33" s="174"/>
-      <c r="AO33" s="174"/>
-      <c r="AP33" s="174"/>
-      <c r="AQ33" s="174"/>
-      <c r="AR33" s="174"/>
-      <c r="AS33" s="175"/>
-      <c r="AT33" s="176" t="s">
+      <c r="AI33" s="180"/>
+      <c r="AJ33" s="180"/>
+      <c r="AK33" s="180"/>
+      <c r="AL33" s="180"/>
+      <c r="AM33" s="180"/>
+      <c r="AN33" s="180"/>
+      <c r="AO33" s="180"/>
+      <c r="AP33" s="180"/>
+      <c r="AQ33" s="180"/>
+      <c r="AR33" s="180"/>
+      <c r="AS33" s="181"/>
+      <c r="AT33" s="149" t="s">
         <v>275</v>
       </c>
-      <c r="AU33" s="177"/>
-      <c r="AV33" s="150" t="s">
+      <c r="AU33" s="150"/>
+      <c r="AV33" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="AW33" s="152"/>
-      <c r="AX33" s="173" t="s">
+      <c r="AW33" s="155"/>
+      <c r="AX33" s="179" t="s">
         <v>319</v>
       </c>
-      <c r="AY33" s="174"/>
-      <c r="AZ33" s="174"/>
-      <c r="BA33" s="174"/>
-      <c r="BB33" s="174"/>
-      <c r="BC33" s="174"/>
-      <c r="BD33" s="175"/>
+      <c r="AY33" s="180"/>
+      <c r="AZ33" s="180"/>
+      <c r="BA33" s="180"/>
+      <c r="BB33" s="180"/>
+      <c r="BC33" s="180"/>
+      <c r="BD33" s="181"/>
       <c r="BE33" s="7"/>
       <c r="BF33" s="7"/>
       <c r="BG33" s="7"/>
@@ -9247,10 +9247,10 @@
         <v>317</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="153" t="s">
+      <c r="E34" s="151" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="153"/>
+      <c r="F34" s="151"/>
       <c r="G34" s="22" t="s">
         <v>321</v>
       </c>
@@ -9266,10 +9266,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="153" t="s">
+      <c r="T34" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="U34" s="153"/>
+      <c r="U34" s="151"/>
       <c r="V34" s="22" t="s">
         <v>325</v>
       </c>
@@ -9298,10 +9298,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="153" t="s">
+      <c r="AT34" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="AU34" s="153"/>
+      <c r="AU34" s="151"/>
       <c r="AV34" s="22" t="s">
         <v>320</v>
       </c>
@@ -9572,33 +9572,33 @@
         <v>326</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="168" t="s">
+      <c r="E39" s="182" t="s">
         <v>273</v>
       </c>
-      <c r="F39" s="169"/>
-      <c r="G39" s="171" t="s">
+      <c r="F39" s="183"/>
+      <c r="G39" s="184" t="s">
         <v>273</v>
       </c>
-      <c r="H39" s="172"/>
+      <c r="H39" s="185"/>
       <c r="I39" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="J39" s="133" t="s">
+      <c r="J39" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="K39" s="134"/>
-      <c r="L39" s="133" t="s">
+      <c r="K39" s="152"/>
+      <c r="L39" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="M39" s="134"/>
-      <c r="N39" s="133" t="s">
+      <c r="M39" s="152"/>
+      <c r="N39" s="143" t="s">
         <v>281</v>
       </c>
-      <c r="O39" s="134"/>
-      <c r="P39" s="133" t="s">
+      <c r="O39" s="152"/>
+      <c r="P39" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="Q39" s="134"/>
+      <c r="Q39" s="152"/>
       <c r="R39" s="103"/>
       <c r="S39" s="103" t="s">
         <v>239</v>
@@ -9607,50 +9607,50 @@
         <v>239</v>
       </c>
       <c r="U39" s="103"/>
-      <c r="V39" s="133" t="s">
+      <c r="V39" s="143" t="s">
         <v>283</v>
       </c>
-      <c r="W39" s="134"/>
-      <c r="X39" s="133" t="s">
+      <c r="W39" s="152"/>
+      <c r="X39" s="143" t="s">
         <v>284</v>
       </c>
-      <c r="Y39" s="134"/>
-      <c r="Z39" s="133" t="s">
+      <c r="Y39" s="152"/>
+      <c r="Z39" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="AA39" s="134"/>
-      <c r="AB39" s="133" t="s">
+      <c r="AA39" s="152"/>
+      <c r="AB39" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="AC39" s="134"/>
-      <c r="AD39" s="129" t="s">
+      <c r="AC39" s="152"/>
+      <c r="AD39" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AE39" s="170"/>
-      <c r="AF39" s="130"/>
-      <c r="AG39" s="133" t="s">
+      <c r="AE39" s="187"/>
+      <c r="AF39" s="148"/>
+      <c r="AG39" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AH39" s="134"/>
+      <c r="AH39" s="152"/>
       <c r="AI39" s="112" t="s">
         <v>319</v>
       </c>
-      <c r="AJ39" s="133" t="s">
+      <c r="AJ39" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="AK39" s="134"/>
-      <c r="AL39" s="133" t="s">
+      <c r="AK39" s="152"/>
+      <c r="AL39" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="AM39" s="134"/>
-      <c r="AN39" s="133" t="s">
+      <c r="AM39" s="152"/>
+      <c r="AN39" s="143" t="s">
         <v>281</v>
       </c>
-      <c r="AO39" s="134"/>
-      <c r="AP39" s="133" t="s">
+      <c r="AO39" s="152"/>
+      <c r="AP39" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="AQ39" s="134"/>
+      <c r="AQ39" s="152"/>
       <c r="AR39" s="103"/>
       <c r="AS39" s="103" t="s">
         <v>239</v>
@@ -9679,14 +9679,14 @@
         <v>351</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="146" t="s">
+      <c r="E40" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="146"/>
-      <c r="G40" s="146" t="s">
+      <c r="F40" s="186"/>
+      <c r="G40" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="H40" s="146"/>
+      <c r="H40" s="186"/>
       <c r="I40" s="113" t="s">
         <v>324</v>
       </c>
@@ -9713,10 +9713,10 @@
       <c r="AD40" s="103"/>
       <c r="AE40" s="103"/>
       <c r="AF40" s="103"/>
-      <c r="AG40" s="146" t="s">
+      <c r="AG40" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="AH40" s="146"/>
+      <c r="AH40" s="186"/>
       <c r="AI40" s="113" t="s">
         <v>328</v>
       </c>
@@ -9752,27 +9752,27 @@
         <v>327</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="133" t="s">
+      <c r="E41" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="134"/>
+      <c r="F41" s="152"/>
       <c r="G41" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="H41" s="133" t="s">
+      <c r="H41" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="I41" s="134"/>
-      <c r="J41" s="133" t="s">
+      <c r="I41" s="152"/>
+      <c r="J41" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="K41" s="134"/>
-      <c r="L41" s="168"/>
-      <c r="M41" s="169"/>
-      <c r="N41" s="171" t="s">
+      <c r="K41" s="152"/>
+      <c r="L41" s="182"/>
+      <c r="M41" s="183"/>
+      <c r="N41" s="184" t="s">
         <v>282</v>
       </c>
-      <c r="O41" s="172"/>
+      <c r="O41" s="185"/>
       <c r="P41" s="103"/>
       <c r="Q41" s="103" t="s">
         <v>239</v>
@@ -9781,50 +9781,50 @@
         <v>239</v>
       </c>
       <c r="S41" s="103"/>
-      <c r="T41" s="133" t="s">
+      <c r="T41" s="143" t="s">
         <v>283</v>
       </c>
-      <c r="U41" s="134"/>
-      <c r="V41" s="133" t="s">
+      <c r="U41" s="152"/>
+      <c r="V41" s="143" t="s">
         <v>284</v>
       </c>
-      <c r="W41" s="134"/>
-      <c r="X41" s="133" t="s">
+      <c r="W41" s="152"/>
+      <c r="X41" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="Y41" s="134"/>
-      <c r="Z41" s="133" t="s">
+      <c r="Y41" s="152"/>
+      <c r="Z41" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="AA41" s="134"/>
-      <c r="AB41" s="129" t="s">
+      <c r="AA41" s="152"/>
+      <c r="AB41" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AC41" s="170"/>
-      <c r="AD41" s="130"/>
-      <c r="AE41" s="133" t="s">
+      <c r="AC41" s="187"/>
+      <c r="AD41" s="148"/>
+      <c r="AE41" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AF41" s="134"/>
+      <c r="AF41" s="152"/>
       <c r="AG41" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="AH41" s="133" t="s">
+      <c r="AH41" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="AI41" s="134"/>
-      <c r="AJ41" s="133" t="s">
+      <c r="AI41" s="152"/>
+      <c r="AJ41" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="AK41" s="134"/>
-      <c r="AL41" s="133" t="s">
+      <c r="AK41" s="152"/>
+      <c r="AL41" s="143" t="s">
         <v>281</v>
       </c>
-      <c r="AM41" s="134"/>
-      <c r="AN41" s="133" t="s">
+      <c r="AM41" s="152"/>
+      <c r="AN41" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="AO41" s="134"/>
+      <c r="AO41" s="152"/>
       <c r="AP41" s="103"/>
       <c r="AQ41" s="103" t="s">
         <v>239</v>
@@ -9833,27 +9833,27 @@
         <v>239</v>
       </c>
       <c r="AS41" s="103"/>
-      <c r="AT41" s="133" t="s">
+      <c r="AT41" s="143" t="s">
         <v>283</v>
       </c>
-      <c r="AU41" s="134"/>
-      <c r="AV41" s="133" t="s">
+      <c r="AU41" s="152"/>
+      <c r="AV41" s="143" t="s">
         <v>284</v>
       </c>
-      <c r="AW41" s="134"/>
-      <c r="AX41" s="133" t="s">
+      <c r="AW41" s="152"/>
+      <c r="AX41" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="AY41" s="134"/>
-      <c r="AZ41" s="133" t="s">
+      <c r="AY41" s="152"/>
+      <c r="AZ41" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="BA41" s="134"/>
-      <c r="BB41" s="129" t="s">
+      <c r="BA41" s="152"/>
+      <c r="BB41" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="BC41" s="170"/>
-      <c r="BD41" s="130"/>
+      <c r="BC41" s="187"/>
+      <c r="BD41" s="148"/>
       <c r="BE41" s="103"/>
       <c r="BF41" s="103"/>
       <c r="BG41" s="103"/>
@@ -9865,10 +9865,10 @@
         <v>352</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="146" t="s">
+      <c r="E42" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="146"/>
+      <c r="F42" s="186"/>
       <c r="G42" s="113" t="s">
         <v>324</v>
       </c>
@@ -9895,10 +9895,10 @@
       <c r="AB42" s="103"/>
       <c r="AC42" s="103"/>
       <c r="AD42" s="103"/>
-      <c r="AE42" s="146" t="s">
+      <c r="AE42" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="AF42" s="146"/>
+      <c r="AF42" s="186"/>
       <c r="AG42" s="113" t="s">
         <v>324</v>
       </c>
@@ -10008,75 +10008,75 @@
       <c r="G44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="165" t="s">
+      <c r="H44" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="I44" s="166"/>
-      <c r="J44" s="166"/>
-      <c r="K44" s="166"/>
-      <c r="L44" s="166"/>
-      <c r="M44" s="166"/>
-      <c r="N44" s="166"/>
-      <c r="O44" s="166"/>
-      <c r="P44" s="166"/>
-      <c r="Q44" s="166"/>
-      <c r="R44" s="166"/>
-      <c r="S44" s="167"/>
-      <c r="T44" s="168" t="s">
+      <c r="I44" s="194"/>
+      <c r="J44" s="194"/>
+      <c r="K44" s="194"/>
+      <c r="L44" s="194"/>
+      <c r="M44" s="194"/>
+      <c r="N44" s="194"/>
+      <c r="O44" s="194"/>
+      <c r="P44" s="194"/>
+      <c r="Q44" s="194"/>
+      <c r="R44" s="194"/>
+      <c r="S44" s="195"/>
+      <c r="T44" s="182" t="s">
         <v>275</v>
       </c>
-      <c r="U44" s="169"/>
-      <c r="V44" s="129" t="s">
+      <c r="U44" s="183"/>
+      <c r="V44" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="W44" s="130"/>
-      <c r="X44" s="165" t="s">
+      <c r="W44" s="148"/>
+      <c r="X44" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="Y44" s="166"/>
-      <c r="Z44" s="166"/>
-      <c r="AA44" s="166"/>
-      <c r="AB44" s="166"/>
-      <c r="AC44" s="166"/>
-      <c r="AD44" s="166"/>
-      <c r="AE44" s="167"/>
+      <c r="Y44" s="194"/>
+      <c r="Z44" s="194"/>
+      <c r="AA44" s="194"/>
+      <c r="AB44" s="194"/>
+      <c r="AC44" s="194"/>
+      <c r="AD44" s="194"/>
+      <c r="AE44" s="195"/>
       <c r="AF44" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH44" s="165" t="s">
+      <c r="AH44" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="AI44" s="166"/>
-      <c r="AJ44" s="166"/>
-      <c r="AK44" s="166"/>
-      <c r="AL44" s="166"/>
-      <c r="AM44" s="166"/>
-      <c r="AN44" s="166"/>
-      <c r="AO44" s="166"/>
-      <c r="AP44" s="166"/>
-      <c r="AQ44" s="166"/>
-      <c r="AR44" s="166"/>
-      <c r="AS44" s="167"/>
-      <c r="AT44" s="133" t="s">
+      <c r="AI44" s="194"/>
+      <c r="AJ44" s="194"/>
+      <c r="AK44" s="194"/>
+      <c r="AL44" s="194"/>
+      <c r="AM44" s="194"/>
+      <c r="AN44" s="194"/>
+      <c r="AO44" s="194"/>
+      <c r="AP44" s="194"/>
+      <c r="AQ44" s="194"/>
+      <c r="AR44" s="194"/>
+      <c r="AS44" s="195"/>
+      <c r="AT44" s="143" t="s">
         <v>275</v>
       </c>
-      <c r="AU44" s="134"/>
-      <c r="AV44" s="129" t="s">
+      <c r="AU44" s="152"/>
+      <c r="AV44" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AW44" s="130"/>
-      <c r="AX44" s="165" t="s">
+      <c r="AW44" s="148"/>
+      <c r="AX44" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="AY44" s="166"/>
-      <c r="AZ44" s="166"/>
-      <c r="BA44" s="166"/>
-      <c r="BB44" s="166"/>
-      <c r="BC44" s="166"/>
-      <c r="BD44" s="167"/>
+      <c r="AY44" s="194"/>
+      <c r="AZ44" s="194"/>
+      <c r="BA44" s="194"/>
+      <c r="BB44" s="194"/>
+      <c r="BC44" s="194"/>
+      <c r="BD44" s="195"/>
       <c r="BE44" s="103"/>
       <c r="BF44" s="103"/>
       <c r="BG44" s="103"/>
@@ -10088,10 +10088,10 @@
         <v>352</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="146" t="s">
+      <c r="E45" s="186" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="146"/>
+      <c r="F45" s="186"/>
       <c r="G45" s="113" t="s">
         <v>321</v>
       </c>
@@ -10107,10 +10107,10 @@
       <c r="Q45" s="116"/>
       <c r="R45" s="116"/>
       <c r="S45" s="103"/>
-      <c r="T45" s="146" t="s">
+      <c r="T45" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="U45" s="146"/>
+      <c r="U45" s="186"/>
       <c r="V45" s="113" t="s">
         <v>325</v>
       </c>
@@ -10139,10 +10139,10 @@
       <c r="AQ45" s="116"/>
       <c r="AR45" s="116"/>
       <c r="AS45" s="103"/>
-      <c r="AT45" s="146" t="s">
+      <c r="AT45" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="AU45" s="146"/>
+      <c r="AU45" s="186"/>
       <c r="AV45" s="113" t="s">
         <v>320</v>
       </c>
@@ -10171,70 +10171,70 @@
       <c r="F46" s="117" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="165" t="s">
+      <c r="G46" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="H46" s="166"/>
-      <c r="I46" s="166"/>
-      <c r="J46" s="166"/>
-      <c r="K46" s="166"/>
-      <c r="L46" s="166"/>
-      <c r="M46" s="166"/>
-      <c r="N46" s="166"/>
-      <c r="O46" s="166"/>
-      <c r="P46" s="166"/>
-      <c r="Q46" s="166"/>
-      <c r="R46" s="166"/>
-      <c r="S46" s="166"/>
-      <c r="T46" s="166"/>
-      <c r="U46" s="166"/>
-      <c r="V46" s="166"/>
-      <c r="W46" s="166"/>
-      <c r="X46" s="166"/>
-      <c r="Y46" s="166"/>
-      <c r="Z46" s="166"/>
-      <c r="AA46" s="166"/>
-      <c r="AB46" s="166"/>
-      <c r="AC46" s="166"/>
-      <c r="AD46" s="166"/>
-      <c r="AE46" s="167"/>
+      <c r="H46" s="194"/>
+      <c r="I46" s="194"/>
+      <c r="J46" s="194"/>
+      <c r="K46" s="194"/>
+      <c r="L46" s="194"/>
+      <c r="M46" s="194"/>
+      <c r="N46" s="194"/>
+      <c r="O46" s="194"/>
+      <c r="P46" s="194"/>
+      <c r="Q46" s="194"/>
+      <c r="R46" s="194"/>
+      <c r="S46" s="194"/>
+      <c r="T46" s="194"/>
+      <c r="U46" s="194"/>
+      <c r="V46" s="194"/>
+      <c r="W46" s="194"/>
+      <c r="X46" s="194"/>
+      <c r="Y46" s="194"/>
+      <c r="Z46" s="194"/>
+      <c r="AA46" s="194"/>
+      <c r="AB46" s="194"/>
+      <c r="AC46" s="194"/>
+      <c r="AD46" s="194"/>
+      <c r="AE46" s="195"/>
       <c r="AF46" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG46" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH46" s="165" t="s">
+      <c r="AH46" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="AI46" s="166"/>
-      <c r="AJ46" s="166"/>
-      <c r="AK46" s="166"/>
-      <c r="AL46" s="166"/>
-      <c r="AM46" s="166"/>
-      <c r="AN46" s="166"/>
-      <c r="AO46" s="166"/>
-      <c r="AP46" s="166"/>
-      <c r="AQ46" s="166"/>
-      <c r="AR46" s="166"/>
-      <c r="AS46" s="167"/>
-      <c r="AT46" s="133" t="s">
+      <c r="AI46" s="194"/>
+      <c r="AJ46" s="194"/>
+      <c r="AK46" s="194"/>
+      <c r="AL46" s="194"/>
+      <c r="AM46" s="194"/>
+      <c r="AN46" s="194"/>
+      <c r="AO46" s="194"/>
+      <c r="AP46" s="194"/>
+      <c r="AQ46" s="194"/>
+      <c r="AR46" s="194"/>
+      <c r="AS46" s="195"/>
+      <c r="AT46" s="143" t="s">
         <v>275</v>
       </c>
-      <c r="AU46" s="134"/>
-      <c r="AV46" s="129" t="s">
+      <c r="AU46" s="152"/>
+      <c r="AV46" s="147" t="s">
         <v>297</v>
       </c>
-      <c r="AW46" s="130"/>
-      <c r="AX46" s="165" t="s">
+      <c r="AW46" s="148"/>
+      <c r="AX46" s="193" t="s">
         <v>319</v>
       </c>
-      <c r="AY46" s="166"/>
-      <c r="AZ46" s="166"/>
-      <c r="BA46" s="166"/>
-      <c r="BB46" s="166"/>
-      <c r="BC46" s="166"/>
-      <c r="BD46" s="167"/>
+      <c r="AY46" s="194"/>
+      <c r="AZ46" s="194"/>
+      <c r="BA46" s="194"/>
+      <c r="BB46" s="194"/>
+      <c r="BC46" s="194"/>
+      <c r="BD46" s="195"/>
       <c r="BE46" s="103"/>
       <c r="BF46" s="103"/>
       <c r="BG46" s="103"/>
@@ -10291,10 +10291,10 @@
       <c r="AQ47" s="116"/>
       <c r="AR47" s="116"/>
       <c r="AS47" s="103"/>
-      <c r="AT47" s="146" t="s">
+      <c r="AT47" s="186" t="s">
         <v>323</v>
       </c>
-      <c r="AU47" s="146"/>
+      <c r="AU47" s="186"/>
       <c r="AV47" s="113" t="s">
         <v>320</v>
       </c>
@@ -10685,20 +10685,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="136" t="s">
+      <c r="E54" s="140" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="137"/>
-      <c r="G54" s="137"/>
-      <c r="H54" s="137"/>
-      <c r="I54" s="137"/>
-      <c r="J54" s="137"/>
-      <c r="K54" s="157"/>
-      <c r="L54" s="136" t="s">
+      <c r="F54" s="141"/>
+      <c r="G54" s="141"/>
+      <c r="H54" s="141"/>
+      <c r="I54" s="141"/>
+      <c r="J54" s="141"/>
+      <c r="K54" s="142"/>
+      <c r="L54" s="140" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="137"/>
-      <c r="N54" s="138"/>
+      <c r="M54" s="141"/>
+      <c r="N54" s="209"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -10819,20 +10819,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="139" t="s">
+      <c r="E56" s="200" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="140"/>
-      <c r="G56" s="140"/>
-      <c r="H56" s="140"/>
-      <c r="I56" s="140"/>
-      <c r="J56" s="140"/>
-      <c r="K56" s="141"/>
-      <c r="L56" s="139" t="s">
+      <c r="F56" s="202"/>
+      <c r="G56" s="202"/>
+      <c r="H56" s="202"/>
+      <c r="I56" s="202"/>
+      <c r="J56" s="202"/>
+      <c r="K56" s="201"/>
+      <c r="L56" s="200" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="140"/>
-      <c r="N56" s="141"/>
+      <c r="M56" s="202"/>
+      <c r="N56" s="201"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -13304,68 +13304,68 @@
         <v>364</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="136" t="s">
+      <c r="E95" s="140" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="137"/>
-      <c r="G95" s="137"/>
-      <c r="H95" s="137"/>
-      <c r="I95" s="137"/>
-      <c r="J95" s="137"/>
-      <c r="K95" s="157"/>
-      <c r="L95" s="136" t="s">
+      <c r="F95" s="141"/>
+      <c r="G95" s="141"/>
+      <c r="H95" s="141"/>
+      <c r="I95" s="141"/>
+      <c r="J95" s="141"/>
+      <c r="K95" s="142"/>
+      <c r="L95" s="140" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="137"/>
-      <c r="N95" s="157"/>
-      <c r="O95" s="147" t="s">
+      <c r="M95" s="141"/>
+      <c r="N95" s="142"/>
+      <c r="O95" s="176" t="s">
         <v>260</v>
       </c>
-      <c r="P95" s="148"/>
-      <c r="Q95" s="148"/>
-      <c r="R95" s="148"/>
-      <c r="S95" s="148"/>
-      <c r="T95" s="149"/>
-      <c r="U95" s="147" t="s">
+      <c r="P95" s="177"/>
+      <c r="Q95" s="177"/>
+      <c r="R95" s="177"/>
+      <c r="S95" s="177"/>
+      <c r="T95" s="178"/>
+      <c r="U95" s="176" t="s">
         <v>260</v>
       </c>
-      <c r="V95" s="148"/>
-      <c r="W95" s="148"/>
-      <c r="X95" s="148"/>
-      <c r="Y95" s="148"/>
-      <c r="Z95" s="148"/>
-      <c r="AA95" s="148"/>
-      <c r="AB95" s="149"/>
-      <c r="AC95" s="147" t="s">
+      <c r="V95" s="177"/>
+      <c r="W95" s="177"/>
+      <c r="X95" s="177"/>
+      <c r="Y95" s="177"/>
+      <c r="Z95" s="177"/>
+      <c r="AA95" s="177"/>
+      <c r="AB95" s="178"/>
+      <c r="AC95" s="176" t="s">
         <v>260</v>
       </c>
-      <c r="AD95" s="148"/>
-      <c r="AE95" s="148"/>
-      <c r="AF95" s="148"/>
-      <c r="AG95" s="148"/>
-      <c r="AH95" s="148"/>
-      <c r="AI95" s="148"/>
-      <c r="AJ95" s="149"/>
-      <c r="AK95" s="147" t="s">
+      <c r="AD95" s="177"/>
+      <c r="AE95" s="177"/>
+      <c r="AF95" s="177"/>
+      <c r="AG95" s="177"/>
+      <c r="AH95" s="177"/>
+      <c r="AI95" s="177"/>
+      <c r="AJ95" s="178"/>
+      <c r="AK95" s="176" t="s">
         <v>260</v>
       </c>
-      <c r="AL95" s="148"/>
-      <c r="AM95" s="148"/>
-      <c r="AN95" s="148"/>
-      <c r="AO95" s="148"/>
-      <c r="AP95" s="148"/>
-      <c r="AQ95" s="148"/>
-      <c r="AR95" s="149"/>
-      <c r="AS95" s="192" t="s">
+      <c r="AL95" s="177"/>
+      <c r="AM95" s="177"/>
+      <c r="AN95" s="177"/>
+      <c r="AO95" s="177"/>
+      <c r="AP95" s="177"/>
+      <c r="AQ95" s="177"/>
+      <c r="AR95" s="178"/>
+      <c r="AS95" s="173" t="s">
         <v>356</v>
       </c>
-      <c r="AT95" s="193"/>
-      <c r="AU95" s="193"/>
-      <c r="AV95" s="193"/>
-      <c r="AW95" s="193"/>
-      <c r="AX95" s="193"/>
-      <c r="AY95" s="193"/>
-      <c r="AZ95" s="194"/>
+      <c r="AT95" s="174"/>
+      <c r="AU95" s="174"/>
+      <c r="AV95" s="174"/>
+      <c r="AW95" s="174"/>
+      <c r="AX95" s="174"/>
+      <c r="AY95" s="174"/>
+      <c r="AZ95" s="175"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -13470,68 +13470,68 @@
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="139" t="s">
+      <c r="E97" s="200" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="140"/>
-      <c r="G97" s="140"/>
-      <c r="H97" s="140"/>
-      <c r="I97" s="140"/>
-      <c r="J97" s="140"/>
-      <c r="K97" s="141"/>
-      <c r="L97" s="139" t="s">
+      <c r="F97" s="202"/>
+      <c r="G97" s="202"/>
+      <c r="H97" s="202"/>
+      <c r="I97" s="202"/>
+      <c r="J97" s="202"/>
+      <c r="K97" s="201"/>
+      <c r="L97" s="200" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="140"/>
-      <c r="N97" s="140"/>
-      <c r="O97" s="139" t="s">
+      <c r="M97" s="202"/>
+      <c r="N97" s="202"/>
+      <c r="O97" s="200" t="s">
         <v>272</v>
       </c>
-      <c r="P97" s="140"/>
-      <c r="Q97" s="140"/>
-      <c r="R97" s="140"/>
-      <c r="S97" s="140"/>
-      <c r="T97" s="141"/>
-      <c r="U97" s="139" t="s">
+      <c r="P97" s="202"/>
+      <c r="Q97" s="202"/>
+      <c r="R97" s="202"/>
+      <c r="S97" s="202"/>
+      <c r="T97" s="201"/>
+      <c r="U97" s="200" t="s">
         <v>229</v>
       </c>
-      <c r="V97" s="140"/>
-      <c r="W97" s="140"/>
-      <c r="X97" s="140"/>
-      <c r="Y97" s="140"/>
-      <c r="Z97" s="140"/>
-      <c r="AA97" s="140"/>
-      <c r="AB97" s="141"/>
-      <c r="AC97" s="139" t="s">
+      <c r="V97" s="202"/>
+      <c r="W97" s="202"/>
+      <c r="X97" s="202"/>
+      <c r="Y97" s="202"/>
+      <c r="Z97" s="202"/>
+      <c r="AA97" s="202"/>
+      <c r="AB97" s="201"/>
+      <c r="AC97" s="200" t="s">
         <v>229</v>
       </c>
-      <c r="AD97" s="140"/>
-      <c r="AE97" s="140"/>
-      <c r="AF97" s="140"/>
-      <c r="AG97" s="140"/>
-      <c r="AH97" s="140"/>
-      <c r="AI97" s="140"/>
-      <c r="AJ97" s="141"/>
-      <c r="AK97" s="139" t="s">
+      <c r="AD97" s="202"/>
+      <c r="AE97" s="202"/>
+      <c r="AF97" s="202"/>
+      <c r="AG97" s="202"/>
+      <c r="AH97" s="202"/>
+      <c r="AI97" s="202"/>
+      <c r="AJ97" s="201"/>
+      <c r="AK97" s="200" t="s">
         <v>229</v>
       </c>
-      <c r="AL97" s="140"/>
-      <c r="AM97" s="140"/>
-      <c r="AN97" s="140"/>
-      <c r="AO97" s="140"/>
-      <c r="AP97" s="140"/>
-      <c r="AQ97" s="140"/>
-      <c r="AR97" s="141"/>
-      <c r="AS97" s="140" t="s">
+      <c r="AL97" s="202"/>
+      <c r="AM97" s="202"/>
+      <c r="AN97" s="202"/>
+      <c r="AO97" s="202"/>
+      <c r="AP97" s="202"/>
+      <c r="AQ97" s="202"/>
+      <c r="AR97" s="201"/>
+      <c r="AS97" s="202" t="s">
         <v>229</v>
       </c>
-      <c r="AT97" s="140"/>
-      <c r="AU97" s="140"/>
-      <c r="AV97" s="140"/>
-      <c r="AW97" s="140"/>
-      <c r="AX97" s="140"/>
-      <c r="AY97" s="140"/>
-      <c r="AZ97" s="141"/>
+      <c r="AT97" s="202"/>
+      <c r="AU97" s="202"/>
+      <c r="AV97" s="202"/>
+      <c r="AW97" s="202"/>
+      <c r="AX97" s="202"/>
+      <c r="AY97" s="202"/>
+      <c r="AZ97" s="201"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -13606,68 +13606,68 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="189" t="s">
+      <c r="E99" s="167" t="s">
         <v>402</v>
       </c>
-      <c r="F99" s="190"/>
-      <c r="G99" s="190"/>
-      <c r="H99" s="190"/>
-      <c r="I99" s="190"/>
-      <c r="J99" s="190"/>
-      <c r="K99" s="191"/>
-      <c r="L99" s="142" t="s">
+      <c r="F99" s="168"/>
+      <c r="G99" s="168"/>
+      <c r="H99" s="168"/>
+      <c r="I99" s="168"/>
+      <c r="J99" s="168"/>
+      <c r="K99" s="169"/>
+      <c r="L99" s="170" t="s">
         <v>246</v>
       </c>
-      <c r="M99" s="143"/>
-      <c r="N99" s="144"/>
-      <c r="O99" s="186" t="s">
+      <c r="M99" s="171"/>
+      <c r="N99" s="172"/>
+      <c r="O99" s="164" t="s">
         <v>235</v>
       </c>
-      <c r="P99" s="187"/>
-      <c r="Q99" s="187"/>
-      <c r="R99" s="187"/>
-      <c r="S99" s="187"/>
-      <c r="T99" s="188"/>
-      <c r="U99" s="186" t="s">
+      <c r="P99" s="165"/>
+      <c r="Q99" s="165"/>
+      <c r="R99" s="165"/>
+      <c r="S99" s="165"/>
+      <c r="T99" s="166"/>
+      <c r="U99" s="164" t="s">
         <v>235</v>
       </c>
-      <c r="V99" s="187"/>
-      <c r="W99" s="187"/>
-      <c r="X99" s="187"/>
-      <c r="Y99" s="187"/>
-      <c r="Z99" s="187"/>
-      <c r="AA99" s="187"/>
-      <c r="AB99" s="188"/>
-      <c r="AC99" s="186" t="s">
+      <c r="V99" s="165"/>
+      <c r="W99" s="165"/>
+      <c r="X99" s="165"/>
+      <c r="Y99" s="165"/>
+      <c r="Z99" s="165"/>
+      <c r="AA99" s="165"/>
+      <c r="AB99" s="166"/>
+      <c r="AC99" s="164" t="s">
         <v>235</v>
       </c>
-      <c r="AD99" s="187"/>
-      <c r="AE99" s="187"/>
-      <c r="AF99" s="187"/>
-      <c r="AG99" s="187"/>
-      <c r="AH99" s="187"/>
-      <c r="AI99" s="187"/>
-      <c r="AJ99" s="188"/>
-      <c r="AK99" s="186" t="s">
+      <c r="AD99" s="165"/>
+      <c r="AE99" s="165"/>
+      <c r="AF99" s="165"/>
+      <c r="AG99" s="165"/>
+      <c r="AH99" s="165"/>
+      <c r="AI99" s="165"/>
+      <c r="AJ99" s="166"/>
+      <c r="AK99" s="164" t="s">
         <v>235</v>
       </c>
-      <c r="AL99" s="187"/>
-      <c r="AM99" s="187"/>
-      <c r="AN99" s="187"/>
-      <c r="AO99" s="187"/>
-      <c r="AP99" s="187"/>
-      <c r="AQ99" s="187"/>
-      <c r="AR99" s="188"/>
-      <c r="AS99" s="186" t="s">
+      <c r="AL99" s="165"/>
+      <c r="AM99" s="165"/>
+      <c r="AN99" s="165"/>
+      <c r="AO99" s="165"/>
+      <c r="AP99" s="165"/>
+      <c r="AQ99" s="165"/>
+      <c r="AR99" s="166"/>
+      <c r="AS99" s="164" t="s">
         <v>301</v>
       </c>
-      <c r="AT99" s="187"/>
-      <c r="AU99" s="187"/>
-      <c r="AV99" s="187"/>
-      <c r="AW99" s="187"/>
-      <c r="AX99" s="187"/>
-      <c r="AY99" s="187"/>
-      <c r="AZ99" s="188"/>
+      <c r="AT99" s="165"/>
+      <c r="AU99" s="165"/>
+      <c r="AV99" s="165"/>
+      <c r="AW99" s="165"/>
+      <c r="AX99" s="165"/>
+      <c r="AY99" s="165"/>
+      <c r="AZ99" s="166"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -13809,68 +13809,68 @@
         <v>367</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="136" t="s">
+      <c r="E102" s="140" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="137"/>
-      <c r="G102" s="137"/>
-      <c r="H102" s="137"/>
-      <c r="I102" s="137"/>
-      <c r="J102" s="137"/>
-      <c r="K102" s="157"/>
-      <c r="L102" s="136" t="s">
+      <c r="F102" s="141"/>
+      <c r="G102" s="141"/>
+      <c r="H102" s="141"/>
+      <c r="I102" s="141"/>
+      <c r="J102" s="141"/>
+      <c r="K102" s="142"/>
+      <c r="L102" s="140" t="s">
         <v>223</v>
       </c>
-      <c r="M102" s="137"/>
-      <c r="N102" s="157"/>
-      <c r="O102" s="136" t="s">
+      <c r="M102" s="141"/>
+      <c r="N102" s="142"/>
+      <c r="O102" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="P102" s="137"/>
-      <c r="Q102" s="137"/>
-      <c r="R102" s="157"/>
-      <c r="S102" s="136" t="s">
+      <c r="P102" s="141"/>
+      <c r="Q102" s="141"/>
+      <c r="R102" s="142"/>
+      <c r="S102" s="140" t="s">
         <v>306</v>
       </c>
-      <c r="T102" s="137"/>
-      <c r="U102" s="137"/>
-      <c r="V102" s="137"/>
-      <c r="W102" s="137"/>
-      <c r="X102" s="137"/>
-      <c r="Y102" s="137"/>
-      <c r="Z102" s="137"/>
-      <c r="AA102" s="137"/>
-      <c r="AB102" s="137"/>
-      <c r="AC102" s="137"/>
-      <c r="AD102" s="157"/>
-      <c r="AE102" s="136" t="s">
+      <c r="T102" s="141"/>
+      <c r="U102" s="141"/>
+      <c r="V102" s="141"/>
+      <c r="W102" s="141"/>
+      <c r="X102" s="141"/>
+      <c r="Y102" s="141"/>
+      <c r="Z102" s="141"/>
+      <c r="AA102" s="141"/>
+      <c r="AB102" s="141"/>
+      <c r="AC102" s="141"/>
+      <c r="AD102" s="142"/>
+      <c r="AE102" s="140" t="s">
         <v>307</v>
       </c>
-      <c r="AF102" s="137"/>
-      <c r="AG102" s="137"/>
-      <c r="AH102" s="137"/>
-      <c r="AI102" s="137"/>
-      <c r="AJ102" s="137"/>
-      <c r="AK102" s="137"/>
-      <c r="AL102" s="137"/>
-      <c r="AM102" s="137"/>
-      <c r="AN102" s="137"/>
-      <c r="AO102" s="137"/>
-      <c r="AP102" s="157"/>
-      <c r="AQ102" s="136" t="s">
+      <c r="AF102" s="141"/>
+      <c r="AG102" s="141"/>
+      <c r="AH102" s="141"/>
+      <c r="AI102" s="141"/>
+      <c r="AJ102" s="141"/>
+      <c r="AK102" s="141"/>
+      <c r="AL102" s="141"/>
+      <c r="AM102" s="141"/>
+      <c r="AN102" s="141"/>
+      <c r="AO102" s="141"/>
+      <c r="AP102" s="142"/>
+      <c r="AQ102" s="140" t="s">
         <v>224</v>
       </c>
-      <c r="AR102" s="157"/>
-      <c r="AS102" s="136" t="s">
+      <c r="AR102" s="142"/>
+      <c r="AS102" s="140" t="s">
         <v>234</v>
       </c>
-      <c r="AT102" s="137"/>
-      <c r="AU102" s="137"/>
-      <c r="AV102" s="137"/>
-      <c r="AW102" s="137"/>
-      <c r="AX102" s="137"/>
-      <c r="AY102" s="137"/>
-      <c r="AZ102" s="157"/>
+      <c r="AT102" s="141"/>
+      <c r="AU102" s="141"/>
+      <c r="AV102" s="141"/>
+      <c r="AW102" s="141"/>
+      <c r="AX102" s="141"/>
+      <c r="AY102" s="141"/>
+      <c r="AZ102" s="142"/>
       <c r="BA102" s="42"/>
       <c r="BB102" s="42"/>
       <c r="BC102" s="42"/>
@@ -13973,68 +13973,68 @@
       <c r="B104" s="42"/>
       <c r="C104" s="42"/>
       <c r="D104" s="42"/>
-      <c r="E104" s="139" t="s">
+      <c r="E104" s="200" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="140"/>
-      <c r="G104" s="140"/>
-      <c r="H104" s="140"/>
-      <c r="I104" s="140"/>
-      <c r="J104" s="140"/>
-      <c r="K104" s="141"/>
-      <c r="L104" s="139" t="s">
+      <c r="F104" s="202"/>
+      <c r="G104" s="202"/>
+      <c r="H104" s="202"/>
+      <c r="I104" s="202"/>
+      <c r="J104" s="202"/>
+      <c r="K104" s="201"/>
+      <c r="L104" s="200" t="s">
         <v>226</v>
       </c>
-      <c r="M104" s="140"/>
-      <c r="N104" s="141"/>
-      <c r="O104" s="139" t="s">
+      <c r="M104" s="202"/>
+      <c r="N104" s="201"/>
+      <c r="O104" s="200" t="s">
         <v>227</v>
       </c>
-      <c r="P104" s="140"/>
-      <c r="Q104" s="140"/>
-      <c r="R104" s="141"/>
-      <c r="S104" s="139" t="s">
+      <c r="P104" s="202"/>
+      <c r="Q104" s="202"/>
+      <c r="R104" s="201"/>
+      <c r="S104" s="200" t="s">
         <v>228</v>
       </c>
-      <c r="T104" s="140"/>
-      <c r="U104" s="140"/>
-      <c r="V104" s="140"/>
-      <c r="W104" s="140"/>
-      <c r="X104" s="140"/>
-      <c r="Y104" s="140"/>
-      <c r="Z104" s="140"/>
-      <c r="AA104" s="140"/>
-      <c r="AB104" s="140"/>
-      <c r="AC104" s="140"/>
-      <c r="AD104" s="141"/>
-      <c r="AE104" s="139" t="s">
+      <c r="T104" s="202"/>
+      <c r="U104" s="202"/>
+      <c r="V104" s="202"/>
+      <c r="W104" s="202"/>
+      <c r="X104" s="202"/>
+      <c r="Y104" s="202"/>
+      <c r="Z104" s="202"/>
+      <c r="AA104" s="202"/>
+      <c r="AB104" s="202"/>
+      <c r="AC104" s="202"/>
+      <c r="AD104" s="201"/>
+      <c r="AE104" s="200" t="s">
         <v>228</v>
       </c>
-      <c r="AF104" s="140"/>
-      <c r="AG104" s="140"/>
-      <c r="AH104" s="140"/>
-      <c r="AI104" s="140"/>
-      <c r="AJ104" s="140"/>
-      <c r="AK104" s="140"/>
-      <c r="AL104" s="140"/>
-      <c r="AM104" s="140"/>
-      <c r="AN104" s="140"/>
-      <c r="AO104" s="140"/>
-      <c r="AP104" s="141"/>
-      <c r="AQ104" s="139" t="s">
+      <c r="AF104" s="202"/>
+      <c r="AG104" s="202"/>
+      <c r="AH104" s="202"/>
+      <c r="AI104" s="202"/>
+      <c r="AJ104" s="202"/>
+      <c r="AK104" s="202"/>
+      <c r="AL104" s="202"/>
+      <c r="AM104" s="202"/>
+      <c r="AN104" s="202"/>
+      <c r="AO104" s="202"/>
+      <c r="AP104" s="201"/>
+      <c r="AQ104" s="200" t="s">
         <v>230</v>
       </c>
-      <c r="AR104" s="141"/>
-      <c r="AS104" s="139" t="s">
+      <c r="AR104" s="201"/>
+      <c r="AS104" s="200" t="s">
         <v>229</v>
       </c>
-      <c r="AT104" s="140"/>
-      <c r="AU104" s="140"/>
-      <c r="AV104" s="140"/>
-      <c r="AW104" s="140"/>
-      <c r="AX104" s="140"/>
-      <c r="AY104" s="140"/>
-      <c r="AZ104" s="141"/>
+      <c r="AT104" s="202"/>
+      <c r="AU104" s="202"/>
+      <c r="AV104" s="202"/>
+      <c r="AW104" s="202"/>
+      <c r="AX104" s="202"/>
+      <c r="AY104" s="202"/>
+      <c r="AZ104" s="201"/>
       <c r="BA104" s="42"/>
       <c r="BB104" s="42"/>
       <c r="BC104" s="42"/>
@@ -14120,11 +14120,11 @@
       <c r="I106" s="76"/>
       <c r="J106" s="76"/>
       <c r="K106" s="77"/>
-      <c r="L106" s="142" t="s">
+      <c r="L106" s="170" t="s">
         <v>246</v>
       </c>
-      <c r="M106" s="143"/>
-      <c r="N106" s="144"/>
+      <c r="M106" s="171"/>
+      <c r="N106" s="172"/>
       <c r="O106" s="53"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="50"/>
@@ -14163,16 +14163,16 @@
       <c r="AR106" s="51">
         <v>0</v>
       </c>
-      <c r="AS106" s="195" t="s">
+      <c r="AS106" s="136" t="s">
         <v>231</v>
       </c>
-      <c r="AT106" s="196"/>
-      <c r="AU106" s="196"/>
-      <c r="AV106" s="196"/>
-      <c r="AW106" s="196"/>
-      <c r="AX106" s="196"/>
-      <c r="AY106" s="196"/>
-      <c r="AZ106" s="197"/>
+      <c r="AT106" s="137"/>
+      <c r="AU106" s="137"/>
+      <c r="AV106" s="137"/>
+      <c r="AW106" s="137"/>
+      <c r="AX106" s="137"/>
+      <c r="AY106" s="137"/>
+      <c r="AZ106" s="138"/>
       <c r="BA106" s="50" t="s">
         <v>316</v>
       </c>
@@ -14238,16 +14238,16 @@
       <c r="AR107" s="51">
         <v>1</v>
       </c>
-      <c r="AS107" s="195" t="s">
+      <c r="AS107" s="136" t="s">
         <v>354</v>
       </c>
-      <c r="AT107" s="196"/>
-      <c r="AU107" s="196"/>
-      <c r="AV107" s="196"/>
-      <c r="AW107" s="196"/>
-      <c r="AX107" s="196"/>
-      <c r="AY107" s="196"/>
-      <c r="AZ107" s="197"/>
+      <c r="AT107" s="137"/>
+      <c r="AU107" s="137"/>
+      <c r="AV107" s="137"/>
+      <c r="AW107" s="137"/>
+      <c r="AX107" s="137"/>
+      <c r="AY107" s="137"/>
+      <c r="AZ107" s="138"/>
       <c r="BA107" s="50" t="s">
         <v>298</v>
       </c>
@@ -14315,16 +14315,16 @@
       <c r="AR108" s="51">
         <v>0</v>
       </c>
-      <c r="AS108" s="195" t="s">
+      <c r="AS108" s="136" t="s">
         <v>353</v>
       </c>
-      <c r="AT108" s="196"/>
-      <c r="AU108" s="196"/>
-      <c r="AV108" s="196"/>
-      <c r="AW108" s="196"/>
-      <c r="AX108" s="196"/>
-      <c r="AY108" s="196"/>
-      <c r="AZ108" s="197"/>
+      <c r="AT108" s="137"/>
+      <c r="AU108" s="137"/>
+      <c r="AV108" s="137"/>
+      <c r="AW108" s="137"/>
+      <c r="AX108" s="137"/>
+      <c r="AY108" s="137"/>
+      <c r="AZ108" s="138"/>
       <c r="BA108" s="50" t="s">
         <v>265</v>
       </c>
@@ -14388,16 +14388,16 @@
       <c r="AR109" s="51">
         <v>1</v>
       </c>
-      <c r="AS109" s="195" t="s">
+      <c r="AS109" s="136" t="s">
         <v>233</v>
       </c>
-      <c r="AT109" s="196"/>
-      <c r="AU109" s="196"/>
-      <c r="AV109" s="196"/>
-      <c r="AW109" s="196"/>
-      <c r="AX109" s="196"/>
-      <c r="AY109" s="196"/>
-      <c r="AZ109" s="197"/>
+      <c r="AT109" s="137"/>
+      <c r="AU109" s="137"/>
+      <c r="AV109" s="137"/>
+      <c r="AW109" s="137"/>
+      <c r="AX109" s="137"/>
+      <c r="AY109" s="137"/>
+      <c r="AZ109" s="138"/>
       <c r="BA109" s="50" t="s">
         <v>260</v>
       </c>
@@ -14553,12 +14553,12 @@
       <c r="L112" s="49"/>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
-      <c r="O112" s="183" t="s">
+      <c r="O112" s="161" t="s">
         <v>232</v>
       </c>
-      <c r="P112" s="184"/>
-      <c r="Q112" s="184"/>
-      <c r="R112" s="185"/>
+      <c r="P112" s="162"/>
+      <c r="Q112" s="162"/>
+      <c r="R112" s="163"/>
       <c r="S112" s="50"/>
       <c r="T112" s="50"/>
       <c r="U112" s="50"/>
@@ -14583,20 +14583,20 @@
       <c r="AN112" s="50"/>
       <c r="AO112" s="50"/>
       <c r="AP112" s="50"/>
-      <c r="AQ112" s="178" t="s">
+      <c r="AQ112" s="156" t="s">
         <v>302</v>
       </c>
-      <c r="AR112" s="179"/>
-      <c r="AS112" s="180" t="s">
+      <c r="AR112" s="157"/>
+      <c r="AS112" s="158" t="s">
         <v>299</v>
       </c>
-      <c r="AT112" s="181"/>
-      <c r="AU112" s="181"/>
-      <c r="AV112" s="181"/>
-      <c r="AW112" s="181"/>
-      <c r="AX112" s="181"/>
-      <c r="AY112" s="181"/>
-      <c r="AZ112" s="182"/>
+      <c r="AT112" s="159"/>
+      <c r="AU112" s="159"/>
+      <c r="AV112" s="159"/>
+      <c r="AW112" s="159"/>
+      <c r="AX112" s="159"/>
+      <c r="AY112" s="159"/>
+      <c r="AZ112" s="160"/>
       <c r="BA112" s="42"/>
       <c r="BB112" s="42"/>
       <c r="BC112" s="42"/>
@@ -15797,20 +15797,20 @@
       <c r="AN130" s="42"/>
       <c r="AO130" s="42"/>
       <c r="AP130" s="42"/>
-      <c r="AQ130" s="178" t="s">
+      <c r="AQ130" s="156" t="s">
         <v>304</v>
       </c>
-      <c r="AR130" s="179"/>
-      <c r="AS130" s="180" t="s">
+      <c r="AR130" s="157"/>
+      <c r="AS130" s="158" t="s">
         <v>355</v>
       </c>
-      <c r="AT130" s="181"/>
-      <c r="AU130" s="181"/>
-      <c r="AV130" s="181"/>
-      <c r="AW130" s="181"/>
-      <c r="AX130" s="181"/>
-      <c r="AY130" s="181"/>
-      <c r="AZ130" s="182"/>
+      <c r="AT130" s="159"/>
+      <c r="AU130" s="159"/>
+      <c r="AV130" s="159"/>
+      <c r="AW130" s="159"/>
+      <c r="AX130" s="159"/>
+      <c r="AY130" s="159"/>
+      <c r="AZ130" s="160"/>
       <c r="BA130" s="42"/>
       <c r="BB130" s="42"/>
       <c r="BC130" s="42"/>
@@ -15864,16 +15864,16 @@
       <c r="AP131" s="42"/>
       <c r="AQ131" s="42"/>
       <c r="AR131" s="42"/>
-      <c r="AS131" s="186" t="s">
+      <c r="AS131" s="164" t="s">
         <v>301</v>
       </c>
-      <c r="AT131" s="187"/>
-      <c r="AU131" s="187"/>
-      <c r="AV131" s="187"/>
-      <c r="AW131" s="187"/>
-      <c r="AX131" s="187"/>
-      <c r="AY131" s="187"/>
-      <c r="AZ131" s="188"/>
+      <c r="AT131" s="165"/>
+      <c r="AU131" s="165"/>
+      <c r="AV131" s="165"/>
+      <c r="AW131" s="165"/>
+      <c r="AX131" s="165"/>
+      <c r="AY131" s="165"/>
+      <c r="AZ131" s="166"/>
       <c r="BA131" s="42"/>
       <c r="BB131" s="42"/>
       <c r="BC131" s="42"/>
@@ -15986,20 +15986,20 @@
       <c r="AN133" s="42"/>
       <c r="AO133" s="42"/>
       <c r="AP133" s="42"/>
-      <c r="AQ133" s="178" t="s">
+      <c r="AQ133" s="156" t="s">
         <v>303</v>
       </c>
-      <c r="AR133" s="179"/>
-      <c r="AS133" s="180" t="s">
+      <c r="AR133" s="157"/>
+      <c r="AS133" s="158" t="s">
         <v>305</v>
       </c>
-      <c r="AT133" s="181"/>
-      <c r="AU133" s="181"/>
-      <c r="AV133" s="181"/>
-      <c r="AW133" s="181"/>
-      <c r="AX133" s="181"/>
-      <c r="AY133" s="181"/>
-      <c r="AZ133" s="182"/>
+      <c r="AT133" s="159"/>
+      <c r="AU133" s="159"/>
+      <c r="AV133" s="159"/>
+      <c r="AW133" s="159"/>
+      <c r="AX133" s="159"/>
+      <c r="AY133" s="159"/>
+      <c r="AZ133" s="160"/>
       <c r="BA133" s="42"/>
       <c r="BB133" s="42"/>
       <c r="BC133" s="42"/>
@@ -18622,6 +18622,193 @@
     </row>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="AZ23:BF23"/>
+    <mergeCell ref="BB24:BF24"/>
+    <mergeCell ref="BD25:BF25"/>
+    <mergeCell ref="AD25:AF25"/>
+    <mergeCell ref="L15:AF15"/>
+    <mergeCell ref="N16:AF16"/>
+    <mergeCell ref="P17:AF17"/>
+    <mergeCell ref="P18:AF18"/>
+    <mergeCell ref="AL15:BF15"/>
+    <mergeCell ref="AN16:BF16"/>
+    <mergeCell ref="AP17:BF17"/>
+    <mergeCell ref="AP18:BF18"/>
+    <mergeCell ref="AX22:BF22"/>
+    <mergeCell ref="AJ15:AK15"/>
+    <mergeCell ref="AV22:AW22"/>
+    <mergeCell ref="AH15:AI15"/>
+    <mergeCell ref="AJ16:AK16"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AT22:AU22"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AX23:AY23"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="U95:AB95"/>
+    <mergeCell ref="O95:T95"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="AQ104:AR104"/>
+    <mergeCell ref="AS104:AZ104"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="AS97:AZ97"/>
+    <mergeCell ref="AK97:AR97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="O104:R104"/>
+    <mergeCell ref="S104:AD104"/>
+    <mergeCell ref="AE104:AP104"/>
+    <mergeCell ref="AC97:AJ97"/>
+    <mergeCell ref="U97:AB97"/>
+    <mergeCell ref="O97:T97"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AQ112:AR112"/>
+    <mergeCell ref="AQ130:AR130"/>
+    <mergeCell ref="AQ133:AR133"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="AS112:AZ112"/>
+    <mergeCell ref="O112:R112"/>
+    <mergeCell ref="AS130:AZ130"/>
+    <mergeCell ref="AS131:AZ131"/>
+    <mergeCell ref="AS133:AZ133"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="U99:AB99"/>
+    <mergeCell ref="AC99:AJ99"/>
+    <mergeCell ref="AK99:AR99"/>
+    <mergeCell ref="AS99:AZ99"/>
+    <mergeCell ref="O99:T99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AS95:AZ95"/>
+    <mergeCell ref="AK95:AR95"/>
+    <mergeCell ref="AC95:AJ95"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
     <mergeCell ref="AS109:AZ109"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="S102:AD102"/>
@@ -18646,193 +18833,6 @@
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="Z30:AA30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="AQ112:AR112"/>
-    <mergeCell ref="AQ130:AR130"/>
-    <mergeCell ref="AQ133:AR133"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="AS112:AZ112"/>
-    <mergeCell ref="O112:R112"/>
-    <mergeCell ref="AS130:AZ130"/>
-    <mergeCell ref="AS131:AZ131"/>
-    <mergeCell ref="AS133:AZ133"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="U99:AB99"/>
-    <mergeCell ref="AC99:AJ99"/>
-    <mergeCell ref="AK99:AR99"/>
-    <mergeCell ref="AS99:AZ99"/>
-    <mergeCell ref="O99:T99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AS95:AZ95"/>
-    <mergeCell ref="AK95:AR95"/>
-    <mergeCell ref="AC95:AJ95"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AQ104:AR104"/>
-    <mergeCell ref="AS104:AZ104"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="AS97:AZ97"/>
-    <mergeCell ref="AK97:AR97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="L104:N104"/>
-    <mergeCell ref="O104:R104"/>
-    <mergeCell ref="S104:AD104"/>
-    <mergeCell ref="AE104:AP104"/>
-    <mergeCell ref="AC97:AJ97"/>
-    <mergeCell ref="U97:AB97"/>
-    <mergeCell ref="O97:T97"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="U95:AB95"/>
-    <mergeCell ref="O95:T95"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="AZ23:BF23"/>
-    <mergeCell ref="BB24:BF24"/>
-    <mergeCell ref="BD25:BF25"/>
-    <mergeCell ref="AD25:AF25"/>
-    <mergeCell ref="L15:AF15"/>
-    <mergeCell ref="N16:AF16"/>
-    <mergeCell ref="P17:AF17"/>
-    <mergeCell ref="P18:AF18"/>
-    <mergeCell ref="AL15:BF15"/>
-    <mergeCell ref="AN16:BF16"/>
-    <mergeCell ref="AP17:BF17"/>
-    <mergeCell ref="AP18:BF18"/>
-    <mergeCell ref="AX22:BF22"/>
-    <mergeCell ref="AJ15:AK15"/>
-    <mergeCell ref="AV22:AW22"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AT22:AU22"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AX23:AY23"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[Slot Doc] Correct chip type with QFN32 package
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1BB6B0-E119-4281-8180-EEE24AE2E3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E651AA9-28BC-4261-A42A-36B377B718A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin mapping EVAL" sheetId="3" r:id="rId1"/>
@@ -1423,13 +1423,13 @@
     <t>Pin Mapping MASTER/SLAVE EFR32xG22 (BRD4182A - QFN 40 pin)</t>
   </si>
   <si>
-    <t>Pin Mapping MASTER (EFR32MG22C224F512IM40 - QFN 32 pin)</t>
-  </si>
-  <si>
-    <t>Pin Mapping SLAVE (EFR32MG22C224F512IM40 - QFN 32 pin)</t>
-  </si>
-  <si>
     <t>Pin Mapping SLAVE EFR32xG22 (BRD4183A - QFN 32 pin)</t>
+  </si>
+  <si>
+    <t>Pin Mapping SLAVE (EFR32MG22C224F512IM32 - QFN 32 pin)</t>
+  </si>
+  <si>
+    <t>Pin Mapping MASTER (EFR32MG22C224F512IM32 - QFN 32 pin)</t>
   </si>
 </sst>
 </file>
@@ -2317,16 +2317,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2335,38 +2353,41 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2375,6 +2396,81 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2419,15 +2515,6 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2437,107 +2524,20 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3617,7 +3617,7 @@
   </sheetPr>
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -3647,7 +3647,7 @@
         <v>447</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="N1" s="5"/>
       <c r="AA1" s="17" t="s">
@@ -6080,8 +6080,8 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,7 +6103,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>449</v>
@@ -7030,21 +7030,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="139"/>
-      <c r="M3" s="139"/>
-      <c r="N3" s="139"/>
-      <c r="O3" s="139"/>
-      <c r="P3" s="139"/>
-      <c r="Q3" s="139"/>
-      <c r="R3" s="139"/>
-      <c r="S3" s="139"/>
+      <c r="E3" s="208"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="208"/>
+      <c r="L3" s="208"/>
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208"/>
+      <c r="P3" s="208"/>
+      <c r="Q3" s="208"/>
+      <c r="R3" s="208"/>
+      <c r="S3" s="208"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -7152,45 +7152,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="197" t="s">
+      <c r="E5" s="164" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="198"/>
-      <c r="G5" s="198"/>
-      <c r="H5" s="198"/>
-      <c r="I5" s="198"/>
-      <c r="J5" s="199"/>
-      <c r="K5" s="188" t="s">
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="168" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="205"/>
-      <c r="M5" s="205"/>
-      <c r="N5" s="205"/>
-      <c r="O5" s="189"/>
-      <c r="P5" s="188" t="s">
+      <c r="L5" s="171"/>
+      <c r="M5" s="171"/>
+      <c r="N5" s="171"/>
+      <c r="O5" s="169"/>
+      <c r="P5" s="168" t="s">
         <v>276</v>
       </c>
-      <c r="Q5" s="189"/>
-      <c r="R5" s="190" t="s">
+      <c r="Q5" s="169"/>
+      <c r="R5" s="172" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="191"/>
-      <c r="T5" s="191"/>
-      <c r="U5" s="191"/>
-      <c r="V5" s="191"/>
-      <c r="W5" s="192"/>
-      <c r="X5" s="188" t="s">
+      <c r="S5" s="173"/>
+      <c r="T5" s="173"/>
+      <c r="U5" s="173"/>
+      <c r="V5" s="173"/>
+      <c r="W5" s="174"/>
+      <c r="X5" s="168" t="s">
         <v>270</v>
       </c>
-      <c r="Y5" s="189"/>
-      <c r="Z5" s="197" t="s">
+      <c r="Y5" s="169"/>
+      <c r="Z5" s="164" t="s">
         <v>339</v>
       </c>
-      <c r="AA5" s="198"/>
-      <c r="AB5" s="198"/>
-      <c r="AC5" s="198"/>
-      <c r="AD5" s="198"/>
-      <c r="AE5" s="199"/>
+      <c r="AA5" s="165"/>
+      <c r="AB5" s="165"/>
+      <c r="AC5" s="165"/>
+      <c r="AD5" s="165"/>
+      <c r="AE5" s="166"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -7225,45 +7225,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="204" t="s">
+      <c r="E6" s="145" t="s">
         <v>395</v>
       </c>
-      <c r="F6" s="204"/>
-      <c r="G6" s="204"/>
-      <c r="H6" s="204"/>
-      <c r="I6" s="204"/>
-      <c r="J6" s="204"/>
-      <c r="K6" s="203" t="s">
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="155" t="s">
         <v>336</v>
       </c>
-      <c r="L6" s="203"/>
-      <c r="M6" s="203"/>
-      <c r="N6" s="203"/>
-      <c r="O6" s="203"/>
-      <c r="P6" s="203" t="s">
+      <c r="L6" s="155"/>
+      <c r="M6" s="155"/>
+      <c r="N6" s="155"/>
+      <c r="O6" s="155"/>
+      <c r="P6" s="155" t="s">
         <v>338</v>
       </c>
-      <c r="Q6" s="203"/>
-      <c r="R6" s="204" t="s">
+      <c r="Q6" s="155"/>
+      <c r="R6" s="145" t="s">
         <v>271</v>
       </c>
-      <c r="S6" s="204"/>
-      <c r="T6" s="204"/>
-      <c r="U6" s="204"/>
-      <c r="V6" s="204"/>
-      <c r="W6" s="204"/>
-      <c r="X6" s="204" t="s">
+      <c r="S6" s="145"/>
+      <c r="T6" s="145"/>
+      <c r="U6" s="145"/>
+      <c r="V6" s="145"/>
+      <c r="W6" s="145"/>
+      <c r="X6" s="145" t="s">
         <v>338</v>
       </c>
-      <c r="Y6" s="204"/>
-      <c r="Z6" s="204" t="s">
+      <c r="Y6" s="145"/>
+      <c r="Z6" s="145" t="s">
         <v>395</v>
       </c>
-      <c r="AA6" s="204"/>
-      <c r="AB6" s="204"/>
-      <c r="AC6" s="204"/>
-      <c r="AD6" s="204"/>
-      <c r="AE6" s="204"/>
+      <c r="AA6" s="145"/>
+      <c r="AB6" s="145"/>
+      <c r="AC6" s="145"/>
+      <c r="AD6" s="145"/>
+      <c r="AE6" s="145"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -7304,29 +7304,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="196" t="s">
+      <c r="K7" s="170" t="s">
         <v>337</v>
       </c>
-      <c r="L7" s="196"/>
-      <c r="M7" s="196"/>
-      <c r="N7" s="196"/>
-      <c r="O7" s="196"/>
-      <c r="P7" s="196" t="s">
+      <c r="L7" s="170"/>
+      <c r="M7" s="170"/>
+      <c r="N7" s="170"/>
+      <c r="O7" s="170"/>
+      <c r="P7" s="170" t="s">
         <v>337</v>
       </c>
-      <c r="Q7" s="196"/>
-      <c r="R7" s="196" t="s">
+      <c r="Q7" s="170"/>
+      <c r="R7" s="170" t="s">
         <v>278</v>
       </c>
-      <c r="S7" s="196"/>
-      <c r="T7" s="196"/>
-      <c r="U7" s="196"/>
-      <c r="V7" s="196"/>
-      <c r="W7" s="196"/>
-      <c r="X7" s="196" t="s">
+      <c r="S7" s="170"/>
+      <c r="T7" s="170"/>
+      <c r="U7" s="170"/>
+      <c r="V7" s="170"/>
+      <c r="W7" s="170"/>
+      <c r="X7" s="170" t="s">
         <v>337</v>
       </c>
-      <c r="Y7" s="196"/>
+      <c r="Y7" s="170"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -7762,7 +7762,7 @@
       <c r="E14" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="144"/>
+      <c r="F14" s="209"/>
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
@@ -7790,7 +7790,7 @@
       <c r="AE14" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="144"/>
+      <c r="AF14" s="209"/>
       <c r="AG14" s="104"/>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
@@ -7833,67 +7833,67 @@
       <c r="G15" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H15" s="145" t="s">
+      <c r="H15" s="141" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="146"/>
-      <c r="J15" s="147" t="s">
+      <c r="I15" s="142"/>
+      <c r="J15" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="148"/>
-      <c r="L15" s="206"/>
-      <c r="M15" s="207"/>
-      <c r="N15" s="207"/>
-      <c r="O15" s="207"/>
-      <c r="P15" s="207"/>
-      <c r="Q15" s="207"/>
-      <c r="R15" s="207"/>
-      <c r="S15" s="207"/>
-      <c r="T15" s="207"/>
-      <c r="U15" s="207"/>
-      <c r="V15" s="207"/>
-      <c r="W15" s="207"/>
-      <c r="X15" s="207"/>
-      <c r="Y15" s="207"/>
-      <c r="Z15" s="207"/>
-      <c r="AA15" s="207"/>
-      <c r="AB15" s="207"/>
-      <c r="AC15" s="207"/>
-      <c r="AD15" s="207"/>
-      <c r="AE15" s="207"/>
-      <c r="AF15" s="208"/>
+      <c r="K15" s="140"/>
+      <c r="L15" s="136"/>
+      <c r="M15" s="137"/>
+      <c r="N15" s="137"/>
+      <c r="O15" s="137"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="137"/>
+      <c r="R15" s="137"/>
+      <c r="S15" s="137"/>
+      <c r="T15" s="137"/>
+      <c r="U15" s="137"/>
+      <c r="V15" s="137"/>
+      <c r="W15" s="137"/>
+      <c r="X15" s="137"/>
+      <c r="Y15" s="137"/>
+      <c r="Z15" s="137"/>
+      <c r="AA15" s="137"/>
+      <c r="AB15" s="137"/>
+      <c r="AC15" s="137"/>
+      <c r="AD15" s="137"/>
+      <c r="AE15" s="137"/>
+      <c r="AF15" s="138"/>
       <c r="AG15" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="AH15" s="145" t="s">
+      <c r="AH15" s="141" t="s">
         <v>279</v>
       </c>
-      <c r="AI15" s="146"/>
-      <c r="AJ15" s="147" t="s">
+      <c r="AI15" s="142"/>
+      <c r="AJ15" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AK15" s="148"/>
-      <c r="AL15" s="206"/>
-      <c r="AM15" s="207"/>
-      <c r="AN15" s="207"/>
-      <c r="AO15" s="207"/>
-      <c r="AP15" s="207"/>
-      <c r="AQ15" s="207"/>
-      <c r="AR15" s="207"/>
-      <c r="AS15" s="207"/>
-      <c r="AT15" s="207"/>
-      <c r="AU15" s="207"/>
-      <c r="AV15" s="207"/>
-      <c r="AW15" s="207"/>
-      <c r="AX15" s="207"/>
-      <c r="AY15" s="207"/>
-      <c r="AZ15" s="207"/>
-      <c r="BA15" s="207"/>
-      <c r="BB15" s="207"/>
-      <c r="BC15" s="207"/>
-      <c r="BD15" s="207"/>
-      <c r="BE15" s="207"/>
-      <c r="BF15" s="207"/>
+      <c r="AK15" s="140"/>
+      <c r="AL15" s="136"/>
+      <c r="AM15" s="137"/>
+      <c r="AN15" s="137"/>
+      <c r="AO15" s="137"/>
+      <c r="AP15" s="137"/>
+      <c r="AQ15" s="137"/>
+      <c r="AR15" s="137"/>
+      <c r="AS15" s="137"/>
+      <c r="AT15" s="137"/>
+      <c r="AU15" s="137"/>
+      <c r="AV15" s="137"/>
+      <c r="AW15" s="137"/>
+      <c r="AX15" s="137"/>
+      <c r="AY15" s="137"/>
+      <c r="AZ15" s="137"/>
+      <c r="BA15" s="137"/>
+      <c r="BB15" s="137"/>
+      <c r="BC15" s="137"/>
+      <c r="BD15" s="137"/>
+      <c r="BE15" s="137"/>
+      <c r="BF15" s="137"/>
       <c r="BG15" s="103"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -7914,33 +7914,33 @@
         <v>287</v>
       </c>
       <c r="I16" s="110"/>
-      <c r="J16" s="145" t="s">
+      <c r="J16" s="141" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="146"/>
-      <c r="L16" s="147" t="s">
+      <c r="K16" s="142"/>
+      <c r="L16" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="M16" s="148"/>
-      <c r="N16" s="206"/>
-      <c r="O16" s="207"/>
-      <c r="P16" s="207"/>
-      <c r="Q16" s="207"/>
-      <c r="R16" s="207"/>
-      <c r="S16" s="207"/>
-      <c r="T16" s="207"/>
-      <c r="U16" s="207"/>
-      <c r="V16" s="207"/>
-      <c r="W16" s="207"/>
-      <c r="X16" s="207"/>
-      <c r="Y16" s="207"/>
-      <c r="Z16" s="207"/>
-      <c r="AA16" s="207"/>
-      <c r="AB16" s="207"/>
-      <c r="AC16" s="207"/>
-      <c r="AD16" s="207"/>
-      <c r="AE16" s="207"/>
-      <c r="AF16" s="208"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="136"/>
+      <c r="O16" s="137"/>
+      <c r="P16" s="137"/>
+      <c r="Q16" s="137"/>
+      <c r="R16" s="137"/>
+      <c r="S16" s="137"/>
+      <c r="T16" s="137"/>
+      <c r="U16" s="137"/>
+      <c r="V16" s="137"/>
+      <c r="W16" s="137"/>
+      <c r="X16" s="137"/>
+      <c r="Y16" s="137"/>
+      <c r="Z16" s="137"/>
+      <c r="AA16" s="137"/>
+      <c r="AB16" s="137"/>
+      <c r="AC16" s="137"/>
+      <c r="AD16" s="137"/>
+      <c r="AE16" s="137"/>
+      <c r="AF16" s="138"/>
       <c r="AG16" s="106" t="s">
         <v>274</v>
       </c>
@@ -7948,33 +7948,33 @@
         <v>287</v>
       </c>
       <c r="AI16" s="110"/>
-      <c r="AJ16" s="145" t="s">
+      <c r="AJ16" s="141" t="s">
         <v>280</v>
       </c>
-      <c r="AK16" s="146"/>
-      <c r="AL16" s="147" t="s">
+      <c r="AK16" s="142"/>
+      <c r="AL16" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AM16" s="148"/>
-      <c r="AN16" s="206"/>
-      <c r="AO16" s="207"/>
-      <c r="AP16" s="207"/>
-      <c r="AQ16" s="207"/>
-      <c r="AR16" s="207"/>
-      <c r="AS16" s="207"/>
-      <c r="AT16" s="207"/>
-      <c r="AU16" s="207"/>
-      <c r="AV16" s="207"/>
-      <c r="AW16" s="207"/>
-      <c r="AX16" s="207"/>
-      <c r="AY16" s="207"/>
-      <c r="AZ16" s="207"/>
-      <c r="BA16" s="207"/>
-      <c r="BB16" s="207"/>
-      <c r="BC16" s="207"/>
-      <c r="BD16" s="207"/>
-      <c r="BE16" s="207"/>
-      <c r="BF16" s="207"/>
+      <c r="AM16" s="140"/>
+      <c r="AN16" s="136"/>
+      <c r="AO16" s="137"/>
+      <c r="AP16" s="137"/>
+      <c r="AQ16" s="137"/>
+      <c r="AR16" s="137"/>
+      <c r="AS16" s="137"/>
+      <c r="AT16" s="137"/>
+      <c r="AU16" s="137"/>
+      <c r="AV16" s="137"/>
+      <c r="AW16" s="137"/>
+      <c r="AX16" s="137"/>
+      <c r="AY16" s="137"/>
+      <c r="AZ16" s="137"/>
+      <c r="BA16" s="137"/>
+      <c r="BB16" s="137"/>
+      <c r="BC16" s="137"/>
+      <c r="BD16" s="137"/>
+      <c r="BE16" s="137"/>
+      <c r="BF16" s="137"/>
       <c r="BG16" s="103"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -7997,31 +7997,31 @@
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
       <c r="K17" s="110"/>
-      <c r="L17" s="145" t="s">
+      <c r="L17" s="141" t="s">
         <v>281</v>
       </c>
-      <c r="M17" s="146"/>
-      <c r="N17" s="147" t="s">
+      <c r="M17" s="142"/>
+      <c r="N17" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="O17" s="148"/>
-      <c r="P17" s="206"/>
-      <c r="Q17" s="207"/>
-      <c r="R17" s="207"/>
-      <c r="S17" s="207"/>
-      <c r="T17" s="207"/>
-      <c r="U17" s="207"/>
-      <c r="V17" s="207"/>
-      <c r="W17" s="207"/>
-      <c r="X17" s="207"/>
-      <c r="Y17" s="207"/>
-      <c r="Z17" s="207"/>
-      <c r="AA17" s="207"/>
-      <c r="AB17" s="207"/>
-      <c r="AC17" s="207"/>
-      <c r="AD17" s="207"/>
-      <c r="AE17" s="207"/>
-      <c r="AF17" s="208"/>
+      <c r="O17" s="140"/>
+      <c r="P17" s="136"/>
+      <c r="Q17" s="137"/>
+      <c r="R17" s="137"/>
+      <c r="S17" s="137"/>
+      <c r="T17" s="137"/>
+      <c r="U17" s="137"/>
+      <c r="V17" s="137"/>
+      <c r="W17" s="137"/>
+      <c r="X17" s="137"/>
+      <c r="Y17" s="137"/>
+      <c r="Z17" s="137"/>
+      <c r="AA17" s="137"/>
+      <c r="AB17" s="137"/>
+      <c r="AC17" s="137"/>
+      <c r="AD17" s="137"/>
+      <c r="AE17" s="137"/>
+      <c r="AF17" s="138"/>
       <c r="AG17" s="106" t="s">
         <v>274</v>
       </c>
@@ -8031,31 +8031,31 @@
       <c r="AI17" s="111"/>
       <c r="AJ17" s="111"/>
       <c r="AK17" s="110"/>
-      <c r="AL17" s="145" t="s">
+      <c r="AL17" s="141" t="s">
         <v>281</v>
       </c>
-      <c r="AM17" s="146"/>
-      <c r="AN17" s="147" t="s">
+      <c r="AM17" s="142"/>
+      <c r="AN17" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AO17" s="148"/>
-      <c r="AP17" s="206"/>
-      <c r="AQ17" s="207"/>
-      <c r="AR17" s="207"/>
-      <c r="AS17" s="207"/>
-      <c r="AT17" s="207"/>
-      <c r="AU17" s="207"/>
-      <c r="AV17" s="207"/>
-      <c r="AW17" s="207"/>
-      <c r="AX17" s="207"/>
-      <c r="AY17" s="207"/>
-      <c r="AZ17" s="207"/>
-      <c r="BA17" s="207"/>
-      <c r="BB17" s="207"/>
-      <c r="BC17" s="207"/>
-      <c r="BD17" s="207"/>
-      <c r="BE17" s="207"/>
-      <c r="BF17" s="207"/>
+      <c r="AO17" s="140"/>
+      <c r="AP17" s="136"/>
+      <c r="AQ17" s="137"/>
+      <c r="AR17" s="137"/>
+      <c r="AS17" s="137"/>
+      <c r="AT17" s="137"/>
+      <c r="AU17" s="137"/>
+      <c r="AV17" s="137"/>
+      <c r="AW17" s="137"/>
+      <c r="AX17" s="137"/>
+      <c r="AY17" s="137"/>
+      <c r="AZ17" s="137"/>
+      <c r="BA17" s="137"/>
+      <c r="BB17" s="137"/>
+      <c r="BC17" s="137"/>
+      <c r="BD17" s="137"/>
+      <c r="BE17" s="137"/>
+      <c r="BF17" s="137"/>
       <c r="BG17" s="103"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -8083,24 +8083,24 @@
       <c r="N18" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="O18" s="152"/>
-      <c r="P18" s="206"/>
-      <c r="Q18" s="207"/>
-      <c r="R18" s="207"/>
-      <c r="S18" s="207"/>
-      <c r="T18" s="207"/>
-      <c r="U18" s="207"/>
-      <c r="V18" s="207"/>
-      <c r="W18" s="207"/>
-      <c r="X18" s="207"/>
-      <c r="Y18" s="207"/>
-      <c r="Z18" s="207"/>
-      <c r="AA18" s="207"/>
-      <c r="AB18" s="207"/>
-      <c r="AC18" s="207"/>
-      <c r="AD18" s="207"/>
-      <c r="AE18" s="207"/>
-      <c r="AF18" s="208"/>
+      <c r="O18" s="144"/>
+      <c r="P18" s="136"/>
+      <c r="Q18" s="137"/>
+      <c r="R18" s="137"/>
+      <c r="S18" s="137"/>
+      <c r="T18" s="137"/>
+      <c r="U18" s="137"/>
+      <c r="V18" s="137"/>
+      <c r="W18" s="137"/>
+      <c r="X18" s="137"/>
+      <c r="Y18" s="137"/>
+      <c r="Z18" s="137"/>
+      <c r="AA18" s="137"/>
+      <c r="AB18" s="137"/>
+      <c r="AC18" s="137"/>
+      <c r="AD18" s="137"/>
+      <c r="AE18" s="137"/>
+      <c r="AF18" s="138"/>
       <c r="AG18" s="106" t="s">
         <v>274</v>
       </c>
@@ -8115,24 +8115,24 @@
       <c r="AN18" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="AO18" s="152"/>
-      <c r="AP18" s="206"/>
-      <c r="AQ18" s="207"/>
-      <c r="AR18" s="207"/>
-      <c r="AS18" s="207"/>
-      <c r="AT18" s="207"/>
-      <c r="AU18" s="207"/>
-      <c r="AV18" s="207"/>
-      <c r="AW18" s="207"/>
-      <c r="AX18" s="207"/>
-      <c r="AY18" s="207"/>
-      <c r="AZ18" s="207"/>
-      <c r="BA18" s="207"/>
-      <c r="BB18" s="207"/>
-      <c r="BC18" s="207"/>
-      <c r="BD18" s="207"/>
-      <c r="BE18" s="207"/>
-      <c r="BF18" s="207"/>
+      <c r="AO18" s="144"/>
+      <c r="AP18" s="136"/>
+      <c r="AQ18" s="137"/>
+      <c r="AR18" s="137"/>
+      <c r="AS18" s="137"/>
+      <c r="AT18" s="137"/>
+      <c r="AU18" s="137"/>
+      <c r="AV18" s="137"/>
+      <c r="AW18" s="137"/>
+      <c r="AX18" s="137"/>
+      <c r="AY18" s="137"/>
+      <c r="AZ18" s="137"/>
+      <c r="BA18" s="137"/>
+      <c r="BB18" s="137"/>
+      <c r="BC18" s="137"/>
+      <c r="BD18" s="137"/>
+      <c r="BE18" s="137"/>
+      <c r="BF18" s="137"/>
       <c r="BG18" s="103"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -8358,23 +8358,23 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
       <c r="S22" s="110"/>
-      <c r="T22" s="145" t="s">
+      <c r="T22" s="141" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="146"/>
-      <c r="V22" s="147" t="s">
+      <c r="U22" s="142"/>
+      <c r="V22" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="W22" s="148"/>
-      <c r="X22" s="206"/>
-      <c r="Y22" s="207"/>
-      <c r="Z22" s="207"/>
-      <c r="AA22" s="207"/>
-      <c r="AB22" s="207"/>
-      <c r="AC22" s="207"/>
-      <c r="AD22" s="207"/>
-      <c r="AE22" s="207"/>
-      <c r="AF22" s="208"/>
+      <c r="W22" s="140"/>
+      <c r="X22" s="136"/>
+      <c r="Y22" s="137"/>
+      <c r="Z22" s="137"/>
+      <c r="AA22" s="137"/>
+      <c r="AB22" s="137"/>
+      <c r="AC22" s="137"/>
+      <c r="AD22" s="137"/>
+      <c r="AE22" s="137"/>
+      <c r="AF22" s="138"/>
       <c r="AG22" s="106" t="s">
         <v>274</v>
       </c>
@@ -8392,23 +8392,23 @@
       <c r="AQ22" s="111"/>
       <c r="AR22" s="111"/>
       <c r="AS22" s="110"/>
-      <c r="AT22" s="145" t="s">
+      <c r="AT22" s="141" t="s">
         <v>283</v>
       </c>
-      <c r="AU22" s="146"/>
-      <c r="AV22" s="147" t="s">
+      <c r="AU22" s="142"/>
+      <c r="AV22" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AW22" s="148"/>
-      <c r="AX22" s="206"/>
-      <c r="AY22" s="207"/>
-      <c r="AZ22" s="207"/>
-      <c r="BA22" s="207"/>
-      <c r="BB22" s="207"/>
-      <c r="BC22" s="207"/>
-      <c r="BD22" s="207"/>
-      <c r="BE22" s="207"/>
-      <c r="BF22" s="207"/>
+      <c r="AW22" s="140"/>
+      <c r="AX22" s="136"/>
+      <c r="AY22" s="137"/>
+      <c r="AZ22" s="137"/>
+      <c r="BA22" s="137"/>
+      <c r="BB22" s="137"/>
+      <c r="BC22" s="137"/>
+      <c r="BD22" s="137"/>
+      <c r="BE22" s="137"/>
+      <c r="BF22" s="137"/>
       <c r="BG22" s="103"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -8441,21 +8441,21 @@
       <c r="S23" s="111"/>
       <c r="T23" s="111"/>
       <c r="U23" s="110"/>
-      <c r="V23" s="145" t="s">
+      <c r="V23" s="141" t="s">
         <v>284</v>
       </c>
-      <c r="W23" s="146"/>
-      <c r="X23" s="147" t="s">
+      <c r="W23" s="142"/>
+      <c r="X23" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="Y23" s="148"/>
-      <c r="Z23" s="206"/>
-      <c r="AA23" s="207"/>
-      <c r="AB23" s="207"/>
-      <c r="AC23" s="207"/>
-      <c r="AD23" s="207"/>
-      <c r="AE23" s="207"/>
-      <c r="AF23" s="208"/>
+      <c r="Y23" s="140"/>
+      <c r="Z23" s="136"/>
+      <c r="AA23" s="137"/>
+      <c r="AB23" s="137"/>
+      <c r="AC23" s="137"/>
+      <c r="AD23" s="137"/>
+      <c r="AE23" s="137"/>
+      <c r="AF23" s="138"/>
       <c r="AG23" s="106" t="s">
         <v>274</v>
       </c>
@@ -8475,21 +8475,21 @@
       <c r="AS23" s="111"/>
       <c r="AT23" s="111"/>
       <c r="AU23" s="110"/>
-      <c r="AV23" s="145" t="s">
+      <c r="AV23" s="141" t="s">
         <v>284</v>
       </c>
-      <c r="AW23" s="146"/>
-      <c r="AX23" s="147" t="s">
+      <c r="AW23" s="142"/>
+      <c r="AX23" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AY23" s="148"/>
-      <c r="AZ23" s="206"/>
-      <c r="BA23" s="207"/>
-      <c r="BB23" s="207"/>
-      <c r="BC23" s="207"/>
-      <c r="BD23" s="207"/>
-      <c r="BE23" s="207"/>
-      <c r="BF23" s="207"/>
+      <c r="AY23" s="140"/>
+      <c r="AZ23" s="136"/>
+      <c r="BA23" s="137"/>
+      <c r="BB23" s="137"/>
+      <c r="BC23" s="137"/>
+      <c r="BD23" s="137"/>
+      <c r="BE23" s="137"/>
+      <c r="BF23" s="137"/>
       <c r="BG23" s="103"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -8524,19 +8524,19 @@
       <c r="U24" s="111"/>
       <c r="V24" s="111"/>
       <c r="W24" s="110"/>
-      <c r="X24" s="145" t="s">
+      <c r="X24" s="141" t="s">
         <v>285</v>
       </c>
-      <c r="Y24" s="146"/>
-      <c r="Z24" s="147" t="s">
+      <c r="Y24" s="142"/>
+      <c r="Z24" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AA24" s="148"/>
-      <c r="AB24" s="206"/>
-      <c r="AC24" s="207"/>
-      <c r="AD24" s="207"/>
-      <c r="AE24" s="207"/>
-      <c r="AF24" s="208"/>
+      <c r="AA24" s="140"/>
+      <c r="AB24" s="136"/>
+      <c r="AC24" s="137"/>
+      <c r="AD24" s="137"/>
+      <c r="AE24" s="137"/>
+      <c r="AF24" s="138"/>
       <c r="AG24" s="106" t="s">
         <v>274</v>
       </c>
@@ -8558,19 +8558,19 @@
       <c r="AU24" s="111"/>
       <c r="AV24" s="111"/>
       <c r="AW24" s="110"/>
-      <c r="AX24" s="145" t="s">
+      <c r="AX24" s="141" t="s">
         <v>285</v>
       </c>
-      <c r="AY24" s="146"/>
-      <c r="AZ24" s="147" t="s">
+      <c r="AY24" s="142"/>
+      <c r="AZ24" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="BA24" s="148"/>
-      <c r="BB24" s="206"/>
-      <c r="BC24" s="207"/>
-      <c r="BD24" s="207"/>
-      <c r="BE24" s="207"/>
-      <c r="BF24" s="207"/>
+      <c r="BA24" s="140"/>
+      <c r="BB24" s="136"/>
+      <c r="BC24" s="137"/>
+      <c r="BD24" s="137"/>
+      <c r="BE24" s="137"/>
+      <c r="BF24" s="137"/>
       <c r="BG24" s="103"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -8610,14 +8610,14 @@
       <c r="Z25" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="AA25" s="152"/>
-      <c r="AB25" s="147" t="s">
+      <c r="AA25" s="144"/>
+      <c r="AB25" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AC25" s="148"/>
-      <c r="AD25" s="206"/>
-      <c r="AE25" s="207"/>
-      <c r="AF25" s="208"/>
+      <c r="AC25" s="140"/>
+      <c r="AD25" s="136"/>
+      <c r="AE25" s="137"/>
+      <c r="AF25" s="138"/>
       <c r="AG25" s="106" t="s">
         <v>274</v>
       </c>
@@ -8644,14 +8644,14 @@
       <c r="AZ25" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="BA25" s="152"/>
-      <c r="BB25" s="147" t="s">
+      <c r="BA25" s="144"/>
+      <c r="BB25" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="BC25" s="148"/>
-      <c r="BD25" s="206"/>
-      <c r="BE25" s="207"/>
-      <c r="BF25" s="207"/>
+      <c r="BC25" s="140"/>
+      <c r="BD25" s="136"/>
+      <c r="BE25" s="137"/>
+      <c r="BF25" s="137"/>
       <c r="BG25" s="103"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -8909,29 +8909,29 @@
         <v>318</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="149" t="s">
+      <c r="E30" s="186" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="150"/>
+      <c r="F30" s="187"/>
       <c r="G30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="149" t="s">
+      <c r="H30" s="186" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="150"/>
-      <c r="J30" s="149" t="s">
+      <c r="I30" s="187"/>
+      <c r="J30" s="186" t="s">
         <v>280</v>
       </c>
-      <c r="K30" s="150"/>
-      <c r="L30" s="149" t="s">
+      <c r="K30" s="187"/>
+      <c r="L30" s="186" t="s">
         <v>281</v>
       </c>
-      <c r="M30" s="150"/>
-      <c r="N30" s="149" t="s">
+      <c r="M30" s="187"/>
+      <c r="N30" s="186" t="s">
         <v>282</v>
       </c>
-      <c r="O30" s="150"/>
+      <c r="O30" s="187"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>239</v>
@@ -8940,50 +8940,50 @@
         <v>239</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="149" t="s">
+      <c r="T30" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="U30" s="150"/>
-      <c r="V30" s="149" t="s">
+      <c r="U30" s="187"/>
+      <c r="V30" s="186" t="s">
         <v>284</v>
       </c>
-      <c r="W30" s="150"/>
-      <c r="X30" s="149" t="s">
+      <c r="W30" s="187"/>
+      <c r="X30" s="186" t="s">
         <v>285</v>
       </c>
-      <c r="Y30" s="150"/>
-      <c r="Z30" s="149" t="s">
+      <c r="Y30" s="187"/>
+      <c r="Z30" s="186" t="s">
         <v>286</v>
       </c>
-      <c r="AA30" s="150"/>
-      <c r="AB30" s="153" t="s">
+      <c r="AA30" s="187"/>
+      <c r="AB30" s="160" t="s">
         <v>297</v>
       </c>
-      <c r="AC30" s="154"/>
-      <c r="AD30" s="155"/>
-      <c r="AE30" s="149" t="s">
+      <c r="AC30" s="161"/>
+      <c r="AD30" s="162"/>
+      <c r="AE30" s="186" t="s">
         <v>273</v>
       </c>
-      <c r="AF30" s="150"/>
+      <c r="AF30" s="187"/>
       <c r="AG30" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="AH30" s="149" t="s">
+      <c r="AH30" s="186" t="s">
         <v>279</v>
       </c>
-      <c r="AI30" s="150"/>
-      <c r="AJ30" s="149" t="s">
+      <c r="AI30" s="187"/>
+      <c r="AJ30" s="186" t="s">
         <v>280</v>
       </c>
-      <c r="AK30" s="150"/>
-      <c r="AL30" s="149" t="s">
+      <c r="AK30" s="187"/>
+      <c r="AL30" s="186" t="s">
         <v>281</v>
       </c>
-      <c r="AM30" s="150"/>
-      <c r="AN30" s="149" t="s">
+      <c r="AM30" s="187"/>
+      <c r="AN30" s="186" t="s">
         <v>282</v>
       </c>
-      <c r="AO30" s="150"/>
+      <c r="AO30" s="187"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>239</v>
@@ -8992,27 +8992,27 @@
         <v>239</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="149" t="s">
+      <c r="AT30" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="AU30" s="150"/>
-      <c r="AV30" s="149" t="s">
+      <c r="AU30" s="187"/>
+      <c r="AV30" s="186" t="s">
         <v>284</v>
       </c>
-      <c r="AW30" s="150"/>
-      <c r="AX30" s="149" t="s">
+      <c r="AW30" s="187"/>
+      <c r="AX30" s="186" t="s">
         <v>285</v>
       </c>
-      <c r="AY30" s="150"/>
-      <c r="AZ30" s="149" t="s">
+      <c r="AY30" s="187"/>
+      <c r="AZ30" s="186" t="s">
         <v>286</v>
       </c>
-      <c r="BA30" s="150"/>
-      <c r="BB30" s="153" t="s">
+      <c r="BA30" s="187"/>
+      <c r="BB30" s="160" t="s">
         <v>297</v>
       </c>
-      <c r="BC30" s="154"/>
-      <c r="BD30" s="155"/>
+      <c r="BC30" s="161"/>
+      <c r="BD30" s="162"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -9024,10 +9024,10 @@
         <v>317</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="151" t="s">
+      <c r="E31" s="163" t="s">
         <v>323</v>
       </c>
-      <c r="F31" s="151"/>
+      <c r="F31" s="163"/>
       <c r="G31" s="22" t="s">
         <v>324</v>
       </c>
@@ -9054,10 +9054,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="151" t="s">
+      <c r="AE31" s="163" t="s">
         <v>323</v>
       </c>
-      <c r="AF31" s="151"/>
+      <c r="AF31" s="163"/>
       <c r="AG31" s="22" t="s">
         <v>324</v>
       </c>
@@ -9167,75 +9167,75 @@
       <c r="G33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="H33" s="179" t="s">
+      <c r="H33" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="I33" s="180"/>
-      <c r="J33" s="180"/>
-      <c r="K33" s="180"/>
-      <c r="L33" s="180"/>
-      <c r="M33" s="180"/>
-      <c r="N33" s="180"/>
-      <c r="O33" s="180"/>
-      <c r="P33" s="180"/>
-      <c r="Q33" s="180"/>
-      <c r="R33" s="180"/>
-      <c r="S33" s="181"/>
-      <c r="T33" s="149" t="s">
+      <c r="I33" s="184"/>
+      <c r="J33" s="184"/>
+      <c r="K33" s="184"/>
+      <c r="L33" s="184"/>
+      <c r="M33" s="184"/>
+      <c r="N33" s="184"/>
+      <c r="O33" s="184"/>
+      <c r="P33" s="184"/>
+      <c r="Q33" s="184"/>
+      <c r="R33" s="184"/>
+      <c r="S33" s="185"/>
+      <c r="T33" s="186" t="s">
         <v>275</v>
       </c>
-      <c r="U33" s="150"/>
-      <c r="V33" s="153" t="s">
+      <c r="U33" s="187"/>
+      <c r="V33" s="160" t="s">
         <v>297</v>
       </c>
-      <c r="W33" s="155"/>
-      <c r="X33" s="179" t="s">
+      <c r="W33" s="162"/>
+      <c r="X33" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="Y33" s="180"/>
-      <c r="Z33" s="180"/>
-      <c r="AA33" s="180"/>
-      <c r="AB33" s="180"/>
-      <c r="AC33" s="180"/>
-      <c r="AD33" s="180"/>
-      <c r="AE33" s="181"/>
+      <c r="Y33" s="184"/>
+      <c r="Z33" s="184"/>
+      <c r="AA33" s="184"/>
+      <c r="AB33" s="184"/>
+      <c r="AC33" s="184"/>
+      <c r="AD33" s="184"/>
+      <c r="AE33" s="185"/>
       <c r="AF33" s="24" t="s">
         <v>273</v>
       </c>
       <c r="AG33" s="102" t="s">
         <v>274</v>
       </c>
-      <c r="AH33" s="179" t="s">
+      <c r="AH33" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="AI33" s="180"/>
-      <c r="AJ33" s="180"/>
-      <c r="AK33" s="180"/>
-      <c r="AL33" s="180"/>
-      <c r="AM33" s="180"/>
-      <c r="AN33" s="180"/>
-      <c r="AO33" s="180"/>
-      <c r="AP33" s="180"/>
-      <c r="AQ33" s="180"/>
-      <c r="AR33" s="180"/>
-      <c r="AS33" s="181"/>
-      <c r="AT33" s="149" t="s">
+      <c r="AI33" s="184"/>
+      <c r="AJ33" s="184"/>
+      <c r="AK33" s="184"/>
+      <c r="AL33" s="184"/>
+      <c r="AM33" s="184"/>
+      <c r="AN33" s="184"/>
+      <c r="AO33" s="184"/>
+      <c r="AP33" s="184"/>
+      <c r="AQ33" s="184"/>
+      <c r="AR33" s="184"/>
+      <c r="AS33" s="185"/>
+      <c r="AT33" s="186" t="s">
         <v>275</v>
       </c>
-      <c r="AU33" s="150"/>
-      <c r="AV33" s="153" t="s">
+      <c r="AU33" s="187"/>
+      <c r="AV33" s="160" t="s">
         <v>297</v>
       </c>
-      <c r="AW33" s="155"/>
-      <c r="AX33" s="179" t="s">
+      <c r="AW33" s="162"/>
+      <c r="AX33" s="183" t="s">
         <v>319</v>
       </c>
-      <c r="AY33" s="180"/>
-      <c r="AZ33" s="180"/>
-      <c r="BA33" s="180"/>
-      <c r="BB33" s="180"/>
-      <c r="BC33" s="180"/>
-      <c r="BD33" s="181"/>
+      <c r="AY33" s="184"/>
+      <c r="AZ33" s="184"/>
+      <c r="BA33" s="184"/>
+      <c r="BB33" s="184"/>
+      <c r="BC33" s="184"/>
+      <c r="BD33" s="185"/>
       <c r="BE33" s="7"/>
       <c r="BF33" s="7"/>
       <c r="BG33" s="7"/>
@@ -9247,10 +9247,10 @@
         <v>317</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="151" t="s">
+      <c r="E34" s="163" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="151"/>
+      <c r="F34" s="163"/>
       <c r="G34" s="22" t="s">
         <v>321</v>
       </c>
@@ -9266,10 +9266,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="151" t="s">
+      <c r="T34" s="163" t="s">
         <v>323</v>
       </c>
-      <c r="U34" s="151"/>
+      <c r="U34" s="163"/>
       <c r="V34" s="22" t="s">
         <v>325</v>
       </c>
@@ -9298,10 +9298,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="151" t="s">
+      <c r="AT34" s="163" t="s">
         <v>323</v>
       </c>
-      <c r="AU34" s="151"/>
+      <c r="AU34" s="163"/>
       <c r="AV34" s="22" t="s">
         <v>320</v>
       </c>
@@ -9572,33 +9572,33 @@
         <v>326</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="182" t="s">
+      <c r="E39" s="178" t="s">
         <v>273</v>
       </c>
-      <c r="F39" s="183"/>
-      <c r="G39" s="184" t="s">
+      <c r="F39" s="179"/>
+      <c r="G39" s="181" t="s">
         <v>273</v>
       </c>
-      <c r="H39" s="185"/>
+      <c r="H39" s="182"/>
       <c r="I39" s="100" t="s">
         <v>319</v>
       </c>
       <c r="J39" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="K39" s="152"/>
+      <c r="K39" s="144"/>
       <c r="L39" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="M39" s="152"/>
+      <c r="M39" s="144"/>
       <c r="N39" s="143" t="s">
         <v>281</v>
       </c>
-      <c r="O39" s="152"/>
+      <c r="O39" s="144"/>
       <c r="P39" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="Q39" s="152"/>
+      <c r="Q39" s="144"/>
       <c r="R39" s="103"/>
       <c r="S39" s="103" t="s">
         <v>239</v>
@@ -9610,47 +9610,47 @@
       <c r="V39" s="143" t="s">
         <v>283</v>
       </c>
-      <c r="W39" s="152"/>
+      <c r="W39" s="144"/>
       <c r="X39" s="143" t="s">
         <v>284</v>
       </c>
-      <c r="Y39" s="152"/>
+      <c r="Y39" s="144"/>
       <c r="Z39" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="AA39" s="152"/>
+      <c r="AA39" s="144"/>
       <c r="AB39" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="AC39" s="152"/>
-      <c r="AD39" s="147" t="s">
+      <c r="AC39" s="144"/>
+      <c r="AD39" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AE39" s="187"/>
-      <c r="AF39" s="148"/>
+      <c r="AE39" s="180"/>
+      <c r="AF39" s="140"/>
       <c r="AG39" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AH39" s="152"/>
+      <c r="AH39" s="144"/>
       <c r="AI39" s="112" t="s">
         <v>319</v>
       </c>
       <c r="AJ39" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="AK39" s="152"/>
+      <c r="AK39" s="144"/>
       <c r="AL39" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="AM39" s="152"/>
+      <c r="AM39" s="144"/>
       <c r="AN39" s="143" t="s">
         <v>281</v>
       </c>
-      <c r="AO39" s="152"/>
+      <c r="AO39" s="144"/>
       <c r="AP39" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="AQ39" s="152"/>
+      <c r="AQ39" s="144"/>
       <c r="AR39" s="103"/>
       <c r="AS39" s="103" t="s">
         <v>239</v>
@@ -9679,14 +9679,14 @@
         <v>351</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="186" t="s">
+      <c r="E40" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="186"/>
-      <c r="G40" s="186" t="s">
+      <c r="F40" s="156"/>
+      <c r="G40" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="H40" s="186"/>
+      <c r="H40" s="156"/>
       <c r="I40" s="113" t="s">
         <v>324</v>
       </c>
@@ -9713,10 +9713,10 @@
       <c r="AD40" s="103"/>
       <c r="AE40" s="103"/>
       <c r="AF40" s="103"/>
-      <c r="AG40" s="186" t="s">
+      <c r="AG40" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="AH40" s="186"/>
+      <c r="AH40" s="156"/>
       <c r="AI40" s="113" t="s">
         <v>328</v>
       </c>
@@ -9755,24 +9755,24 @@
       <c r="E41" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="152"/>
+      <c r="F41" s="144"/>
       <c r="G41" s="100" t="s">
         <v>319</v>
       </c>
       <c r="H41" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="I41" s="152"/>
+      <c r="I41" s="144"/>
       <c r="J41" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="K41" s="152"/>
-      <c r="L41" s="182"/>
-      <c r="M41" s="183"/>
-      <c r="N41" s="184" t="s">
+      <c r="K41" s="144"/>
+      <c r="L41" s="178"/>
+      <c r="M41" s="179"/>
+      <c r="N41" s="181" t="s">
         <v>282</v>
       </c>
-      <c r="O41" s="185"/>
+      <c r="O41" s="182"/>
       <c r="P41" s="103"/>
       <c r="Q41" s="103" t="s">
         <v>239</v>
@@ -9784,47 +9784,47 @@
       <c r="T41" s="143" t="s">
         <v>283</v>
       </c>
-      <c r="U41" s="152"/>
+      <c r="U41" s="144"/>
       <c r="V41" s="143" t="s">
         <v>284</v>
       </c>
-      <c r="W41" s="152"/>
+      <c r="W41" s="144"/>
       <c r="X41" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="Y41" s="152"/>
+      <c r="Y41" s="144"/>
       <c r="Z41" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="AA41" s="152"/>
-      <c r="AB41" s="147" t="s">
+      <c r="AA41" s="144"/>
+      <c r="AB41" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AC41" s="187"/>
-      <c r="AD41" s="148"/>
+      <c r="AC41" s="180"/>
+      <c r="AD41" s="140"/>
       <c r="AE41" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AF41" s="152"/>
+      <c r="AF41" s="144"/>
       <c r="AG41" s="100" t="s">
         <v>319</v>
       </c>
       <c r="AH41" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="AI41" s="152"/>
+      <c r="AI41" s="144"/>
       <c r="AJ41" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="AK41" s="152"/>
+      <c r="AK41" s="144"/>
       <c r="AL41" s="143" t="s">
         <v>281</v>
       </c>
-      <c r="AM41" s="152"/>
+      <c r="AM41" s="144"/>
       <c r="AN41" s="143" t="s">
         <v>282</v>
       </c>
-      <c r="AO41" s="152"/>
+      <c r="AO41" s="144"/>
       <c r="AP41" s="103"/>
       <c r="AQ41" s="103" t="s">
         <v>239</v>
@@ -9836,24 +9836,24 @@
       <c r="AT41" s="143" t="s">
         <v>283</v>
       </c>
-      <c r="AU41" s="152"/>
+      <c r="AU41" s="144"/>
       <c r="AV41" s="143" t="s">
         <v>284</v>
       </c>
-      <c r="AW41" s="152"/>
+      <c r="AW41" s="144"/>
       <c r="AX41" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="AY41" s="152"/>
+      <c r="AY41" s="144"/>
       <c r="AZ41" s="143" t="s">
         <v>286</v>
       </c>
-      <c r="BA41" s="152"/>
-      <c r="BB41" s="147" t="s">
+      <c r="BA41" s="144"/>
+      <c r="BB41" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="BC41" s="187"/>
-      <c r="BD41" s="148"/>
+      <c r="BC41" s="180"/>
+      <c r="BD41" s="140"/>
       <c r="BE41" s="103"/>
       <c r="BF41" s="103"/>
       <c r="BG41" s="103"/>
@@ -9865,10 +9865,10 @@
         <v>352</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="186" t="s">
+      <c r="E42" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="186"/>
+      <c r="F42" s="156"/>
       <c r="G42" s="113" t="s">
         <v>324</v>
       </c>
@@ -9895,10 +9895,10 @@
       <c r="AB42" s="103"/>
       <c r="AC42" s="103"/>
       <c r="AD42" s="103"/>
-      <c r="AE42" s="186" t="s">
+      <c r="AE42" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="AF42" s="186"/>
+      <c r="AF42" s="156"/>
       <c r="AG42" s="113" t="s">
         <v>324</v>
       </c>
@@ -10008,75 +10008,75 @@
       <c r="G44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="193" t="s">
+      <c r="H44" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="I44" s="194"/>
-      <c r="J44" s="194"/>
-      <c r="K44" s="194"/>
-      <c r="L44" s="194"/>
-      <c r="M44" s="194"/>
-      <c r="N44" s="194"/>
-      <c r="O44" s="194"/>
-      <c r="P44" s="194"/>
-      <c r="Q44" s="194"/>
-      <c r="R44" s="194"/>
-      <c r="S44" s="195"/>
-      <c r="T44" s="182" t="s">
+      <c r="I44" s="176"/>
+      <c r="J44" s="176"/>
+      <c r="K44" s="176"/>
+      <c r="L44" s="176"/>
+      <c r="M44" s="176"/>
+      <c r="N44" s="176"/>
+      <c r="O44" s="176"/>
+      <c r="P44" s="176"/>
+      <c r="Q44" s="176"/>
+      <c r="R44" s="176"/>
+      <c r="S44" s="177"/>
+      <c r="T44" s="178" t="s">
         <v>275</v>
       </c>
-      <c r="U44" s="183"/>
-      <c r="V44" s="147" t="s">
+      <c r="U44" s="179"/>
+      <c r="V44" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="W44" s="148"/>
-      <c r="X44" s="193" t="s">
+      <c r="W44" s="140"/>
+      <c r="X44" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="Y44" s="194"/>
-      <c r="Z44" s="194"/>
-      <c r="AA44" s="194"/>
-      <c r="AB44" s="194"/>
-      <c r="AC44" s="194"/>
-      <c r="AD44" s="194"/>
-      <c r="AE44" s="195"/>
+      <c r="Y44" s="176"/>
+      <c r="Z44" s="176"/>
+      <c r="AA44" s="176"/>
+      <c r="AB44" s="176"/>
+      <c r="AC44" s="176"/>
+      <c r="AD44" s="176"/>
+      <c r="AE44" s="177"/>
       <c r="AF44" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG44" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH44" s="193" t="s">
+      <c r="AH44" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="AI44" s="194"/>
-      <c r="AJ44" s="194"/>
-      <c r="AK44" s="194"/>
-      <c r="AL44" s="194"/>
-      <c r="AM44" s="194"/>
-      <c r="AN44" s="194"/>
-      <c r="AO44" s="194"/>
-      <c r="AP44" s="194"/>
-      <c r="AQ44" s="194"/>
-      <c r="AR44" s="194"/>
-      <c r="AS44" s="195"/>
+      <c r="AI44" s="176"/>
+      <c r="AJ44" s="176"/>
+      <c r="AK44" s="176"/>
+      <c r="AL44" s="176"/>
+      <c r="AM44" s="176"/>
+      <c r="AN44" s="176"/>
+      <c r="AO44" s="176"/>
+      <c r="AP44" s="176"/>
+      <c r="AQ44" s="176"/>
+      <c r="AR44" s="176"/>
+      <c r="AS44" s="177"/>
       <c r="AT44" s="143" t="s">
         <v>275</v>
       </c>
-      <c r="AU44" s="152"/>
-      <c r="AV44" s="147" t="s">
+      <c r="AU44" s="144"/>
+      <c r="AV44" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AW44" s="148"/>
-      <c r="AX44" s="193" t="s">
+      <c r="AW44" s="140"/>
+      <c r="AX44" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="AY44" s="194"/>
-      <c r="AZ44" s="194"/>
-      <c r="BA44" s="194"/>
-      <c r="BB44" s="194"/>
-      <c r="BC44" s="194"/>
-      <c r="BD44" s="195"/>
+      <c r="AY44" s="176"/>
+      <c r="AZ44" s="176"/>
+      <c r="BA44" s="176"/>
+      <c r="BB44" s="176"/>
+      <c r="BC44" s="176"/>
+      <c r="BD44" s="177"/>
       <c r="BE44" s="103"/>
       <c r="BF44" s="103"/>
       <c r="BG44" s="103"/>
@@ -10088,10 +10088,10 @@
         <v>352</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="186" t="s">
+      <c r="E45" s="156" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="186"/>
+      <c r="F45" s="156"/>
       <c r="G45" s="113" t="s">
         <v>321</v>
       </c>
@@ -10107,10 +10107,10 @@
       <c r="Q45" s="116"/>
       <c r="R45" s="116"/>
       <c r="S45" s="103"/>
-      <c r="T45" s="186" t="s">
+      <c r="T45" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="U45" s="186"/>
+      <c r="U45" s="156"/>
       <c r="V45" s="113" t="s">
         <v>325</v>
       </c>
@@ -10139,10 +10139,10 @@
       <c r="AQ45" s="116"/>
       <c r="AR45" s="116"/>
       <c r="AS45" s="103"/>
-      <c r="AT45" s="186" t="s">
+      <c r="AT45" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="AU45" s="186"/>
+      <c r="AU45" s="156"/>
       <c r="AV45" s="113" t="s">
         <v>320</v>
       </c>
@@ -10171,70 +10171,70 @@
       <c r="F46" s="117" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="193" t="s">
+      <c r="G46" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="H46" s="194"/>
-      <c r="I46" s="194"/>
-      <c r="J46" s="194"/>
-      <c r="K46" s="194"/>
-      <c r="L46" s="194"/>
-      <c r="M46" s="194"/>
-      <c r="N46" s="194"/>
-      <c r="O46" s="194"/>
-      <c r="P46" s="194"/>
-      <c r="Q46" s="194"/>
-      <c r="R46" s="194"/>
-      <c r="S46" s="194"/>
-      <c r="T46" s="194"/>
-      <c r="U46" s="194"/>
-      <c r="V46" s="194"/>
-      <c r="W46" s="194"/>
-      <c r="X46" s="194"/>
-      <c r="Y46" s="194"/>
-      <c r="Z46" s="194"/>
-      <c r="AA46" s="194"/>
-      <c r="AB46" s="194"/>
-      <c r="AC46" s="194"/>
-      <c r="AD46" s="194"/>
-      <c r="AE46" s="195"/>
+      <c r="H46" s="176"/>
+      <c r="I46" s="176"/>
+      <c r="J46" s="176"/>
+      <c r="K46" s="176"/>
+      <c r="L46" s="176"/>
+      <c r="M46" s="176"/>
+      <c r="N46" s="176"/>
+      <c r="O46" s="176"/>
+      <c r="P46" s="176"/>
+      <c r="Q46" s="176"/>
+      <c r="R46" s="176"/>
+      <c r="S46" s="176"/>
+      <c r="T46" s="176"/>
+      <c r="U46" s="176"/>
+      <c r="V46" s="176"/>
+      <c r="W46" s="176"/>
+      <c r="X46" s="176"/>
+      <c r="Y46" s="176"/>
+      <c r="Z46" s="176"/>
+      <c r="AA46" s="176"/>
+      <c r="AB46" s="176"/>
+      <c r="AC46" s="176"/>
+      <c r="AD46" s="176"/>
+      <c r="AE46" s="177"/>
       <c r="AF46" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AG46" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="AH46" s="193" t="s">
+      <c r="AH46" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="AI46" s="194"/>
-      <c r="AJ46" s="194"/>
-      <c r="AK46" s="194"/>
-      <c r="AL46" s="194"/>
-      <c r="AM46" s="194"/>
-      <c r="AN46" s="194"/>
-      <c r="AO46" s="194"/>
-      <c r="AP46" s="194"/>
-      <c r="AQ46" s="194"/>
-      <c r="AR46" s="194"/>
-      <c r="AS46" s="195"/>
+      <c r="AI46" s="176"/>
+      <c r="AJ46" s="176"/>
+      <c r="AK46" s="176"/>
+      <c r="AL46" s="176"/>
+      <c r="AM46" s="176"/>
+      <c r="AN46" s="176"/>
+      <c r="AO46" s="176"/>
+      <c r="AP46" s="176"/>
+      <c r="AQ46" s="176"/>
+      <c r="AR46" s="176"/>
+      <c r="AS46" s="177"/>
       <c r="AT46" s="143" t="s">
         <v>275</v>
       </c>
-      <c r="AU46" s="152"/>
-      <c r="AV46" s="147" t="s">
+      <c r="AU46" s="144"/>
+      <c r="AV46" s="139" t="s">
         <v>297</v>
       </c>
-      <c r="AW46" s="148"/>
-      <c r="AX46" s="193" t="s">
+      <c r="AW46" s="140"/>
+      <c r="AX46" s="175" t="s">
         <v>319</v>
       </c>
-      <c r="AY46" s="194"/>
-      <c r="AZ46" s="194"/>
-      <c r="BA46" s="194"/>
-      <c r="BB46" s="194"/>
-      <c r="BC46" s="194"/>
-      <c r="BD46" s="195"/>
+      <c r="AY46" s="176"/>
+      <c r="AZ46" s="176"/>
+      <c r="BA46" s="176"/>
+      <c r="BB46" s="176"/>
+      <c r="BC46" s="176"/>
+      <c r="BD46" s="177"/>
       <c r="BE46" s="103"/>
       <c r="BF46" s="103"/>
       <c r="BG46" s="103"/>
@@ -10291,10 +10291,10 @@
       <c r="AQ47" s="116"/>
       <c r="AR47" s="116"/>
       <c r="AS47" s="103"/>
-      <c r="AT47" s="186" t="s">
+      <c r="AT47" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="AU47" s="186"/>
+      <c r="AU47" s="156"/>
       <c r="AV47" s="113" t="s">
         <v>320</v>
       </c>
@@ -10685,20 +10685,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="140" t="s">
+      <c r="E54" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="141"/>
-      <c r="G54" s="141"/>
-      <c r="H54" s="141"/>
-      <c r="I54" s="141"/>
-      <c r="J54" s="141"/>
-      <c r="K54" s="142"/>
-      <c r="L54" s="140" t="s">
+      <c r="F54" s="147"/>
+      <c r="G54" s="147"/>
+      <c r="H54" s="147"/>
+      <c r="I54" s="147"/>
+      <c r="J54" s="147"/>
+      <c r="K54" s="167"/>
+      <c r="L54" s="146" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="141"/>
-      <c r="N54" s="209"/>
+      <c r="M54" s="147"/>
+      <c r="N54" s="148"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -10819,20 +10819,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="200" t="s">
+      <c r="E56" s="149" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="202"/>
-      <c r="G56" s="202"/>
-      <c r="H56" s="202"/>
-      <c r="I56" s="202"/>
-      <c r="J56" s="202"/>
-      <c r="K56" s="201"/>
-      <c r="L56" s="200" t="s">
+      <c r="F56" s="150"/>
+      <c r="G56" s="150"/>
+      <c r="H56" s="150"/>
+      <c r="I56" s="150"/>
+      <c r="J56" s="150"/>
+      <c r="K56" s="151"/>
+      <c r="L56" s="149" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="202"/>
-      <c r="N56" s="201"/>
+      <c r="M56" s="150"/>
+      <c r="N56" s="151"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -13304,68 +13304,68 @@
         <v>364</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="140" t="s">
+      <c r="E95" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="141"/>
-      <c r="G95" s="141"/>
-      <c r="H95" s="141"/>
-      <c r="I95" s="141"/>
-      <c r="J95" s="141"/>
-      <c r="K95" s="142"/>
-      <c r="L95" s="140" t="s">
+      <c r="F95" s="147"/>
+      <c r="G95" s="147"/>
+      <c r="H95" s="147"/>
+      <c r="I95" s="147"/>
+      <c r="J95" s="147"/>
+      <c r="K95" s="167"/>
+      <c r="L95" s="146" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="141"/>
-      <c r="N95" s="142"/>
-      <c r="O95" s="176" t="s">
+      <c r="M95" s="147"/>
+      <c r="N95" s="167"/>
+      <c r="O95" s="157" t="s">
         <v>260</v>
       </c>
-      <c r="P95" s="177"/>
-      <c r="Q95" s="177"/>
-      <c r="R95" s="177"/>
-      <c r="S95" s="177"/>
-      <c r="T95" s="178"/>
-      <c r="U95" s="176" t="s">
+      <c r="P95" s="158"/>
+      <c r="Q95" s="158"/>
+      <c r="R95" s="158"/>
+      <c r="S95" s="158"/>
+      <c r="T95" s="159"/>
+      <c r="U95" s="157" t="s">
         <v>260</v>
       </c>
-      <c r="V95" s="177"/>
-      <c r="W95" s="177"/>
-      <c r="X95" s="177"/>
-      <c r="Y95" s="177"/>
-      <c r="Z95" s="177"/>
-      <c r="AA95" s="177"/>
-      <c r="AB95" s="178"/>
-      <c r="AC95" s="176" t="s">
+      <c r="V95" s="158"/>
+      <c r="W95" s="158"/>
+      <c r="X95" s="158"/>
+      <c r="Y95" s="158"/>
+      <c r="Z95" s="158"/>
+      <c r="AA95" s="158"/>
+      <c r="AB95" s="159"/>
+      <c r="AC95" s="157" t="s">
         <v>260</v>
       </c>
-      <c r="AD95" s="177"/>
-      <c r="AE95" s="177"/>
-      <c r="AF95" s="177"/>
-      <c r="AG95" s="177"/>
-      <c r="AH95" s="177"/>
-      <c r="AI95" s="177"/>
-      <c r="AJ95" s="178"/>
-      <c r="AK95" s="176" t="s">
+      <c r="AD95" s="158"/>
+      <c r="AE95" s="158"/>
+      <c r="AF95" s="158"/>
+      <c r="AG95" s="158"/>
+      <c r="AH95" s="158"/>
+      <c r="AI95" s="158"/>
+      <c r="AJ95" s="159"/>
+      <c r="AK95" s="157" t="s">
         <v>260</v>
       </c>
-      <c r="AL95" s="177"/>
-      <c r="AM95" s="177"/>
-      <c r="AN95" s="177"/>
-      <c r="AO95" s="177"/>
-      <c r="AP95" s="177"/>
-      <c r="AQ95" s="177"/>
-      <c r="AR95" s="178"/>
-      <c r="AS95" s="173" t="s">
+      <c r="AL95" s="158"/>
+      <c r="AM95" s="158"/>
+      <c r="AN95" s="158"/>
+      <c r="AO95" s="158"/>
+      <c r="AP95" s="158"/>
+      <c r="AQ95" s="158"/>
+      <c r="AR95" s="159"/>
+      <c r="AS95" s="202" t="s">
         <v>356</v>
       </c>
-      <c r="AT95" s="174"/>
-      <c r="AU95" s="174"/>
-      <c r="AV95" s="174"/>
-      <c r="AW95" s="174"/>
-      <c r="AX95" s="174"/>
-      <c r="AY95" s="174"/>
-      <c r="AZ95" s="175"/>
+      <c r="AT95" s="203"/>
+      <c r="AU95" s="203"/>
+      <c r="AV95" s="203"/>
+      <c r="AW95" s="203"/>
+      <c r="AX95" s="203"/>
+      <c r="AY95" s="203"/>
+      <c r="AZ95" s="204"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -13470,68 +13470,68 @@
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="200" t="s">
+      <c r="E97" s="149" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="202"/>
-      <c r="G97" s="202"/>
-      <c r="H97" s="202"/>
-      <c r="I97" s="202"/>
-      <c r="J97" s="202"/>
-      <c r="K97" s="201"/>
-      <c r="L97" s="200" t="s">
+      <c r="F97" s="150"/>
+      <c r="G97" s="150"/>
+      <c r="H97" s="150"/>
+      <c r="I97" s="150"/>
+      <c r="J97" s="150"/>
+      <c r="K97" s="151"/>
+      <c r="L97" s="149" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="202"/>
-      <c r="N97" s="202"/>
-      <c r="O97" s="200" t="s">
+      <c r="M97" s="150"/>
+      <c r="N97" s="150"/>
+      <c r="O97" s="149" t="s">
         <v>272</v>
       </c>
-      <c r="P97" s="202"/>
-      <c r="Q97" s="202"/>
-      <c r="R97" s="202"/>
-      <c r="S97" s="202"/>
-      <c r="T97" s="201"/>
-      <c r="U97" s="200" t="s">
+      <c r="P97" s="150"/>
+      <c r="Q97" s="150"/>
+      <c r="R97" s="150"/>
+      <c r="S97" s="150"/>
+      <c r="T97" s="151"/>
+      <c r="U97" s="149" t="s">
         <v>229</v>
       </c>
-      <c r="V97" s="202"/>
-      <c r="W97" s="202"/>
-      <c r="X97" s="202"/>
-      <c r="Y97" s="202"/>
-      <c r="Z97" s="202"/>
-      <c r="AA97" s="202"/>
-      <c r="AB97" s="201"/>
-      <c r="AC97" s="200" t="s">
+      <c r="V97" s="150"/>
+      <c r="W97" s="150"/>
+      <c r="X97" s="150"/>
+      <c r="Y97" s="150"/>
+      <c r="Z97" s="150"/>
+      <c r="AA97" s="150"/>
+      <c r="AB97" s="151"/>
+      <c r="AC97" s="149" t="s">
         <v>229</v>
       </c>
-      <c r="AD97" s="202"/>
-      <c r="AE97" s="202"/>
-      <c r="AF97" s="202"/>
-      <c r="AG97" s="202"/>
-      <c r="AH97" s="202"/>
-      <c r="AI97" s="202"/>
-      <c r="AJ97" s="201"/>
-      <c r="AK97" s="200" t="s">
+      <c r="AD97" s="150"/>
+      <c r="AE97" s="150"/>
+      <c r="AF97" s="150"/>
+      <c r="AG97" s="150"/>
+      <c r="AH97" s="150"/>
+      <c r="AI97" s="150"/>
+      <c r="AJ97" s="151"/>
+      <c r="AK97" s="149" t="s">
         <v>229</v>
       </c>
-      <c r="AL97" s="202"/>
-      <c r="AM97" s="202"/>
-      <c r="AN97" s="202"/>
-      <c r="AO97" s="202"/>
-      <c r="AP97" s="202"/>
-      <c r="AQ97" s="202"/>
-      <c r="AR97" s="201"/>
-      <c r="AS97" s="202" t="s">
+      <c r="AL97" s="150"/>
+      <c r="AM97" s="150"/>
+      <c r="AN97" s="150"/>
+      <c r="AO97" s="150"/>
+      <c r="AP97" s="150"/>
+      <c r="AQ97" s="150"/>
+      <c r="AR97" s="151"/>
+      <c r="AS97" s="150" t="s">
         <v>229</v>
       </c>
-      <c r="AT97" s="202"/>
-      <c r="AU97" s="202"/>
-      <c r="AV97" s="202"/>
-      <c r="AW97" s="202"/>
-      <c r="AX97" s="202"/>
-      <c r="AY97" s="202"/>
-      <c r="AZ97" s="201"/>
+      <c r="AT97" s="150"/>
+      <c r="AU97" s="150"/>
+      <c r="AV97" s="150"/>
+      <c r="AW97" s="150"/>
+      <c r="AX97" s="150"/>
+      <c r="AY97" s="150"/>
+      <c r="AZ97" s="151"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -13606,68 +13606,68 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="167" t="s">
+      <c r="E99" s="199" t="s">
         <v>402</v>
       </c>
-      <c r="F99" s="168"/>
-      <c r="G99" s="168"/>
-      <c r="H99" s="168"/>
-      <c r="I99" s="168"/>
-      <c r="J99" s="168"/>
-      <c r="K99" s="169"/>
-      <c r="L99" s="170" t="s">
+      <c r="F99" s="200"/>
+      <c r="G99" s="200"/>
+      <c r="H99" s="200"/>
+      <c r="I99" s="200"/>
+      <c r="J99" s="200"/>
+      <c r="K99" s="201"/>
+      <c r="L99" s="152" t="s">
         <v>246</v>
       </c>
-      <c r="M99" s="171"/>
-      <c r="N99" s="172"/>
-      <c r="O99" s="164" t="s">
+      <c r="M99" s="153"/>
+      <c r="N99" s="154"/>
+      <c r="O99" s="196" t="s">
         <v>235</v>
       </c>
-      <c r="P99" s="165"/>
-      <c r="Q99" s="165"/>
-      <c r="R99" s="165"/>
-      <c r="S99" s="165"/>
-      <c r="T99" s="166"/>
-      <c r="U99" s="164" t="s">
+      <c r="P99" s="197"/>
+      <c r="Q99" s="197"/>
+      <c r="R99" s="197"/>
+      <c r="S99" s="197"/>
+      <c r="T99" s="198"/>
+      <c r="U99" s="196" t="s">
         <v>235</v>
       </c>
-      <c r="V99" s="165"/>
-      <c r="W99" s="165"/>
-      <c r="X99" s="165"/>
-      <c r="Y99" s="165"/>
-      <c r="Z99" s="165"/>
-      <c r="AA99" s="165"/>
-      <c r="AB99" s="166"/>
-      <c r="AC99" s="164" t="s">
+      <c r="V99" s="197"/>
+      <c r="W99" s="197"/>
+      <c r="X99" s="197"/>
+      <c r="Y99" s="197"/>
+      <c r="Z99" s="197"/>
+      <c r="AA99" s="197"/>
+      <c r="AB99" s="198"/>
+      <c r="AC99" s="196" t="s">
         <v>235</v>
       </c>
-      <c r="AD99" s="165"/>
-      <c r="AE99" s="165"/>
-      <c r="AF99" s="165"/>
-      <c r="AG99" s="165"/>
-      <c r="AH99" s="165"/>
-      <c r="AI99" s="165"/>
-      <c r="AJ99" s="166"/>
-      <c r="AK99" s="164" t="s">
+      <c r="AD99" s="197"/>
+      <c r="AE99" s="197"/>
+      <c r="AF99" s="197"/>
+      <c r="AG99" s="197"/>
+      <c r="AH99" s="197"/>
+      <c r="AI99" s="197"/>
+      <c r="AJ99" s="198"/>
+      <c r="AK99" s="196" t="s">
         <v>235</v>
       </c>
-      <c r="AL99" s="165"/>
-      <c r="AM99" s="165"/>
-      <c r="AN99" s="165"/>
-      <c r="AO99" s="165"/>
-      <c r="AP99" s="165"/>
-      <c r="AQ99" s="165"/>
-      <c r="AR99" s="166"/>
-      <c r="AS99" s="164" t="s">
+      <c r="AL99" s="197"/>
+      <c r="AM99" s="197"/>
+      <c r="AN99" s="197"/>
+      <c r="AO99" s="197"/>
+      <c r="AP99" s="197"/>
+      <c r="AQ99" s="197"/>
+      <c r="AR99" s="198"/>
+      <c r="AS99" s="196" t="s">
         <v>301</v>
       </c>
-      <c r="AT99" s="165"/>
-      <c r="AU99" s="165"/>
-      <c r="AV99" s="165"/>
-      <c r="AW99" s="165"/>
-      <c r="AX99" s="165"/>
-      <c r="AY99" s="165"/>
-      <c r="AZ99" s="166"/>
+      <c r="AT99" s="197"/>
+      <c r="AU99" s="197"/>
+      <c r="AV99" s="197"/>
+      <c r="AW99" s="197"/>
+      <c r="AX99" s="197"/>
+      <c r="AY99" s="197"/>
+      <c r="AZ99" s="198"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -13809,68 +13809,68 @@
         <v>367</v>
       </c>
       <c r="D102" s="42"/>
-      <c r="E102" s="140" t="s">
+      <c r="E102" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="141"/>
-      <c r="G102" s="141"/>
-      <c r="H102" s="141"/>
-      <c r="I102" s="141"/>
-      <c r="J102" s="141"/>
-      <c r="K102" s="142"/>
-      <c r="L102" s="140" t="s">
+      <c r="F102" s="147"/>
+      <c r="G102" s="147"/>
+      <c r="H102" s="147"/>
+      <c r="I102" s="147"/>
+      <c r="J102" s="147"/>
+      <c r="K102" s="167"/>
+      <c r="L102" s="146" t="s">
         <v>223</v>
       </c>
-      <c r="M102" s="141"/>
-      <c r="N102" s="142"/>
-      <c r="O102" s="140" t="s">
+      <c r="M102" s="147"/>
+      <c r="N102" s="167"/>
+      <c r="O102" s="146" t="s">
         <v>232</v>
       </c>
-      <c r="P102" s="141"/>
-      <c r="Q102" s="141"/>
-      <c r="R102" s="142"/>
-      <c r="S102" s="140" t="s">
+      <c r="P102" s="147"/>
+      <c r="Q102" s="147"/>
+      <c r="R102" s="167"/>
+      <c r="S102" s="146" t="s">
         <v>306</v>
       </c>
-      <c r="T102" s="141"/>
-      <c r="U102" s="141"/>
-      <c r="V102" s="141"/>
-      <c r="W102" s="141"/>
-      <c r="X102" s="141"/>
-      <c r="Y102" s="141"/>
-      <c r="Z102" s="141"/>
-      <c r="AA102" s="141"/>
-      <c r="AB102" s="141"/>
-      <c r="AC102" s="141"/>
-      <c r="AD102" s="142"/>
-      <c r="AE102" s="140" t="s">
+      <c r="T102" s="147"/>
+      <c r="U102" s="147"/>
+      <c r="V102" s="147"/>
+      <c r="W102" s="147"/>
+      <c r="X102" s="147"/>
+      <c r="Y102" s="147"/>
+      <c r="Z102" s="147"/>
+      <c r="AA102" s="147"/>
+      <c r="AB102" s="147"/>
+      <c r="AC102" s="147"/>
+      <c r="AD102" s="167"/>
+      <c r="AE102" s="146" t="s">
         <v>307</v>
       </c>
-      <c r="AF102" s="141"/>
-      <c r="AG102" s="141"/>
-      <c r="AH102" s="141"/>
-      <c r="AI102" s="141"/>
-      <c r="AJ102" s="141"/>
-      <c r="AK102" s="141"/>
-      <c r="AL102" s="141"/>
-      <c r="AM102" s="141"/>
-      <c r="AN102" s="141"/>
-      <c r="AO102" s="141"/>
-      <c r="AP102" s="142"/>
-      <c r="AQ102" s="140" t="s">
+      <c r="AF102" s="147"/>
+      <c r="AG102" s="147"/>
+      <c r="AH102" s="147"/>
+      <c r="AI102" s="147"/>
+      <c r="AJ102" s="147"/>
+      <c r="AK102" s="147"/>
+      <c r="AL102" s="147"/>
+      <c r="AM102" s="147"/>
+      <c r="AN102" s="147"/>
+      <c r="AO102" s="147"/>
+      <c r="AP102" s="167"/>
+      <c r="AQ102" s="146" t="s">
         <v>224</v>
       </c>
-      <c r="AR102" s="142"/>
-      <c r="AS102" s="140" t="s">
+      <c r="AR102" s="167"/>
+      <c r="AS102" s="146" t="s">
         <v>234</v>
       </c>
-      <c r="AT102" s="141"/>
-      <c r="AU102" s="141"/>
-      <c r="AV102" s="141"/>
-      <c r="AW102" s="141"/>
-      <c r="AX102" s="141"/>
-      <c r="AY102" s="141"/>
-      <c r="AZ102" s="142"/>
+      <c r="AT102" s="147"/>
+      <c r="AU102" s="147"/>
+      <c r="AV102" s="147"/>
+      <c r="AW102" s="147"/>
+      <c r="AX102" s="147"/>
+      <c r="AY102" s="147"/>
+      <c r="AZ102" s="167"/>
       <c r="BA102" s="42"/>
       <c r="BB102" s="42"/>
       <c r="BC102" s="42"/>
@@ -13973,68 +13973,68 @@
       <c r="B104" s="42"/>
       <c r="C104" s="42"/>
       <c r="D104" s="42"/>
-      <c r="E104" s="200" t="s">
+      <c r="E104" s="149" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="202"/>
-      <c r="G104" s="202"/>
-      <c r="H104" s="202"/>
-      <c r="I104" s="202"/>
-      <c r="J104" s="202"/>
-      <c r="K104" s="201"/>
-      <c r="L104" s="200" t="s">
+      <c r="F104" s="150"/>
+      <c r="G104" s="150"/>
+      <c r="H104" s="150"/>
+      <c r="I104" s="150"/>
+      <c r="J104" s="150"/>
+      <c r="K104" s="151"/>
+      <c r="L104" s="149" t="s">
         <v>226</v>
       </c>
-      <c r="M104" s="202"/>
-      <c r="N104" s="201"/>
-      <c r="O104" s="200" t="s">
+      <c r="M104" s="150"/>
+      <c r="N104" s="151"/>
+      <c r="O104" s="149" t="s">
         <v>227</v>
       </c>
-      <c r="P104" s="202"/>
-      <c r="Q104" s="202"/>
-      <c r="R104" s="201"/>
-      <c r="S104" s="200" t="s">
+      <c r="P104" s="150"/>
+      <c r="Q104" s="150"/>
+      <c r="R104" s="151"/>
+      <c r="S104" s="149" t="s">
         <v>228</v>
       </c>
-      <c r="T104" s="202"/>
-      <c r="U104" s="202"/>
-      <c r="V104" s="202"/>
-      <c r="W104" s="202"/>
-      <c r="X104" s="202"/>
-      <c r="Y104" s="202"/>
-      <c r="Z104" s="202"/>
-      <c r="AA104" s="202"/>
-      <c r="AB104" s="202"/>
-      <c r="AC104" s="202"/>
-      <c r="AD104" s="201"/>
-      <c r="AE104" s="200" t="s">
+      <c r="T104" s="150"/>
+      <c r="U104" s="150"/>
+      <c r="V104" s="150"/>
+      <c r="W104" s="150"/>
+      <c r="X104" s="150"/>
+      <c r="Y104" s="150"/>
+      <c r="Z104" s="150"/>
+      <c r="AA104" s="150"/>
+      <c r="AB104" s="150"/>
+      <c r="AC104" s="150"/>
+      <c r="AD104" s="151"/>
+      <c r="AE104" s="149" t="s">
         <v>228</v>
       </c>
-      <c r="AF104" s="202"/>
-      <c r="AG104" s="202"/>
-      <c r="AH104" s="202"/>
-      <c r="AI104" s="202"/>
-      <c r="AJ104" s="202"/>
-      <c r="AK104" s="202"/>
-      <c r="AL104" s="202"/>
-      <c r="AM104" s="202"/>
-      <c r="AN104" s="202"/>
-      <c r="AO104" s="202"/>
-      <c r="AP104" s="201"/>
-      <c r="AQ104" s="200" t="s">
+      <c r="AF104" s="150"/>
+      <c r="AG104" s="150"/>
+      <c r="AH104" s="150"/>
+      <c r="AI104" s="150"/>
+      <c r="AJ104" s="150"/>
+      <c r="AK104" s="150"/>
+      <c r="AL104" s="150"/>
+      <c r="AM104" s="150"/>
+      <c r="AN104" s="150"/>
+      <c r="AO104" s="150"/>
+      <c r="AP104" s="151"/>
+      <c r="AQ104" s="149" t="s">
         <v>230</v>
       </c>
-      <c r="AR104" s="201"/>
-      <c r="AS104" s="200" t="s">
+      <c r="AR104" s="151"/>
+      <c r="AS104" s="149" t="s">
         <v>229</v>
       </c>
-      <c r="AT104" s="202"/>
-      <c r="AU104" s="202"/>
-      <c r="AV104" s="202"/>
-      <c r="AW104" s="202"/>
-      <c r="AX104" s="202"/>
-      <c r="AY104" s="202"/>
-      <c r="AZ104" s="201"/>
+      <c r="AT104" s="150"/>
+      <c r="AU104" s="150"/>
+      <c r="AV104" s="150"/>
+      <c r="AW104" s="150"/>
+      <c r="AX104" s="150"/>
+      <c r="AY104" s="150"/>
+      <c r="AZ104" s="151"/>
       <c r="BA104" s="42"/>
       <c r="BB104" s="42"/>
       <c r="BC104" s="42"/>
@@ -14120,11 +14120,11 @@
       <c r="I106" s="76"/>
       <c r="J106" s="76"/>
       <c r="K106" s="77"/>
-      <c r="L106" s="170" t="s">
+      <c r="L106" s="152" t="s">
         <v>246</v>
       </c>
-      <c r="M106" s="171"/>
-      <c r="N106" s="172"/>
+      <c r="M106" s="153"/>
+      <c r="N106" s="154"/>
       <c r="O106" s="53"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="50"/>
@@ -14163,16 +14163,16 @@
       <c r="AR106" s="51">
         <v>0</v>
       </c>
-      <c r="AS106" s="136" t="s">
+      <c r="AS106" s="205" t="s">
         <v>231</v>
       </c>
-      <c r="AT106" s="137"/>
-      <c r="AU106" s="137"/>
-      <c r="AV106" s="137"/>
-      <c r="AW106" s="137"/>
-      <c r="AX106" s="137"/>
-      <c r="AY106" s="137"/>
-      <c r="AZ106" s="138"/>
+      <c r="AT106" s="206"/>
+      <c r="AU106" s="206"/>
+      <c r="AV106" s="206"/>
+      <c r="AW106" s="206"/>
+      <c r="AX106" s="206"/>
+      <c r="AY106" s="206"/>
+      <c r="AZ106" s="207"/>
       <c r="BA106" s="50" t="s">
         <v>316</v>
       </c>
@@ -14238,16 +14238,16 @@
       <c r="AR107" s="51">
         <v>1</v>
       </c>
-      <c r="AS107" s="136" t="s">
+      <c r="AS107" s="205" t="s">
         <v>354</v>
       </c>
-      <c r="AT107" s="137"/>
-      <c r="AU107" s="137"/>
-      <c r="AV107" s="137"/>
-      <c r="AW107" s="137"/>
-      <c r="AX107" s="137"/>
-      <c r="AY107" s="137"/>
-      <c r="AZ107" s="138"/>
+      <c r="AT107" s="206"/>
+      <c r="AU107" s="206"/>
+      <c r="AV107" s="206"/>
+      <c r="AW107" s="206"/>
+      <c r="AX107" s="206"/>
+      <c r="AY107" s="206"/>
+      <c r="AZ107" s="207"/>
       <c r="BA107" s="50" t="s">
         <v>298</v>
       </c>
@@ -14315,16 +14315,16 @@
       <c r="AR108" s="51">
         <v>0</v>
       </c>
-      <c r="AS108" s="136" t="s">
+      <c r="AS108" s="205" t="s">
         <v>353</v>
       </c>
-      <c r="AT108" s="137"/>
-      <c r="AU108" s="137"/>
-      <c r="AV108" s="137"/>
-      <c r="AW108" s="137"/>
-      <c r="AX108" s="137"/>
-      <c r="AY108" s="137"/>
-      <c r="AZ108" s="138"/>
+      <c r="AT108" s="206"/>
+      <c r="AU108" s="206"/>
+      <c r="AV108" s="206"/>
+      <c r="AW108" s="206"/>
+      <c r="AX108" s="206"/>
+      <c r="AY108" s="206"/>
+      <c r="AZ108" s="207"/>
       <c r="BA108" s="50" t="s">
         <v>265</v>
       </c>
@@ -14388,16 +14388,16 @@
       <c r="AR109" s="51">
         <v>1</v>
       </c>
-      <c r="AS109" s="136" t="s">
+      <c r="AS109" s="205" t="s">
         <v>233</v>
       </c>
-      <c r="AT109" s="137"/>
-      <c r="AU109" s="137"/>
-      <c r="AV109" s="137"/>
-      <c r="AW109" s="137"/>
-      <c r="AX109" s="137"/>
-      <c r="AY109" s="137"/>
-      <c r="AZ109" s="138"/>
+      <c r="AT109" s="206"/>
+      <c r="AU109" s="206"/>
+      <c r="AV109" s="206"/>
+      <c r="AW109" s="206"/>
+      <c r="AX109" s="206"/>
+      <c r="AY109" s="206"/>
+      <c r="AZ109" s="207"/>
       <c r="BA109" s="50" t="s">
         <v>260</v>
       </c>
@@ -14553,12 +14553,12 @@
       <c r="L112" s="49"/>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
-      <c r="O112" s="161" t="s">
+      <c r="O112" s="193" t="s">
         <v>232</v>
       </c>
-      <c r="P112" s="162"/>
-      <c r="Q112" s="162"/>
-      <c r="R112" s="163"/>
+      <c r="P112" s="194"/>
+      <c r="Q112" s="194"/>
+      <c r="R112" s="195"/>
       <c r="S112" s="50"/>
       <c r="T112" s="50"/>
       <c r="U112" s="50"/>
@@ -14583,20 +14583,20 @@
       <c r="AN112" s="50"/>
       <c r="AO112" s="50"/>
       <c r="AP112" s="50"/>
-      <c r="AQ112" s="156" t="s">
+      <c r="AQ112" s="188" t="s">
         <v>302</v>
       </c>
-      <c r="AR112" s="157"/>
-      <c r="AS112" s="158" t="s">
+      <c r="AR112" s="189"/>
+      <c r="AS112" s="190" t="s">
         <v>299</v>
       </c>
-      <c r="AT112" s="159"/>
-      <c r="AU112" s="159"/>
-      <c r="AV112" s="159"/>
-      <c r="AW112" s="159"/>
-      <c r="AX112" s="159"/>
-      <c r="AY112" s="159"/>
-      <c r="AZ112" s="160"/>
+      <c r="AT112" s="191"/>
+      <c r="AU112" s="191"/>
+      <c r="AV112" s="191"/>
+      <c r="AW112" s="191"/>
+      <c r="AX112" s="191"/>
+      <c r="AY112" s="191"/>
+      <c r="AZ112" s="192"/>
       <c r="BA112" s="42"/>
       <c r="BB112" s="42"/>
       <c r="BC112" s="42"/>
@@ -15797,20 +15797,20 @@
       <c r="AN130" s="42"/>
       <c r="AO130" s="42"/>
       <c r="AP130" s="42"/>
-      <c r="AQ130" s="156" t="s">
+      <c r="AQ130" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="AR130" s="157"/>
-      <c r="AS130" s="158" t="s">
+      <c r="AR130" s="189"/>
+      <c r="AS130" s="190" t="s">
         <v>355</v>
       </c>
-      <c r="AT130" s="159"/>
-      <c r="AU130" s="159"/>
-      <c r="AV130" s="159"/>
-      <c r="AW130" s="159"/>
-      <c r="AX130" s="159"/>
-      <c r="AY130" s="159"/>
-      <c r="AZ130" s="160"/>
+      <c r="AT130" s="191"/>
+      <c r="AU130" s="191"/>
+      <c r="AV130" s="191"/>
+      <c r="AW130" s="191"/>
+      <c r="AX130" s="191"/>
+      <c r="AY130" s="191"/>
+      <c r="AZ130" s="192"/>
       <c r="BA130" s="42"/>
       <c r="BB130" s="42"/>
       <c r="BC130" s="42"/>
@@ -15864,16 +15864,16 @@
       <c r="AP131" s="42"/>
       <c r="AQ131" s="42"/>
       <c r="AR131" s="42"/>
-      <c r="AS131" s="164" t="s">
+      <c r="AS131" s="196" t="s">
         <v>301</v>
       </c>
-      <c r="AT131" s="165"/>
-      <c r="AU131" s="165"/>
-      <c r="AV131" s="165"/>
-      <c r="AW131" s="165"/>
-      <c r="AX131" s="165"/>
-      <c r="AY131" s="165"/>
-      <c r="AZ131" s="166"/>
+      <c r="AT131" s="197"/>
+      <c r="AU131" s="197"/>
+      <c r="AV131" s="197"/>
+      <c r="AW131" s="197"/>
+      <c r="AX131" s="197"/>
+      <c r="AY131" s="197"/>
+      <c r="AZ131" s="198"/>
       <c r="BA131" s="42"/>
       <c r="BB131" s="42"/>
       <c r="BC131" s="42"/>
@@ -15986,20 +15986,20 @@
       <c r="AN133" s="42"/>
       <c r="AO133" s="42"/>
       <c r="AP133" s="42"/>
-      <c r="AQ133" s="156" t="s">
+      <c r="AQ133" s="188" t="s">
         <v>303</v>
       </c>
-      <c r="AR133" s="157"/>
-      <c r="AS133" s="158" t="s">
+      <c r="AR133" s="189"/>
+      <c r="AS133" s="190" t="s">
         <v>305</v>
       </c>
-      <c r="AT133" s="159"/>
-      <c r="AU133" s="159"/>
-      <c r="AV133" s="159"/>
-      <c r="AW133" s="159"/>
-      <c r="AX133" s="159"/>
-      <c r="AY133" s="159"/>
-      <c r="AZ133" s="160"/>
+      <c r="AT133" s="191"/>
+      <c r="AU133" s="191"/>
+      <c r="AV133" s="191"/>
+      <c r="AW133" s="191"/>
+      <c r="AX133" s="191"/>
+      <c r="AY133" s="191"/>
+      <c r="AZ133" s="192"/>
       <c r="BA133" s="42"/>
       <c r="BB133" s="42"/>
       <c r="BC133" s="42"/>
@@ -18622,6 +18622,193 @@
     </row>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="AS109:AZ109"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="S102:AD102"/>
+    <mergeCell ref="AQ102:AR102"/>
+    <mergeCell ref="AS102:AZ102"/>
+    <mergeCell ref="AE102:AP102"/>
+    <mergeCell ref="E102:K102"/>
+    <mergeCell ref="L102:N102"/>
+    <mergeCell ref="O102:R102"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="AS106:AZ106"/>
+    <mergeCell ref="AS107:AZ107"/>
+    <mergeCell ref="AS108:AZ108"/>
+    <mergeCell ref="AV46:AW46"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE30:AF30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="AQ112:AR112"/>
+    <mergeCell ref="AQ130:AR130"/>
+    <mergeCell ref="AQ133:AR133"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="AS112:AZ112"/>
+    <mergeCell ref="O112:R112"/>
+    <mergeCell ref="AS130:AZ130"/>
+    <mergeCell ref="AS131:AZ131"/>
+    <mergeCell ref="AS133:AZ133"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="U99:AB99"/>
+    <mergeCell ref="AC99:AJ99"/>
+    <mergeCell ref="AK99:AR99"/>
+    <mergeCell ref="AS99:AZ99"/>
+    <mergeCell ref="O99:T99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AS95:AZ95"/>
+    <mergeCell ref="AK95:AR95"/>
+    <mergeCell ref="AC95:AJ95"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="AQ104:AR104"/>
+    <mergeCell ref="AS104:AZ104"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="AS97:AZ97"/>
+    <mergeCell ref="AK97:AR97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="O104:R104"/>
+    <mergeCell ref="S104:AD104"/>
+    <mergeCell ref="AE104:AP104"/>
+    <mergeCell ref="AC97:AJ97"/>
+    <mergeCell ref="U97:AB97"/>
+    <mergeCell ref="O97:T97"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="U95:AB95"/>
+    <mergeCell ref="O95:T95"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
     <mergeCell ref="AZ23:BF23"/>
     <mergeCell ref="BB24:BF24"/>
     <mergeCell ref="BD25:BF25"/>
@@ -18646,193 +18833,6 @@
     <mergeCell ref="AT22:AU22"/>
     <mergeCell ref="AV23:AW23"/>
     <mergeCell ref="AX23:AY23"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="U95:AB95"/>
-    <mergeCell ref="O95:T95"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="AQ104:AR104"/>
-    <mergeCell ref="AS104:AZ104"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="AS97:AZ97"/>
-    <mergeCell ref="AK97:AR97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="L104:N104"/>
-    <mergeCell ref="O104:R104"/>
-    <mergeCell ref="S104:AD104"/>
-    <mergeCell ref="AE104:AP104"/>
-    <mergeCell ref="AC97:AJ97"/>
-    <mergeCell ref="U97:AB97"/>
-    <mergeCell ref="O97:T97"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AQ112:AR112"/>
-    <mergeCell ref="AQ130:AR130"/>
-    <mergeCell ref="AQ133:AR133"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="AS112:AZ112"/>
-    <mergeCell ref="O112:R112"/>
-    <mergeCell ref="AS130:AZ130"/>
-    <mergeCell ref="AS131:AZ131"/>
-    <mergeCell ref="AS133:AZ133"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="U99:AB99"/>
-    <mergeCell ref="AC99:AJ99"/>
-    <mergeCell ref="AK99:AR99"/>
-    <mergeCell ref="AS99:AZ99"/>
-    <mergeCell ref="O99:T99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AS95:AZ95"/>
-    <mergeCell ref="AK95:AR95"/>
-    <mergeCell ref="AC95:AJ95"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="AS109:AZ109"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="S102:AD102"/>
-    <mergeCell ref="AQ102:AR102"/>
-    <mergeCell ref="AS102:AZ102"/>
-    <mergeCell ref="AE102:AP102"/>
-    <mergeCell ref="E102:K102"/>
-    <mergeCell ref="L102:N102"/>
-    <mergeCell ref="O102:R102"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="AS106:AZ106"/>
-    <mergeCell ref="AS107:AZ107"/>
-    <mergeCell ref="AS108:AZ108"/>
-    <mergeCell ref="AV46:AW46"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[Slot Doc] Correction for TX/RX_ERR and RSSI/LQI
</commit_message>
<xml_diff>
--- a/Doc/Slot_EFR32x (version 1).xlsx
+++ b/Doc/Slot_EFR32x (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SiLabs\Eval\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0B4AB7-A28D-410D-B440-369330BE4ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A7569C-917B-46C8-9FC2-E92B65336CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{FAB646C4-5574-4E39-84B4-67E265388564}"/>
   </bookViews>
@@ -1923,28 +1923,28 @@
     <t>RSSI / LQI</t>
   </si>
   <si>
-    <t>RSSI (MSB) &amp; LQI (LSB) / Non signed 8 bits (0-255/0xFF)</t>
-  </si>
-  <si>
-    <t>RSSI: 1 bit = 0.1 dBm / Offset = xx / [-xx… 20 dBm ] / OOR = [0xFFF]</t>
-  </si>
-  <si>
-    <t>LQI: 1 bit = N/A / Offset = 0 / [0… 255] / OOR = N/A</t>
-  </si>
-  <si>
     <t>CH=0x07</t>
   </si>
   <si>
     <t>TX_ERR / RX_ERR</t>
   </si>
   <si>
-    <t>TX_ERR rate (MSB) &amp; RX_ERR rate (LSB) / Non signed 8 bits (0-255/0xFF)</t>
-  </si>
-  <si>
-    <t>TX_ERR: 1 bit = 0.5% / Offset = 0% / [0 … 100%] / OOR = N/A</t>
-  </si>
-  <si>
-    <t>RX_ERR: 1 bit = 0.5% / Offset = 0% / [0 … 100%] / OOR = N/A</t>
+    <t>RSSI: 1 bit = 0.4 dBm / Offset = xx / [-xx… 20 dBm ] / OOR = N/A</t>
+  </si>
+  <si>
+    <t>TX_ERR rate (MSB) &amp; RX_ERR rate (LSB) / Non signed 6 bits (0-64/0x3F)</t>
+  </si>
+  <si>
+    <t>RSSI (MSB) &amp; LQI (LSB) / Non signed 6 bits (0-63/0x3F)</t>
+  </si>
+  <si>
+    <t>LQI: 1 bit = N/A / Offset = 0 / [0… 63] / OOR = N/A</t>
+  </si>
+  <si>
+    <t>TX_ERR: 1 bit = 0.01% / Offset = 0% / [0 … 0.62%] / OOR = [0x3F]</t>
+  </si>
+  <si>
+    <t>RX_ERR: 1 bit = 0.01% / Offset = 0% / [0 … 0.62%] / OOR = [0x3F]</t>
   </si>
 </sst>
 </file>
@@ -3029,35 +3029,42 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3065,7 +3072,16 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3077,19 +3093,49 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3101,31 +3147,55 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3146,108 +3216,38 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14375,8 +14375,8 @@
   </sheetPr>
   <dimension ref="A1:BG205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="AO168" sqref="AO168"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="AO162" sqref="AO162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14515,21 +14515,21 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="209"/>
-      <c r="G3" s="209"/>
-      <c r="H3" s="209"/>
-      <c r="I3" s="209"/>
-      <c r="J3" s="209"/>
-      <c r="K3" s="209"/>
-      <c r="L3" s="209"/>
-      <c r="M3" s="209"/>
-      <c r="N3" s="209"/>
-      <c r="O3" s="209"/>
-      <c r="P3" s="209"/>
-      <c r="Q3" s="209"/>
-      <c r="R3" s="209"/>
-      <c r="S3" s="209"/>
+      <c r="E3" s="185"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="185"/>
+      <c r="L3" s="185"/>
+      <c r="M3" s="185"/>
+      <c r="N3" s="185"/>
+      <c r="O3" s="185"/>
+      <c r="P3" s="185"/>
+      <c r="Q3" s="185"/>
+      <c r="R3" s="185"/>
+      <c r="S3" s="185"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -14637,45 +14637,45 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="174" t="s">
+      <c r="E5" s="223" t="s">
         <v>323</v>
       </c>
-      <c r="F5" s="175"/>
-      <c r="G5" s="175"/>
-      <c r="H5" s="175"/>
-      <c r="I5" s="175"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="178" t="s">
+      <c r="F5" s="224"/>
+      <c r="G5" s="224"/>
+      <c r="H5" s="224"/>
+      <c r="I5" s="224"/>
+      <c r="J5" s="225"/>
+      <c r="K5" s="214" t="s">
         <v>261</v>
       </c>
-      <c r="L5" s="181"/>
-      <c r="M5" s="181"/>
-      <c r="N5" s="181"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="178" t="s">
+      <c r="L5" s="228"/>
+      <c r="M5" s="228"/>
+      <c r="N5" s="228"/>
+      <c r="O5" s="215"/>
+      <c r="P5" s="214" t="s">
         <v>268</v>
       </c>
-      <c r="Q5" s="179"/>
-      <c r="R5" s="182" t="s">
+      <c r="Q5" s="215"/>
+      <c r="R5" s="216" t="s">
         <v>262</v>
       </c>
-      <c r="S5" s="183"/>
-      <c r="T5" s="183"/>
-      <c r="U5" s="183"/>
-      <c r="V5" s="183"/>
-      <c r="W5" s="184"/>
-      <c r="X5" s="178" t="s">
+      <c r="S5" s="217"/>
+      <c r="T5" s="217"/>
+      <c r="U5" s="217"/>
+      <c r="V5" s="217"/>
+      <c r="W5" s="218"/>
+      <c r="X5" s="214" t="s">
         <v>263</v>
       </c>
-      <c r="Y5" s="179"/>
-      <c r="Z5" s="174" t="s">
+      <c r="Y5" s="215"/>
+      <c r="Z5" s="223" t="s">
         <v>322</v>
       </c>
-      <c r="AA5" s="175"/>
-      <c r="AB5" s="175"/>
-      <c r="AC5" s="175"/>
-      <c r="AD5" s="175"/>
-      <c r="AE5" s="176"/>
+      <c r="AA5" s="224"/>
+      <c r="AB5" s="224"/>
+      <c r="AC5" s="224"/>
+      <c r="AD5" s="224"/>
+      <c r="AE5" s="225"/>
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="18"/>
@@ -14710,45 +14710,45 @@
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="158" t="s">
+      <c r="E6" s="227" t="s">
         <v>375</v>
       </c>
-      <c r="F6" s="158"/>
-      <c r="G6" s="158"/>
-      <c r="H6" s="158"/>
-      <c r="I6" s="158"/>
-      <c r="J6" s="158"/>
-      <c r="K6" s="168" t="s">
+      <c r="F6" s="227"/>
+      <c r="G6" s="227"/>
+      <c r="H6" s="227"/>
+      <c r="I6" s="227"/>
+      <c r="J6" s="227"/>
+      <c r="K6" s="226" t="s">
         <v>319</v>
       </c>
-      <c r="L6" s="168"/>
-      <c r="M6" s="168"/>
-      <c r="N6" s="168"/>
-      <c r="O6" s="168"/>
-      <c r="P6" s="168" t="s">
+      <c r="L6" s="226"/>
+      <c r="M6" s="226"/>
+      <c r="N6" s="226"/>
+      <c r="O6" s="226"/>
+      <c r="P6" s="226" t="s">
         <v>321</v>
       </c>
-      <c r="Q6" s="168"/>
-      <c r="R6" s="158" t="s">
+      <c r="Q6" s="226"/>
+      <c r="R6" s="227" t="s">
         <v>264</v>
       </c>
-      <c r="S6" s="158"/>
-      <c r="T6" s="158"/>
-      <c r="U6" s="158"/>
-      <c r="V6" s="158"/>
-      <c r="W6" s="158"/>
-      <c r="X6" s="158" t="s">
+      <c r="S6" s="227"/>
+      <c r="T6" s="227"/>
+      <c r="U6" s="227"/>
+      <c r="V6" s="227"/>
+      <c r="W6" s="227"/>
+      <c r="X6" s="227" t="s">
         <v>321</v>
       </c>
-      <c r="Y6" s="158"/>
-      <c r="Z6" s="158" t="s">
+      <c r="Y6" s="227"/>
+      <c r="Z6" s="227" t="s">
         <v>375</v>
       </c>
-      <c r="AA6" s="158"/>
-      <c r="AB6" s="158"/>
-      <c r="AC6" s="158"/>
-      <c r="AD6" s="158"/>
-      <c r="AE6" s="158"/>
+      <c r="AA6" s="227"/>
+      <c r="AB6" s="227"/>
+      <c r="AC6" s="227"/>
+      <c r="AD6" s="227"/>
+      <c r="AE6" s="227"/>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -14789,29 +14789,29 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="180" t="s">
+      <c r="K7" s="222" t="s">
         <v>320</v>
       </c>
-      <c r="L7" s="180"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="180"/>
-      <c r="P7" s="180" t="s">
+      <c r="L7" s="222"/>
+      <c r="M7" s="222"/>
+      <c r="N7" s="222"/>
+      <c r="O7" s="222"/>
+      <c r="P7" s="222" t="s">
         <v>320</v>
       </c>
-      <c r="Q7" s="180"/>
-      <c r="R7" s="180" t="s">
+      <c r="Q7" s="222"/>
+      <c r="R7" s="222" t="s">
         <v>270</v>
       </c>
-      <c r="S7" s="180"/>
-      <c r="T7" s="180"/>
-      <c r="U7" s="180"/>
-      <c r="V7" s="180"/>
-      <c r="W7" s="180"/>
-      <c r="X7" s="180" t="s">
+      <c r="S7" s="222"/>
+      <c r="T7" s="222"/>
+      <c r="U7" s="222"/>
+      <c r="V7" s="222"/>
+      <c r="W7" s="222"/>
+      <c r="X7" s="222" t="s">
         <v>320</v>
       </c>
-      <c r="Y7" s="180"/>
+      <c r="Y7" s="222"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
@@ -15244,10 +15244,10 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="156" t="s">
+      <c r="E14" s="186" t="s">
         <v>265</v>
       </c>
-      <c r="F14" s="210"/>
+      <c r="F14" s="187"/>
       <c r="G14" s="97"/>
       <c r="H14" s="97"/>
       <c r="I14" s="97"/>
@@ -15272,10 +15272,10 @@
       <c r="AB14" s="101"/>
       <c r="AC14" s="101"/>
       <c r="AD14" s="101"/>
-      <c r="AE14" s="156" t="s">
+      <c r="AE14" s="186" t="s">
         <v>265</v>
       </c>
-      <c r="AF14" s="210"/>
+      <c r="AF14" s="187"/>
       <c r="AG14" s="97"/>
       <c r="AH14" s="97"/>
       <c r="AI14" s="97"/>
@@ -15318,67 +15318,67 @@
       <c r="G15" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="H15" s="154" t="s">
+      <c r="H15" s="188" t="s">
         <v>271</v>
       </c>
-      <c r="I15" s="155"/>
-      <c r="J15" s="152" t="s">
+      <c r="I15" s="189"/>
+      <c r="J15" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="K15" s="153"/>
-      <c r="L15" s="149"/>
-      <c r="M15" s="150"/>
-      <c r="N15" s="150"/>
-      <c r="O15" s="150"/>
-      <c r="P15" s="150"/>
-      <c r="Q15" s="150"/>
-      <c r="R15" s="150"/>
-      <c r="S15" s="150"/>
-      <c r="T15" s="150"/>
-      <c r="U15" s="150"/>
-      <c r="V15" s="150"/>
-      <c r="W15" s="150"/>
-      <c r="X15" s="150"/>
-      <c r="Y15" s="150"/>
-      <c r="Z15" s="150"/>
-      <c r="AA15" s="150"/>
-      <c r="AB15" s="150"/>
-      <c r="AC15" s="150"/>
-      <c r="AD15" s="150"/>
-      <c r="AE15" s="150"/>
-      <c r="AF15" s="151"/>
+      <c r="K15" s="191"/>
+      <c r="L15" s="229"/>
+      <c r="M15" s="230"/>
+      <c r="N15" s="230"/>
+      <c r="O15" s="230"/>
+      <c r="P15" s="230"/>
+      <c r="Q15" s="230"/>
+      <c r="R15" s="230"/>
+      <c r="S15" s="230"/>
+      <c r="T15" s="230"/>
+      <c r="U15" s="230"/>
+      <c r="V15" s="230"/>
+      <c r="W15" s="230"/>
+      <c r="X15" s="230"/>
+      <c r="Y15" s="230"/>
+      <c r="Z15" s="230"/>
+      <c r="AA15" s="230"/>
+      <c r="AB15" s="230"/>
+      <c r="AC15" s="230"/>
+      <c r="AD15" s="230"/>
+      <c r="AE15" s="230"/>
+      <c r="AF15" s="231"/>
       <c r="AG15" s="99" t="s">
         <v>266</v>
       </c>
-      <c r="AH15" s="154" t="s">
+      <c r="AH15" s="188" t="s">
         <v>271</v>
       </c>
-      <c r="AI15" s="155"/>
-      <c r="AJ15" s="152" t="s">
+      <c r="AI15" s="189"/>
+      <c r="AJ15" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AK15" s="153"/>
-      <c r="AL15" s="149"/>
-      <c r="AM15" s="150"/>
-      <c r="AN15" s="150"/>
-      <c r="AO15" s="150"/>
-      <c r="AP15" s="150"/>
-      <c r="AQ15" s="150"/>
-      <c r="AR15" s="150"/>
-      <c r="AS15" s="150"/>
-      <c r="AT15" s="150"/>
-      <c r="AU15" s="150"/>
-      <c r="AV15" s="150"/>
-      <c r="AW15" s="150"/>
-      <c r="AX15" s="150"/>
-      <c r="AY15" s="150"/>
-      <c r="AZ15" s="150"/>
-      <c r="BA15" s="150"/>
-      <c r="BB15" s="150"/>
-      <c r="BC15" s="150"/>
-      <c r="BD15" s="150"/>
-      <c r="BE15" s="150"/>
-      <c r="BF15" s="150"/>
+      <c r="AK15" s="191"/>
+      <c r="AL15" s="229"/>
+      <c r="AM15" s="230"/>
+      <c r="AN15" s="230"/>
+      <c r="AO15" s="230"/>
+      <c r="AP15" s="230"/>
+      <c r="AQ15" s="230"/>
+      <c r="AR15" s="230"/>
+      <c r="AS15" s="230"/>
+      <c r="AT15" s="230"/>
+      <c r="AU15" s="230"/>
+      <c r="AV15" s="230"/>
+      <c r="AW15" s="230"/>
+      <c r="AX15" s="230"/>
+      <c r="AY15" s="230"/>
+      <c r="AZ15" s="230"/>
+      <c r="BA15" s="230"/>
+      <c r="BB15" s="230"/>
+      <c r="BC15" s="230"/>
+      <c r="BD15" s="230"/>
+      <c r="BE15" s="230"/>
+      <c r="BF15" s="230"/>
       <c r="BG15" s="96"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
@@ -15399,33 +15399,33 @@
         <v>279</v>
       </c>
       <c r="I16" s="103"/>
-      <c r="J16" s="154" t="s">
+      <c r="J16" s="188" t="s">
         <v>272</v>
       </c>
-      <c r="K16" s="155"/>
-      <c r="L16" s="152" t="s">
+      <c r="K16" s="189"/>
+      <c r="L16" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="M16" s="153"/>
-      <c r="N16" s="149"/>
-      <c r="O16" s="150"/>
-      <c r="P16" s="150"/>
-      <c r="Q16" s="150"/>
-      <c r="R16" s="150"/>
-      <c r="S16" s="150"/>
-      <c r="T16" s="150"/>
-      <c r="U16" s="150"/>
-      <c r="V16" s="150"/>
-      <c r="W16" s="150"/>
-      <c r="X16" s="150"/>
-      <c r="Y16" s="150"/>
-      <c r="Z16" s="150"/>
-      <c r="AA16" s="150"/>
-      <c r="AB16" s="150"/>
-      <c r="AC16" s="150"/>
-      <c r="AD16" s="150"/>
-      <c r="AE16" s="150"/>
-      <c r="AF16" s="151"/>
+      <c r="M16" s="191"/>
+      <c r="N16" s="229"/>
+      <c r="O16" s="230"/>
+      <c r="P16" s="230"/>
+      <c r="Q16" s="230"/>
+      <c r="R16" s="230"/>
+      <c r="S16" s="230"/>
+      <c r="T16" s="230"/>
+      <c r="U16" s="230"/>
+      <c r="V16" s="230"/>
+      <c r="W16" s="230"/>
+      <c r="X16" s="230"/>
+      <c r="Y16" s="230"/>
+      <c r="Z16" s="230"/>
+      <c r="AA16" s="230"/>
+      <c r="AB16" s="230"/>
+      <c r="AC16" s="230"/>
+      <c r="AD16" s="230"/>
+      <c r="AE16" s="230"/>
+      <c r="AF16" s="231"/>
       <c r="AG16" s="99" t="s">
         <v>266</v>
       </c>
@@ -15433,33 +15433,33 @@
         <v>279</v>
       </c>
       <c r="AI16" s="103"/>
-      <c r="AJ16" s="154" t="s">
+      <c r="AJ16" s="188" t="s">
         <v>272</v>
       </c>
-      <c r="AK16" s="155"/>
-      <c r="AL16" s="152" t="s">
+      <c r="AK16" s="189"/>
+      <c r="AL16" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AM16" s="153"/>
-      <c r="AN16" s="149"/>
-      <c r="AO16" s="150"/>
-      <c r="AP16" s="150"/>
-      <c r="AQ16" s="150"/>
-      <c r="AR16" s="150"/>
-      <c r="AS16" s="150"/>
-      <c r="AT16" s="150"/>
-      <c r="AU16" s="150"/>
-      <c r="AV16" s="150"/>
-      <c r="AW16" s="150"/>
-      <c r="AX16" s="150"/>
-      <c r="AY16" s="150"/>
-      <c r="AZ16" s="150"/>
-      <c r="BA16" s="150"/>
-      <c r="BB16" s="150"/>
-      <c r="BC16" s="150"/>
-      <c r="BD16" s="150"/>
-      <c r="BE16" s="150"/>
-      <c r="BF16" s="150"/>
+      <c r="AM16" s="191"/>
+      <c r="AN16" s="229"/>
+      <c r="AO16" s="230"/>
+      <c r="AP16" s="230"/>
+      <c r="AQ16" s="230"/>
+      <c r="AR16" s="230"/>
+      <c r="AS16" s="230"/>
+      <c r="AT16" s="230"/>
+      <c r="AU16" s="230"/>
+      <c r="AV16" s="230"/>
+      <c r="AW16" s="230"/>
+      <c r="AX16" s="230"/>
+      <c r="AY16" s="230"/>
+      <c r="AZ16" s="230"/>
+      <c r="BA16" s="230"/>
+      <c r="BB16" s="230"/>
+      <c r="BC16" s="230"/>
+      <c r="BD16" s="230"/>
+      <c r="BE16" s="230"/>
+      <c r="BF16" s="230"/>
       <c r="BG16" s="96"/>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
@@ -15482,31 +15482,31 @@
       <c r="I17" s="104"/>
       <c r="J17" s="104"/>
       <c r="K17" s="103"/>
-      <c r="L17" s="154" t="s">
+      <c r="L17" s="188" t="s">
         <v>273</v>
       </c>
-      <c r="M17" s="155"/>
-      <c r="N17" s="152" t="s">
+      <c r="M17" s="189"/>
+      <c r="N17" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="O17" s="153"/>
-      <c r="P17" s="149"/>
-      <c r="Q17" s="150"/>
-      <c r="R17" s="150"/>
-      <c r="S17" s="150"/>
-      <c r="T17" s="150"/>
-      <c r="U17" s="150"/>
-      <c r="V17" s="150"/>
-      <c r="W17" s="150"/>
-      <c r="X17" s="150"/>
-      <c r="Y17" s="150"/>
-      <c r="Z17" s="150"/>
-      <c r="AA17" s="150"/>
-      <c r="AB17" s="150"/>
-      <c r="AC17" s="150"/>
-      <c r="AD17" s="150"/>
-      <c r="AE17" s="150"/>
-      <c r="AF17" s="151"/>
+      <c r="O17" s="191"/>
+      <c r="P17" s="229"/>
+      <c r="Q17" s="230"/>
+      <c r="R17" s="230"/>
+      <c r="S17" s="230"/>
+      <c r="T17" s="230"/>
+      <c r="U17" s="230"/>
+      <c r="V17" s="230"/>
+      <c r="W17" s="230"/>
+      <c r="X17" s="230"/>
+      <c r="Y17" s="230"/>
+      <c r="Z17" s="230"/>
+      <c r="AA17" s="230"/>
+      <c r="AB17" s="230"/>
+      <c r="AC17" s="230"/>
+      <c r="AD17" s="230"/>
+      <c r="AE17" s="230"/>
+      <c r="AF17" s="231"/>
       <c r="AG17" s="99" t="s">
         <v>266</v>
       </c>
@@ -15516,31 +15516,31 @@
       <c r="AI17" s="104"/>
       <c r="AJ17" s="104"/>
       <c r="AK17" s="103"/>
-      <c r="AL17" s="154" t="s">
+      <c r="AL17" s="188" t="s">
         <v>273</v>
       </c>
-      <c r="AM17" s="155"/>
-      <c r="AN17" s="152" t="s">
+      <c r="AM17" s="189"/>
+      <c r="AN17" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AO17" s="153"/>
-      <c r="AP17" s="149"/>
-      <c r="AQ17" s="150"/>
-      <c r="AR17" s="150"/>
-      <c r="AS17" s="150"/>
-      <c r="AT17" s="150"/>
-      <c r="AU17" s="150"/>
-      <c r="AV17" s="150"/>
-      <c r="AW17" s="150"/>
-      <c r="AX17" s="150"/>
-      <c r="AY17" s="150"/>
-      <c r="AZ17" s="150"/>
-      <c r="BA17" s="150"/>
-      <c r="BB17" s="150"/>
-      <c r="BC17" s="150"/>
-      <c r="BD17" s="150"/>
-      <c r="BE17" s="150"/>
-      <c r="BF17" s="150"/>
+      <c r="AO17" s="191"/>
+      <c r="AP17" s="229"/>
+      <c r="AQ17" s="230"/>
+      <c r="AR17" s="230"/>
+      <c r="AS17" s="230"/>
+      <c r="AT17" s="230"/>
+      <c r="AU17" s="230"/>
+      <c r="AV17" s="230"/>
+      <c r="AW17" s="230"/>
+      <c r="AX17" s="230"/>
+      <c r="AY17" s="230"/>
+      <c r="AZ17" s="230"/>
+      <c r="BA17" s="230"/>
+      <c r="BB17" s="230"/>
+      <c r="BC17" s="230"/>
+      <c r="BD17" s="230"/>
+      <c r="BE17" s="230"/>
+      <c r="BF17" s="230"/>
       <c r="BG17" s="96"/>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
@@ -15565,27 +15565,27 @@
       <c r="K18" s="104"/>
       <c r="L18" s="104"/>
       <c r="M18" s="103"/>
-      <c r="N18" s="156" t="s">
+      <c r="N18" s="186" t="s">
         <v>274</v>
       </c>
-      <c r="O18" s="157"/>
-      <c r="P18" s="149"/>
-      <c r="Q18" s="150"/>
-      <c r="R18" s="150"/>
-      <c r="S18" s="150"/>
-      <c r="T18" s="150"/>
-      <c r="U18" s="150"/>
-      <c r="V18" s="150"/>
-      <c r="W18" s="150"/>
-      <c r="X18" s="150"/>
-      <c r="Y18" s="150"/>
-      <c r="Z18" s="150"/>
-      <c r="AA18" s="150"/>
-      <c r="AB18" s="150"/>
-      <c r="AC18" s="150"/>
-      <c r="AD18" s="150"/>
-      <c r="AE18" s="150"/>
-      <c r="AF18" s="151"/>
+      <c r="O18" s="195"/>
+      <c r="P18" s="229"/>
+      <c r="Q18" s="230"/>
+      <c r="R18" s="230"/>
+      <c r="S18" s="230"/>
+      <c r="T18" s="230"/>
+      <c r="U18" s="230"/>
+      <c r="V18" s="230"/>
+      <c r="W18" s="230"/>
+      <c r="X18" s="230"/>
+      <c r="Y18" s="230"/>
+      <c r="Z18" s="230"/>
+      <c r="AA18" s="230"/>
+      <c r="AB18" s="230"/>
+      <c r="AC18" s="230"/>
+      <c r="AD18" s="230"/>
+      <c r="AE18" s="230"/>
+      <c r="AF18" s="231"/>
       <c r="AG18" s="99" t="s">
         <v>266</v>
       </c>
@@ -15597,27 +15597,27 @@
       <c r="AK18" s="104"/>
       <c r="AL18" s="104"/>
       <c r="AM18" s="103"/>
-      <c r="AN18" s="156" t="s">
+      <c r="AN18" s="186" t="s">
         <v>274</v>
       </c>
-      <c r="AO18" s="157"/>
-      <c r="AP18" s="149"/>
-      <c r="AQ18" s="150"/>
-      <c r="AR18" s="150"/>
-      <c r="AS18" s="150"/>
-      <c r="AT18" s="150"/>
-      <c r="AU18" s="150"/>
-      <c r="AV18" s="150"/>
-      <c r="AW18" s="150"/>
-      <c r="AX18" s="150"/>
-      <c r="AY18" s="150"/>
-      <c r="AZ18" s="150"/>
-      <c r="BA18" s="150"/>
-      <c r="BB18" s="150"/>
-      <c r="BC18" s="150"/>
-      <c r="BD18" s="150"/>
-      <c r="BE18" s="150"/>
-      <c r="BF18" s="150"/>
+      <c r="AO18" s="195"/>
+      <c r="AP18" s="229"/>
+      <c r="AQ18" s="230"/>
+      <c r="AR18" s="230"/>
+      <c r="AS18" s="230"/>
+      <c r="AT18" s="230"/>
+      <c r="AU18" s="230"/>
+      <c r="AV18" s="230"/>
+      <c r="AW18" s="230"/>
+      <c r="AX18" s="230"/>
+      <c r="AY18" s="230"/>
+      <c r="AZ18" s="230"/>
+      <c r="BA18" s="230"/>
+      <c r="BB18" s="230"/>
+      <c r="BC18" s="230"/>
+      <c r="BD18" s="230"/>
+      <c r="BE18" s="230"/>
+      <c r="BF18" s="230"/>
       <c r="BG18" s="96"/>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
@@ -15843,23 +15843,23 @@
       <c r="Q22" s="104"/>
       <c r="R22" s="104"/>
       <c r="S22" s="103"/>
-      <c r="T22" s="154" t="s">
+      <c r="T22" s="188" t="s">
         <v>275</v>
       </c>
-      <c r="U22" s="155"/>
-      <c r="V22" s="152" t="s">
+      <c r="U22" s="189"/>
+      <c r="V22" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="W22" s="153"/>
-      <c r="X22" s="149"/>
-      <c r="Y22" s="150"/>
-      <c r="Z22" s="150"/>
-      <c r="AA22" s="150"/>
-      <c r="AB22" s="150"/>
-      <c r="AC22" s="150"/>
-      <c r="AD22" s="150"/>
-      <c r="AE22" s="150"/>
-      <c r="AF22" s="151"/>
+      <c r="W22" s="191"/>
+      <c r="X22" s="229"/>
+      <c r="Y22" s="230"/>
+      <c r="Z22" s="230"/>
+      <c r="AA22" s="230"/>
+      <c r="AB22" s="230"/>
+      <c r="AC22" s="230"/>
+      <c r="AD22" s="230"/>
+      <c r="AE22" s="230"/>
+      <c r="AF22" s="231"/>
       <c r="AG22" s="99" t="s">
         <v>266</v>
       </c>
@@ -15877,23 +15877,23 @@
       <c r="AQ22" s="104"/>
       <c r="AR22" s="104"/>
       <c r="AS22" s="103"/>
-      <c r="AT22" s="154" t="s">
+      <c r="AT22" s="188" t="s">
         <v>275</v>
       </c>
-      <c r="AU22" s="155"/>
-      <c r="AV22" s="152" t="s">
+      <c r="AU22" s="189"/>
+      <c r="AV22" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AW22" s="153"/>
-      <c r="AX22" s="149"/>
-      <c r="AY22" s="150"/>
-      <c r="AZ22" s="150"/>
-      <c r="BA22" s="150"/>
-      <c r="BB22" s="150"/>
-      <c r="BC22" s="150"/>
-      <c r="BD22" s="150"/>
-      <c r="BE22" s="150"/>
-      <c r="BF22" s="150"/>
+      <c r="AW22" s="191"/>
+      <c r="AX22" s="229"/>
+      <c r="AY22" s="230"/>
+      <c r="AZ22" s="230"/>
+      <c r="BA22" s="230"/>
+      <c r="BB22" s="230"/>
+      <c r="BC22" s="230"/>
+      <c r="BD22" s="230"/>
+      <c r="BE22" s="230"/>
+      <c r="BF22" s="230"/>
       <c r="BG22" s="96"/>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -15926,21 +15926,21 @@
       <c r="S23" s="104"/>
       <c r="T23" s="104"/>
       <c r="U23" s="103"/>
-      <c r="V23" s="154" t="s">
+      <c r="V23" s="188" t="s">
         <v>276</v>
       </c>
-      <c r="W23" s="155"/>
-      <c r="X23" s="152" t="s">
+      <c r="W23" s="189"/>
+      <c r="X23" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="Y23" s="153"/>
-      <c r="Z23" s="149"/>
-      <c r="AA23" s="150"/>
-      <c r="AB23" s="150"/>
-      <c r="AC23" s="150"/>
-      <c r="AD23" s="150"/>
-      <c r="AE23" s="150"/>
-      <c r="AF23" s="151"/>
+      <c r="Y23" s="191"/>
+      <c r="Z23" s="229"/>
+      <c r="AA23" s="230"/>
+      <c r="AB23" s="230"/>
+      <c r="AC23" s="230"/>
+      <c r="AD23" s="230"/>
+      <c r="AE23" s="230"/>
+      <c r="AF23" s="231"/>
       <c r="AG23" s="99" t="s">
         <v>266</v>
       </c>
@@ -15960,21 +15960,21 @@
       <c r="AS23" s="104"/>
       <c r="AT23" s="104"/>
       <c r="AU23" s="103"/>
-      <c r="AV23" s="154" t="s">
+      <c r="AV23" s="188" t="s">
         <v>276</v>
       </c>
-      <c r="AW23" s="155"/>
-      <c r="AX23" s="152" t="s">
+      <c r="AW23" s="189"/>
+      <c r="AX23" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AY23" s="153"/>
-      <c r="AZ23" s="149"/>
-      <c r="BA23" s="150"/>
-      <c r="BB23" s="150"/>
-      <c r="BC23" s="150"/>
-      <c r="BD23" s="150"/>
-      <c r="BE23" s="150"/>
-      <c r="BF23" s="150"/>
+      <c r="AY23" s="191"/>
+      <c r="AZ23" s="229"/>
+      <c r="BA23" s="230"/>
+      <c r="BB23" s="230"/>
+      <c r="BC23" s="230"/>
+      <c r="BD23" s="230"/>
+      <c r="BE23" s="230"/>
+      <c r="BF23" s="230"/>
       <c r="BG23" s="96"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -16009,19 +16009,19 @@
       <c r="U24" s="104"/>
       <c r="V24" s="104"/>
       <c r="W24" s="103"/>
-      <c r="X24" s="154" t="s">
+      <c r="X24" s="188" t="s">
         <v>277</v>
       </c>
-      <c r="Y24" s="155"/>
-      <c r="Z24" s="152" t="s">
+      <c r="Y24" s="189"/>
+      <c r="Z24" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AA24" s="153"/>
-      <c r="AB24" s="149"/>
-      <c r="AC24" s="150"/>
-      <c r="AD24" s="150"/>
-      <c r="AE24" s="150"/>
-      <c r="AF24" s="151"/>
+      <c r="AA24" s="191"/>
+      <c r="AB24" s="229"/>
+      <c r="AC24" s="230"/>
+      <c r="AD24" s="230"/>
+      <c r="AE24" s="230"/>
+      <c r="AF24" s="231"/>
       <c r="AG24" s="99" t="s">
         <v>266</v>
       </c>
@@ -16043,19 +16043,19 @@
       <c r="AU24" s="104"/>
       <c r="AV24" s="104"/>
       <c r="AW24" s="103"/>
-      <c r="AX24" s="154" t="s">
+      <c r="AX24" s="188" t="s">
         <v>277</v>
       </c>
-      <c r="AY24" s="155"/>
-      <c r="AZ24" s="152" t="s">
+      <c r="AY24" s="189"/>
+      <c r="AZ24" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="BA24" s="153"/>
-      <c r="BB24" s="149"/>
-      <c r="BC24" s="150"/>
-      <c r="BD24" s="150"/>
-      <c r="BE24" s="150"/>
-      <c r="BF24" s="150"/>
+      <c r="BA24" s="191"/>
+      <c r="BB24" s="229"/>
+      <c r="BC24" s="230"/>
+      <c r="BD24" s="230"/>
+      <c r="BE24" s="230"/>
+      <c r="BF24" s="230"/>
       <c r="BG24" s="96"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -16092,17 +16092,17 @@
       <c r="W25" s="104"/>
       <c r="X25" s="104"/>
       <c r="Y25" s="103"/>
-      <c r="Z25" s="156" t="s">
+      <c r="Z25" s="186" t="s">
         <v>278</v>
       </c>
-      <c r="AA25" s="157"/>
-      <c r="AB25" s="152" t="s">
+      <c r="AA25" s="195"/>
+      <c r="AB25" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AC25" s="153"/>
-      <c r="AD25" s="149"/>
-      <c r="AE25" s="150"/>
-      <c r="AF25" s="151"/>
+      <c r="AC25" s="191"/>
+      <c r="AD25" s="229"/>
+      <c r="AE25" s="230"/>
+      <c r="AF25" s="231"/>
       <c r="AG25" s="99" t="s">
         <v>266</v>
       </c>
@@ -16126,17 +16126,17 @@
       <c r="AW25" s="104"/>
       <c r="AX25" s="104"/>
       <c r="AY25" s="103"/>
-      <c r="AZ25" s="156" t="s">
+      <c r="AZ25" s="186" t="s">
         <v>278</v>
       </c>
-      <c r="BA25" s="157"/>
-      <c r="BB25" s="152" t="s">
+      <c r="BA25" s="195"/>
+      <c r="BB25" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="BC25" s="153"/>
-      <c r="BD25" s="149"/>
-      <c r="BE25" s="150"/>
-      <c r="BF25" s="150"/>
+      <c r="BC25" s="191"/>
+      <c r="BD25" s="229"/>
+      <c r="BE25" s="230"/>
+      <c r="BF25" s="230"/>
       <c r="BG25" s="96"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -16394,29 +16394,29 @@
         <v>301</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="196" t="s">
+      <c r="E30" s="192" t="s">
         <v>265</v>
       </c>
-      <c r="F30" s="197"/>
+      <c r="F30" s="193"/>
       <c r="G30" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="H30" s="196" t="s">
+      <c r="H30" s="192" t="s">
         <v>271</v>
       </c>
-      <c r="I30" s="197"/>
-      <c r="J30" s="196" t="s">
+      <c r="I30" s="193"/>
+      <c r="J30" s="192" t="s">
         <v>272</v>
       </c>
-      <c r="K30" s="197"/>
-      <c r="L30" s="196" t="s">
+      <c r="K30" s="193"/>
+      <c r="L30" s="192" t="s">
         <v>273</v>
       </c>
-      <c r="M30" s="197"/>
-      <c r="N30" s="196" t="s">
+      <c r="M30" s="193"/>
+      <c r="N30" s="192" t="s">
         <v>274</v>
       </c>
-      <c r="O30" s="197"/>
+      <c r="O30" s="193"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="s">
         <v>234</v>
@@ -16425,50 +16425,50 @@
         <v>234</v>
       </c>
       <c r="S30" s="7"/>
-      <c r="T30" s="196" t="s">
+      <c r="T30" s="192" t="s">
         <v>275</v>
       </c>
-      <c r="U30" s="197"/>
-      <c r="V30" s="196" t="s">
+      <c r="U30" s="193"/>
+      <c r="V30" s="192" t="s">
         <v>276</v>
       </c>
-      <c r="W30" s="197"/>
-      <c r="X30" s="196" t="s">
+      <c r="W30" s="193"/>
+      <c r="X30" s="192" t="s">
         <v>277</v>
       </c>
-      <c r="Y30" s="197"/>
-      <c r="Z30" s="196" t="s">
+      <c r="Y30" s="193"/>
+      <c r="Z30" s="192" t="s">
         <v>278</v>
       </c>
-      <c r="AA30" s="197"/>
-      <c r="AB30" s="170" t="s">
+      <c r="AA30" s="193"/>
+      <c r="AB30" s="196" t="s">
         <v>289</v>
       </c>
-      <c r="AC30" s="171"/>
-      <c r="AD30" s="172"/>
-      <c r="AE30" s="196" t="s">
+      <c r="AC30" s="197"/>
+      <c r="AD30" s="198"/>
+      <c r="AE30" s="192" t="s">
         <v>265</v>
       </c>
-      <c r="AF30" s="197"/>
+      <c r="AF30" s="193"/>
       <c r="AG30" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="AH30" s="196" t="s">
+      <c r="AH30" s="192" t="s">
         <v>271</v>
       </c>
-      <c r="AI30" s="197"/>
-      <c r="AJ30" s="196" t="s">
+      <c r="AI30" s="193"/>
+      <c r="AJ30" s="192" t="s">
         <v>272</v>
       </c>
-      <c r="AK30" s="197"/>
-      <c r="AL30" s="196" t="s">
+      <c r="AK30" s="193"/>
+      <c r="AL30" s="192" t="s">
         <v>273</v>
       </c>
-      <c r="AM30" s="197"/>
-      <c r="AN30" s="196" t="s">
+      <c r="AM30" s="193"/>
+      <c r="AN30" s="192" t="s">
         <v>274</v>
       </c>
-      <c r="AO30" s="197"/>
+      <c r="AO30" s="193"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7" t="s">
         <v>234</v>
@@ -16477,27 +16477,27 @@
         <v>234</v>
       </c>
       <c r="AS30" s="7"/>
-      <c r="AT30" s="196" t="s">
+      <c r="AT30" s="192" t="s">
         <v>275</v>
       </c>
-      <c r="AU30" s="197"/>
-      <c r="AV30" s="196" t="s">
+      <c r="AU30" s="193"/>
+      <c r="AV30" s="192" t="s">
         <v>276</v>
       </c>
-      <c r="AW30" s="197"/>
-      <c r="AX30" s="196" t="s">
+      <c r="AW30" s="193"/>
+      <c r="AX30" s="192" t="s">
         <v>277</v>
       </c>
-      <c r="AY30" s="197"/>
-      <c r="AZ30" s="196" t="s">
+      <c r="AY30" s="193"/>
+      <c r="AZ30" s="192" t="s">
         <v>278</v>
       </c>
-      <c r="BA30" s="197"/>
-      <c r="BB30" s="170" t="s">
+      <c r="BA30" s="193"/>
+      <c r="BB30" s="196" t="s">
         <v>289</v>
       </c>
-      <c r="BC30" s="171"/>
-      <c r="BD30" s="172"/>
+      <c r="BC30" s="197"/>
+      <c r="BD30" s="198"/>
       <c r="BE30" s="7"/>
       <c r="BF30" s="7"/>
       <c r="BG30" s="7"/>
@@ -16509,10 +16509,10 @@
         <v>300</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="173" t="s">
+      <c r="E31" s="194" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="173"/>
+      <c r="F31" s="194"/>
       <c r="G31" s="22" t="s">
         <v>307</v>
       </c>
@@ -16539,10 +16539,10 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
-      <c r="AE31" s="173" t="s">
+      <c r="AE31" s="194" t="s">
         <v>306</v>
       </c>
-      <c r="AF31" s="173"/>
+      <c r="AF31" s="194"/>
       <c r="AG31" s="22" t="s">
         <v>307</v>
       </c>
@@ -16652,75 +16652,75 @@
       <c r="G33" s="95" t="s">
         <v>266</v>
       </c>
-      <c r="H33" s="193" t="s">
+      <c r="H33" s="205" t="s">
         <v>302</v>
       </c>
-      <c r="I33" s="194"/>
-      <c r="J33" s="194"/>
-      <c r="K33" s="194"/>
-      <c r="L33" s="194"/>
-      <c r="M33" s="194"/>
-      <c r="N33" s="194"/>
-      <c r="O33" s="194"/>
-      <c r="P33" s="194"/>
-      <c r="Q33" s="194"/>
-      <c r="R33" s="194"/>
-      <c r="S33" s="195"/>
-      <c r="T33" s="196" t="s">
+      <c r="I33" s="206"/>
+      <c r="J33" s="206"/>
+      <c r="K33" s="206"/>
+      <c r="L33" s="206"/>
+      <c r="M33" s="206"/>
+      <c r="N33" s="206"/>
+      <c r="O33" s="206"/>
+      <c r="P33" s="206"/>
+      <c r="Q33" s="206"/>
+      <c r="R33" s="206"/>
+      <c r="S33" s="207"/>
+      <c r="T33" s="192" t="s">
         <v>267</v>
       </c>
-      <c r="U33" s="197"/>
-      <c r="V33" s="170" t="s">
+      <c r="U33" s="193"/>
+      <c r="V33" s="196" t="s">
         <v>289</v>
       </c>
-      <c r="W33" s="172"/>
-      <c r="X33" s="193" t="s">
+      <c r="W33" s="198"/>
+      <c r="X33" s="205" t="s">
         <v>302</v>
       </c>
-      <c r="Y33" s="194"/>
-      <c r="Z33" s="194"/>
-      <c r="AA33" s="194"/>
-      <c r="AB33" s="194"/>
-      <c r="AC33" s="194"/>
-      <c r="AD33" s="194"/>
-      <c r="AE33" s="195"/>
+      <c r="Y33" s="206"/>
+      <c r="Z33" s="206"/>
+      <c r="AA33" s="206"/>
+      <c r="AB33" s="206"/>
+      <c r="AC33" s="206"/>
+      <c r="AD33" s="206"/>
+      <c r="AE33" s="207"/>
       <c r="AF33" s="24" t="s">
         <v>265</v>
       </c>
       <c r="AG33" s="95" t="s">
         <v>266</v>
       </c>
-      <c r="AH33" s="193" t="s">
+      <c r="AH33" s="205" t="s">
         <v>302</v>
       </c>
-      <c r="AI33" s="194"/>
-      <c r="AJ33" s="194"/>
-      <c r="AK33" s="194"/>
-      <c r="AL33" s="194"/>
-      <c r="AM33" s="194"/>
-      <c r="AN33" s="194"/>
-      <c r="AO33" s="194"/>
-      <c r="AP33" s="194"/>
-      <c r="AQ33" s="194"/>
-      <c r="AR33" s="194"/>
-      <c r="AS33" s="195"/>
-      <c r="AT33" s="196" t="s">
+      <c r="AI33" s="206"/>
+      <c r="AJ33" s="206"/>
+      <c r="AK33" s="206"/>
+      <c r="AL33" s="206"/>
+      <c r="AM33" s="206"/>
+      <c r="AN33" s="206"/>
+      <c r="AO33" s="206"/>
+      <c r="AP33" s="206"/>
+      <c r="AQ33" s="206"/>
+      <c r="AR33" s="206"/>
+      <c r="AS33" s="207"/>
+      <c r="AT33" s="192" t="s">
         <v>267</v>
       </c>
-      <c r="AU33" s="197"/>
-      <c r="AV33" s="170" t="s">
+      <c r="AU33" s="193"/>
+      <c r="AV33" s="196" t="s">
         <v>289</v>
       </c>
-      <c r="AW33" s="172"/>
-      <c r="AX33" s="193" t="s">
+      <c r="AW33" s="198"/>
+      <c r="AX33" s="205" t="s">
         <v>302</v>
       </c>
-      <c r="AY33" s="194"/>
-      <c r="AZ33" s="194"/>
-      <c r="BA33" s="194"/>
-      <c r="BB33" s="194"/>
-      <c r="BC33" s="194"/>
-      <c r="BD33" s="195"/>
+      <c r="AY33" s="206"/>
+      <c r="AZ33" s="206"/>
+      <c r="BA33" s="206"/>
+      <c r="BB33" s="206"/>
+      <c r="BC33" s="206"/>
+      <c r="BD33" s="207"/>
       <c r="BE33" s="7"/>
       <c r="BF33" s="7"/>
       <c r="BG33" s="7"/>
@@ -16732,10 +16732,10 @@
         <v>300</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="173" t="s">
+      <c r="E34" s="194" t="s">
         <v>305</v>
       </c>
-      <c r="F34" s="173"/>
+      <c r="F34" s="194"/>
       <c r="G34" s="22" t="s">
         <v>304</v>
       </c>
@@ -16751,10 +16751,10 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="173" t="s">
+      <c r="T34" s="194" t="s">
         <v>306</v>
       </c>
-      <c r="U34" s="173"/>
+      <c r="U34" s="194"/>
       <c r="V34" s="22" t="s">
         <v>308</v>
       </c>
@@ -16783,10 +16783,10 @@
       <c r="AQ34" s="21"/>
       <c r="AR34" s="21"/>
       <c r="AS34" s="7"/>
-      <c r="AT34" s="173" t="s">
+      <c r="AT34" s="194" t="s">
         <v>306</v>
       </c>
-      <c r="AU34" s="173"/>
+      <c r="AU34" s="194"/>
       <c r="AV34" s="22" t="s">
         <v>303</v>
       </c>
@@ -17057,33 +17057,33 @@
         <v>309</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="188" t="s">
+      <c r="E39" s="208" t="s">
         <v>265</v>
       </c>
-      <c r="F39" s="189"/>
-      <c r="G39" s="191" t="s">
+      <c r="F39" s="209"/>
+      <c r="G39" s="210" t="s">
         <v>265</v>
       </c>
-      <c r="H39" s="192"/>
+      <c r="H39" s="211"/>
       <c r="I39" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="J39" s="156" t="s">
+      <c r="J39" s="186" t="s">
         <v>271</v>
       </c>
-      <c r="K39" s="157"/>
-      <c r="L39" s="156" t="s">
+      <c r="K39" s="195"/>
+      <c r="L39" s="186" t="s">
         <v>272</v>
       </c>
-      <c r="M39" s="157"/>
-      <c r="N39" s="156" t="s">
+      <c r="M39" s="195"/>
+      <c r="N39" s="186" t="s">
         <v>273</v>
       </c>
-      <c r="O39" s="157"/>
-      <c r="P39" s="156" t="s">
+      <c r="O39" s="195"/>
+      <c r="P39" s="186" t="s">
         <v>274</v>
       </c>
-      <c r="Q39" s="157"/>
+      <c r="Q39" s="195"/>
       <c r="R39" s="96"/>
       <c r="S39" s="96" t="s">
         <v>234</v>
@@ -17092,50 +17092,50 @@
         <v>234</v>
       </c>
       <c r="U39" s="96"/>
-      <c r="V39" s="156" t="s">
+      <c r="V39" s="186" t="s">
         <v>275</v>
       </c>
-      <c r="W39" s="157"/>
-      <c r="X39" s="156" t="s">
+      <c r="W39" s="195"/>
+      <c r="X39" s="186" t="s">
         <v>276</v>
       </c>
-      <c r="Y39" s="157"/>
-      <c r="Z39" s="156" t="s">
+      <c r="Y39" s="195"/>
+      <c r="Z39" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="AA39" s="157"/>
-      <c r="AB39" s="156" t="s">
+      <c r="AA39" s="195"/>
+      <c r="AB39" s="186" t="s">
         <v>278</v>
       </c>
-      <c r="AC39" s="157"/>
-      <c r="AD39" s="152" t="s">
+      <c r="AC39" s="195"/>
+      <c r="AD39" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AE39" s="190"/>
-      <c r="AF39" s="153"/>
-      <c r="AG39" s="156" t="s">
+      <c r="AE39" s="213"/>
+      <c r="AF39" s="191"/>
+      <c r="AG39" s="186" t="s">
         <v>265</v>
       </c>
-      <c r="AH39" s="157"/>
+      <c r="AH39" s="195"/>
       <c r="AI39" s="105" t="s">
         <v>302</v>
       </c>
-      <c r="AJ39" s="156" t="s">
+      <c r="AJ39" s="186" t="s">
         <v>271</v>
       </c>
-      <c r="AK39" s="157"/>
-      <c r="AL39" s="156" t="s">
+      <c r="AK39" s="195"/>
+      <c r="AL39" s="186" t="s">
         <v>272</v>
       </c>
-      <c r="AM39" s="157"/>
-      <c r="AN39" s="156" t="s">
+      <c r="AM39" s="195"/>
+      <c r="AN39" s="186" t="s">
         <v>273</v>
       </c>
-      <c r="AO39" s="157"/>
-      <c r="AP39" s="156" t="s">
+      <c r="AO39" s="195"/>
+      <c r="AP39" s="186" t="s">
         <v>274</v>
       </c>
-      <c r="AQ39" s="157"/>
+      <c r="AQ39" s="195"/>
       <c r="AR39" s="96"/>
       <c r="AS39" s="96" t="s">
         <v>234</v>
@@ -17164,14 +17164,14 @@
         <v>334</v>
       </c>
       <c r="D40" s="26"/>
-      <c r="E40" s="169" t="s">
+      <c r="E40" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="F40" s="169"/>
-      <c r="G40" s="169" t="s">
+      <c r="F40" s="212"/>
+      <c r="G40" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="H40" s="169"/>
+      <c r="H40" s="212"/>
       <c r="I40" s="106" t="s">
         <v>307</v>
       </c>
@@ -17198,10 +17198,10 @@
       <c r="AD40" s="96"/>
       <c r="AE40" s="96"/>
       <c r="AF40" s="96"/>
-      <c r="AG40" s="169" t="s">
+      <c r="AG40" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="AH40" s="169"/>
+      <c r="AH40" s="212"/>
       <c r="AI40" s="106" t="s">
         <v>311</v>
       </c>
@@ -17237,27 +17237,27 @@
         <v>310</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="156" t="s">
+      <c r="E41" s="186" t="s">
         <v>265</v>
       </c>
-      <c r="F41" s="157"/>
+      <c r="F41" s="195"/>
       <c r="G41" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="H41" s="156" t="s">
+      <c r="H41" s="186" t="s">
         <v>271</v>
       </c>
-      <c r="I41" s="157"/>
-      <c r="J41" s="156" t="s">
+      <c r="I41" s="195"/>
+      <c r="J41" s="186" t="s">
         <v>272</v>
       </c>
-      <c r="K41" s="157"/>
-      <c r="L41" s="188"/>
-      <c r="M41" s="189"/>
-      <c r="N41" s="191" t="s">
+      <c r="K41" s="195"/>
+      <c r="L41" s="208"/>
+      <c r="M41" s="209"/>
+      <c r="N41" s="210" t="s">
         <v>274</v>
       </c>
-      <c r="O41" s="192"/>
+      <c r="O41" s="211"/>
       <c r="P41" s="96"/>
       <c r="Q41" s="96" t="s">
         <v>234</v>
@@ -17266,50 +17266,50 @@
         <v>234</v>
       </c>
       <c r="S41" s="96"/>
-      <c r="T41" s="156" t="s">
+      <c r="T41" s="186" t="s">
         <v>275</v>
       </c>
-      <c r="U41" s="157"/>
-      <c r="V41" s="156" t="s">
+      <c r="U41" s="195"/>
+      <c r="V41" s="186" t="s">
         <v>276</v>
       </c>
-      <c r="W41" s="157"/>
-      <c r="X41" s="156" t="s">
+      <c r="W41" s="195"/>
+      <c r="X41" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="Y41" s="157"/>
-      <c r="Z41" s="156" t="s">
+      <c r="Y41" s="195"/>
+      <c r="Z41" s="186" t="s">
         <v>278</v>
       </c>
-      <c r="AA41" s="157"/>
-      <c r="AB41" s="152" t="s">
+      <c r="AA41" s="195"/>
+      <c r="AB41" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AC41" s="190"/>
-      <c r="AD41" s="153"/>
-      <c r="AE41" s="156" t="s">
+      <c r="AC41" s="213"/>
+      <c r="AD41" s="191"/>
+      <c r="AE41" s="186" t="s">
         <v>265</v>
       </c>
-      <c r="AF41" s="157"/>
+      <c r="AF41" s="195"/>
       <c r="AG41" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="AH41" s="156" t="s">
+      <c r="AH41" s="186" t="s">
         <v>271</v>
       </c>
-      <c r="AI41" s="157"/>
-      <c r="AJ41" s="156" t="s">
+      <c r="AI41" s="195"/>
+      <c r="AJ41" s="186" t="s">
         <v>272</v>
       </c>
-      <c r="AK41" s="157"/>
-      <c r="AL41" s="156" t="s">
+      <c r="AK41" s="195"/>
+      <c r="AL41" s="186" t="s">
         <v>273</v>
       </c>
-      <c r="AM41" s="157"/>
-      <c r="AN41" s="156" t="s">
+      <c r="AM41" s="195"/>
+      <c r="AN41" s="186" t="s">
         <v>274</v>
       </c>
-      <c r="AO41" s="157"/>
+      <c r="AO41" s="195"/>
       <c r="AP41" s="96"/>
       <c r="AQ41" s="96" t="s">
         <v>234</v>
@@ -17318,27 +17318,27 @@
         <v>234</v>
       </c>
       <c r="AS41" s="96"/>
-      <c r="AT41" s="156" t="s">
+      <c r="AT41" s="186" t="s">
         <v>275</v>
       </c>
-      <c r="AU41" s="157"/>
-      <c r="AV41" s="156" t="s">
+      <c r="AU41" s="195"/>
+      <c r="AV41" s="186" t="s">
         <v>276</v>
       </c>
-      <c r="AW41" s="157"/>
-      <c r="AX41" s="156" t="s">
+      <c r="AW41" s="195"/>
+      <c r="AX41" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="AY41" s="157"/>
-      <c r="AZ41" s="156" t="s">
+      <c r="AY41" s="195"/>
+      <c r="AZ41" s="186" t="s">
         <v>278</v>
       </c>
-      <c r="BA41" s="157"/>
-      <c r="BB41" s="152" t="s">
+      <c r="BA41" s="195"/>
+      <c r="BB41" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="BC41" s="190"/>
-      <c r="BD41" s="153"/>
+      <c r="BC41" s="213"/>
+      <c r="BD41" s="191"/>
       <c r="BE41" s="96"/>
       <c r="BF41" s="96"/>
       <c r="BG41" s="96"/>
@@ -17350,10 +17350,10 @@
         <v>335</v>
       </c>
       <c r="D42" s="26"/>
-      <c r="E42" s="169" t="s">
+      <c r="E42" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="F42" s="169"/>
+      <c r="F42" s="212"/>
       <c r="G42" s="106" t="s">
         <v>307</v>
       </c>
@@ -17380,10 +17380,10 @@
       <c r="AB42" s="96"/>
       <c r="AC42" s="96"/>
       <c r="AD42" s="96"/>
-      <c r="AE42" s="169" t="s">
+      <c r="AE42" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="AF42" s="169"/>
+      <c r="AF42" s="212"/>
       <c r="AG42" s="106" t="s">
         <v>307</v>
       </c>
@@ -17493,75 +17493,75 @@
       <c r="G44" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="H44" s="185" t="s">
+      <c r="H44" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="I44" s="186"/>
-      <c r="J44" s="186"/>
-      <c r="K44" s="186"/>
-      <c r="L44" s="186"/>
-      <c r="M44" s="186"/>
-      <c r="N44" s="186"/>
-      <c r="O44" s="186"/>
-      <c r="P44" s="186"/>
-      <c r="Q44" s="186"/>
-      <c r="R44" s="186"/>
-      <c r="S44" s="187"/>
-      <c r="T44" s="188" t="s">
+      <c r="I44" s="220"/>
+      <c r="J44" s="220"/>
+      <c r="K44" s="220"/>
+      <c r="L44" s="220"/>
+      <c r="M44" s="220"/>
+      <c r="N44" s="220"/>
+      <c r="O44" s="220"/>
+      <c r="P44" s="220"/>
+      <c r="Q44" s="220"/>
+      <c r="R44" s="220"/>
+      <c r="S44" s="221"/>
+      <c r="T44" s="208" t="s">
         <v>267</v>
       </c>
-      <c r="U44" s="189"/>
-      <c r="V44" s="152" t="s">
+      <c r="U44" s="209"/>
+      <c r="V44" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="W44" s="153"/>
-      <c r="X44" s="185" t="s">
+      <c r="W44" s="191"/>
+      <c r="X44" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="Y44" s="186"/>
-      <c r="Z44" s="186"/>
-      <c r="AA44" s="186"/>
-      <c r="AB44" s="186"/>
-      <c r="AC44" s="186"/>
-      <c r="AD44" s="186"/>
-      <c r="AE44" s="187"/>
+      <c r="Y44" s="220"/>
+      <c r="Z44" s="220"/>
+      <c r="AA44" s="220"/>
+      <c r="AB44" s="220"/>
+      <c r="AC44" s="220"/>
+      <c r="AD44" s="220"/>
+      <c r="AE44" s="221"/>
       <c r="AF44" s="108" t="s">
         <v>265</v>
       </c>
       <c r="AG44" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="AH44" s="185" t="s">
+      <c r="AH44" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="AI44" s="186"/>
-      <c r="AJ44" s="186"/>
-      <c r="AK44" s="186"/>
-      <c r="AL44" s="186"/>
-      <c r="AM44" s="186"/>
-      <c r="AN44" s="186"/>
-      <c r="AO44" s="186"/>
-      <c r="AP44" s="186"/>
-      <c r="AQ44" s="186"/>
-      <c r="AR44" s="186"/>
-      <c r="AS44" s="187"/>
-      <c r="AT44" s="156" t="s">
+      <c r="AI44" s="220"/>
+      <c r="AJ44" s="220"/>
+      <c r="AK44" s="220"/>
+      <c r="AL44" s="220"/>
+      <c r="AM44" s="220"/>
+      <c r="AN44" s="220"/>
+      <c r="AO44" s="220"/>
+      <c r="AP44" s="220"/>
+      <c r="AQ44" s="220"/>
+      <c r="AR44" s="220"/>
+      <c r="AS44" s="221"/>
+      <c r="AT44" s="186" t="s">
         <v>267</v>
       </c>
-      <c r="AU44" s="157"/>
-      <c r="AV44" s="152" t="s">
+      <c r="AU44" s="195"/>
+      <c r="AV44" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AW44" s="153"/>
-      <c r="AX44" s="185" t="s">
+      <c r="AW44" s="191"/>
+      <c r="AX44" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="AY44" s="186"/>
-      <c r="AZ44" s="186"/>
-      <c r="BA44" s="186"/>
-      <c r="BB44" s="186"/>
-      <c r="BC44" s="186"/>
-      <c r="BD44" s="187"/>
+      <c r="AY44" s="220"/>
+      <c r="AZ44" s="220"/>
+      <c r="BA44" s="220"/>
+      <c r="BB44" s="220"/>
+      <c r="BC44" s="220"/>
+      <c r="BD44" s="221"/>
       <c r="BE44" s="96"/>
       <c r="BF44" s="96"/>
       <c r="BG44" s="96"/>
@@ -17573,10 +17573,10 @@
         <v>335</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="169" t="s">
+      <c r="E45" s="212" t="s">
         <v>305</v>
       </c>
-      <c r="F45" s="169"/>
+      <c r="F45" s="212"/>
       <c r="G45" s="106" t="s">
         <v>304</v>
       </c>
@@ -17592,10 +17592,10 @@
       <c r="Q45" s="109"/>
       <c r="R45" s="109"/>
       <c r="S45" s="96"/>
-      <c r="T45" s="169" t="s">
+      <c r="T45" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="U45" s="169"/>
+      <c r="U45" s="212"/>
       <c r="V45" s="106" t="s">
         <v>308</v>
       </c>
@@ -17624,10 +17624,10 @@
       <c r="AQ45" s="109"/>
       <c r="AR45" s="109"/>
       <c r="AS45" s="96"/>
-      <c r="AT45" s="169" t="s">
+      <c r="AT45" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="AU45" s="169"/>
+      <c r="AU45" s="212"/>
       <c r="AV45" s="106" t="s">
         <v>303</v>
       </c>
@@ -17656,70 +17656,70 @@
       <c r="F46" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="G46" s="185" t="s">
+      <c r="G46" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="H46" s="186"/>
-      <c r="I46" s="186"/>
-      <c r="J46" s="186"/>
-      <c r="K46" s="186"/>
-      <c r="L46" s="186"/>
-      <c r="M46" s="186"/>
-      <c r="N46" s="186"/>
-      <c r="O46" s="186"/>
-      <c r="P46" s="186"/>
-      <c r="Q46" s="186"/>
-      <c r="R46" s="186"/>
-      <c r="S46" s="186"/>
-      <c r="T46" s="186"/>
-      <c r="U46" s="186"/>
-      <c r="V46" s="186"/>
-      <c r="W46" s="186"/>
-      <c r="X46" s="186"/>
-      <c r="Y46" s="186"/>
-      <c r="Z46" s="186"/>
-      <c r="AA46" s="186"/>
-      <c r="AB46" s="186"/>
-      <c r="AC46" s="186"/>
-      <c r="AD46" s="186"/>
-      <c r="AE46" s="187"/>
+      <c r="H46" s="220"/>
+      <c r="I46" s="220"/>
+      <c r="J46" s="220"/>
+      <c r="K46" s="220"/>
+      <c r="L46" s="220"/>
+      <c r="M46" s="220"/>
+      <c r="N46" s="220"/>
+      <c r="O46" s="220"/>
+      <c r="P46" s="220"/>
+      <c r="Q46" s="220"/>
+      <c r="R46" s="220"/>
+      <c r="S46" s="220"/>
+      <c r="T46" s="220"/>
+      <c r="U46" s="220"/>
+      <c r="V46" s="220"/>
+      <c r="W46" s="220"/>
+      <c r="X46" s="220"/>
+      <c r="Y46" s="220"/>
+      <c r="Z46" s="220"/>
+      <c r="AA46" s="220"/>
+      <c r="AB46" s="220"/>
+      <c r="AC46" s="220"/>
+      <c r="AD46" s="220"/>
+      <c r="AE46" s="221"/>
       <c r="AF46" s="108" t="s">
         <v>265</v>
       </c>
       <c r="AG46" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="AH46" s="185" t="s">
+      <c r="AH46" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="AI46" s="186"/>
-      <c r="AJ46" s="186"/>
-      <c r="AK46" s="186"/>
-      <c r="AL46" s="186"/>
-      <c r="AM46" s="186"/>
-      <c r="AN46" s="186"/>
-      <c r="AO46" s="186"/>
-      <c r="AP46" s="186"/>
-      <c r="AQ46" s="186"/>
-      <c r="AR46" s="186"/>
-      <c r="AS46" s="187"/>
-      <c r="AT46" s="156" t="s">
+      <c r="AI46" s="220"/>
+      <c r="AJ46" s="220"/>
+      <c r="AK46" s="220"/>
+      <c r="AL46" s="220"/>
+      <c r="AM46" s="220"/>
+      <c r="AN46" s="220"/>
+      <c r="AO46" s="220"/>
+      <c r="AP46" s="220"/>
+      <c r="AQ46" s="220"/>
+      <c r="AR46" s="220"/>
+      <c r="AS46" s="221"/>
+      <c r="AT46" s="186" t="s">
         <v>267</v>
       </c>
-      <c r="AU46" s="157"/>
-      <c r="AV46" s="152" t="s">
+      <c r="AU46" s="195"/>
+      <c r="AV46" s="190" t="s">
         <v>289</v>
       </c>
-      <c r="AW46" s="153"/>
-      <c r="AX46" s="185" t="s">
+      <c r="AW46" s="191"/>
+      <c r="AX46" s="219" t="s">
         <v>302</v>
       </c>
-      <c r="AY46" s="186"/>
-      <c r="AZ46" s="186"/>
-      <c r="BA46" s="186"/>
-      <c r="BB46" s="186"/>
-      <c r="BC46" s="186"/>
-      <c r="BD46" s="187"/>
+      <c r="AY46" s="220"/>
+      <c r="AZ46" s="220"/>
+      <c r="BA46" s="220"/>
+      <c r="BB46" s="220"/>
+      <c r="BC46" s="220"/>
+      <c r="BD46" s="221"/>
       <c r="BE46" s="96"/>
       <c r="BF46" s="96"/>
       <c r="BG46" s="96"/>
@@ -17776,10 +17776,10 @@
       <c r="AQ47" s="109"/>
       <c r="AR47" s="109"/>
       <c r="AS47" s="96"/>
-      <c r="AT47" s="169" t="s">
+      <c r="AT47" s="212" t="s">
         <v>306</v>
       </c>
-      <c r="AU47" s="169"/>
+      <c r="AU47" s="212"/>
       <c r="AV47" s="106" t="s">
         <v>303</v>
       </c>
@@ -18170,20 +18170,20 @@
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
-      <c r="E54" s="159" t="s">
+      <c r="E54" s="172" t="s">
         <v>222</v>
       </c>
-      <c r="F54" s="160"/>
-      <c r="G54" s="160"/>
-      <c r="H54" s="160"/>
-      <c r="I54" s="160"/>
-      <c r="J54" s="160"/>
-      <c r="K54" s="177"/>
-      <c r="L54" s="159" t="s">
+      <c r="F54" s="173"/>
+      <c r="G54" s="173"/>
+      <c r="H54" s="173"/>
+      <c r="I54" s="173"/>
+      <c r="J54" s="173"/>
+      <c r="K54" s="174"/>
+      <c r="L54" s="172" t="s">
         <v>223</v>
       </c>
-      <c r="M54" s="160"/>
-      <c r="N54" s="161"/>
+      <c r="M54" s="173"/>
+      <c r="N54" s="232"/>
       <c r="O54" s="42"/>
       <c r="P54" s="42"/>
       <c r="Q54" s="42"/>
@@ -18304,20 +18304,20 @@
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
-      <c r="E56" s="162" t="s">
+      <c r="E56" s="178" t="s">
         <v>225</v>
       </c>
-      <c r="F56" s="163"/>
-      <c r="G56" s="163"/>
-      <c r="H56" s="163"/>
-      <c r="I56" s="163"/>
-      <c r="J56" s="163"/>
-      <c r="K56" s="164"/>
-      <c r="L56" s="162" t="s">
+      <c r="F56" s="179"/>
+      <c r="G56" s="179"/>
+      <c r="H56" s="179"/>
+      <c r="I56" s="179"/>
+      <c r="J56" s="179"/>
+      <c r="K56" s="180"/>
+      <c r="L56" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="M56" s="163"/>
-      <c r="N56" s="164"/>
+      <c r="M56" s="179"/>
+      <c r="N56" s="180"/>
       <c r="O56" s="42"/>
       <c r="P56" s="42"/>
       <c r="Q56" s="42"/>
@@ -20789,66 +20789,66 @@
         <v>344</v>
       </c>
       <c r="D95" s="42"/>
-      <c r="E95" s="159" t="s">
+      <c r="E95" s="172" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="160"/>
-      <c r="G95" s="160"/>
-      <c r="H95" s="160"/>
-      <c r="I95" s="160"/>
-      <c r="J95" s="160"/>
-      <c r="K95" s="177"/>
-      <c r="L95" s="159" t="s">
+      <c r="F95" s="173"/>
+      <c r="G95" s="173"/>
+      <c r="H95" s="173"/>
+      <c r="I95" s="173"/>
+      <c r="J95" s="173"/>
+      <c r="K95" s="174"/>
+      <c r="L95" s="172" t="s">
         <v>223</v>
       </c>
-      <c r="M95" s="160"/>
-      <c r="N95" s="177"/>
-      <c r="O95" s="159" t="s">
+      <c r="M95" s="173"/>
+      <c r="N95" s="174"/>
+      <c r="O95" s="172" t="s">
         <v>570</v>
       </c>
-      <c r="P95" s="160"/>
-      <c r="Q95" s="160"/>
-      <c r="R95" s="160"/>
-      <c r="S95" s="160"/>
-      <c r="T95" s="160"/>
-      <c r="U95" s="160"/>
-      <c r="V95" s="160"/>
-      <c r="W95" s="160"/>
-      <c r="X95" s="160"/>
-      <c r="Y95" s="160"/>
-      <c r="Z95" s="177"/>
-      <c r="AA95" s="159" t="s">
+      <c r="P95" s="173"/>
+      <c r="Q95" s="173"/>
+      <c r="R95" s="173"/>
+      <c r="S95" s="173"/>
+      <c r="T95" s="173"/>
+      <c r="U95" s="173"/>
+      <c r="V95" s="173"/>
+      <c r="W95" s="173"/>
+      <c r="X95" s="173"/>
+      <c r="Y95" s="173"/>
+      <c r="Z95" s="174"/>
+      <c r="AA95" s="172" t="s">
         <v>571</v>
       </c>
-      <c r="AB95" s="160"/>
-      <c r="AC95" s="160"/>
-      <c r="AD95" s="160"/>
-      <c r="AE95" s="160"/>
-      <c r="AF95" s="160"/>
-      <c r="AG95" s="160"/>
-      <c r="AH95" s="177"/>
-      <c r="AI95" s="159" t="s">
+      <c r="AB95" s="173"/>
+      <c r="AC95" s="173"/>
+      <c r="AD95" s="173"/>
+      <c r="AE95" s="173"/>
+      <c r="AF95" s="173"/>
+      <c r="AG95" s="173"/>
+      <c r="AH95" s="174"/>
+      <c r="AI95" s="172" t="s">
         <v>572</v>
       </c>
-      <c r="AJ95" s="160"/>
-      <c r="AK95" s="160"/>
-      <c r="AL95" s="160"/>
-      <c r="AM95" s="160"/>
-      <c r="AN95" s="160"/>
-      <c r="AO95" s="160"/>
-      <c r="AP95" s="160"/>
-      <c r="AQ95" s="160"/>
-      <c r="AR95" s="160"/>
-      <c r="AS95" s="160"/>
-      <c r="AT95" s="177"/>
-      <c r="AU95" s="203" t="s">
+      <c r="AJ95" s="173"/>
+      <c r="AK95" s="173"/>
+      <c r="AL95" s="173"/>
+      <c r="AM95" s="173"/>
+      <c r="AN95" s="173"/>
+      <c r="AO95" s="173"/>
+      <c r="AP95" s="173"/>
+      <c r="AQ95" s="173"/>
+      <c r="AR95" s="173"/>
+      <c r="AS95" s="173"/>
+      <c r="AT95" s="174"/>
+      <c r="AU95" s="175" t="s">
         <v>290</v>
       </c>
-      <c r="AV95" s="204"/>
-      <c r="AW95" s="204"/>
-      <c r="AX95" s="204"/>
-      <c r="AY95" s="204"/>
-      <c r="AZ95" s="205"/>
+      <c r="AV95" s="176"/>
+      <c r="AW95" s="176"/>
+      <c r="AX95" s="176"/>
+      <c r="AY95" s="176"/>
+      <c r="AZ95" s="177"/>
       <c r="BA95" s="42"/>
       <c r="BB95" s="42"/>
       <c r="BC95" s="42"/>
@@ -20953,66 +20953,66 @@
       </c>
       <c r="C97" s="42"/>
       <c r="D97" s="42"/>
-      <c r="E97" s="162" t="s">
+      <c r="E97" s="178" t="s">
         <v>225</v>
       </c>
-      <c r="F97" s="163"/>
-      <c r="G97" s="163"/>
-      <c r="H97" s="163"/>
-      <c r="I97" s="163"/>
-      <c r="J97" s="163"/>
-      <c r="K97" s="164"/>
-      <c r="L97" s="162" t="s">
+      <c r="F97" s="179"/>
+      <c r="G97" s="179"/>
+      <c r="H97" s="179"/>
+      <c r="I97" s="179"/>
+      <c r="J97" s="179"/>
+      <c r="K97" s="180"/>
+      <c r="L97" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="M97" s="163"/>
-      <c r="N97" s="163"/>
-      <c r="O97" s="162" t="s">
+      <c r="M97" s="179"/>
+      <c r="N97" s="179"/>
+      <c r="O97" s="178" t="s">
         <v>559</v>
       </c>
-      <c r="P97" s="163"/>
-      <c r="Q97" s="163"/>
-      <c r="R97" s="163"/>
-      <c r="S97" s="163"/>
-      <c r="T97" s="163"/>
-      <c r="U97" s="163"/>
-      <c r="V97" s="163"/>
-      <c r="W97" s="163"/>
-      <c r="X97" s="163"/>
-      <c r="Y97" s="163"/>
-      <c r="Z97" s="164"/>
-      <c r="AA97" s="162" t="s">
+      <c r="P97" s="179"/>
+      <c r="Q97" s="179"/>
+      <c r="R97" s="179"/>
+      <c r="S97" s="179"/>
+      <c r="T97" s="179"/>
+      <c r="U97" s="179"/>
+      <c r="V97" s="179"/>
+      <c r="W97" s="179"/>
+      <c r="X97" s="179"/>
+      <c r="Y97" s="179"/>
+      <c r="Z97" s="180"/>
+      <c r="AA97" s="178" t="s">
         <v>561</v>
       </c>
-      <c r="AB97" s="163"/>
-      <c r="AC97" s="163"/>
-      <c r="AD97" s="163"/>
-      <c r="AE97" s="163"/>
-      <c r="AF97" s="163"/>
-      <c r="AG97" s="163"/>
-      <c r="AH97" s="164"/>
-      <c r="AI97" s="162" t="s">
+      <c r="AB97" s="179"/>
+      <c r="AC97" s="179"/>
+      <c r="AD97" s="179"/>
+      <c r="AE97" s="179"/>
+      <c r="AF97" s="179"/>
+      <c r="AG97" s="179"/>
+      <c r="AH97" s="180"/>
+      <c r="AI97" s="178" t="s">
         <v>559</v>
       </c>
-      <c r="AJ97" s="163"/>
-      <c r="AK97" s="163"/>
-      <c r="AL97" s="163"/>
-      <c r="AM97" s="163"/>
-      <c r="AN97" s="163"/>
-      <c r="AO97" s="163"/>
-      <c r="AP97" s="163"/>
-      <c r="AQ97" s="163"/>
-      <c r="AR97" s="163"/>
-      <c r="AS97" s="163"/>
-      <c r="AT97" s="164"/>
-      <c r="AU97" s="213" t="s">
+      <c r="AJ97" s="179"/>
+      <c r="AK97" s="179"/>
+      <c r="AL97" s="179"/>
+      <c r="AM97" s="179"/>
+      <c r="AN97" s="179"/>
+      <c r="AO97" s="179"/>
+      <c r="AP97" s="179"/>
+      <c r="AQ97" s="179"/>
+      <c r="AR97" s="179"/>
+      <c r="AS97" s="179"/>
+      <c r="AT97" s="180"/>
+      <c r="AU97" s="151" t="s">
         <v>573</v>
       </c>
-      <c r="AV97" s="214"/>
-      <c r="AW97" s="214"/>
-      <c r="AX97" s="214"/>
-      <c r="AY97" s="214"/>
-      <c r="AZ97" s="215"/>
+      <c r="AV97" s="152"/>
+      <c r="AW97" s="152"/>
+      <c r="AX97" s="152"/>
+      <c r="AY97" s="152"/>
+      <c r="AZ97" s="153"/>
       <c r="BA97" s="42"/>
       <c r="BB97" s="42"/>
       <c r="BC97" s="42"/>
@@ -21022,10 +21022,10 @@
       <c r="BG97" s="42"/>
     </row>
     <row r="98" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A98" s="229">
+      <c r="A98" s="166">
         <v>255</v>
       </c>
-      <c r="B98" s="231">
+      <c r="B98" s="168">
         <v>20</v>
       </c>
       <c r="C98" s="42"/>
@@ -21091,20 +21091,20 @@
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
       <c r="D99" s="42"/>
-      <c r="E99" s="200" t="s">
+      <c r="E99" s="199" t="s">
         <v>589</v>
       </c>
-      <c r="F99" s="201"/>
-      <c r="G99" s="201"/>
-      <c r="H99" s="201"/>
-      <c r="I99" s="201"/>
-      <c r="J99" s="201"/>
-      <c r="K99" s="202"/>
-      <c r="L99" s="165" t="s">
+      <c r="F99" s="200"/>
+      <c r="G99" s="200"/>
+      <c r="H99" s="200"/>
+      <c r="I99" s="200"/>
+      <c r="J99" s="200"/>
+      <c r="K99" s="201"/>
+      <c r="L99" s="202" t="s">
         <v>241</v>
       </c>
-      <c r="M99" s="166"/>
-      <c r="N99" s="167"/>
+      <c r="M99" s="203"/>
+      <c r="N99" s="204"/>
       <c r="O99" s="67" t="s">
         <v>574</v>
       </c>
@@ -21143,14 +21143,14 @@
       <c r="AR99" s="68"/>
       <c r="AS99" s="68"/>
       <c r="AT99" s="69"/>
-      <c r="AU99" s="228" t="s">
+      <c r="AU99" s="165" t="s">
         <v>583</v>
       </c>
-      <c r="AV99" s="219"/>
-      <c r="AW99" s="219"/>
-      <c r="AX99" s="219"/>
-      <c r="AY99" s="219"/>
-      <c r="AZ99" s="220"/>
+      <c r="AV99" s="156"/>
+      <c r="AW99" s="156"/>
+      <c r="AX99" s="156"/>
+      <c r="AY99" s="156"/>
+      <c r="AZ99" s="157"/>
       <c r="BA99" s="42"/>
       <c r="BB99" s="42"/>
       <c r="BC99" s="42"/>
@@ -21560,68 +21560,68 @@
         <v>347</v>
       </c>
       <c r="D106" s="42"/>
-      <c r="E106" s="159" t="s">
+      <c r="E106" s="172" t="s">
         <v>222</v>
       </c>
-      <c r="F106" s="160"/>
-      <c r="G106" s="160"/>
-      <c r="H106" s="160"/>
-      <c r="I106" s="160"/>
-      <c r="J106" s="160"/>
-      <c r="K106" s="177"/>
-      <c r="L106" s="159" t="s">
+      <c r="F106" s="173"/>
+      <c r="G106" s="173"/>
+      <c r="H106" s="173"/>
+      <c r="I106" s="173"/>
+      <c r="J106" s="173"/>
+      <c r="K106" s="174"/>
+      <c r="L106" s="172" t="s">
         <v>223</v>
       </c>
-      <c r="M106" s="160"/>
-      <c r="N106" s="177"/>
-      <c r="O106" s="159" t="s">
+      <c r="M106" s="173"/>
+      <c r="N106" s="174"/>
+      <c r="O106" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="P106" s="160"/>
-      <c r="Q106" s="160"/>
-      <c r="R106" s="159" t="s">
+      <c r="P106" s="173"/>
+      <c r="Q106" s="173"/>
+      <c r="R106" s="172" t="s">
         <v>297</v>
       </c>
-      <c r="S106" s="160"/>
-      <c r="T106" s="160"/>
-      <c r="U106" s="160"/>
-      <c r="V106" s="160"/>
-      <c r="W106" s="160"/>
-      <c r="X106" s="160"/>
-      <c r="Y106" s="160"/>
-      <c r="Z106" s="160"/>
-      <c r="AA106" s="160"/>
-      <c r="AB106" s="160"/>
-      <c r="AC106" s="177"/>
-      <c r="AD106" s="159" t="s">
+      <c r="S106" s="173"/>
+      <c r="T106" s="173"/>
+      <c r="U106" s="173"/>
+      <c r="V106" s="173"/>
+      <c r="W106" s="173"/>
+      <c r="X106" s="173"/>
+      <c r="Y106" s="173"/>
+      <c r="Z106" s="173"/>
+      <c r="AA106" s="173"/>
+      <c r="AB106" s="173"/>
+      <c r="AC106" s="174"/>
+      <c r="AD106" s="172" t="s">
         <v>298</v>
       </c>
-      <c r="AE106" s="160"/>
-      <c r="AF106" s="160"/>
-      <c r="AG106" s="160"/>
-      <c r="AH106" s="160"/>
-      <c r="AI106" s="160"/>
-      <c r="AJ106" s="160"/>
-      <c r="AK106" s="177"/>
-      <c r="AL106" s="159" t="s">
+      <c r="AE106" s="173"/>
+      <c r="AF106" s="173"/>
+      <c r="AG106" s="173"/>
+      <c r="AH106" s="173"/>
+      <c r="AI106" s="173"/>
+      <c r="AJ106" s="173"/>
+      <c r="AK106" s="174"/>
+      <c r="AL106" s="172" t="s">
         <v>224</v>
       </c>
-      <c r="AM106" s="160"/>
-      <c r="AN106" s="177"/>
-      <c r="AO106" s="159" t="s">
+      <c r="AM106" s="173"/>
+      <c r="AN106" s="174"/>
+      <c r="AO106" s="172" t="s">
         <v>229</v>
       </c>
-      <c r="AP106" s="160"/>
-      <c r="AQ106" s="160"/>
-      <c r="AR106" s="160"/>
-      <c r="AS106" s="160"/>
-      <c r="AT106" s="160"/>
-      <c r="AU106" s="160"/>
-      <c r="AV106" s="160"/>
-      <c r="AW106" s="160"/>
-      <c r="AX106" s="160"/>
-      <c r="AY106" s="160"/>
-      <c r="AZ106" s="177"/>
+      <c r="AP106" s="173"/>
+      <c r="AQ106" s="173"/>
+      <c r="AR106" s="173"/>
+      <c r="AS106" s="173"/>
+      <c r="AT106" s="173"/>
+      <c r="AU106" s="173"/>
+      <c r="AV106" s="173"/>
+      <c r="AW106" s="173"/>
+      <c r="AX106" s="173"/>
+      <c r="AY106" s="173"/>
+      <c r="AZ106" s="174"/>
       <c r="BA106" s="42"/>
       <c r="BB106" s="42"/>
       <c r="BC106" s="42"/>
@@ -21728,68 +21728,68 @@
       </c>
       <c r="C108" s="50"/>
       <c r="D108" s="42"/>
-      <c r="E108" s="162" t="s">
+      <c r="E108" s="178" t="s">
         <v>225</v>
       </c>
-      <c r="F108" s="163"/>
-      <c r="G108" s="163"/>
-      <c r="H108" s="163"/>
-      <c r="I108" s="163"/>
-      <c r="J108" s="163"/>
-      <c r="K108" s="164"/>
-      <c r="L108" s="162" t="s">
+      <c r="F108" s="179"/>
+      <c r="G108" s="179"/>
+      <c r="H108" s="179"/>
+      <c r="I108" s="179"/>
+      <c r="J108" s="179"/>
+      <c r="K108" s="180"/>
+      <c r="L108" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="M108" s="163"/>
-      <c r="N108" s="164"/>
-      <c r="O108" s="162" t="s">
+      <c r="M108" s="179"/>
+      <c r="N108" s="180"/>
+      <c r="O108" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="P108" s="163"/>
-      <c r="Q108" s="163"/>
-      <c r="R108" s="162" t="s">
+      <c r="P108" s="179"/>
+      <c r="Q108" s="179"/>
+      <c r="R108" s="178" t="s">
         <v>559</v>
       </c>
-      <c r="S108" s="163"/>
-      <c r="T108" s="163"/>
-      <c r="U108" s="163"/>
-      <c r="V108" s="163"/>
-      <c r="W108" s="163"/>
-      <c r="X108" s="163"/>
-      <c r="Y108" s="163"/>
-      <c r="Z108" s="163"/>
-      <c r="AA108" s="163"/>
-      <c r="AB108" s="163"/>
-      <c r="AC108" s="164"/>
-      <c r="AD108" s="162" t="s">
+      <c r="S108" s="179"/>
+      <c r="T108" s="179"/>
+      <c r="U108" s="179"/>
+      <c r="V108" s="179"/>
+      <c r="W108" s="179"/>
+      <c r="X108" s="179"/>
+      <c r="Y108" s="179"/>
+      <c r="Z108" s="179"/>
+      <c r="AA108" s="179"/>
+      <c r="AB108" s="179"/>
+      <c r="AC108" s="180"/>
+      <c r="AD108" s="178" t="s">
         <v>561</v>
       </c>
-      <c r="AE108" s="163"/>
-      <c r="AF108" s="163"/>
-      <c r="AG108" s="163"/>
-      <c r="AH108" s="163"/>
-      <c r="AI108" s="163"/>
-      <c r="AJ108" s="163"/>
-      <c r="AK108" s="164"/>
-      <c r="AL108" s="162" t="s">
+      <c r="AE108" s="179"/>
+      <c r="AF108" s="179"/>
+      <c r="AG108" s="179"/>
+      <c r="AH108" s="179"/>
+      <c r="AI108" s="179"/>
+      <c r="AJ108" s="179"/>
+      <c r="AK108" s="180"/>
+      <c r="AL108" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="AM108" s="163"/>
-      <c r="AN108" s="164"/>
-      <c r="AO108" s="162" t="s">
+      <c r="AM108" s="179"/>
+      <c r="AN108" s="180"/>
+      <c r="AO108" s="178" t="s">
         <v>559</v>
       </c>
-      <c r="AP108" s="163"/>
-      <c r="AQ108" s="163"/>
-      <c r="AR108" s="163"/>
-      <c r="AS108" s="163"/>
-      <c r="AT108" s="163"/>
-      <c r="AU108" s="163"/>
-      <c r="AV108" s="163"/>
-      <c r="AW108" s="163"/>
-      <c r="AX108" s="163"/>
-      <c r="AY108" s="163"/>
-      <c r="AZ108" s="164"/>
+      <c r="AP108" s="179"/>
+      <c r="AQ108" s="179"/>
+      <c r="AR108" s="179"/>
+      <c r="AS108" s="179"/>
+      <c r="AT108" s="179"/>
+      <c r="AU108" s="179"/>
+      <c r="AV108" s="179"/>
+      <c r="AW108" s="179"/>
+      <c r="AX108" s="179"/>
+      <c r="AY108" s="179"/>
+      <c r="AZ108" s="180"/>
       <c r="BA108" s="42"/>
       <c r="BB108" s="42"/>
       <c r="BC108" s="42"/>
@@ -21799,10 +21799,10 @@
       <c r="BG108" s="42"/>
     </row>
     <row r="109" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A109" s="229">
+      <c r="A109" s="166">
         <v>1</v>
       </c>
-      <c r="B109" s="231">
+      <c r="B109" s="168">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C109" s="50"/>
@@ -21867,7 +21867,7 @@
       <c r="A110" s="42">
         <v>2</v>
       </c>
-      <c r="B110" s="231">
+      <c r="B110" s="168">
         <v>0.31</v>
       </c>
       <c r="C110" s="50"/>
@@ -21883,11 +21883,11 @@
       <c r="I110" s="73"/>
       <c r="J110" s="73"/>
       <c r="K110" s="74"/>
-      <c r="L110" s="165" t="s">
+      <c r="L110" s="202" t="s">
         <v>241</v>
       </c>
-      <c r="M110" s="166"/>
-      <c r="N110" s="167"/>
+      <c r="M110" s="203"/>
+      <c r="N110" s="204"/>
       <c r="O110" s="53"/>
       <c r="P110" s="50"/>
       <c r="Q110" s="50"/>
@@ -21924,20 +21924,20 @@
       <c r="AN110" s="51">
         <v>0</v>
       </c>
-      <c r="AO110" s="206" t="s">
+      <c r="AO110" s="181" t="s">
         <v>227</v>
       </c>
-      <c r="AP110" s="207"/>
-      <c r="AQ110" s="207"/>
-      <c r="AR110" s="207"/>
-      <c r="AS110" s="207"/>
-      <c r="AT110" s="207"/>
-      <c r="AU110" s="207"/>
-      <c r="AV110" s="207"/>
-      <c r="AW110" s="207"/>
-      <c r="AX110" s="207"/>
-      <c r="AY110" s="207"/>
-      <c r="AZ110" s="208"/>
+      <c r="AP110" s="182"/>
+      <c r="AQ110" s="182"/>
+      <c r="AR110" s="182"/>
+      <c r="AS110" s="182"/>
+      <c r="AT110" s="182"/>
+      <c r="AU110" s="182"/>
+      <c r="AV110" s="182"/>
+      <c r="AW110" s="182"/>
+      <c r="AX110" s="182"/>
+      <c r="AY110" s="182"/>
+      <c r="AZ110" s="183"/>
       <c r="BA110" s="50" t="s">
         <v>299</v>
       </c>
@@ -21952,7 +21952,7 @@
       <c r="A111" s="42">
         <v>3</v>
       </c>
-      <c r="B111" s="231">
+      <c r="B111" s="168">
         <f>(B110+0.2)</f>
         <v>0.51</v>
       </c>
@@ -22006,20 +22006,20 @@
       <c r="AN111" s="51">
         <v>1</v>
       </c>
-      <c r="AO111" s="206" t="s">
+      <c r="AO111" s="181" t="s">
         <v>337</v>
       </c>
-      <c r="AP111" s="207"/>
-      <c r="AQ111" s="207"/>
-      <c r="AR111" s="207"/>
-      <c r="AS111" s="207"/>
-      <c r="AT111" s="207"/>
-      <c r="AU111" s="207"/>
-      <c r="AV111" s="207"/>
-      <c r="AW111" s="207"/>
-      <c r="AX111" s="207"/>
-      <c r="AY111" s="207"/>
-      <c r="AZ111" s="208"/>
+      <c r="AP111" s="182"/>
+      <c r="AQ111" s="182"/>
+      <c r="AR111" s="182"/>
+      <c r="AS111" s="182"/>
+      <c r="AT111" s="182"/>
+      <c r="AU111" s="182"/>
+      <c r="AV111" s="182"/>
+      <c r="AW111" s="182"/>
+      <c r="AX111" s="182"/>
+      <c r="AY111" s="182"/>
+      <c r="AZ111" s="183"/>
       <c r="BA111" s="50" t="s">
         <v>290</v>
       </c>
@@ -22034,7 +22034,7 @@
       <c r="A112" s="42">
         <v>4</v>
       </c>
-      <c r="B112" s="231">
+      <c r="B112" s="168">
         <f>(B111+0.2)</f>
         <v>0.71</v>
       </c>
@@ -22090,20 +22090,20 @@
       <c r="AN112" s="51">
         <v>0</v>
       </c>
-      <c r="AO112" s="206" t="s">
+      <c r="AO112" s="181" t="s">
         <v>336</v>
       </c>
-      <c r="AP112" s="207"/>
-      <c r="AQ112" s="207"/>
-      <c r="AR112" s="207"/>
-      <c r="AS112" s="207"/>
-      <c r="AT112" s="207"/>
-      <c r="AU112" s="207"/>
-      <c r="AV112" s="207"/>
-      <c r="AW112" s="207"/>
-      <c r="AX112" s="207"/>
-      <c r="AY112" s="207"/>
-      <c r="AZ112" s="208"/>
+      <c r="AP112" s="182"/>
+      <c r="AQ112" s="182"/>
+      <c r="AR112" s="182"/>
+      <c r="AS112" s="182"/>
+      <c r="AT112" s="182"/>
+      <c r="AU112" s="182"/>
+      <c r="AV112" s="182"/>
+      <c r="AW112" s="182"/>
+      <c r="AX112" s="182"/>
+      <c r="AY112" s="182"/>
+      <c r="AZ112" s="183"/>
       <c r="BA112" s="50" t="s">
         <v>258</v>
       </c>
@@ -22118,7 +22118,7 @@
       <c r="A113" s="42">
         <v>5</v>
       </c>
-      <c r="B113" s="231">
+      <c r="B113" s="168">
         <f>(B112+0.2)</f>
         <v>0.90999999999999992</v>
       </c>
@@ -22170,20 +22170,20 @@
       <c r="AN113" s="51">
         <v>1</v>
       </c>
-      <c r="AO113" s="206" t="s">
+      <c r="AO113" s="181" t="s">
         <v>599</v>
       </c>
-      <c r="AP113" s="207"/>
-      <c r="AQ113" s="207"/>
-      <c r="AR113" s="207"/>
-      <c r="AS113" s="207"/>
-      <c r="AT113" s="207"/>
-      <c r="AU113" s="207"/>
-      <c r="AV113" s="207"/>
-      <c r="AW113" s="207"/>
-      <c r="AX113" s="207"/>
-      <c r="AY113" s="207"/>
-      <c r="AZ113" s="208"/>
+      <c r="AP113" s="182"/>
+      <c r="AQ113" s="182"/>
+      <c r="AR113" s="182"/>
+      <c r="AS113" s="182"/>
+      <c r="AT113" s="182"/>
+      <c r="AU113" s="182"/>
+      <c r="AV113" s="182"/>
+      <c r="AW113" s="182"/>
+      <c r="AX113" s="182"/>
+      <c r="AY113" s="182"/>
+      <c r="AZ113" s="183"/>
       <c r="BA113" s="50" t="s">
         <v>590</v>
       </c>
@@ -22196,10 +22196,10 @@
     </row>
     <row r="114" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A114" s="42"/>
-      <c r="B114" s="232" t="s">
+      <c r="B114" s="169" t="s">
         <v>234</v>
       </c>
-      <c r="C114" s="230"/>
+      <c r="C114" s="167"/>
       <c r="D114" s="42"/>
       <c r="E114" s="49"/>
       <c r="F114" s="50"/>
@@ -22247,20 +22247,20 @@
       <c r="AN114" s="51">
         <v>0</v>
       </c>
-      <c r="AO114" s="206" t="s">
+      <c r="AO114" s="181" t="s">
         <v>600</v>
       </c>
-      <c r="AP114" s="207"/>
-      <c r="AQ114" s="207"/>
-      <c r="AR114" s="207"/>
-      <c r="AS114" s="207"/>
-      <c r="AT114" s="207"/>
-      <c r="AU114" s="207"/>
-      <c r="AV114" s="207"/>
-      <c r="AW114" s="207"/>
-      <c r="AX114" s="207"/>
-      <c r="AY114" s="207"/>
-      <c r="AZ114" s="208"/>
+      <c r="AP114" s="182"/>
+      <c r="AQ114" s="182"/>
+      <c r="AR114" s="182"/>
+      <c r="AS114" s="182"/>
+      <c r="AT114" s="182"/>
+      <c r="AU114" s="182"/>
+      <c r="AV114" s="182"/>
+      <c r="AW114" s="182"/>
+      <c r="AX114" s="182"/>
+      <c r="AY114" s="182"/>
+      <c r="AZ114" s="183"/>
       <c r="BA114" s="50" t="s">
         <v>591</v>
       </c>
@@ -22273,10 +22273,10 @@
     </row>
     <row r="115" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A115" s="42"/>
-      <c r="B115" s="232" t="s">
+      <c r="B115" s="169" t="s">
         <v>234</v>
       </c>
-      <c r="C115" s="230"/>
+      <c r="C115" s="167"/>
       <c r="D115" s="42"/>
       <c r="E115" s="49"/>
       <c r="F115" s="50"/>
@@ -22288,29 +22288,29 @@
       <c r="L115" s="52"/>
       <c r="M115" s="53"/>
       <c r="N115" s="53"/>
-      <c r="O115" s="216"/>
-      <c r="P115" s="216"/>
-      <c r="Q115" s="216"/>
-      <c r="R115" s="216"/>
+      <c r="O115" s="154"/>
+      <c r="P115" s="154"/>
+      <c r="Q115" s="154"/>
+      <c r="R115" s="154"/>
       <c r="S115" s="50"/>
       <c r="T115" s="50"/>
       <c r="U115" s="50"/>
-      <c r="V115" s="216"/>
-      <c r="W115" s="216"/>
-      <c r="X115" s="216"/>
-      <c r="Y115" s="216"/>
-      <c r="Z115" s="216"/>
-      <c r="AA115" s="216"/>
-      <c r="AB115" s="216"/>
-      <c r="AC115" s="216"/>
-      <c r="AD115" s="216"/>
-      <c r="AE115" s="216"/>
-      <c r="AF115" s="216"/>
-      <c r="AG115" s="216"/>
-      <c r="AH115" s="216"/>
-      <c r="AI115" s="216"/>
-      <c r="AJ115" s="216"/>
-      <c r="AK115" s="216"/>
+      <c r="V115" s="154"/>
+      <c r="W115" s="154"/>
+      <c r="X115" s="154"/>
+      <c r="Y115" s="154"/>
+      <c r="Z115" s="154"/>
+      <c r="AA115" s="154"/>
+      <c r="AB115" s="154"/>
+      <c r="AC115" s="154"/>
+      <c r="AD115" s="154"/>
+      <c r="AE115" s="154"/>
+      <c r="AF115" s="154"/>
+      <c r="AG115" s="154"/>
+      <c r="AH115" s="154"/>
+      <c r="AI115" s="154"/>
+      <c r="AJ115" s="154"/>
+      <c r="AK115" s="154"/>
       <c r="AL115" s="51">
         <v>1</v>
       </c>
@@ -22320,20 +22320,20 @@
       <c r="AN115" s="51">
         <v>1</v>
       </c>
-      <c r="AO115" s="206" t="s">
+      <c r="AO115" s="181" t="s">
         <v>601</v>
       </c>
-      <c r="AP115" s="207"/>
-      <c r="AQ115" s="207"/>
-      <c r="AR115" s="207"/>
-      <c r="AS115" s="207"/>
-      <c r="AT115" s="207"/>
-      <c r="AU115" s="207"/>
-      <c r="AV115" s="207"/>
-      <c r="AW115" s="207"/>
-      <c r="AX115" s="207"/>
-      <c r="AY115" s="207"/>
-      <c r="AZ115" s="208"/>
+      <c r="AP115" s="182"/>
+      <c r="AQ115" s="182"/>
+      <c r="AR115" s="182"/>
+      <c r="AS115" s="182"/>
+      <c r="AT115" s="182"/>
+      <c r="AU115" s="182"/>
+      <c r="AV115" s="182"/>
+      <c r="AW115" s="182"/>
+      <c r="AX115" s="182"/>
+      <c r="AY115" s="182"/>
+      <c r="AZ115" s="183"/>
       <c r="BA115" s="50" t="s">
         <v>592</v>
       </c>
@@ -22348,7 +22348,7 @@
       <c r="A116" s="42">
         <v>97</v>
       </c>
-      <c r="B116" s="231">
+      <c r="B116" s="168">
         <f>((97-2)*0.2+0.31)</f>
         <v>19.309999999999999</v>
       </c>
@@ -22375,22 +22375,22 @@
       <c r="S116" s="50"/>
       <c r="T116" s="50"/>
       <c r="U116" s="50"/>
-      <c r="V116" s="216"/>
-      <c r="W116" s="216"/>
-      <c r="X116" s="216"/>
-      <c r="Y116" s="216"/>
-      <c r="Z116" s="216"/>
-      <c r="AA116" s="216"/>
-      <c r="AB116" s="216"/>
-      <c r="AC116" s="216"/>
-      <c r="AD116" s="216"/>
-      <c r="AE116" s="216"/>
-      <c r="AF116" s="216"/>
-      <c r="AG116" s="216"/>
-      <c r="AH116" s="216"/>
-      <c r="AI116" s="216"/>
-      <c r="AJ116" s="216"/>
-      <c r="AK116" s="216"/>
+      <c r="V116" s="154"/>
+      <c r="W116" s="154"/>
+      <c r="X116" s="154"/>
+      <c r="Y116" s="154"/>
+      <c r="Z116" s="154"/>
+      <c r="AA116" s="154"/>
+      <c r="AB116" s="154"/>
+      <c r="AC116" s="154"/>
+      <c r="AD116" s="154"/>
+      <c r="AE116" s="154"/>
+      <c r="AF116" s="154"/>
+      <c r="AG116" s="154"/>
+      <c r="AH116" s="154"/>
+      <c r="AI116" s="154"/>
+      <c r="AJ116" s="154"/>
+      <c r="AK116" s="154"/>
       <c r="AL116" s="51">
         <v>1</v>
       </c>
@@ -22400,20 +22400,20 @@
       <c r="AN116" s="51">
         <v>0</v>
       </c>
-      <c r="AO116" s="206" t="s">
+      <c r="AO116" s="181" t="s">
         <v>602</v>
       </c>
-      <c r="AP116" s="207"/>
-      <c r="AQ116" s="207"/>
-      <c r="AR116" s="207"/>
-      <c r="AS116" s="207"/>
-      <c r="AT116" s="207"/>
-      <c r="AU116" s="207"/>
-      <c r="AV116" s="207"/>
-      <c r="AW116" s="207"/>
-      <c r="AX116" s="207"/>
-      <c r="AY116" s="207"/>
-      <c r="AZ116" s="208"/>
+      <c r="AP116" s="182"/>
+      <c r="AQ116" s="182"/>
+      <c r="AR116" s="182"/>
+      <c r="AS116" s="182"/>
+      <c r="AT116" s="182"/>
+      <c r="AU116" s="182"/>
+      <c r="AV116" s="182"/>
+      <c r="AW116" s="182"/>
+      <c r="AX116" s="182"/>
+      <c r="AY116" s="182"/>
+      <c r="AZ116" s="183"/>
       <c r="BA116" s="50" t="s">
         <v>593</v>
       </c>
@@ -22428,7 +22428,7 @@
       <c r="A117" s="42">
         <v>98</v>
       </c>
-      <c r="B117" s="231">
+      <c r="B117" s="168">
         <f>(B116+0.2)</f>
         <v>19.509999999999998</v>
       </c>
@@ -22444,31 +22444,31 @@
       <c r="L117" s="52"/>
       <c r="M117" s="53"/>
       <c r="N117" s="53"/>
-      <c r="O117" s="203" t="s">
+      <c r="O117" s="175" t="s">
         <v>228</v>
       </c>
-      <c r="P117" s="204"/>
-      <c r="Q117" s="205"/>
+      <c r="P117" s="176"/>
+      <c r="Q117" s="177"/>
       <c r="R117" s="50"/>
       <c r="S117" s="50"/>
       <c r="T117" s="50"/>
       <c r="U117" s="50"/>
-      <c r="V117" s="216"/>
-      <c r="W117" s="216"/>
-      <c r="X117" s="216"/>
-      <c r="Y117" s="216"/>
-      <c r="Z117" s="216"/>
-      <c r="AA117" s="216"/>
-      <c r="AB117" s="216"/>
-      <c r="AC117" s="216"/>
-      <c r="AD117" s="216"/>
-      <c r="AE117" s="216"/>
-      <c r="AF117" s="216"/>
-      <c r="AG117" s="216"/>
-      <c r="AH117" s="216"/>
-      <c r="AI117" s="216"/>
-      <c r="AJ117" s="216"/>
-      <c r="AK117" s="216"/>
+      <c r="V117" s="154"/>
+      <c r="W117" s="154"/>
+      <c r="X117" s="154"/>
+      <c r="Y117" s="154"/>
+      <c r="Z117" s="154"/>
+      <c r="AA117" s="154"/>
+      <c r="AB117" s="154"/>
+      <c r="AC117" s="154"/>
+      <c r="AD117" s="154"/>
+      <c r="AE117" s="154"/>
+      <c r="AF117" s="154"/>
+      <c r="AG117" s="154"/>
+      <c r="AH117" s="154"/>
+      <c r="AI117" s="154"/>
+      <c r="AJ117" s="154"/>
+      <c r="AK117" s="154"/>
       <c r="AL117" s="51">
         <v>1</v>
       </c>
@@ -22478,20 +22478,20 @@
       <c r="AN117" s="51">
         <v>1</v>
       </c>
-      <c r="AO117" s="206" t="s">
+      <c r="AO117" s="181" t="s">
         <v>564</v>
       </c>
-      <c r="AP117" s="207"/>
-      <c r="AQ117" s="207"/>
-      <c r="AR117" s="207"/>
-      <c r="AS117" s="207"/>
-      <c r="AT117" s="207"/>
-      <c r="AU117" s="207"/>
-      <c r="AV117" s="207"/>
-      <c r="AW117" s="207"/>
-      <c r="AX117" s="207"/>
-      <c r="AY117" s="207"/>
-      <c r="AZ117" s="208"/>
+      <c r="AP117" s="182"/>
+      <c r="AQ117" s="182"/>
+      <c r="AR117" s="182"/>
+      <c r="AS117" s="182"/>
+      <c r="AT117" s="182"/>
+      <c r="AU117" s="182"/>
+      <c r="AV117" s="182"/>
+      <c r="AW117" s="182"/>
+      <c r="AX117" s="182"/>
+      <c r="AY117" s="182"/>
+      <c r="AZ117" s="183"/>
       <c r="BA117" s="50" t="s">
         <v>594</v>
       </c>
@@ -22506,7 +22506,7 @@
       <c r="A118" s="42">
         <v>99</v>
       </c>
-      <c r="B118" s="231">
+      <c r="B118" s="168">
         <f>(B117+0.2)</f>
         <v>19.709999999999997</v>
       </c>
@@ -22522,9 +22522,9 @@
       <c r="L118" s="49"/>
       <c r="M118" s="50"/>
       <c r="N118" s="50"/>
-      <c r="O118" s="211"/>
-      <c r="P118" s="211"/>
-      <c r="Q118" s="212">
+      <c r="O118" s="149"/>
+      <c r="P118" s="149"/>
+      <c r="Q118" s="150">
         <v>1</v>
       </c>
       <c r="R118" s="67" t="s">
@@ -22576,7 +22576,7 @@
       <c r="A119" s="42">
         <v>100</v>
       </c>
-      <c r="B119" s="231">
+      <c r="B119" s="168">
         <f>(B118+0.2)</f>
         <v>19.909999999999997</v>
       </c>
@@ -22689,24 +22689,24 @@
       <c r="AJ120" s="50"/>
       <c r="AK120" s="50"/>
       <c r="AL120" s="50"/>
-      <c r="AM120" s="217" t="s">
+      <c r="AM120" s="184" t="s">
         <v>293</v>
       </c>
-      <c r="AN120" s="217"/>
-      <c r="AO120" s="159" t="s">
+      <c r="AN120" s="184"/>
+      <c r="AO120" s="172" t="s">
         <v>291</v>
       </c>
-      <c r="AP120" s="160"/>
-      <c r="AQ120" s="160"/>
-      <c r="AR120" s="160"/>
-      <c r="AS120" s="160"/>
-      <c r="AT120" s="160"/>
-      <c r="AU120" s="160"/>
-      <c r="AV120" s="160"/>
-      <c r="AW120" s="160"/>
-      <c r="AX120" s="160"/>
-      <c r="AY120" s="160"/>
-      <c r="AZ120" s="177"/>
+      <c r="AP120" s="173"/>
+      <c r="AQ120" s="173"/>
+      <c r="AR120" s="173"/>
+      <c r="AS120" s="173"/>
+      <c r="AT120" s="173"/>
+      <c r="AU120" s="173"/>
+      <c r="AV120" s="173"/>
+      <c r="AW120" s="173"/>
+      <c r="AX120" s="173"/>
+      <c r="AY120" s="173"/>
+      <c r="AZ120" s="174"/>
       <c r="BA120" s="42"/>
       <c r="BB120" s="42"/>
       <c r="BC120" s="42"/>
@@ -22756,18 +22756,18 @@
       <c r="AL121" s="42"/>
       <c r="AM121" s="42"/>
       <c r="AN121" s="42"/>
-      <c r="AO121" s="211"/>
-      <c r="AP121" s="211"/>
-      <c r="AQ121" s="211"/>
-      <c r="AR121" s="211"/>
-      <c r="AS121" s="211"/>
-      <c r="AT121" s="211"/>
-      <c r="AU121" s="211"/>
-      <c r="AV121" s="211"/>
-      <c r="AW121" s="211"/>
-      <c r="AX121" s="211"/>
-      <c r="AY121" s="211"/>
-      <c r="AZ121" s="212">
+      <c r="AO121" s="149"/>
+      <c r="AP121" s="149"/>
+      <c r="AQ121" s="149"/>
+      <c r="AR121" s="149"/>
+      <c r="AS121" s="149"/>
+      <c r="AT121" s="149"/>
+      <c r="AU121" s="149"/>
+      <c r="AV121" s="149"/>
+      <c r="AW121" s="149"/>
+      <c r="AX121" s="149"/>
+      <c r="AY121" s="149"/>
+      <c r="AZ121" s="150">
         <v>1</v>
       </c>
       <c r="BA121" s="78" t="s">
@@ -23619,7 +23619,7 @@
       <c r="AN134" s="79" t="s">
         <v>361</v>
       </c>
-      <c r="AO134" s="218">
+      <c r="AO134" s="155">
         <v>0</v>
       </c>
       <c r="AP134" s="77">
@@ -23629,7 +23629,7 @@
         <v>1</v>
       </c>
       <c r="AR134" s="77"/>
-      <c r="AS134" s="218"/>
+      <c r="AS134" s="155"/>
       <c r="AT134" s="77"/>
       <c r="AU134" s="77"/>
       <c r="AV134" s="77"/>
@@ -24021,24 +24021,24 @@
       <c r="AJ140" s="42"/>
       <c r="AK140" s="42"/>
       <c r="AL140" s="42"/>
-      <c r="AM140" s="198" t="s">
+      <c r="AM140" s="170" t="s">
         <v>295</v>
       </c>
-      <c r="AN140" s="199"/>
-      <c r="AO140" s="159" t="s">
+      <c r="AN140" s="171"/>
+      <c r="AO140" s="172" t="s">
         <v>338</v>
       </c>
-      <c r="AP140" s="160"/>
-      <c r="AQ140" s="160"/>
-      <c r="AR140" s="160"/>
-      <c r="AS140" s="160"/>
-      <c r="AT140" s="160"/>
-      <c r="AU140" s="160"/>
-      <c r="AV140" s="160"/>
-      <c r="AW140" s="160"/>
-      <c r="AX140" s="160"/>
-      <c r="AY140" s="160"/>
-      <c r="AZ140" s="177"/>
+      <c r="AP140" s="173"/>
+      <c r="AQ140" s="173"/>
+      <c r="AR140" s="173"/>
+      <c r="AS140" s="173"/>
+      <c r="AT140" s="173"/>
+      <c r="AU140" s="173"/>
+      <c r="AV140" s="173"/>
+      <c r="AW140" s="173"/>
+      <c r="AX140" s="173"/>
+      <c r="AY140" s="173"/>
+      <c r="AZ140" s="174"/>
       <c r="BA140" s="42"/>
       <c r="BB140" s="42"/>
       <c r="BC140" s="42"/>
@@ -24088,20 +24088,20 @@
       <c r="AL141" s="42"/>
       <c r="AM141" s="42"/>
       <c r="AN141" s="42"/>
-      <c r="AO141" s="225" t="s">
+      <c r="AO141" s="162" t="s">
         <v>584</v>
       </c>
-      <c r="AP141" s="226"/>
-      <c r="AQ141" s="226"/>
-      <c r="AR141" s="226"/>
-      <c r="AS141" s="226"/>
-      <c r="AT141" s="226"/>
-      <c r="AU141" s="226"/>
-      <c r="AV141" s="226"/>
-      <c r="AW141" s="226"/>
-      <c r="AX141" s="226"/>
-      <c r="AY141" s="226"/>
-      <c r="AZ141" s="227"/>
+      <c r="AP141" s="163"/>
+      <c r="AQ141" s="163"/>
+      <c r="AR141" s="163"/>
+      <c r="AS141" s="163"/>
+      <c r="AT141" s="163"/>
+      <c r="AU141" s="163"/>
+      <c r="AV141" s="163"/>
+      <c r="AW141" s="163"/>
+      <c r="AX141" s="163"/>
+      <c r="AY141" s="163"/>
+      <c r="AZ141" s="164"/>
       <c r="BA141" s="42"/>
       <c r="BB141" s="42"/>
       <c r="BC141" s="42"/>
@@ -24210,24 +24210,24 @@
       <c r="AJ143" s="42"/>
       <c r="AK143" s="42"/>
       <c r="AL143" s="42"/>
-      <c r="AM143" s="198" t="s">
+      <c r="AM143" s="170" t="s">
         <v>294</v>
       </c>
-      <c r="AN143" s="199"/>
-      <c r="AO143" s="159" t="s">
+      <c r="AN143" s="171"/>
+      <c r="AO143" s="172" t="s">
         <v>296</v>
       </c>
-      <c r="AP143" s="160"/>
-      <c r="AQ143" s="160"/>
-      <c r="AR143" s="160"/>
-      <c r="AS143" s="160"/>
-      <c r="AT143" s="160"/>
-      <c r="AU143" s="160"/>
-      <c r="AV143" s="160"/>
-      <c r="AW143" s="160"/>
-      <c r="AX143" s="160"/>
-      <c r="AY143" s="160"/>
-      <c r="AZ143" s="177"/>
+      <c r="AP143" s="173"/>
+      <c r="AQ143" s="173"/>
+      <c r="AR143" s="173"/>
+      <c r="AS143" s="173"/>
+      <c r="AT143" s="173"/>
+      <c r="AU143" s="173"/>
+      <c r="AV143" s="173"/>
+      <c r="AW143" s="173"/>
+      <c r="AX143" s="173"/>
+      <c r="AY143" s="173"/>
+      <c r="AZ143" s="174"/>
       <c r="BA143" s="42"/>
       <c r="BB143" s="42"/>
       <c r="BC143" s="42"/>
@@ -24277,20 +24277,20 @@
       <c r="AL144" s="42"/>
       <c r="AM144" s="42"/>
       <c r="AN144" s="42"/>
-      <c r="AO144" s="222" t="s">
+      <c r="AO144" s="159" t="s">
         <v>603</v>
       </c>
-      <c r="AP144" s="221"/>
-      <c r="AQ144" s="221"/>
-      <c r="AR144" s="221"/>
-      <c r="AS144" s="223"/>
-      <c r="AT144" s="221"/>
-      <c r="AU144" s="221"/>
-      <c r="AV144" s="221"/>
-      <c r="AW144" s="221"/>
-      <c r="AX144" s="221"/>
-      <c r="AY144" s="221"/>
-      <c r="AZ144" s="224"/>
+      <c r="AP144" s="158"/>
+      <c r="AQ144" s="158"/>
+      <c r="AR144" s="158"/>
+      <c r="AS144" s="160"/>
+      <c r="AT144" s="158"/>
+      <c r="AU144" s="158"/>
+      <c r="AV144" s="158"/>
+      <c r="AW144" s="158"/>
+      <c r="AX144" s="158"/>
+      <c r="AY144" s="158"/>
+      <c r="AZ144" s="161"/>
       <c r="BA144" s="42"/>
       <c r="BB144" s="42"/>
       <c r="BC144" s="42"/>
@@ -24462,24 +24462,24 @@
       <c r="AJ147" s="42"/>
       <c r="AK147" s="42"/>
       <c r="AL147" s="42"/>
-      <c r="AM147" s="198" t="s">
+      <c r="AM147" s="170" t="s">
         <v>605</v>
       </c>
-      <c r="AN147" s="199"/>
-      <c r="AO147" s="159" t="s">
+      <c r="AN147" s="171"/>
+      <c r="AO147" s="172" t="s">
         <v>590</v>
       </c>
-      <c r="AP147" s="160"/>
-      <c r="AQ147" s="160"/>
-      <c r="AR147" s="160"/>
-      <c r="AS147" s="160"/>
-      <c r="AT147" s="160"/>
-      <c r="AU147" s="160"/>
-      <c r="AV147" s="160"/>
-      <c r="AW147" s="160"/>
-      <c r="AX147" s="160"/>
-      <c r="AY147" s="160"/>
-      <c r="AZ147" s="177"/>
+      <c r="AP147" s="173"/>
+      <c r="AQ147" s="173"/>
+      <c r="AR147" s="173"/>
+      <c r="AS147" s="173"/>
+      <c r="AT147" s="173"/>
+      <c r="AU147" s="173"/>
+      <c r="AV147" s="173"/>
+      <c r="AW147" s="173"/>
+      <c r="AX147" s="173"/>
+      <c r="AY147" s="173"/>
+      <c r="AZ147" s="174"/>
       <c r="BA147" s="42"/>
       <c r="BB147" s="42"/>
       <c r="BC147" s="42"/>
@@ -24529,20 +24529,20 @@
       <c r="AL148" s="42"/>
       <c r="AM148" s="42"/>
       <c r="AN148" s="42"/>
-      <c r="AO148" s="222" t="s">
+      <c r="AO148" s="159" t="s">
         <v>606</v>
       </c>
-      <c r="AP148" s="221"/>
-      <c r="AQ148" s="221"/>
-      <c r="AR148" s="221"/>
-      <c r="AS148" s="223"/>
-      <c r="AT148" s="221"/>
-      <c r="AU148" s="221"/>
-      <c r="AV148" s="221"/>
-      <c r="AW148" s="221"/>
-      <c r="AX148" s="221"/>
-      <c r="AY148" s="221"/>
-      <c r="AZ148" s="224"/>
+      <c r="AP148" s="158"/>
+      <c r="AQ148" s="158"/>
+      <c r="AR148" s="158"/>
+      <c r="AS148" s="160"/>
+      <c r="AT148" s="158"/>
+      <c r="AU148" s="158"/>
+      <c r="AV148" s="158"/>
+      <c r="AW148" s="158"/>
+      <c r="AX148" s="158"/>
+      <c r="AY148" s="158"/>
+      <c r="AZ148" s="161"/>
       <c r="BA148" s="42"/>
       <c r="BB148" s="42"/>
       <c r="BC148" s="42"/>
@@ -24714,24 +24714,24 @@
       <c r="AJ151" s="42"/>
       <c r="AK151" s="42"/>
       <c r="AL151" s="42"/>
-      <c r="AM151" s="198" t="s">
+      <c r="AM151" s="170" t="s">
         <v>608</v>
       </c>
-      <c r="AN151" s="199"/>
-      <c r="AO151" s="159" t="s">
+      <c r="AN151" s="171"/>
+      <c r="AO151" s="172" t="s">
         <v>591</v>
       </c>
-      <c r="AP151" s="160"/>
-      <c r="AQ151" s="160"/>
-      <c r="AR151" s="160"/>
-      <c r="AS151" s="160"/>
-      <c r="AT151" s="160"/>
-      <c r="AU151" s="160"/>
-      <c r="AV151" s="160"/>
-      <c r="AW151" s="160"/>
-      <c r="AX151" s="160"/>
-      <c r="AY151" s="160"/>
-      <c r="AZ151" s="177"/>
+      <c r="AP151" s="173"/>
+      <c r="AQ151" s="173"/>
+      <c r="AR151" s="173"/>
+      <c r="AS151" s="173"/>
+      <c r="AT151" s="173"/>
+      <c r="AU151" s="173"/>
+      <c r="AV151" s="173"/>
+      <c r="AW151" s="173"/>
+      <c r="AX151" s="173"/>
+      <c r="AY151" s="173"/>
+      <c r="AZ151" s="174"/>
       <c r="BA151" s="42"/>
       <c r="BB151" s="42"/>
       <c r="BC151" s="42"/>
@@ -24781,20 +24781,20 @@
       <c r="AL152" s="42"/>
       <c r="AM152" s="42"/>
       <c r="AN152" s="42"/>
-      <c r="AO152" s="222" t="s">
+      <c r="AO152" s="159" t="s">
         <v>609</v>
       </c>
-      <c r="AP152" s="221"/>
-      <c r="AQ152" s="221"/>
-      <c r="AR152" s="221"/>
-      <c r="AS152" s="223"/>
-      <c r="AT152" s="221"/>
-      <c r="AU152" s="221"/>
-      <c r="AV152" s="221"/>
-      <c r="AW152" s="221"/>
-      <c r="AX152" s="221"/>
-      <c r="AY152" s="221"/>
-      <c r="AZ152" s="224"/>
+      <c r="AP152" s="158"/>
+      <c r="AQ152" s="158"/>
+      <c r="AR152" s="158"/>
+      <c r="AS152" s="160"/>
+      <c r="AT152" s="158"/>
+      <c r="AU152" s="158"/>
+      <c r="AV152" s="158"/>
+      <c r="AW152" s="158"/>
+      <c r="AX152" s="158"/>
+      <c r="AY152" s="158"/>
+      <c r="AZ152" s="161"/>
       <c r="BA152" s="42"/>
       <c r="BB152" s="42"/>
       <c r="BC152" s="42"/>
@@ -24966,24 +24966,24 @@
       <c r="AJ155" s="42"/>
       <c r="AK155" s="42"/>
       <c r="AL155" s="42"/>
-      <c r="AM155" s="198" t="s">
+      <c r="AM155" s="170" t="s">
         <v>610</v>
       </c>
-      <c r="AN155" s="199"/>
-      <c r="AO155" s="159" t="s">
+      <c r="AN155" s="171"/>
+      <c r="AO155" s="172" t="s">
         <v>592</v>
       </c>
-      <c r="AP155" s="160"/>
-      <c r="AQ155" s="160"/>
-      <c r="AR155" s="160"/>
-      <c r="AS155" s="160"/>
-      <c r="AT155" s="160"/>
-      <c r="AU155" s="160"/>
-      <c r="AV155" s="160"/>
-      <c r="AW155" s="160"/>
-      <c r="AX155" s="160"/>
-      <c r="AY155" s="160"/>
-      <c r="AZ155" s="177"/>
+      <c r="AP155" s="173"/>
+      <c r="AQ155" s="173"/>
+      <c r="AR155" s="173"/>
+      <c r="AS155" s="173"/>
+      <c r="AT155" s="173"/>
+      <c r="AU155" s="173"/>
+      <c r="AV155" s="173"/>
+      <c r="AW155" s="173"/>
+      <c r="AX155" s="173"/>
+      <c r="AY155" s="173"/>
+      <c r="AZ155" s="174"/>
       <c r="BA155" s="42"/>
       <c r="BB155" s="42"/>
       <c r="BC155" s="42"/>
@@ -25033,20 +25033,20 @@
       <c r="AL156" s="42"/>
       <c r="AM156" s="42"/>
       <c r="AN156" s="42"/>
-      <c r="AO156" s="222" t="s">
+      <c r="AO156" s="159" t="s">
         <v>611</v>
       </c>
-      <c r="AP156" s="221"/>
-      <c r="AQ156" s="221"/>
-      <c r="AR156" s="221"/>
-      <c r="AS156" s="223"/>
-      <c r="AT156" s="221"/>
-      <c r="AU156" s="221"/>
-      <c r="AV156" s="221"/>
-      <c r="AW156" s="221"/>
-      <c r="AX156" s="221"/>
-      <c r="AY156" s="221"/>
-      <c r="AZ156" s="224"/>
+      <c r="AP156" s="158"/>
+      <c r="AQ156" s="158"/>
+      <c r="AR156" s="158"/>
+      <c r="AS156" s="160"/>
+      <c r="AT156" s="158"/>
+      <c r="AU156" s="158"/>
+      <c r="AV156" s="158"/>
+      <c r="AW156" s="158"/>
+      <c r="AX156" s="158"/>
+      <c r="AY156" s="158"/>
+      <c r="AZ156" s="161"/>
       <c r="BA156" s="42"/>
       <c r="BB156" s="42"/>
       <c r="BC156" s="42"/>
@@ -25218,24 +25218,24 @@
       <c r="AJ159" s="42"/>
       <c r="AK159" s="42"/>
       <c r="AL159" s="42"/>
-      <c r="AM159" s="198" t="s">
+      <c r="AM159" s="170" t="s">
         <v>612</v>
       </c>
-      <c r="AN159" s="199"/>
-      <c r="AO159" s="159" t="s">
+      <c r="AN159" s="171"/>
+      <c r="AO159" s="172" t="s">
         <v>613</v>
       </c>
-      <c r="AP159" s="160"/>
-      <c r="AQ159" s="160"/>
-      <c r="AR159" s="160"/>
-      <c r="AS159" s="160"/>
-      <c r="AT159" s="160"/>
-      <c r="AU159" s="160"/>
-      <c r="AV159" s="160"/>
-      <c r="AW159" s="160"/>
-      <c r="AX159" s="160"/>
-      <c r="AY159" s="160"/>
-      <c r="AZ159" s="177"/>
+      <c r="AP159" s="173"/>
+      <c r="AQ159" s="173"/>
+      <c r="AR159" s="173"/>
+      <c r="AS159" s="173"/>
+      <c r="AT159" s="173"/>
+      <c r="AU159" s="173"/>
+      <c r="AV159" s="173"/>
+      <c r="AW159" s="173"/>
+      <c r="AX159" s="173"/>
+      <c r="AY159" s="173"/>
+      <c r="AZ159" s="174"/>
       <c r="BA159" s="42"/>
       <c r="BB159" s="42"/>
       <c r="BC159" s="42"/>
@@ -25285,20 +25285,20 @@
       <c r="AL160" s="42"/>
       <c r="AM160" s="42"/>
       <c r="AN160" s="42"/>
-      <c r="AO160" s="222" t="s">
-        <v>614</v>
-      </c>
-      <c r="AP160" s="221"/>
-      <c r="AQ160" s="221"/>
-      <c r="AR160" s="221"/>
-      <c r="AS160" s="223"/>
-      <c r="AT160" s="221"/>
-      <c r="AU160" s="221"/>
-      <c r="AV160" s="221"/>
-      <c r="AW160" s="221"/>
-      <c r="AX160" s="221"/>
-      <c r="AY160" s="221"/>
-      <c r="AZ160" s="224"/>
+      <c r="AO160" s="159" t="s">
+        <v>618</v>
+      </c>
+      <c r="AP160" s="158"/>
+      <c r="AQ160" s="158"/>
+      <c r="AR160" s="158"/>
+      <c r="AS160" s="160"/>
+      <c r="AT160" s="158"/>
+      <c r="AU160" s="158"/>
+      <c r="AV160" s="158"/>
+      <c r="AW160" s="158"/>
+      <c r="AX160" s="158"/>
+      <c r="AY160" s="158"/>
+      <c r="AZ160" s="161"/>
       <c r="BA160" s="42"/>
       <c r="BB160" s="42"/>
       <c r="BC160" s="42"/>
@@ -25349,7 +25349,7 @@
       <c r="AM161" s="42"/>
       <c r="AN161" s="42"/>
       <c r="AO161" s="67" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="AP161" s="70"/>
       <c r="AQ161" s="70"/>
@@ -25412,7 +25412,7 @@
       <c r="AM162" s="42"/>
       <c r="AN162" s="42"/>
       <c r="AO162" s="67" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="AP162" s="70"/>
       <c r="AQ162" s="70"/>
@@ -25533,24 +25533,24 @@
       <c r="AJ164" s="42"/>
       <c r="AK164" s="42"/>
       <c r="AL164" s="42"/>
-      <c r="AM164" s="198" t="s">
-        <v>617</v>
-      </c>
-      <c r="AN164" s="199"/>
-      <c r="AO164" s="159" t="s">
-        <v>618</v>
-      </c>
-      <c r="AP164" s="160"/>
-      <c r="AQ164" s="160"/>
-      <c r="AR164" s="160"/>
-      <c r="AS164" s="160"/>
-      <c r="AT164" s="160"/>
-      <c r="AU164" s="160"/>
-      <c r="AV164" s="160"/>
-      <c r="AW164" s="160"/>
-      <c r="AX164" s="160"/>
-      <c r="AY164" s="160"/>
-      <c r="AZ164" s="177"/>
+      <c r="AM164" s="170" t="s">
+        <v>614</v>
+      </c>
+      <c r="AN164" s="171"/>
+      <c r="AO164" s="172" t="s">
+        <v>615</v>
+      </c>
+      <c r="AP164" s="173"/>
+      <c r="AQ164" s="173"/>
+      <c r="AR164" s="173"/>
+      <c r="AS164" s="173"/>
+      <c r="AT164" s="173"/>
+      <c r="AU164" s="173"/>
+      <c r="AV164" s="173"/>
+      <c r="AW164" s="173"/>
+      <c r="AX164" s="173"/>
+      <c r="AY164" s="173"/>
+      <c r="AZ164" s="174"/>
       <c r="BA164" s="42"/>
       <c r="BB164" s="42"/>
       <c r="BC164" s="42"/>
@@ -25600,20 +25600,20 @@
       <c r="AL165" s="42"/>
       <c r="AM165" s="42"/>
       <c r="AN165" s="42"/>
-      <c r="AO165" s="222" t="s">
-        <v>619</v>
-      </c>
-      <c r="AP165" s="221"/>
-      <c r="AQ165" s="221"/>
-      <c r="AR165" s="221"/>
-      <c r="AS165" s="223"/>
-      <c r="AT165" s="221"/>
-      <c r="AU165" s="221"/>
-      <c r="AV165" s="221"/>
-      <c r="AW165" s="221"/>
-      <c r="AX165" s="221"/>
-      <c r="AY165" s="221"/>
-      <c r="AZ165" s="224"/>
+      <c r="AO165" s="159" t="s">
+        <v>617</v>
+      </c>
+      <c r="AP165" s="158"/>
+      <c r="AQ165" s="158"/>
+      <c r="AR165" s="158"/>
+      <c r="AS165" s="160"/>
+      <c r="AT165" s="158"/>
+      <c r="AU165" s="158"/>
+      <c r="AV165" s="158"/>
+      <c r="AW165" s="158"/>
+      <c r="AX165" s="158"/>
+      <c r="AY165" s="158"/>
+      <c r="AZ165" s="161"/>
       <c r="BA165" s="42"/>
       <c r="BB165" s="42"/>
       <c r="BC165" s="42"/>
@@ -28110,16 +28110,188 @@
     </row>
   </sheetData>
   <mergeCells count="216">
-    <mergeCell ref="AM147:AN147"/>
-    <mergeCell ref="AO147:AZ147"/>
-    <mergeCell ref="AM151:AN151"/>
-    <mergeCell ref="AO151:AZ151"/>
-    <mergeCell ref="AM155:AN155"/>
-    <mergeCell ref="AO155:AZ155"/>
-    <mergeCell ref="AM159:AN159"/>
-    <mergeCell ref="AO159:AZ159"/>
-    <mergeCell ref="AM164:AN164"/>
-    <mergeCell ref="AO164:AZ164"/>
+    <mergeCell ref="AX23:AY23"/>
+    <mergeCell ref="L110:N110"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="AB30:AD30"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="AD25:AF25"/>
+    <mergeCell ref="L15:AF15"/>
+    <mergeCell ref="N16:AF16"/>
+    <mergeCell ref="P17:AF17"/>
+    <mergeCell ref="P18:AF18"/>
+    <mergeCell ref="E108:K108"/>
+    <mergeCell ref="L108:N108"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="Z23:AF23"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="E56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="AX41:AY41"/>
+    <mergeCell ref="AZ41:BA41"/>
+    <mergeCell ref="BB41:BD41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="AE42:AF42"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="Z6:AE6"/>
+    <mergeCell ref="AZ23:BF23"/>
+    <mergeCell ref="BB24:BF24"/>
+    <mergeCell ref="BD25:BF25"/>
+    <mergeCell ref="AL15:BF15"/>
+    <mergeCell ref="AN16:BF16"/>
+    <mergeCell ref="AP17:BF17"/>
+    <mergeCell ref="AP18:BF18"/>
+    <mergeCell ref="AX22:BF22"/>
+    <mergeCell ref="AJ15:AK15"/>
+    <mergeCell ref="AV22:AW22"/>
+    <mergeCell ref="AH15:AI15"/>
+    <mergeCell ref="AJ16:AK16"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AX46:BD46"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="G46:AE46"/>
+    <mergeCell ref="AH46:AS46"/>
+    <mergeCell ref="AT46:AU46"/>
+    <mergeCell ref="X44:AE44"/>
+    <mergeCell ref="AH44:AS44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:BD44"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="AT45:AU45"/>
+    <mergeCell ref="H44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="AT41:AU41"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AT22:AU22"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AG40:AH40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AD39:AF39"/>
+    <mergeCell ref="AG39:AH39"/>
+    <mergeCell ref="AH41:AI41"/>
+    <mergeCell ref="AJ41:AK41"/>
+    <mergeCell ref="AL41:AM41"/>
+    <mergeCell ref="AN41:AO41"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="AX33:BD33"/>
+    <mergeCell ref="X33:AE33"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="AV33:AW33"/>
+    <mergeCell ref="AT34:AU34"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="AH33:AS33"/>
+    <mergeCell ref="AN39:AO39"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="BB30:BD30"/>
+    <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="R108:AC108"/>
+    <mergeCell ref="AL108:AN108"/>
+    <mergeCell ref="AL106:AN106"/>
+    <mergeCell ref="AD106:AK106"/>
+    <mergeCell ref="AD108:AK108"/>
+    <mergeCell ref="R106:AC106"/>
+    <mergeCell ref="AM120:AN120"/>
+    <mergeCell ref="AO120:AZ120"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E106:K106"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="AV46:AW46"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE30:AF30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="AM140:AN140"/>
     <mergeCell ref="AM143:AN143"/>
     <mergeCell ref="AO140:AZ140"/>
@@ -28144,188 +28316,16 @@
     <mergeCell ref="AO115:AZ115"/>
     <mergeCell ref="O106:Q106"/>
     <mergeCell ref="O108:Q108"/>
-    <mergeCell ref="R108:AC108"/>
-    <mergeCell ref="AL108:AN108"/>
-    <mergeCell ref="AL106:AN106"/>
-    <mergeCell ref="AD106:AK106"/>
-    <mergeCell ref="AD108:AK108"/>
-    <mergeCell ref="R106:AC106"/>
-    <mergeCell ref="AM120:AN120"/>
-    <mergeCell ref="AO120:AZ120"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E106:K106"/>
-    <mergeCell ref="L106:N106"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="AV46:AW46"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="BB30:BD30"/>
-    <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="AX33:BD33"/>
-    <mergeCell ref="X33:AE33"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="AV33:AW33"/>
-    <mergeCell ref="AT34:AU34"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="AH33:AS33"/>
-    <mergeCell ref="AN39:AO39"/>
-    <mergeCell ref="AP39:AQ39"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL39:AM39"/>
-    <mergeCell ref="AG40:AH40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AD39:AF39"/>
-    <mergeCell ref="AG39:AH39"/>
-    <mergeCell ref="AH41:AI41"/>
-    <mergeCell ref="AJ41:AK41"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AN41:AO41"/>
-    <mergeCell ref="AT41:AU41"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="AX46:BD46"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="G46:AE46"/>
-    <mergeCell ref="AH46:AS46"/>
-    <mergeCell ref="AT46:AU46"/>
-    <mergeCell ref="X44:AE44"/>
-    <mergeCell ref="AH44:AS44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:BD44"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="AT45:AU45"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="AX41:AY41"/>
-    <mergeCell ref="AZ41:BA41"/>
-    <mergeCell ref="BB41:BD41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="E108:K108"/>
-    <mergeCell ref="L108:N108"/>
-    <mergeCell ref="E54:K54"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="Z6:AE6"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="Z23:AF23"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="E56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L110:N110"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="AZ23:BF23"/>
-    <mergeCell ref="BB24:BF24"/>
-    <mergeCell ref="BD25:BF25"/>
-    <mergeCell ref="AD25:AF25"/>
-    <mergeCell ref="L15:AF15"/>
-    <mergeCell ref="N16:AF16"/>
-    <mergeCell ref="P17:AF17"/>
-    <mergeCell ref="P18:AF18"/>
-    <mergeCell ref="AL15:BF15"/>
-    <mergeCell ref="AN16:BF16"/>
-    <mergeCell ref="AP17:BF17"/>
-    <mergeCell ref="AP18:BF18"/>
-    <mergeCell ref="AX22:BF22"/>
-    <mergeCell ref="AJ15:AK15"/>
-    <mergeCell ref="AV22:AW22"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AT22:AU22"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AX23:AY23"/>
+    <mergeCell ref="AM147:AN147"/>
+    <mergeCell ref="AO147:AZ147"/>
+    <mergeCell ref="AM151:AN151"/>
+    <mergeCell ref="AO151:AZ151"/>
+    <mergeCell ref="AM155:AN155"/>
+    <mergeCell ref="AO155:AZ155"/>
+    <mergeCell ref="AM159:AN159"/>
+    <mergeCell ref="AO159:AZ159"/>
+    <mergeCell ref="AM164:AN164"/>
+    <mergeCell ref="AO164:AZ164"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>